<commit_message>
e-Questrian/pages/landing: Whats new section added - content needs to be added
</commit_message>
<xml_diff>
--- a/apps/e-questrian/e-Questrian - To do list.xlsx
+++ b/apps/e-questrian/e-Questrian - To do list.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rferreira/sigmafox/apps/e-questrian/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6D20C18-69A1-9B43-89B5-BC8ECC7766F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50D5CC8A-2550-304E-9168-C1A9D5E635F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="740" windowWidth="34560" windowHeight="21600" activeTab="2" xr2:uid="{DC2B379E-A936-2146-8C4F-53C43AECE05C}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="19820" activeTab="2" xr2:uid="{DC2B379E-A936-2146-8C4F-53C43AECE05C}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary of completion" sheetId="3" r:id="rId1"/>
@@ -22,7 +22,7 @@
   </definedNames>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="10" r:id="rId4"/>
+    <pivotCache cacheId="4" r:id="rId4"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="859" uniqueCount="215">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="860" uniqueCount="215">
   <si>
     <t>Sections</t>
   </si>
@@ -812,7 +812,7 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Ruben Ferreira" refreshedDate="45309.547474074076" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="117" xr:uid="{AEB2BF63-68F2-404E-AE9B-E794DFB00774}">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Ruben Ferreira" refreshedDate="45310.2627931713" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="117" xr:uid="{AEB2BF63-68F2-404E-AE9B-E794DFB00774}">
   <cacheSource type="worksheet">
     <worksheetSource ref="A1:M1048576" sheet="Issues 3-1-24"/>
   </cacheSource>
@@ -871,6 +871,246 @@
 <file path=xl/pivotCache/pivotCacheRecords1.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" count="117">
   <r>
+    <n v="53"/>
+    <s v="Calendar/Appointments"/>
+    <s v="Appointments modal"/>
+    <s v="Cancelling/Voiding"/>
+    <s v="If an appointment is cancelled but that have been previously invoiced - then this needs to be credit noted"/>
+    <s v="Does not function as expected"/>
+    <s v="USP"/>
+    <s v="Major change to current component"/>
+    <n v="8"/>
+    <n v="10"/>
+    <n v="200"/>
+    <n v="77"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <n v="6"/>
+    <s v="Navbar"/>
+    <s v="Login Button"/>
+    <m/>
+    <s v="Should be added to Navbar"/>
+    <s v="Poor UX"/>
+    <s v="New feature"/>
+    <s v="Minor change to current component"/>
+    <n v="4"/>
+    <n v="7"/>
+    <n v="98"/>
+    <n v="1"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <n v="77"/>
+    <s v="Finance - Payments"/>
+    <s v="Payment modal"/>
+    <m/>
+    <s v="Voiding payments does not work"/>
+    <s v="Does not function as expected"/>
+    <s v="Feature enhancement/fix"/>
+    <s v="Investigation and change"/>
+    <n v="8"/>
+    <n v="6"/>
+    <n v="96"/>
+    <m/>
+    <x v="0"/>
+  </r>
+  <r>
+    <n v="90"/>
+    <s v="Clients"/>
+    <s v="Client modal"/>
+    <m/>
+    <s v="Remove client is not working"/>
+    <s v="Does not function as expected"/>
+    <s v="Feature enhancement/fix"/>
+    <s v="Investigation and change"/>
+    <n v="8"/>
+    <n v="6"/>
+    <n v="96"/>
+    <m/>
+    <x v="0"/>
+  </r>
+  <r>
+    <n v="112"/>
+    <s v="Finance - Reports"/>
+    <s v="Statement runs"/>
+    <m/>
+    <s v="Statements do not show credit notes (where required)"/>
+    <s v="Does not function as expected"/>
+    <s v="Feature enhancement/fix"/>
+    <s v="Investigation and change"/>
+    <n v="8"/>
+    <n v="6"/>
+    <n v="96"/>
+    <n v="53"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <n v="114"/>
+    <s v="Finance - Payments"/>
+    <s v="Payment modal"/>
+    <m/>
+    <s v="Payment are not being recorded correctly "/>
+    <s v="Does not function as expected"/>
+    <s v="Feature enhancement/fix"/>
+    <s v="Investigation and change"/>
+    <n v="8"/>
+    <n v="6"/>
+    <n v="96"/>
+    <m/>
+    <x v="0"/>
+  </r>
+  <r>
+    <n v="45"/>
+    <s v="Calendar/Appointments"/>
+    <s v="Calendar"/>
+    <s v="Date picker"/>
+    <s v="Should have a date picker at the top of the calendar"/>
+    <s v="Poor UX"/>
+    <s v="Feature enhancement/fix"/>
+    <s v="Minor change to current component"/>
+    <n v="4"/>
+    <n v="6"/>
+    <n v="72"/>
+    <m/>
+    <x v="0"/>
+  </r>
+  <r>
+    <n v="116"/>
+    <s v="Marketing"/>
+    <s v="Landing Page"/>
+    <s v="Our Features Section"/>
+    <s v="Update content for the features section of the landing page"/>
+    <s v="Poor UX"/>
+    <s v="Feature enhancement/fix"/>
+    <s v="Minor change to current component"/>
+    <n v="4"/>
+    <n v="6"/>
+    <n v="72"/>
+    <n v="2"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <n v="32"/>
+    <s v="Navbar"/>
+    <s v="Logo "/>
+    <m/>
+    <s v="On hovering the logo the cursor should be pointer"/>
+    <s v="Poor UX"/>
+    <s v="Improved UX"/>
+    <s v="Minor tweak"/>
+    <n v="4"/>
+    <n v="4"/>
+    <n v="64"/>
+    <m/>
+    <x v="0"/>
+  </r>
+  <r>
+    <n v="113"/>
+    <s v="Login/Register"/>
+    <s v="Register modal"/>
+    <m/>
+    <s v="Needs to be a modal specfically for registrations"/>
+    <s v="Does not function as expected"/>
+    <s v="Feature enhancement/fix"/>
+    <s v="New component/service with simple integration"/>
+    <n v="8"/>
+    <n v="6"/>
+    <n v="57.6"/>
+    <m/>
+    <x v="0"/>
+  </r>
+  <r>
+    <n v="25"/>
+    <s v="User Management"/>
+    <s v="Sign in Modal"/>
+    <m/>
+    <s v="After trying to register (and assuming it fails) and attempts in future to sign in will result in a registration attempt"/>
+    <s v="Breaks App"/>
+    <s v="Improved UX"/>
+    <s v="Investigation and change"/>
+    <n v="10"/>
+    <n v="4"/>
+    <n v="53.333333333333336"/>
+    <m/>
+    <x v="0"/>
+  </r>
+  <r>
+    <n v="59"/>
+    <s v="Finance - Invoicing"/>
+    <s v="Invoice view"/>
+    <m/>
+    <s v="The detail should reference the instructor"/>
+    <s v="Nice to have"/>
+    <s v="USP"/>
+    <s v="Minor change to current component"/>
+    <n v="1"/>
+    <n v="10"/>
+    <n v="50"/>
+    <n v="60"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <n v="60"/>
+    <s v="Calendar/Appointments"/>
+    <s v="Appointments modal"/>
+    <m/>
+    <s v="New appointments should be able select an instructor"/>
+    <s v="Nice to have"/>
+    <s v="USP"/>
+    <s v="Minor change to current component"/>
+    <n v="1"/>
+    <n v="10"/>
+    <n v="50"/>
+    <n v="62"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <n v="61"/>
+    <s v="Calendar/Appointments"/>
+    <s v="Appointments modal"/>
+    <m/>
+    <s v="New appointments should be able select an horse"/>
+    <s v="Nice to have"/>
+    <s v="USP"/>
+    <s v="Minor change to current component"/>
+    <n v="1"/>
+    <n v="10"/>
+    <n v="50"/>
+    <n v="63"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <n v="64"/>
+    <s v="Finance - Invoicing"/>
+    <s v="Invoice view"/>
+    <m/>
+    <s v="The detail should reference the horse"/>
+    <s v="Nice to have"/>
+    <s v="USP"/>
+    <s v="Minor change to current component"/>
+    <n v="1"/>
+    <n v="10"/>
+    <n v="50"/>
+    <n v="61"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <n v="40"/>
+    <s v="Calendar/Appointments"/>
+    <s v="Calendar"/>
+    <m/>
+    <s v="Not able to scroll down the calendar when required"/>
+    <s v="Does not function as expected"/>
+    <s v="Improved UX"/>
+    <s v="Investigation and change"/>
+    <n v="8"/>
+    <n v="4"/>
+    <n v="42.666666666666664"/>
+    <m/>
+    <x v="0"/>
+  </r>
+  <r>
     <n v="1"/>
     <s v="Marketing"/>
     <s v="Landing Page"/>
@@ -889,7 +1129,7 @@
     <n v="2"/>
     <s v="Marketing"/>
     <s v="Landing Page"/>
-    <s v="Our Features Section"/>
+    <s v="Features Section"/>
     <s v="Should be added to Landing page"/>
     <s v="Poor UX"/>
     <s v="New feature"/>
@@ -913,7 +1153,7 @@
     <n v="7"/>
     <n v="39.200000000000003"/>
     <m/>
-    <x v="1"/>
+    <x v="0"/>
   </r>
   <r>
     <n v="5"/>
@@ -931,19 +1171,34 @@
     <x v="1"/>
   </r>
   <r>
-    <n v="6"/>
-    <s v="Navbar"/>
-    <s v="Login Button"/>
-    <m/>
-    <s v="Should be added to Navbar"/>
+    <n v="18"/>
+    <s v="Marketing"/>
+    <s v="Landing Page"/>
+    <s v="What's New Section"/>
+    <s v="Should be added to Landing page"/>
     <s v="Poor UX"/>
     <s v="New feature"/>
-    <s v="Minor change to current component"/>
+    <s v="New component/service with simple integration"/>
     <n v="4"/>
     <n v="7"/>
-    <n v="98"/>
-    <n v="1"/>
-    <x v="0"/>
+    <n v="39.200000000000003"/>
+    <m/>
+    <x v="1"/>
+  </r>
+  <r>
+    <n v="24"/>
+    <s v="User Management"/>
+    <s v="Sign in Modal"/>
+    <s v="User details modal"/>
+    <s v="After registering - User should be presented with a basis users detail form with:_x000a_First name_x000a_Last name_x000a_Contact number_x000a_User should also presented the option to skip_x000a_Should be place on top of the main menu page (for now - will be replaced by dash board)"/>
+    <s v="Poor UX"/>
+    <s v="New feature"/>
+    <s v="New component/service with simple integration"/>
+    <n v="4"/>
+    <n v="7"/>
+    <n v="39.200000000000003"/>
+    <m/>
+    <x v="1"/>
   </r>
   <r>
     <n v="7"/>
@@ -957,21 +1212,6 @@
     <n v="4"/>
     <n v="4"/>
     <n v="32"/>
-    <m/>
-    <x v="1"/>
-  </r>
-  <r>
-    <n v="8"/>
-    <s v="User Management"/>
-    <s v="Sign in Modal"/>
-    <s v="Login error warnings"/>
-    <s v="Error modals"/>
-    <s v="Poor UX"/>
-    <s v="New feature"/>
-    <s v="New component/service with complex integration"/>
-    <n v="4"/>
-    <n v="7"/>
-    <n v="28"/>
     <m/>
     <x v="1"/>
   </r>
@@ -1096,111 +1336,6 @@
     <x v="1"/>
   </r>
   <r>
-    <n v="17"/>
-    <s v="User Management"/>
-    <s v="Sign in Modal"/>
-    <s v="Forgot password"/>
-    <s v="No way for users to reset forgotten passwords"/>
-    <s v="Poor UX"/>
-    <s v="Feature enhancement/fix"/>
-    <s v="New component/service with complex integration"/>
-    <n v="4"/>
-    <n v="6"/>
-    <n v="20.571428571428573"/>
-    <m/>
-    <x v="1"/>
-  </r>
-  <r>
-    <n v="18"/>
-    <s v="User Management"/>
-    <s v="Sign in Modal"/>
-    <s v="Forgot password"/>
-    <s v="Third party login - Facebook"/>
-    <s v="Poor UX"/>
-    <s v="Feature enhancement/fix"/>
-    <s v="New component/service with complex integration"/>
-    <n v="4"/>
-    <n v="6"/>
-    <n v="20.571428571428573"/>
-    <m/>
-    <x v="1"/>
-  </r>
-  <r>
-    <n v="57"/>
-    <s v="Marketing"/>
-    <s v="Landing Page"/>
-    <s v="What's New Section"/>
-    <s v="Should be added to Landing page"/>
-    <s v="Poor UX"/>
-    <s v="New feature"/>
-    <s v="New component/service with simple integration"/>
-    <n v="4"/>
-    <n v="7"/>
-    <n v="39.200000000000003"/>
-    <m/>
-    <x v="1"/>
-  </r>
-  <r>
-    <n v="19"/>
-    <s v="User Management"/>
-    <s v="Sign in Modal"/>
-    <s v="Forgot password"/>
-    <s v="Third party login - Google"/>
-    <s v="Poor UX"/>
-    <s v="Feature enhancement/fix"/>
-    <s v="New component/service with complex integration"/>
-    <n v="4"/>
-    <n v="6"/>
-    <n v="20.571428571428573"/>
-    <m/>
-    <x v="1"/>
-  </r>
-  <r>
-    <n v="20"/>
-    <s v="User Management"/>
-    <s v="Sign in Modal"/>
-    <s v="Forgot password"/>
-    <s v="Third party login - LinkedIn"/>
-    <s v="Poor UX"/>
-    <s v="Feature enhancement/fix"/>
-    <s v="New component/service with complex integration"/>
-    <n v="4"/>
-    <n v="6"/>
-    <n v="20.571428571428573"/>
-    <m/>
-    <x v="1"/>
-  </r>
-  <r>
-    <n v="21"/>
-    <s v="User Management"/>
-    <s v="Sign in Modal"/>
-    <s v="Forgot password"/>
-    <s v="Third party login - Microsoft"/>
-    <s v="Poor UX"/>
-    <s v="Feature enhancement/fix"/>
-    <s v="New component/service with complex integration"/>
-    <n v="4"/>
-    <n v="6"/>
-    <n v="20.571428571428573"/>
-    <m/>
-    <x v="1"/>
-  </r>
-  <r>
-    <n v="22"/>
-    <s v="User Management"/>
-    <s v="Sign in Modal"/>
-    <m/>
-    <s v="On small devices the inputs on the modal are mis-aligned (Use 340*635 spec)"/>
-    <s v="Poor UI"/>
-    <s v="Improved UI"/>
-    <s v="Minor tweak"/>
-    <n v="3"/>
-    <n v="3"/>
-    <n v="27"/>
-    <m/>
-    <x v="1"/>
-  </r>
-  <r>
     <n v="23"/>
     <s v="User Management"/>
     <s v="Register modal"/>
@@ -1216,111 +1351,6 @@
     <x v="1"/>
   </r>
   <r>
-    <n v="24"/>
-    <s v="User Management"/>
-    <s v="Sign in Modal"/>
-    <s v="User details modal"/>
-    <s v="After registering - User should be presented with a basis users detail form with:_x000a_First name_x000a_Last name_x000a_Contact number_x000a_User should also presented the option to skip_x000a_Should be place on top of the main menu page (for now - will be replaced by dash board)"/>
-    <s v="Poor UX"/>
-    <s v="New feature"/>
-    <s v="New component/service with simple integration"/>
-    <n v="4"/>
-    <n v="7"/>
-    <n v="39.200000000000003"/>
-    <m/>
-    <x v="1"/>
-  </r>
-  <r>
-    <n v="25"/>
-    <s v="User Management"/>
-    <s v="Sign in Modal"/>
-    <m/>
-    <s v="After trying to register (and assuming it fails) and attempts in future to sign in will result in a registration attempt"/>
-    <s v="Breaks App"/>
-    <s v="Improved UX"/>
-    <s v="Investigation and change"/>
-    <n v="10"/>
-    <n v="4"/>
-    <n v="53.333333333333336"/>
-    <m/>
-    <x v="0"/>
-  </r>
-  <r>
-    <n v="26"/>
-    <s v="Dashboard and Main Menu"/>
-    <s v="Main menu"/>
-    <m/>
-    <s v="As the screen gets wider - the buttons tend to lower - needs to be consistent"/>
-    <s v="Poor UI"/>
-    <s v="Improved UI"/>
-    <s v="Investigation and change"/>
-    <n v="3"/>
-    <n v="3"/>
-    <n v="9"/>
-    <m/>
-    <x v="1"/>
-  </r>
-  <r>
-    <n v="27"/>
-    <s v="General"/>
-    <s v="Utility services"/>
-    <m/>
-    <s v="There needs to be a service that determine whether the view should be mobile or desktop"/>
-    <s v="Poor UI"/>
-    <s v="Refactor/Tech debt"/>
-    <s v="New component/service with complex integration"/>
-    <n v="3"/>
-    <n v="1"/>
-    <n v="0.42857142857142855"/>
-    <m/>
-    <x v="1"/>
-  </r>
-  <r>
-    <n v="28"/>
-    <s v="Dashboard and Main Menu"/>
-    <s v="Main menu"/>
-    <m/>
-    <s v="There should be a view for desktop where the button become a grid of square buttons with icons"/>
-    <s v="Poor UI"/>
-    <s v="Improved UI"/>
-    <s v="Major change to current component"/>
-    <n v="3"/>
-    <n v="3"/>
-    <n v="6.75"/>
-    <m/>
-    <x v="1"/>
-  </r>
-  <r>
-    <n v="29"/>
-    <s v="Dashboard and Main Menu"/>
-    <s v="Main menu"/>
-    <m/>
-    <s v="Needs to use the new view service to determine its required state"/>
-    <s v="Poor UI"/>
-    <s v="Refactor/Tech debt"/>
-    <s v="Minor change to current component"/>
-    <n v="3"/>
-    <n v="1"/>
-    <n v="1.5"/>
-    <n v="27"/>
-    <x v="1"/>
-  </r>
-  <r>
-    <n v="30"/>
-    <s v="Navbar"/>
-    <m/>
-    <m/>
-    <s v="Needs to use the new view service to determine its required state"/>
-    <s v="Poor UI"/>
-    <s v="Refactor/Tech debt"/>
-    <s v="Minor change to current component"/>
-    <n v="3"/>
-    <n v="1"/>
-    <n v="1.5"/>
-    <n v="27"/>
-    <x v="1"/>
-  </r>
-  <r>
     <n v="31"/>
     <s v="Navbar"/>
     <s v="Drop down menu"/>
@@ -1332,36 +1362,6 @@
     <n v="4"/>
     <n v="4"/>
     <n v="32"/>
-    <m/>
-    <x v="1"/>
-  </r>
-  <r>
-    <n v="32"/>
-    <s v="Navbar"/>
-    <s v="Logo "/>
-    <m/>
-    <s v="On hovering the logo the cursor should be pointer"/>
-    <s v="Poor UX"/>
-    <s v="Improved UX"/>
-    <s v="Minor tweak"/>
-    <n v="4"/>
-    <n v="4"/>
-    <n v="64"/>
-    <m/>
-    <x v="0"/>
-  </r>
-  <r>
-    <n v="33"/>
-    <s v="Dashboard and Main Menu"/>
-    <s v="Dashboard"/>
-    <m/>
-    <s v="New page: Dashboard_x000a_Should only be available on desktop_x000a_Should have a option to go to the main menu_x000a_Will contain a variety of reports and summaries"/>
-    <s v="Nice to have"/>
-    <s v="USP"/>
-    <s v="Whole new section"/>
-    <n v="1"/>
-    <n v="10"/>
-    <n v="10"/>
     <m/>
     <x v="1"/>
   </r>
@@ -1381,291 +1381,6 @@
     <x v="1"/>
   </r>
   <r>
-    <n v="35"/>
-    <s v="Navbar"/>
-    <s v="Drop down menu"/>
-    <m/>
-    <s v="Should not down the screen - but should hover above the current screen content"/>
-    <s v="Poor UI"/>
-    <s v="Improved UI"/>
-    <s v="Minor change to current component"/>
-    <n v="3"/>
-    <n v="3"/>
-    <n v="13.5"/>
-    <m/>
-    <x v="1"/>
-  </r>
-  <r>
-    <n v="36"/>
-    <s v="Dashboard and Main Menu"/>
-    <s v="Main menu"/>
-    <s v="Log out"/>
-    <s v="On clicking logout - should warn user before doing so"/>
-    <s v="Poor UX"/>
-    <s v="Improved UX"/>
-    <s v="New component/service with simple integration"/>
-    <n v="4"/>
-    <n v="4"/>
-    <n v="12.8"/>
-    <m/>
-    <x v="1"/>
-  </r>
-  <r>
-    <n v="37"/>
-    <s v="Navbar"/>
-    <s v="Drop down menu"/>
-    <s v="Log out"/>
-    <s v="On clicking logout - should warn user before doing so"/>
-    <s v="Poor UX"/>
-    <s v="Improved UX"/>
-    <s v="New component/service with simple integration"/>
-    <n v="4"/>
-    <n v="4"/>
-    <n v="12.8"/>
-    <m/>
-    <x v="1"/>
-  </r>
-  <r>
-    <n v="38"/>
-    <s v="Calendar/Appointments"/>
-    <s v="Calendar"/>
-    <m/>
-    <s v="On taller screens - the schedule slots should be have a great height to fill the remainder of the screen"/>
-    <s v="Poor UI"/>
-    <s v="Improved UI"/>
-    <s v="Minor change to current component"/>
-    <n v="3"/>
-    <n v="3"/>
-    <n v="13.5"/>
-    <m/>
-    <x v="1"/>
-  </r>
-  <r>
-    <n v="39"/>
-    <s v="Calendar/Appointments"/>
-    <s v="Calendar"/>
-    <m/>
-    <s v="On shorter screens - Schedule slot should have a minimum height"/>
-    <s v="Poor UI"/>
-    <s v="Improved UI"/>
-    <s v="Investigation and change"/>
-    <n v="3"/>
-    <n v="3"/>
-    <n v="9"/>
-    <m/>
-    <x v="1"/>
-  </r>
-  <r>
-    <n v="40"/>
-    <s v="Calendar/Appointments"/>
-    <s v="Calendar"/>
-    <m/>
-    <s v="Not able to scroll down the calendar when required"/>
-    <s v="Does not function as expected"/>
-    <s v="Improved UX"/>
-    <s v="Investigation and change"/>
-    <n v="8"/>
-    <n v="4"/>
-    <n v="42.666666666666664"/>
-    <m/>
-    <x v="0"/>
-  </r>
-  <r>
-    <n v="41"/>
-    <s v="Calendar/Appointments"/>
-    <s v="Calendar"/>
-    <s v="Your calendar drop down"/>
-    <s v="The your calendar header should be a drop down that allows the user to see other staff members calendars_x000a_The drop down menu should be multi select_x000a_The differently coloured appointment blocks should have a border indicating whose calendar the appointment is from_x000a_"/>
-    <s v="Nice to have"/>
-    <s v="USP"/>
-    <s v="Whole new feature"/>
-    <n v="1"/>
-    <n v="10"/>
-    <n v="12.5"/>
-    <m/>
-    <x v="1"/>
-  </r>
-  <r>
-    <n v="42"/>
-    <s v="Calendar/Appointments"/>
-    <s v="Appointments modal"/>
-    <m/>
-    <s v="On smaller screens the Date input is too far right"/>
-    <s v="Poor UI"/>
-    <s v="Improved UI"/>
-    <s v="Investigation and change"/>
-    <n v="3"/>
-    <n v="3"/>
-    <n v="9"/>
-    <m/>
-    <x v="1"/>
-  </r>
-  <r>
-    <n v="43"/>
-    <s v="Calendar/Appointments"/>
-    <s v="Calendar"/>
-    <m/>
-    <s v="The heights of the appointment blocks should match there duration"/>
-    <s v="Poor UI"/>
-    <s v="Feature enhancement/fix"/>
-    <s v="Major change to current component"/>
-    <n v="3"/>
-    <n v="6"/>
-    <n v="27"/>
-    <m/>
-    <x v="1"/>
-  </r>
-  <r>
-    <n v="44"/>
-    <s v="Calendar/Appointments"/>
-    <s v="Calendar"/>
-    <m/>
-    <s v="When too many appointment in a slot - the blocks become cramped… need to find a more elegant way to stack appointment blocks when there are too many appointments"/>
-    <s v="Poor UI"/>
-    <s v="Feature enhancement/fix"/>
-    <s v="Major change to current component"/>
-    <n v="3"/>
-    <n v="6"/>
-    <n v="27"/>
-    <m/>
-    <x v="1"/>
-  </r>
-  <r>
-    <n v="45"/>
-    <s v="Calendar/Appointments"/>
-    <s v="Calendar"/>
-    <s v="Date picker"/>
-    <s v="Should have a date picker at the top of the calendar"/>
-    <s v="Poor UX"/>
-    <s v="Feature enhancement/fix"/>
-    <s v="Minor change to current component"/>
-    <n v="4"/>
-    <n v="6"/>
-    <n v="72"/>
-    <m/>
-    <x v="0"/>
-  </r>
-  <r>
-    <n v="46"/>
-    <s v="Calendar/Appointments"/>
-    <s v="Appointments modal"/>
-    <m/>
-    <s v="On smaller screen the alignments need to be improved - specifically in the view only mode"/>
-    <s v="Poor UI"/>
-    <s v="Improved UI"/>
-    <s v="Investigation and change"/>
-    <n v="3"/>
-    <n v="3"/>
-    <n v="9"/>
-    <m/>
-    <x v="1"/>
-  </r>
-  <r>
-    <n v="47"/>
-    <s v="Calendar/Appointments"/>
-    <s v="Appointments modal"/>
-    <s v="Cancelling/Voiding"/>
-    <s v="Cancelling the appointment should warn the user before the appointment is actually cancelled"/>
-    <s v="Poor UX"/>
-    <s v="Improved UX"/>
-    <s v="New component/service with simple integration"/>
-    <n v="4"/>
-    <n v="4"/>
-    <n v="12.8"/>
-    <m/>
-    <x v="1"/>
-  </r>
-  <r>
-    <n v="48"/>
-    <s v="Calendar/Appointments"/>
-    <s v="Appointments modal"/>
-    <m/>
-    <s v="The cancel changes button on and edited appointment should be darker"/>
-    <s v="Poor UI"/>
-    <s v="Improved UI"/>
-    <s v="Minor tweak"/>
-    <n v="3"/>
-    <n v="3"/>
-    <n v="27"/>
-    <m/>
-    <x v="1"/>
-  </r>
-  <r>
-    <n v="49"/>
-    <s v="Calendar/Appointments"/>
-    <s v="Appointments modal"/>
-    <m/>
-    <s v="When changes are made - the save button appears - but it should always appear - just be disabled"/>
-    <s v="Poor UX"/>
-    <s v="Improved UX"/>
-    <s v="Investigation and change"/>
-    <n v="4"/>
-    <n v="4"/>
-    <n v="21.333333333333332"/>
-    <m/>
-    <x v="1"/>
-  </r>
-  <r>
-    <n v="50"/>
-    <s v="Calendar/Appointments"/>
-    <s v="Appointments modal"/>
-    <s v="Cancelling/Voiding"/>
-    <s v="On cancelling a new appointment (after changes are made) should warn the user that changes will be lost"/>
-    <s v="Poor UX"/>
-    <s v="Improved UX"/>
-    <s v="New component/service with simple integration"/>
-    <n v="4"/>
-    <n v="4"/>
-    <n v="12.8"/>
-    <m/>
-    <x v="1"/>
-  </r>
-  <r>
-    <n v="51"/>
-    <s v="General"/>
-    <s v="Warnings"/>
-    <m/>
-    <s v="Warnings should have an option to allow users to not see them again"/>
-    <s v="Nice to have"/>
-    <s v="New feature"/>
-    <s v="New component/service with complex integration"/>
-    <n v="1"/>
-    <n v="7"/>
-    <n v="7"/>
-    <m/>
-    <x v="1"/>
-  </r>
-  <r>
-    <n v="52"/>
-    <s v="Finance - Payments"/>
-    <s v="Bulk uploads"/>
-    <m/>
-    <s v="Should be able to bulk upload payments_x000a_Should have a standard template_x000a_Should remember the reference - and assign based on that (where this has been seen before)"/>
-    <s v="Nice to have"/>
-    <s v="USP"/>
-    <s v="Whole new feature"/>
-    <n v="1"/>
-    <n v="10"/>
-    <n v="12.5"/>
-    <m/>
-    <x v="1"/>
-  </r>
-  <r>
-    <n v="53"/>
-    <s v="Calendar/Appointments"/>
-    <s v="Appointments modal"/>
-    <s v="Cancelling/Voiding"/>
-    <s v="If an appointment is cancelled but that have been previously invoiced - then this needs to be credit noted"/>
-    <s v="Does not function as expected"/>
-    <s v="USP"/>
-    <s v="Major change to current component"/>
-    <n v="8"/>
-    <n v="10"/>
-    <n v="200"/>
-    <n v="77"/>
-    <x v="0"/>
-  </r>
-  <r>
     <n v="54"/>
     <s v="Calendar/Appointments"/>
     <s v="Appointments modal"/>
@@ -1696,36 +1411,6 @@
     <x v="1"/>
   </r>
   <r>
-    <n v="56"/>
-    <s v="Calendar/Appointments"/>
-    <s v="Appointments modal"/>
-    <m/>
-    <s v="When cancelling an invoiced appoint and additional warning of the credit not needs to be provided"/>
-    <s v="Poor UX"/>
-    <s v="Improved UX"/>
-    <s v="New component/service with simple integration"/>
-    <n v="4"/>
-    <n v="4"/>
-    <n v="12.8"/>
-    <m/>
-    <x v="1"/>
-  </r>
-  <r>
-    <n v="57"/>
-    <s v="Finance - Invoicing"/>
-    <s v="Invoice view"/>
-    <m/>
-    <s v="Lesson (and other sub headings) should be underlined"/>
-    <s v="Poor UI"/>
-    <s v="Improved UI"/>
-    <s v="Minor tweak"/>
-    <n v="3"/>
-    <n v="3"/>
-    <n v="27"/>
-    <m/>
-    <x v="1"/>
-  </r>
-  <r>
     <n v="58"/>
     <s v="Finance - Invoicing"/>
     <s v="Invoice view"/>
@@ -1741,126 +1426,6 @@
     <x v="1"/>
   </r>
   <r>
-    <n v="59"/>
-    <s v="Finance - Invoicing"/>
-    <s v="Invoice view"/>
-    <m/>
-    <s v="The detail should reference the instructor"/>
-    <s v="Nice to have"/>
-    <s v="USP"/>
-    <s v="Minor change to current component"/>
-    <n v="1"/>
-    <n v="10"/>
-    <n v="50"/>
-    <n v="60"/>
-    <x v="1"/>
-  </r>
-  <r>
-    <n v="60"/>
-    <s v="Calendar/Appointments"/>
-    <s v="Appointments modal"/>
-    <m/>
-    <s v="New appointments should be able select an instructor"/>
-    <s v="Nice to have"/>
-    <s v="USP"/>
-    <s v="Minor change to current component"/>
-    <n v="1"/>
-    <n v="10"/>
-    <n v="50"/>
-    <n v="62"/>
-    <x v="1"/>
-  </r>
-  <r>
-    <n v="61"/>
-    <s v="Calendar/Appointments"/>
-    <s v="Appointments modal"/>
-    <m/>
-    <s v="New appointments should be able select an horse"/>
-    <s v="Nice to have"/>
-    <s v="USP"/>
-    <s v="Minor change to current component"/>
-    <n v="1"/>
-    <n v="10"/>
-    <n v="50"/>
-    <n v="63"/>
-    <x v="1"/>
-  </r>
-  <r>
-    <n v="62"/>
-    <s v="Equipment/Assets"/>
-    <m/>
-    <m/>
-    <s v="New section required to add instructor to the client"/>
-    <s v="Nice to have"/>
-    <s v="USP"/>
-    <s v="Whole new section"/>
-    <n v="1"/>
-    <n v="10"/>
-    <n v="10"/>
-    <m/>
-    <x v="1"/>
-  </r>
-  <r>
-    <n v="63"/>
-    <s v="Staff management"/>
-    <m/>
-    <m/>
-    <s v="New section required to add horse to the client"/>
-    <s v="Nice to have"/>
-    <s v="USP"/>
-    <s v="Whole new section"/>
-    <n v="1"/>
-    <n v="10"/>
-    <n v="10"/>
-    <m/>
-    <x v="1"/>
-  </r>
-  <r>
-    <n v="64"/>
-    <s v="Finance - Invoicing"/>
-    <s v="Invoice view"/>
-    <m/>
-    <s v="The detail should reference the horse"/>
-    <s v="Nice to have"/>
-    <s v="USP"/>
-    <s v="Minor change to current component"/>
-    <n v="1"/>
-    <n v="10"/>
-    <n v="50"/>
-    <n v="61"/>
-    <x v="1"/>
-  </r>
-  <r>
-    <n v="65"/>
-    <s v="Finance - Invoicing"/>
-    <s v="PDF export"/>
-    <m/>
-    <s v="Should be able to export the invoice to PDF_x000a_Will required a lot more client and company detail_x000a_Should ask the user where to save it"/>
-    <s v="Nice to have"/>
-    <s v="USP"/>
-    <s v="Whole new feature"/>
-    <n v="1"/>
-    <n v="10"/>
-    <n v="12.5"/>
-    <m/>
-    <x v="1"/>
-  </r>
-  <r>
-    <n v="66"/>
-    <s v="Finance - Invoicing"/>
-    <s v="Invoice view"/>
-    <m/>
-    <s v="On clicking the lesson on the  viewed invoice - Should bring up the appointment modal - with no option to edit"/>
-    <s v="Nice to have"/>
-    <s v="Feature enhancement/fix"/>
-    <s v="Minor change to current component"/>
-    <n v="1"/>
-    <n v="6"/>
-    <n v="18"/>
-    <m/>
-    <x v="1"/>
-  </r>
-  <r>
     <n v="67"/>
     <s v="Finance - Invoicing"/>
     <s v="Invoice view"/>
@@ -1876,246 +1441,6 @@
     <x v="1"/>
   </r>
   <r>
-    <n v="68"/>
-    <s v="Finance - Invoicing"/>
-    <s v="Invoice list"/>
-    <m/>
-    <s v="Should have the ability to filter the list"/>
-    <s v="Nice to have"/>
-    <s v="Feature enhancement/fix"/>
-    <s v="Major change to current component"/>
-    <n v="1"/>
-    <n v="6"/>
-    <n v="9"/>
-    <m/>
-    <x v="1"/>
-  </r>
-  <r>
-    <n v="69"/>
-    <s v="Finance - Invoicing"/>
-    <s v="Invoice list"/>
-    <m/>
-    <s v="Should have the ability to sort the list"/>
-    <s v="Nice to have"/>
-    <s v="Feature enhancement/fix"/>
-    <s v="Major change to current component"/>
-    <n v="1"/>
-    <n v="6"/>
-    <n v="9"/>
-    <m/>
-    <x v="1"/>
-  </r>
-  <r>
-    <n v="70"/>
-    <s v="Finance - Invoicing"/>
-    <s v="Invoice list"/>
-    <m/>
-    <s v="List should be paginated"/>
-    <s v="Nice to have"/>
-    <s v="Feature enhancement/fix"/>
-    <s v="Major change to current component"/>
-    <n v="1"/>
-    <n v="6"/>
-    <n v="9"/>
-    <m/>
-    <x v="1"/>
-  </r>
-  <r>
-    <n v="71"/>
-    <s v="Finance - Invoicing"/>
-    <s v="Generate invoices"/>
-    <s v="Generate invoices params"/>
-    <s v="The radio should be better group - they are too far apart to make sense"/>
-    <s v="Poor UI"/>
-    <s v="Improved UI"/>
-    <s v="Minor change to current component"/>
-    <n v="3"/>
-    <n v="3"/>
-    <n v="13.5"/>
-    <m/>
-    <x v="1"/>
-  </r>
-  <r>
-    <n v="72"/>
-    <s v="Finance - Invoicing"/>
-    <s v="Generate invoices"/>
-    <s v="Generate invoices params"/>
-    <s v="Group of buttons should have a little border to show better relations logic"/>
-    <s v="Poor UI"/>
-    <s v="Improved UI"/>
-    <s v="Minor change to current component"/>
-    <n v="3"/>
-    <n v="3"/>
-    <n v="13.5"/>
-    <m/>
-    <x v="1"/>
-  </r>
-  <r>
-    <n v="73"/>
-    <s v="Finance - Invoicing"/>
-    <s v="Generate invoices"/>
-    <s v="Generate invoices params"/>
-    <s v="The generate invoices button should not be available if the form is not completed correctly"/>
-    <s v="Poor UX"/>
-    <s v="Improved UX"/>
-    <s v="Major change to current component"/>
-    <n v="4"/>
-    <n v="4"/>
-    <n v="16"/>
-    <m/>
-    <x v="1"/>
-  </r>
-  <r>
-    <n v="74"/>
-    <s v="Finance - Invoicing"/>
-    <s v="Generate invoices"/>
-    <s v="Generate invoices params"/>
-    <s v="On smaller screens you can see the whole modal and scroll down"/>
-    <s v="Poor UX"/>
-    <s v="Improved UX"/>
-    <s v="Investigation and change"/>
-    <n v="4"/>
-    <n v="4"/>
-    <n v="21.333333333333332"/>
-    <m/>
-    <x v="1"/>
-  </r>
-  <r>
-    <n v="75"/>
-    <s v="Finance - Invoicing"/>
-    <s v="Generate invoices"/>
-    <s v="Generate invoices results"/>
-    <s v="Needs to produce a summary of the invoices generated:_x000a_Number of invoices_x000a_Lessons invoices_x000a_Total revenue_x000a_Average revenue per invoices_x000a_Median invoice revenue_x000a_Largest and smallest invoices by revenue"/>
-    <s v="Nice to have"/>
-    <s v="Feature enhancement/fix"/>
-    <s v="Major change to current component"/>
-    <n v="1"/>
-    <n v="6"/>
-    <n v="9"/>
-    <m/>
-    <x v="1"/>
-  </r>
-  <r>
-    <n v="76"/>
-    <s v="Finance - Payments"/>
-    <s v="Payment view"/>
-    <m/>
-    <s v="On clicking the payment on the payment list - Should the payment modal in view only mode"/>
-    <s v="Nice to have"/>
-    <s v="Feature enhancement/fix"/>
-    <s v="Minor change to current component"/>
-    <n v="1"/>
-    <n v="6"/>
-    <n v="18"/>
-    <m/>
-    <x v="1"/>
-  </r>
-  <r>
-    <n v="77"/>
-    <s v="Finance - Payments"/>
-    <s v="Payment modal"/>
-    <m/>
-    <s v="Voiding payments does not work"/>
-    <s v="Does not function as expected"/>
-    <s v="Feature enhancement/fix"/>
-    <s v="Investigation and change"/>
-    <n v="8"/>
-    <n v="6"/>
-    <n v="96"/>
-    <m/>
-    <x v="0"/>
-  </r>
-  <r>
-    <n v="78"/>
-    <s v="Finance - Payments"/>
-    <s v="Payment modal"/>
-    <m/>
-    <s v="Payments should have a Type property (EFT vs Cash)"/>
-    <s v="Nice to have"/>
-    <s v="Feature enhancement/fix"/>
-    <s v="Major change to current component"/>
-    <n v="1"/>
-    <n v="6"/>
-    <n v="9"/>
-    <m/>
-    <x v="1"/>
-  </r>
-  <r>
-    <n v="79"/>
-    <s v="Finance - Payments"/>
-    <s v="Payment modal"/>
-    <m/>
-    <s v="On viewing a payment - When trying to record a new payment - the details of the old payment are brought up (as well at the void button)"/>
-    <s v="Poor UX"/>
-    <s v="Improved UX"/>
-    <s v="Investigation and change"/>
-    <n v="4"/>
-    <n v="4"/>
-    <n v="21.333333333333332"/>
-    <m/>
-    <x v="1"/>
-  </r>
-  <r>
-    <n v="80"/>
-    <s v="Finance - Invoicing"/>
-    <s v="Invoice view"/>
-    <m/>
-    <s v="On the statement when you click an invoice - you view the invoice detail - but when you click back it doesn't take you to the statement"/>
-    <s v="Poor UX"/>
-    <s v="Improved UX"/>
-    <s v="Investigation and change"/>
-    <n v="4"/>
-    <n v="4"/>
-    <n v="21.333333333333332"/>
-    <m/>
-    <x v="1"/>
-  </r>
-  <r>
-    <n v="81"/>
-    <s v="Finance - Payments"/>
-    <s v="Payment modal"/>
-    <m/>
-    <s v="On the statement when you click an payment - you view the payment modal - but when you click back it doesn't take you to the statement"/>
-    <s v="Poor UX"/>
-    <s v="Improved UX"/>
-    <s v="Investigation and change"/>
-    <n v="4"/>
-    <n v="4"/>
-    <n v="21.333333333333332"/>
-    <m/>
-    <x v="1"/>
-  </r>
-  <r>
-    <n v="82"/>
-    <s v="Finance - Accounting"/>
-    <s v="Bank statement importer"/>
-    <m/>
-    <s v="Should be able import a bank statement:_x000a_Would require use to allocate transactions_x000a_Transaction are to be remembered for future use_x000a_Should perform a quick recon calculation_x000a_Expenses should be able to be captured when paid (Later will be done on a invoice basis and then payments are allocated to supplier dues)"/>
-    <s v="Nice to have"/>
-    <s v="USP"/>
-    <s v="Whole new section"/>
-    <n v="1"/>
-    <n v="10"/>
-    <n v="10"/>
-    <m/>
-    <x v="1"/>
-  </r>
-  <r>
-    <n v="83"/>
-    <s v="Finance - Reports"/>
-    <s v="Profit and lose report"/>
-    <m/>
-    <s v="Mini profit and loss report_x000a_Should be able to select for a period "/>
-    <s v="Nice to have"/>
-    <s v="USP"/>
-    <s v="Whole new feature"/>
-    <n v="1"/>
-    <n v="10"/>
-    <n v="12.5"/>
-    <m/>
-    <x v="1"/>
-  </r>
-  <r>
     <n v="84"/>
     <s v="Clients"/>
     <s v="Client lists"/>
@@ -2131,66 +1456,6 @@
     <x v="1"/>
   </r>
   <r>
-    <n v="85"/>
-    <s v="Clients"/>
-    <s v="Client lists"/>
-    <m/>
-    <s v="List on smaller screens are squashed"/>
-    <s v="Poor UI"/>
-    <s v="Improved UI"/>
-    <s v="Minor change to current component"/>
-    <n v="3"/>
-    <n v="3"/>
-    <n v="13.5"/>
-    <m/>
-    <x v="1"/>
-  </r>
-  <r>
-    <n v="86"/>
-    <s v="Clients"/>
-    <s v="Client lists"/>
-    <m/>
-    <s v="Lines on the list should have alternating colours"/>
-    <s v="Poor UI"/>
-    <s v="Improved UI"/>
-    <s v="Minor change to current component"/>
-    <n v="3"/>
-    <n v="3"/>
-    <n v="13.5"/>
-    <m/>
-    <x v="1"/>
-  </r>
-  <r>
-    <n v="87"/>
-    <s v="Clients"/>
-    <s v="Client modal"/>
-    <m/>
-    <s v="On viewing a client - When trying to record a new client - the details of the old client are brought up"/>
-    <s v="Poor UX"/>
-    <s v="Improved UX"/>
-    <s v="Investigation and change"/>
-    <n v="4"/>
-    <n v="4"/>
-    <n v="21.333333333333332"/>
-    <m/>
-    <x v="1"/>
-  </r>
-  <r>
-    <n v="88"/>
-    <s v="Clients"/>
-    <s v="Client modal"/>
-    <m/>
-    <s v="On cancelling adding a new client, should take you menu not the list (if you can from the menu)"/>
-    <s v="Poor UX"/>
-    <s v="Improved UX"/>
-    <s v="Investigation and change"/>
-    <n v="4"/>
-    <n v="4"/>
-    <n v="21.333333333333332"/>
-    <m/>
-    <x v="1"/>
-  </r>
-  <r>
     <n v="89"/>
     <s v="Clients"/>
     <s v="Client lists"/>
@@ -2204,261 +1469,6 @@
     <n v="32"/>
     <m/>
     <x v="1"/>
-  </r>
-  <r>
-    <n v="90"/>
-    <s v="Clients"/>
-    <s v="Client modal"/>
-    <m/>
-    <s v="Remove client is not working"/>
-    <s v="Does not function as expected"/>
-    <s v="Feature enhancement/fix"/>
-    <s v="Investigation and change"/>
-    <n v="8"/>
-    <n v="6"/>
-    <n v="96"/>
-    <m/>
-    <x v="0"/>
-  </r>
-  <r>
-    <n v="91"/>
-    <s v="Finance - Reports"/>
-    <s v="Report - Review by instructor"/>
-    <m/>
-    <s v="Required to be built"/>
-    <s v="Nice to have"/>
-    <s v="USP"/>
-    <s v="New component/service with complex integration"/>
-    <n v="1"/>
-    <n v="10"/>
-    <n v="14.285714285714286"/>
-    <n v="59"/>
-    <x v="1"/>
-  </r>
-  <r>
-    <n v="92"/>
-    <s v="Finance - Reports"/>
-    <s v="Report - Review by horse"/>
-    <m/>
-    <s v="Required to be built"/>
-    <s v="Nice to have"/>
-    <s v="USP"/>
-    <s v="New component/service with complex integration"/>
-    <n v="1"/>
-    <n v="10"/>
-    <n v="14.285714285714286"/>
-    <n v="64"/>
-    <x v="1"/>
-  </r>
-  <r>
-    <n v="93"/>
-    <s v="Finance - Reports"/>
-    <s v="Report - Expenses by instructor"/>
-    <m/>
-    <s v="Required to be built"/>
-    <s v="Nice to have"/>
-    <s v="USP"/>
-    <s v="New component/service with complex integration"/>
-    <n v="1"/>
-    <n v="10"/>
-    <n v="14.285714285714286"/>
-    <n v="59"/>
-    <x v="1"/>
-  </r>
-  <r>
-    <n v="94"/>
-    <s v="Finance - Reports"/>
-    <s v="Report - Expenses by horse"/>
-    <m/>
-    <s v="Required to be built"/>
-    <s v="Nice to have"/>
-    <s v="USP"/>
-    <s v="New component/service with complex integration"/>
-    <n v="1"/>
-    <n v="10"/>
-    <n v="14.285714285714286"/>
-    <n v="64"/>
-    <x v="1"/>
-  </r>
-  <r>
-    <n v="95"/>
-    <s v="Finance - Reports"/>
-    <s v="Report - Contribution by instructor"/>
-    <m/>
-    <s v="Required to be built"/>
-    <s v="Nice to have"/>
-    <s v="USP"/>
-    <s v="New component/service with complex integration"/>
-    <n v="1"/>
-    <n v="10"/>
-    <n v="14.285714285714286"/>
-    <n v="59"/>
-    <x v="1"/>
-  </r>
-  <r>
-    <n v="96"/>
-    <s v="Finance - Reports"/>
-    <s v="Report - Contribution by horse"/>
-    <m/>
-    <s v="Required to be built"/>
-    <s v="Nice to have"/>
-    <s v="USP"/>
-    <s v="New component/service with complex integration"/>
-    <n v="1"/>
-    <n v="10"/>
-    <n v="14.285714285714286"/>
-    <n v="64"/>
-    <x v="1"/>
-  </r>
-  <r>
-    <n v="97"/>
-    <s v="Finance - Accounting"/>
-    <s v="Bank statement importer"/>
-    <m/>
-    <s v="If expenses are allocated to instructors should be able to allocate per instructor"/>
-    <s v="Nice to have"/>
-    <s v="USP"/>
-    <s v="New component/service with complex integration"/>
-    <n v="1"/>
-    <n v="10"/>
-    <n v="14.285714285714286"/>
-    <n v="59"/>
-    <x v="1"/>
-  </r>
-  <r>
-    <n v="98"/>
-    <s v="Finance - Accounting"/>
-    <s v="Bank statement importer"/>
-    <m/>
-    <s v="If expenses are allocated to instructors should be able to allocate per instructor"/>
-    <s v="Nice to have"/>
-    <s v="USP"/>
-    <s v="New component/service with complex integration"/>
-    <n v="1"/>
-    <n v="10"/>
-    <n v="14.285714285714286"/>
-    <n v="64"/>
-    <x v="1"/>
-  </r>
-  <r>
-    <n v="99"/>
-    <s v="Booking"/>
-    <s v="Lesson booking platform"/>
-    <m/>
-    <s v="A platform where a customer of the client can book their lessons, based on the slots the client has deemed and allowed as open"/>
-    <s v="Nice to have"/>
-    <s v="USP"/>
-    <s v="Whole new section"/>
-    <n v="1"/>
-    <n v="10"/>
-    <n v="10"/>
-    <m/>
-    <x v="1"/>
-  </r>
-  <r>
-    <n v="100"/>
-    <s v="Clients"/>
-    <s v="Lesson booking platform"/>
-    <m/>
-    <s v="On adding a new client - the client needs to be sent and email/SMS/text with a link to where they can book their own lessons"/>
-    <s v="Nice to have"/>
-    <s v="USP"/>
-    <s v="New component/service with complex integration"/>
-    <n v="1"/>
-    <n v="10"/>
-    <n v="14.285714285714286"/>
-    <n v="99"/>
-    <x v="1"/>
-  </r>
-  <r>
-    <n v="101"/>
-    <s v="Clients"/>
-    <s v="Lesson booking platform"/>
-    <m/>
-    <s v="Client should be able to add themselves as a new client - when on  the booking platform"/>
-    <s v="Nice to have"/>
-    <s v="USP"/>
-    <s v="New component/service with complex integration"/>
-    <n v="1"/>
-    <n v="10"/>
-    <n v="14.285714285714286"/>
-    <n v="100"/>
-    <x v="1"/>
-  </r>
-  <r>
-    <n v="102"/>
-    <s v="Finance - Accounting"/>
-    <s v="Statement runs"/>
-    <m/>
-    <s v="Client should be able to perform a statement run with a simple flow process_x000a_All clients statements are to be PDDd and saved to their folder along with their backing fin documents (invoice, credit notes etc , payment receipts)_x000a_User should be able to determine where the batch of documents is saved"/>
-    <s v="Nice to have"/>
-    <s v="USP"/>
-    <s v="Whole new feature"/>
-    <n v="1"/>
-    <n v="10"/>
-    <n v="12.5"/>
-    <m/>
-    <x v="1"/>
-  </r>
-  <r>
-    <n v="103"/>
-    <s v="Finance - Accounting"/>
-    <s v="Statement runs"/>
-    <m/>
-    <s v="Should be able perform a link batch disperse where the use is sent a link to where their invoices can be found on the platform"/>
-    <s v="Nice to have"/>
-    <s v="USP"/>
-    <s v="New component/service with complex integration"/>
-    <n v="1"/>
-    <n v="10"/>
-    <n v="14.285714285714286"/>
-    <n v="102"/>
-    <x v="1"/>
-  </r>
-  <r>
-    <n v="104"/>
-    <s v="Finance - Accounting"/>
-    <s v="Statement runs"/>
-    <m/>
-    <s v="Should be able to email the documents and statements to the client"/>
-    <s v="Nice to have"/>
-    <s v="USP"/>
-    <s v="New component/service with complex integration"/>
-    <n v="1"/>
-    <n v="10"/>
-    <n v="14.285714285714286"/>
-    <n v="103"/>
-    <x v="1"/>
-  </r>
-  <r>
-    <n v="105"/>
-    <s v="User Management"/>
-    <s v="Profile portal"/>
-    <m/>
-    <s v="A portal where the client can_x000a_Update their details_x000a_Add new users to their account_x000a_Any other preferences they want"/>
-    <s v="Nice to have"/>
-    <s v="USP"/>
-    <s v="Whole new feature"/>
-    <n v="1"/>
-    <n v="10"/>
-    <n v="12.5"/>
-    <m/>
-    <x v="1"/>
-  </r>
-  <r>
-    <n v="106"/>
-    <s v="General"/>
-    <m/>
-    <m/>
-    <s v="Update favicon with new logo"/>
-    <s v="Poor UI"/>
-    <s v="Improved UI"/>
-    <s v="Minor tweak"/>
-    <n v="3"/>
-    <n v="3"/>
-    <n v="27"/>
-    <m/>
-    <x v="0"/>
   </r>
   <r>
     <n v="107"/>
@@ -2506,81 +1516,6 @@
     <x v="1"/>
   </r>
   <r>
-    <n v="110"/>
-    <s v="General"/>
-    <m/>
-    <m/>
-    <s v="Modal screens are still scrollable - when the sheath should prevent that"/>
-    <s v="Poor UI"/>
-    <s v="Improved UI"/>
-    <s v="Investigation and change"/>
-    <n v="3"/>
-    <n v="3"/>
-    <n v="9"/>
-    <m/>
-    <x v="1"/>
-  </r>
-  <r>
-    <n v="111"/>
-    <s v="Finance - Invoicing"/>
-    <s v="Generate invoices"/>
-    <m/>
-    <s v="Invoices do not need a voided property as they can't be voided - only credit noted"/>
-    <s v="Poor UX"/>
-    <s v="Refactor/Tech debt"/>
-    <s v="Minor change to current component"/>
-    <n v="4"/>
-    <n v="1"/>
-    <n v="2"/>
-    <m/>
-    <x v="1"/>
-  </r>
-  <r>
-    <n v="112"/>
-    <s v="Finance - Reports"/>
-    <s v="Statement runs"/>
-    <m/>
-    <s v="Statements do not show credit notes (where required)"/>
-    <s v="Does not function as expected"/>
-    <s v="Feature enhancement/fix"/>
-    <s v="Investigation and change"/>
-    <n v="8"/>
-    <n v="6"/>
-    <n v="96"/>
-    <n v="53"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <n v="113"/>
-    <s v="Login/Register"/>
-    <s v="Register modal"/>
-    <m/>
-    <s v="Needs to be a modal specfically for registrations"/>
-    <s v="Does not function as expected"/>
-    <s v="Feature enhancement/fix"/>
-    <s v="New component/service with simple integration"/>
-    <n v="8"/>
-    <n v="6"/>
-    <n v="57.6"/>
-    <m/>
-    <x v="0"/>
-  </r>
-  <r>
-    <n v="114"/>
-    <s v="Finance - Payments"/>
-    <s v="Payment modal"/>
-    <m/>
-    <s v="Payment are not being recorded correctly "/>
-    <s v="Does not function as expected"/>
-    <s v="Feature enhancement/fix"/>
-    <s v="Investigation and change"/>
-    <n v="8"/>
-    <n v="6"/>
-    <n v="96"/>
-    <m/>
-    <x v="0"/>
-  </r>
-  <r>
     <n v="115"/>
     <s v="User Management"/>
     <s v="Register modal"/>
@@ -2596,18 +1531,1083 @@
     <x v="1"/>
   </r>
   <r>
-    <n v="116"/>
-    <s v="Marketing"/>
-    <s v="Landing Page"/>
-    <s v="Our Features Section"/>
-    <s v="Update content for the features section of the landing page"/>
+    <n v="8"/>
+    <s v="User Management"/>
+    <s v="Sign in Modal"/>
+    <s v="Login error warnings"/>
+    <s v="Error modals"/>
+    <s v="Poor UX"/>
+    <s v="New feature"/>
+    <s v="New component/service with complex integration"/>
+    <n v="4"/>
+    <n v="7"/>
+    <n v="28"/>
+    <m/>
+    <x v="1"/>
+  </r>
+  <r>
+    <n v="22"/>
+    <s v="User Management"/>
+    <s v="Sign in Modal"/>
+    <m/>
+    <s v="On small devices the inputs on the modal are mis-aligned (Use 340*635 spec)"/>
+    <s v="Poor UI"/>
+    <s v="Improved UI"/>
+    <s v="Minor tweak"/>
+    <n v="3"/>
+    <n v="3"/>
+    <n v="27"/>
+    <m/>
+    <x v="1"/>
+  </r>
+  <r>
+    <n v="43"/>
+    <s v="Calendar/Appointments"/>
+    <s v="Calendar"/>
+    <m/>
+    <s v="The heights of the appointment blocks should match there duration"/>
+    <s v="Poor UI"/>
+    <s v="Feature enhancement/fix"/>
+    <s v="Major change to current component"/>
+    <n v="3"/>
+    <n v="6"/>
+    <n v="27"/>
+    <m/>
+    <x v="1"/>
+  </r>
+  <r>
+    <n v="44"/>
+    <s v="Calendar/Appointments"/>
+    <s v="Calendar"/>
+    <m/>
+    <s v="When too many appointment in a slot - the blocks become cramped… need to find a more elegant way to stack appointment blocks when there are too many appointments"/>
+    <s v="Poor UI"/>
+    <s v="Feature enhancement/fix"/>
+    <s v="Major change to current component"/>
+    <n v="3"/>
+    <n v="6"/>
+    <n v="27"/>
+    <m/>
+    <x v="1"/>
+  </r>
+  <r>
+    <n v="48"/>
+    <s v="Calendar/Appointments"/>
+    <s v="Appointments modal"/>
+    <m/>
+    <s v="The cancel changes button on and edited appointment should be darker"/>
+    <s v="Poor UI"/>
+    <s v="Improved UI"/>
+    <s v="Minor tweak"/>
+    <n v="3"/>
+    <n v="3"/>
+    <n v="27"/>
+    <m/>
+    <x v="1"/>
+  </r>
+  <r>
+    <n v="57"/>
+    <s v="Finance - Invoicing"/>
+    <s v="Invoice view"/>
+    <m/>
+    <s v="Lesson (and other sub headings) should be underlined"/>
+    <s v="Poor UI"/>
+    <s v="Improved UI"/>
+    <s v="Minor tweak"/>
+    <n v="3"/>
+    <n v="3"/>
+    <n v="27"/>
+    <m/>
+    <x v="1"/>
+  </r>
+  <r>
+    <n v="106"/>
+    <s v="General"/>
+    <m/>
+    <m/>
+    <s v="Update favicon with new logo"/>
+    <s v="Poor UI"/>
+    <s v="Improved UI"/>
+    <s v="Minor tweak"/>
+    <n v="3"/>
+    <n v="3"/>
+    <n v="27"/>
+    <m/>
+    <x v="0"/>
+  </r>
+  <r>
+    <n v="49"/>
+    <s v="Calendar/Appointments"/>
+    <s v="Appointments modal"/>
+    <m/>
+    <s v="When changes are made - the save button appears - but it should always appear - just be disabled"/>
+    <s v="Poor UX"/>
+    <s v="Improved UX"/>
+    <s v="Investigation and change"/>
+    <n v="4"/>
+    <n v="4"/>
+    <n v="21.333333333333332"/>
+    <m/>
+    <x v="1"/>
+  </r>
+  <r>
+    <n v="74"/>
+    <s v="Finance - Invoicing"/>
+    <s v="Generate invoices"/>
+    <s v="Generate invoices params"/>
+    <s v="On smaller screens you can see the whole modal and scroll down"/>
+    <s v="Poor UX"/>
+    <s v="Improved UX"/>
+    <s v="Investigation and change"/>
+    <n v="4"/>
+    <n v="4"/>
+    <n v="21.333333333333332"/>
+    <m/>
+    <x v="1"/>
+  </r>
+  <r>
+    <n v="79"/>
+    <s v="Finance - Payments"/>
+    <s v="Payment modal"/>
+    <m/>
+    <s v="On viewing a payment - When trying to record a new payment - the details of the old payment are brought up (as well at the void button)"/>
+    <s v="Poor UX"/>
+    <s v="Improved UX"/>
+    <s v="Investigation and change"/>
+    <n v="4"/>
+    <n v="4"/>
+    <n v="21.333333333333332"/>
+    <m/>
+    <x v="1"/>
+  </r>
+  <r>
+    <n v="80"/>
+    <s v="Finance - Invoicing"/>
+    <s v="Invoice view"/>
+    <m/>
+    <s v="On the statement when you click an invoice - you view the invoice detail - but when you click back it doesn't take you to the statement"/>
+    <s v="Poor UX"/>
+    <s v="Improved UX"/>
+    <s v="Investigation and change"/>
+    <n v="4"/>
+    <n v="4"/>
+    <n v="21.333333333333332"/>
+    <m/>
+    <x v="1"/>
+  </r>
+  <r>
+    <n v="81"/>
+    <s v="Finance - Payments"/>
+    <s v="Payment modal"/>
+    <m/>
+    <s v="On the statement when you click an payment - you view the payment modal - but when you click back it doesn't take you to the statement"/>
+    <s v="Poor UX"/>
+    <s v="Improved UX"/>
+    <s v="Investigation and change"/>
+    <n v="4"/>
+    <n v="4"/>
+    <n v="21.333333333333332"/>
+    <m/>
+    <x v="1"/>
+  </r>
+  <r>
+    <n v="87"/>
+    <s v="Clients"/>
+    <s v="Client modal"/>
+    <m/>
+    <s v="On viewing a client - When trying to record a new client - the details of the old client are brought up"/>
+    <s v="Poor UX"/>
+    <s v="Improved UX"/>
+    <s v="Investigation and change"/>
+    <n v="4"/>
+    <n v="4"/>
+    <n v="21.333333333333332"/>
+    <m/>
+    <x v="1"/>
+  </r>
+  <r>
+    <n v="88"/>
+    <s v="Clients"/>
+    <s v="Client modal"/>
+    <m/>
+    <s v="On cancelling adding a new client, should take you menu not the list (if you can from the menu)"/>
+    <s v="Poor UX"/>
+    <s v="Improved UX"/>
+    <s v="Investigation and change"/>
+    <n v="4"/>
+    <n v="4"/>
+    <n v="21.333333333333332"/>
+    <m/>
+    <x v="1"/>
+  </r>
+  <r>
+    <n v="17"/>
+    <s v="User Management"/>
+    <s v="Sign in Modal"/>
+    <s v="Forgot password"/>
+    <s v="No way for users to reset forgotten passwords"/>
     <s v="Poor UX"/>
     <s v="Feature enhancement/fix"/>
+    <s v="New component/service with complex integration"/>
+    <n v="4"/>
+    <n v="6"/>
+    <n v="20.571428571428573"/>
+    <m/>
+    <x v="1"/>
+  </r>
+  <r>
+    <n v="18"/>
+    <s v="User Management"/>
+    <s v="Sign in Modal"/>
+    <s v="Forgot password"/>
+    <s v="Third party login - Facebook"/>
+    <s v="Poor UX"/>
+    <s v="Feature enhancement/fix"/>
+    <s v="New component/service with complex integration"/>
+    <n v="4"/>
+    <n v="6"/>
+    <n v="20.571428571428573"/>
+    <m/>
+    <x v="1"/>
+  </r>
+  <r>
+    <n v="19"/>
+    <s v="User Management"/>
+    <s v="Sign in Modal"/>
+    <s v="Forgot password"/>
+    <s v="Third party login - Google"/>
+    <s v="Poor UX"/>
+    <s v="Feature enhancement/fix"/>
+    <s v="New component/service with complex integration"/>
+    <n v="4"/>
+    <n v="6"/>
+    <n v="20.571428571428573"/>
+    <m/>
+    <x v="1"/>
+  </r>
+  <r>
+    <n v="20"/>
+    <s v="User Management"/>
+    <s v="Sign in Modal"/>
+    <s v="Forgot password"/>
+    <s v="Third party login - LinkedIn"/>
+    <s v="Poor UX"/>
+    <s v="Feature enhancement/fix"/>
+    <s v="New component/service with complex integration"/>
+    <n v="4"/>
+    <n v="6"/>
+    <n v="20.571428571428573"/>
+    <m/>
+    <x v="1"/>
+  </r>
+  <r>
+    <n v="21"/>
+    <s v="User Management"/>
+    <s v="Sign in Modal"/>
+    <s v="Forgot password"/>
+    <s v="Third party login - Microsoft"/>
+    <s v="Poor UX"/>
+    <s v="Feature enhancement/fix"/>
+    <s v="New component/service with complex integration"/>
+    <n v="4"/>
+    <n v="6"/>
+    <n v="20.571428571428573"/>
+    <m/>
+    <x v="1"/>
+  </r>
+  <r>
+    <n v="66"/>
+    <s v="Finance - Invoicing"/>
+    <s v="Invoice view"/>
+    <m/>
+    <s v="On clicking the lesson on the  viewed invoice - Should bring up the appointment modal - with no option to edit"/>
+    <s v="Nice to have"/>
+    <s v="Feature enhancement/fix"/>
+    <s v="Minor change to current component"/>
+    <n v="1"/>
+    <n v="6"/>
+    <n v="18"/>
+    <m/>
+    <x v="1"/>
+  </r>
+  <r>
+    <n v="76"/>
+    <s v="Finance - Payments"/>
+    <s v="Payment view"/>
+    <m/>
+    <s v="On clicking the payment on the payment list - Should the payment modal in view only mode"/>
+    <s v="Nice to have"/>
+    <s v="Feature enhancement/fix"/>
+    <s v="Minor change to current component"/>
+    <n v="1"/>
+    <n v="6"/>
+    <n v="18"/>
+    <m/>
+    <x v="1"/>
+  </r>
+  <r>
+    <n v="73"/>
+    <s v="Finance - Invoicing"/>
+    <s v="Generate invoices"/>
+    <s v="Generate invoices params"/>
+    <s v="The generate invoices button should not be available if the form is not completed correctly"/>
+    <s v="Poor UX"/>
+    <s v="Improved UX"/>
+    <s v="Major change to current component"/>
+    <n v="4"/>
+    <n v="4"/>
+    <n v="16"/>
+    <m/>
+    <x v="1"/>
+  </r>
+  <r>
+    <n v="91"/>
+    <s v="Finance - Reports"/>
+    <s v="Report - Review by instructor"/>
+    <m/>
+    <s v="Required to be built"/>
+    <s v="Nice to have"/>
+    <s v="USP"/>
+    <s v="New component/service with complex integration"/>
+    <n v="1"/>
+    <n v="10"/>
+    <n v="14.285714285714286"/>
+    <n v="59"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <n v="92"/>
+    <s v="Finance - Reports"/>
+    <s v="Report - Review by horse"/>
+    <m/>
+    <s v="Required to be built"/>
+    <s v="Nice to have"/>
+    <s v="USP"/>
+    <s v="New component/service with complex integration"/>
+    <n v="1"/>
+    <n v="10"/>
+    <n v="14.285714285714286"/>
+    <n v="64"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <n v="93"/>
+    <s v="Finance - Reports"/>
+    <s v="Report - Expenses by instructor"/>
+    <m/>
+    <s v="Required to be built"/>
+    <s v="Nice to have"/>
+    <s v="USP"/>
+    <s v="New component/service with complex integration"/>
+    <n v="1"/>
+    <n v="10"/>
+    <n v="14.285714285714286"/>
+    <n v="59"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <n v="94"/>
+    <s v="Finance - Reports"/>
+    <s v="Report - Expenses by horse"/>
+    <m/>
+    <s v="Required to be built"/>
+    <s v="Nice to have"/>
+    <s v="USP"/>
+    <s v="New component/service with complex integration"/>
+    <n v="1"/>
+    <n v="10"/>
+    <n v="14.285714285714286"/>
+    <n v="64"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <n v="95"/>
+    <s v="Finance - Reports"/>
+    <s v="Report - Contribution by instructor"/>
+    <m/>
+    <s v="Required to be built"/>
+    <s v="Nice to have"/>
+    <s v="USP"/>
+    <s v="New component/service with complex integration"/>
+    <n v="1"/>
+    <n v="10"/>
+    <n v="14.285714285714286"/>
+    <n v="59"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <n v="96"/>
+    <s v="Finance - Reports"/>
+    <s v="Report - Contribution by horse"/>
+    <m/>
+    <s v="Required to be built"/>
+    <s v="Nice to have"/>
+    <s v="USP"/>
+    <s v="New component/service with complex integration"/>
+    <n v="1"/>
+    <n v="10"/>
+    <n v="14.285714285714286"/>
+    <n v="64"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <n v="97"/>
+    <s v="Finance - Accounting"/>
+    <s v="Bank statement importer"/>
+    <m/>
+    <s v="If expenses are allocated to instructors should be able to allocate per instructor"/>
+    <s v="Nice to have"/>
+    <s v="USP"/>
+    <s v="New component/service with complex integration"/>
+    <n v="1"/>
+    <n v="10"/>
+    <n v="14.285714285714286"/>
+    <n v="59"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <n v="98"/>
+    <s v="Finance - Accounting"/>
+    <s v="Bank statement importer"/>
+    <m/>
+    <s v="If expenses are allocated to instructors should be able to allocate per instructor"/>
+    <s v="Nice to have"/>
+    <s v="USP"/>
+    <s v="New component/service with complex integration"/>
+    <n v="1"/>
+    <n v="10"/>
+    <n v="14.285714285714286"/>
+    <n v="64"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <n v="100"/>
+    <s v="Clients"/>
+    <s v="Lesson booking platform"/>
+    <m/>
+    <s v="On adding a new client - the client needs to be sent and email/SMS/text with a link to where they can book their own lessons"/>
+    <s v="Nice to have"/>
+    <s v="USP"/>
+    <s v="New component/service with complex integration"/>
+    <n v="1"/>
+    <n v="10"/>
+    <n v="14.285714285714286"/>
+    <n v="99"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <n v="101"/>
+    <s v="Clients"/>
+    <s v="Lesson booking platform"/>
+    <m/>
+    <s v="Client should be able to add themselves as a new client - when on  the booking platform"/>
+    <s v="Nice to have"/>
+    <s v="USP"/>
+    <s v="New component/service with complex integration"/>
+    <n v="1"/>
+    <n v="10"/>
+    <n v="14.285714285714286"/>
+    <n v="100"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <n v="103"/>
+    <s v="Finance - Accounting"/>
+    <s v="Statement runs"/>
+    <m/>
+    <s v="Should be able perform a link batch disperse where the use is sent a link to where their invoices can be found on the platform"/>
+    <s v="Nice to have"/>
+    <s v="USP"/>
+    <s v="New component/service with complex integration"/>
+    <n v="1"/>
+    <n v="10"/>
+    <n v="14.285714285714286"/>
+    <n v="102"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <n v="104"/>
+    <s v="Finance - Accounting"/>
+    <s v="Statement runs"/>
+    <m/>
+    <s v="Should be able to email the documents and statements to the client"/>
+    <s v="Nice to have"/>
+    <s v="USP"/>
+    <s v="New component/service with complex integration"/>
+    <n v="1"/>
+    <n v="10"/>
+    <n v="14.285714285714286"/>
+    <n v="103"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <n v="35"/>
+    <s v="Navbar"/>
+    <s v="Drop down menu"/>
+    <m/>
+    <s v="Should not down the screen - but should hover above the current screen content"/>
+    <s v="Poor UI"/>
+    <s v="Improved UI"/>
+    <s v="Minor change to current component"/>
+    <n v="3"/>
+    <n v="3"/>
+    <n v="13.5"/>
+    <m/>
+    <x v="1"/>
+  </r>
+  <r>
+    <n v="38"/>
+    <s v="Calendar/Appointments"/>
+    <s v="Calendar"/>
+    <m/>
+    <s v="On taller screens - the schedule slots should be have a great height to fill the remainder of the screen"/>
+    <s v="Poor UI"/>
+    <s v="Improved UI"/>
+    <s v="Minor change to current component"/>
+    <n v="3"/>
+    <n v="3"/>
+    <n v="13.5"/>
+    <m/>
+    <x v="1"/>
+  </r>
+  <r>
+    <n v="71"/>
+    <s v="Finance - Invoicing"/>
+    <s v="Generate invoices"/>
+    <s v="Generate invoices params"/>
+    <s v="The radio should be better group - they are too far apart to make sense"/>
+    <s v="Poor UI"/>
+    <s v="Improved UI"/>
+    <s v="Minor change to current component"/>
+    <n v="3"/>
+    <n v="3"/>
+    <n v="13.5"/>
+    <m/>
+    <x v="1"/>
+  </r>
+  <r>
+    <n v="72"/>
+    <s v="Finance - Invoicing"/>
+    <s v="Generate invoices"/>
+    <s v="Generate invoices params"/>
+    <s v="Group of buttons should have a little border to show better relations logic"/>
+    <s v="Poor UI"/>
+    <s v="Improved UI"/>
+    <s v="Minor change to current component"/>
+    <n v="3"/>
+    <n v="3"/>
+    <n v="13.5"/>
+    <m/>
+    <x v="1"/>
+  </r>
+  <r>
+    <n v="85"/>
+    <s v="Clients"/>
+    <s v="Client lists"/>
+    <m/>
+    <s v="List on smaller screens are squashed"/>
+    <s v="Poor UI"/>
+    <s v="Improved UI"/>
+    <s v="Minor change to current component"/>
+    <n v="3"/>
+    <n v="3"/>
+    <n v="13.5"/>
+    <m/>
+    <x v="1"/>
+  </r>
+  <r>
+    <n v="86"/>
+    <s v="Clients"/>
+    <s v="Client lists"/>
+    <m/>
+    <s v="Lines on the list should have alternating colours"/>
+    <s v="Poor UI"/>
+    <s v="Improved UI"/>
+    <s v="Minor change to current component"/>
+    <n v="3"/>
+    <n v="3"/>
+    <n v="13.5"/>
+    <m/>
+    <x v="1"/>
+  </r>
+  <r>
+    <n v="36"/>
+    <s v="Dashboard and Main Menu"/>
+    <s v="Main menu"/>
+    <s v="Log out"/>
+    <s v="On clicking logout - should warn user before doing so"/>
+    <s v="Poor UX"/>
+    <s v="Improved UX"/>
+    <s v="New component/service with simple integration"/>
+    <n v="4"/>
+    <n v="4"/>
+    <n v="12.8"/>
+    <m/>
+    <x v="1"/>
+  </r>
+  <r>
+    <n v="37"/>
+    <s v="Navbar"/>
+    <s v="Drop down menu"/>
+    <s v="Log out"/>
+    <s v="On clicking logout - should warn user before doing so"/>
+    <s v="Poor UX"/>
+    <s v="Improved UX"/>
+    <s v="New component/service with simple integration"/>
+    <n v="4"/>
+    <n v="4"/>
+    <n v="12.8"/>
+    <m/>
+    <x v="1"/>
+  </r>
+  <r>
+    <n v="47"/>
+    <s v="Calendar/Appointments"/>
+    <s v="Appointments modal"/>
+    <s v="Cancelling/Voiding"/>
+    <s v="Cancelling the appointment should warn the user before the appointment is actually cancelled"/>
+    <s v="Poor UX"/>
+    <s v="Improved UX"/>
+    <s v="New component/service with simple integration"/>
+    <n v="4"/>
+    <n v="4"/>
+    <n v="12.8"/>
+    <m/>
+    <x v="1"/>
+  </r>
+  <r>
+    <n v="50"/>
+    <s v="Calendar/Appointments"/>
+    <s v="Appointments modal"/>
+    <s v="Cancelling/Voiding"/>
+    <s v="On cancelling a new appointment (after changes are made) should warn the user that changes will be lost"/>
+    <s v="Poor UX"/>
+    <s v="Improved UX"/>
+    <s v="New component/service with simple integration"/>
+    <n v="4"/>
+    <n v="4"/>
+    <n v="12.8"/>
+    <m/>
+    <x v="1"/>
+  </r>
+  <r>
+    <n v="56"/>
+    <s v="Calendar/Appointments"/>
+    <s v="Appointments modal"/>
+    <m/>
+    <s v="When cancelling an invoiced appoint and additional warning of the credit not needs to be provided"/>
+    <s v="Poor UX"/>
+    <s v="Improved UX"/>
+    <s v="New component/service with simple integration"/>
+    <n v="4"/>
+    <n v="4"/>
+    <n v="12.8"/>
+    <m/>
+    <x v="1"/>
+  </r>
+  <r>
+    <n v="41"/>
+    <s v="Calendar/Appointments"/>
+    <s v="Calendar"/>
+    <s v="Your calendar drop down"/>
+    <s v="The your calendar header should be a drop down that allows the user to see other staff members calendars_x000a_The drop down menu should be multi select_x000a_The differently coloured appointment blocks should have a border indicating whose calendar the appointment is from_x000a_"/>
+    <s v="Nice to have"/>
+    <s v="USP"/>
+    <s v="Whole new feature"/>
+    <n v="1"/>
+    <n v="10"/>
+    <n v="12.5"/>
+    <m/>
+    <x v="1"/>
+  </r>
+  <r>
+    <n v="52"/>
+    <s v="Finance - Payments"/>
+    <s v="Bulk uploads"/>
+    <m/>
+    <s v="Should be able to bulk upload payments_x000a_Should have a standard template_x000a_Should remember the reference - and assign based on that (where this has been seen before)"/>
+    <s v="Nice to have"/>
+    <s v="USP"/>
+    <s v="Whole new feature"/>
+    <n v="1"/>
+    <n v="10"/>
+    <n v="12.5"/>
+    <m/>
+    <x v="1"/>
+  </r>
+  <r>
+    <n v="65"/>
+    <s v="Finance - Invoicing"/>
+    <s v="PDF export"/>
+    <m/>
+    <s v="Should be able to export the invoice to PDF_x000a_Will required a lot more client and company detail_x000a_Should ask the user where to save it"/>
+    <s v="Nice to have"/>
+    <s v="USP"/>
+    <s v="Whole new feature"/>
+    <n v="1"/>
+    <n v="10"/>
+    <n v="12.5"/>
+    <m/>
+    <x v="1"/>
+  </r>
+  <r>
+    <n v="83"/>
+    <s v="Finance - Reports"/>
+    <s v="Profit and lose report"/>
+    <m/>
+    <s v="Mini profit and loss report_x000a_Should be able to select for a period "/>
+    <s v="Nice to have"/>
+    <s v="USP"/>
+    <s v="Whole new feature"/>
+    <n v="1"/>
+    <n v="10"/>
+    <n v="12.5"/>
+    <m/>
+    <x v="1"/>
+  </r>
+  <r>
+    <n v="102"/>
+    <s v="Finance - Accounting"/>
+    <s v="Statement runs"/>
+    <m/>
+    <s v="Client should be able to perform a statement run with a simple flow process_x000a_All clients statements are to be PDDd and saved to their folder along with their backing fin documents (invoice, credit notes etc , payment receipts)_x000a_User should be able to determine where the batch of documents is saved"/>
+    <s v="Nice to have"/>
+    <s v="USP"/>
+    <s v="Whole new feature"/>
+    <n v="1"/>
+    <n v="10"/>
+    <n v="12.5"/>
+    <m/>
+    <x v="1"/>
+  </r>
+  <r>
+    <n v="105"/>
+    <s v="User Management"/>
+    <s v="Profile portal"/>
+    <m/>
+    <s v="A portal where the client can_x000a_Update their details_x000a_Add new users to their account_x000a_Any other preferences they want"/>
+    <s v="Nice to have"/>
+    <s v="USP"/>
+    <s v="Whole new feature"/>
+    <n v="1"/>
+    <n v="10"/>
+    <n v="12.5"/>
+    <m/>
+    <x v="1"/>
+  </r>
+  <r>
+    <n v="33"/>
+    <s v="Dashboard and Main Menu"/>
+    <s v="Dashboard"/>
+    <m/>
+    <s v="New page: Dashboard_x000a_Should only be available on desktop_x000a_Should have a option to go to the main menu_x000a_Will contain a variety of reports and summaries"/>
+    <s v="Nice to have"/>
+    <s v="USP"/>
+    <s v="Whole new section"/>
+    <n v="1"/>
+    <n v="10"/>
+    <n v="10"/>
+    <m/>
+    <x v="1"/>
+  </r>
+  <r>
+    <n v="62"/>
+    <s v="Equipment/Assets"/>
+    <m/>
+    <m/>
+    <s v="New section required to add instructor to the client"/>
+    <s v="Nice to have"/>
+    <s v="USP"/>
+    <s v="Whole new section"/>
+    <n v="1"/>
+    <n v="10"/>
+    <n v="10"/>
+    <m/>
+    <x v="1"/>
+  </r>
+  <r>
+    <n v="63"/>
+    <s v="Staff management"/>
+    <m/>
+    <m/>
+    <s v="New section required to add horse to the client"/>
+    <s v="Nice to have"/>
+    <s v="USP"/>
+    <s v="Whole new section"/>
+    <n v="1"/>
+    <n v="10"/>
+    <n v="10"/>
+    <m/>
+    <x v="1"/>
+  </r>
+  <r>
+    <n v="82"/>
+    <s v="Finance - Accounting"/>
+    <s v="Bank statement importer"/>
+    <m/>
+    <s v="Should be able import a bank statement:_x000a_Would require use to allocate transactions_x000a_Transaction are to be remembered for future use_x000a_Should perform a quick recon calculation_x000a_Expenses should be able to be captured when paid (Later will be done on a invoice basis and then payments are allocated to supplier dues)"/>
+    <s v="Nice to have"/>
+    <s v="USP"/>
+    <s v="Whole new section"/>
+    <n v="1"/>
+    <n v="10"/>
+    <n v="10"/>
+    <m/>
+    <x v="1"/>
+  </r>
+  <r>
+    <n v="99"/>
+    <s v="Booking"/>
+    <s v="Lesson booking platform"/>
+    <m/>
+    <s v="A platform where a customer of the client can book their lessons, based on the slots the client has deemed and allowed as open"/>
+    <s v="Nice to have"/>
+    <s v="USP"/>
+    <s v="Whole new section"/>
+    <n v="1"/>
+    <n v="10"/>
+    <n v="10"/>
+    <m/>
+    <x v="1"/>
+  </r>
+  <r>
+    <n v="26"/>
+    <s v="Dashboard and Main Menu"/>
+    <s v="Main menu"/>
+    <m/>
+    <s v="As the screen gets wider - the buttons tend to lower - needs to be consistent"/>
+    <s v="Poor UI"/>
+    <s v="Improved UI"/>
+    <s v="Investigation and change"/>
+    <n v="3"/>
+    <n v="3"/>
+    <n v="9"/>
+    <m/>
+    <x v="1"/>
+  </r>
+  <r>
+    <n v="39"/>
+    <s v="Calendar/Appointments"/>
+    <s v="Calendar"/>
+    <m/>
+    <s v="On shorter screens - Schedule slot should have a minimum height"/>
+    <s v="Poor UI"/>
+    <s v="Improved UI"/>
+    <s v="Investigation and change"/>
+    <n v="3"/>
+    <n v="3"/>
+    <n v="9"/>
+    <m/>
+    <x v="1"/>
+  </r>
+  <r>
+    <n v="42"/>
+    <s v="Calendar/Appointments"/>
+    <s v="Appointments modal"/>
+    <m/>
+    <s v="On smaller screens the Date input is too far right"/>
+    <s v="Poor UI"/>
+    <s v="Improved UI"/>
+    <s v="Investigation and change"/>
+    <n v="3"/>
+    <n v="3"/>
+    <n v="9"/>
+    <m/>
+    <x v="1"/>
+  </r>
+  <r>
+    <n v="46"/>
+    <s v="Calendar/Appointments"/>
+    <s v="Appointments modal"/>
+    <m/>
+    <s v="On smaller screen the alignments need to be improved - specifically in the view only mode"/>
+    <s v="Poor UI"/>
+    <s v="Improved UI"/>
+    <s v="Investigation and change"/>
+    <n v="3"/>
+    <n v="3"/>
+    <n v="9"/>
+    <m/>
+    <x v="1"/>
+  </r>
+  <r>
+    <n v="68"/>
+    <s v="Finance - Invoicing"/>
+    <s v="Invoice list"/>
+    <m/>
+    <s v="Should have the ability to filter the list"/>
+    <s v="Nice to have"/>
+    <s v="Feature enhancement/fix"/>
+    <s v="Major change to current component"/>
+    <n v="1"/>
+    <n v="6"/>
+    <n v="9"/>
+    <m/>
+    <x v="1"/>
+  </r>
+  <r>
+    <n v="69"/>
+    <s v="Finance - Invoicing"/>
+    <s v="Invoice list"/>
+    <m/>
+    <s v="Should have the ability to sort the list"/>
+    <s v="Nice to have"/>
+    <s v="Feature enhancement/fix"/>
+    <s v="Major change to current component"/>
+    <n v="1"/>
+    <n v="6"/>
+    <n v="9"/>
+    <m/>
+    <x v="1"/>
+  </r>
+  <r>
+    <n v="70"/>
+    <s v="Finance - Invoicing"/>
+    <s v="Invoice list"/>
+    <m/>
+    <s v="List should be paginated"/>
+    <s v="Nice to have"/>
+    <s v="Feature enhancement/fix"/>
+    <s v="Major change to current component"/>
+    <n v="1"/>
+    <n v="6"/>
+    <n v="9"/>
+    <m/>
+    <x v="1"/>
+  </r>
+  <r>
+    <n v="75"/>
+    <s v="Finance - Invoicing"/>
+    <s v="Generate invoices"/>
+    <s v="Generate invoices results"/>
+    <s v="Needs to produce a summary of the invoices generated:_x000a_Number of invoices_x000a_Lessons invoices_x000a_Total revenue_x000a_Average revenue per invoices_x000a_Median invoice revenue_x000a_Largest and smallest invoices by revenue"/>
+    <s v="Nice to have"/>
+    <s v="Feature enhancement/fix"/>
+    <s v="Major change to current component"/>
+    <n v="1"/>
+    <n v="6"/>
+    <n v="9"/>
+    <m/>
+    <x v="1"/>
+  </r>
+  <r>
+    <n v="78"/>
+    <s v="Finance - Payments"/>
+    <s v="Payment modal"/>
+    <m/>
+    <s v="Payments should have a Type property (EFT vs Cash)"/>
+    <s v="Nice to have"/>
+    <s v="Feature enhancement/fix"/>
+    <s v="Major change to current component"/>
+    <n v="1"/>
+    <n v="6"/>
+    <n v="9"/>
+    <m/>
+    <x v="1"/>
+  </r>
+  <r>
+    <n v="110"/>
+    <s v="General"/>
+    <m/>
+    <m/>
+    <s v="Modal screens are still scrollable - when the sheath should prevent that"/>
+    <s v="Poor UI"/>
+    <s v="Improved UI"/>
+    <s v="Investigation and change"/>
+    <n v="3"/>
+    <n v="3"/>
+    <n v="9"/>
+    <m/>
+    <x v="1"/>
+  </r>
+  <r>
+    <n v="51"/>
+    <s v="General"/>
+    <s v="Warnings"/>
+    <m/>
+    <s v="Warnings should have an option to allow users to not see them again"/>
+    <s v="Nice to have"/>
+    <s v="New feature"/>
+    <s v="New component/service with complex integration"/>
+    <n v="1"/>
+    <n v="7"/>
+    <n v="7"/>
+    <m/>
+    <x v="1"/>
+  </r>
+  <r>
+    <n v="28"/>
+    <s v="Dashboard and Main Menu"/>
+    <s v="Main menu"/>
+    <m/>
+    <s v="There should be a view for desktop where the button become a grid of square buttons with icons"/>
+    <s v="Poor UI"/>
+    <s v="Improved UI"/>
+    <s v="Major change to current component"/>
+    <n v="3"/>
+    <n v="3"/>
+    <n v="6.75"/>
+    <m/>
+    <x v="1"/>
+  </r>
+  <r>
+    <n v="111"/>
+    <s v="Finance - Invoicing"/>
+    <s v="Generate invoices"/>
+    <m/>
+    <s v="Invoices do not need a voided property as they can't be voided - only credit noted"/>
+    <s v="Poor UX"/>
+    <s v="Refactor/Tech debt"/>
     <s v="Minor change to current component"/>
     <n v="4"/>
-    <n v="6"/>
-    <n v="72"/>
+    <n v="1"/>
     <n v="2"/>
+    <m/>
+    <x v="1"/>
+  </r>
+  <r>
+    <n v="29"/>
+    <s v="Dashboard and Main Menu"/>
+    <s v="Main menu"/>
+    <m/>
+    <s v="Needs to use the new view service to determine its required state"/>
+    <s v="Poor UI"/>
+    <s v="Refactor/Tech debt"/>
+    <s v="Minor change to current component"/>
+    <n v="3"/>
+    <n v="1"/>
+    <n v="1.5"/>
+    <n v="27"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <n v="30"/>
+    <s v="Navbar"/>
+    <m/>
+    <m/>
+    <s v="Needs to use the new view service to determine its required state"/>
+    <s v="Poor UI"/>
+    <s v="Refactor/Tech debt"/>
+    <s v="Minor change to current component"/>
+    <n v="3"/>
+    <n v="1"/>
+    <n v="1.5"/>
+    <n v="27"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <n v="27"/>
+    <s v="General"/>
+    <s v="Utility services"/>
+    <m/>
+    <s v="There needs to be a service that determine whether the view should be mobile or desktop"/>
+    <s v="Poor UI"/>
+    <s v="Refactor/Tech debt"/>
+    <s v="New component/service with complex integration"/>
+    <n v="3"/>
+    <n v="1"/>
+    <n v="0.42857142857142855"/>
+    <m/>
     <x v="1"/>
   </r>
   <r>
@@ -2629,7 +2629,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{936C0618-B7B4-0144-93D9-409C5361BBD7}" name="PivotTable7" cacheId="10" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{936C0618-B7B4-0144-93D9-409C5361BBD7}" name="PivotTable7" cacheId="4" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A7:D9" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="13">
     <pivotField showAll="0"/>
@@ -2685,7 +2685,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{4A183E6E-2837-3A40-90CB-E731BF47E9C0}" name="PivotTable6" cacheId="10" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{4A183E6E-2837-3A40-90CB-E731BF47E9C0}" name="PivotTable6" cacheId="4" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A1:D3" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="13">
     <pivotField showAll="0"/>
@@ -2741,7 +2741,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{4DCC3165-0959-AA43-80CF-D9170B1DCB64}" name="PivotTable8" cacheId="10" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{4DCC3165-0959-AA43-80CF-D9170B1DCB64}" name="PivotTable8" cacheId="4" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A13:D15" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="13">
     <pivotField showAll="0"/>
@@ -3096,7 +3096,7 @@
   <dimension ref="A1:D17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3128,10 +3128,10 @@
         <v>206</v>
       </c>
       <c r="B3" s="8">
-        <v>1077</v>
+        <v>1116.2</v>
       </c>
       <c r="C3" s="8">
-        <v>2150.5976190476176</v>
+        <v>2111.3976190476178</v>
       </c>
       <c r="D3" s="8">
         <v>3227.5976190476176</v>
@@ -3140,7 +3140,7 @@
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="D5" s="7">
         <f>GETPIVOTDATA("Priority S",$A$1,"Status","Done")/GETPIVOTDATA("Priority S",$A$1)</f>
-        <v>0.33368471758812224</v>
+        <v>0.34582997379002978</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
@@ -3164,10 +3164,10 @@
         <v>183</v>
       </c>
       <c r="B9" s="8">
-        <v>89</v>
+        <v>93</v>
       </c>
       <c r="C9" s="8">
-        <v>283</v>
+        <v>279</v>
       </c>
       <c r="D9" s="8">
         <v>372</v>
@@ -3176,7 +3176,7 @@
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="D11" s="7">
         <f>GETPIVOTDATA("Importance S",$A$7,"Status","Done")/GETPIVOTDATA("Importance S",$A$7)</f>
-        <v>0.239247311827957</v>
+        <v>0.25</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
@@ -3200,10 +3200,10 @@
         <v>184</v>
       </c>
       <c r="B15" s="8">
-        <v>82</v>
+        <v>89</v>
       </c>
       <c r="C15" s="8">
-        <v>591</v>
+        <v>584</v>
       </c>
       <c r="D15" s="8">
         <v>673</v>
@@ -3212,7 +3212,7 @@
     <row r="17" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D17" s="7">
         <f>GETPIVOTDATA("Impact S",$A$13,"Status","Done")/GETPIVOTDATA("Impact S",$A$13)</f>
-        <v>0.12184249628528974</v>
+        <v>0.13224368499257058</v>
       </c>
     </row>
   </sheetData>
@@ -3647,7 +3647,7 @@
   <dimension ref="A1:XEX117"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+      <selection activeCell="A20" sqref="A20:XFD20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="34.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -9471,41 +9471,45 @@
       </c>
     </row>
     <row r="20" spans="1:13" ht="17" x14ac:dyDescent="0.2">
-      <c r="A20">
+      <c r="A20" s="3">
         <v>4</v>
       </c>
-      <c r="B20" t="s">
+      <c r="B20" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="C20" t="s">
+      <c r="C20" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="D20" t="s">
+      <c r="D20" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="E20" s="2" t="s">
+      <c r="E20" s="4" t="s">
         <v>95</v>
       </c>
-      <c r="F20" t="s">
+      <c r="F20" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="G20" t="s">
+      <c r="G20" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="H20" t="s">
+      <c r="H20" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="I20" s="1">
+      <c r="I20" s="5">
         <f>VLOOKUP(F20,'Source lists'!$E$1:F21,2,FALSE)</f>
         <v>4</v>
       </c>
-      <c r="J20" s="1">
+      <c r="J20" s="5">
         <f>VLOOKUP(G20,'Source lists'!$H$1:I22,2,FALSE)</f>
         <v>7</v>
       </c>
-      <c r="K20" s="1">
+      <c r="K20" s="5">
         <f>VLOOKUP(F20,'Source lists'!$E$2:$F$6,2,FALSE)*(VLOOKUP(G20,'Source lists'!$H$2:$I$7,2,FALSE)^2)/VLOOKUP(H20,'Source lists'!$K$2:$L$9,2,FALSE)</f>
         <v>39.200000000000003</v>
+      </c>
+      <c r="L20" s="3"/>
+      <c r="M20" s="3" t="s">
+        <v>176</v>
       </c>
     </row>
     <row r="21" spans="1:13" ht="17" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
e-Questrian/pages/landing: Overall minor styling improvements made
</commit_message>
<xml_diff>
--- a/apps/e-questrian/e-Questrian - To do list.xlsx
+++ b/apps/e-questrian/e-Questrian - To do list.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rferreira/sigmafox/apps/e-questrian/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50D5CC8A-2550-304E-9168-C1A9D5E635F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A6B1278-B0D5-614F-BA21-F33C67100DDE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="19820" activeTab="2" xr2:uid="{DC2B379E-A936-2146-8C4F-53C43AECE05C}"/>
+    <workbookView xWindow="0" yWindow="740" windowWidth="34560" windowHeight="21600" activeTab="2" xr2:uid="{DC2B379E-A936-2146-8C4F-53C43AECE05C}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary of completion" sheetId="3" r:id="rId1"/>
@@ -22,7 +22,7 @@
   </definedNames>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="4" r:id="rId4"/>
+    <pivotCache cacheId="0" r:id="rId4"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="860" uniqueCount="215">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="869" uniqueCount="216">
   <si>
     <t>Sections</t>
   </si>
@@ -723,6 +723,9 @@
   </si>
   <si>
     <t>Features Section</t>
+  </si>
+  <si>
+    <t>Why us section</t>
   </si>
 </sst>
 </file>
@@ -778,7 +781,7 @@
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -791,7 +794,6 @@
     <xf numFmtId="43" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -2629,7 +2631,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{936C0618-B7B4-0144-93D9-409C5361BBD7}" name="PivotTable7" cacheId="4" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{936C0618-B7B4-0144-93D9-409C5361BBD7}" name="PivotTable7" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A7:D9" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="13">
     <pivotField showAll="0"/>
@@ -2685,7 +2687,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{4A183E6E-2837-3A40-90CB-E731BF47E9C0}" name="PivotTable6" cacheId="4" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{4A183E6E-2837-3A40-90CB-E731BF47E9C0}" name="PivotTable6" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A1:D3" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="13">
     <pivotField showAll="0"/>
@@ -2741,7 +2743,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{4DCC3165-0959-AA43-80CF-D9170B1DCB64}" name="PivotTable8" cacheId="4" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{4DCC3165-0959-AA43-80CF-D9170B1DCB64}" name="PivotTable8" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A13:D15" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="13">
     <pivotField showAll="0"/>
@@ -3127,13 +3129,13 @@
       <c r="A3" t="s">
         <v>206</v>
       </c>
-      <c r="B3" s="8">
+      <c r="B3">
         <v>1116.2</v>
       </c>
-      <c r="C3" s="8">
+      <c r="C3">
         <v>2111.3976190476178</v>
       </c>
-      <c r="D3" s="8">
+      <c r="D3">
         <v>3227.5976190476176</v>
       </c>
     </row>
@@ -3163,13 +3165,13 @@
       <c r="A9" t="s">
         <v>183</v>
       </c>
-      <c r="B9" s="8">
+      <c r="B9">
         <v>93</v>
       </c>
-      <c r="C9" s="8">
+      <c r="C9">
         <v>279</v>
       </c>
-      <c r="D9" s="8">
+      <c r="D9">
         <v>372</v>
       </c>
     </row>
@@ -3199,13 +3201,13 @@
       <c r="A15" t="s">
         <v>184</v>
       </c>
-      <c r="B15" s="8">
+      <c r="B15">
         <v>89</v>
       </c>
-      <c r="C15" s="8">
+      <c r="C15">
         <v>584</v>
       </c>
-      <c r="D15" s="8">
+      <c r="D15">
         <v>673</v>
       </c>
     </row>
@@ -3225,7 +3227,7 @@
   <dimension ref="A1:L33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3563,6 +3565,9 @@
       <c r="B19" t="s">
         <v>128</v>
       </c>
+      <c r="C19" t="s">
+        <v>215</v>
+      </c>
     </row>
     <row r="20" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B20" t="s">
@@ -3644,10 +3649,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1EB57299-5CFD-7049-BDE4-6415040FFB14}">
-  <dimension ref="A1:XEX117"/>
+  <dimension ref="A1:XEX118"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="A20" sqref="A20:XFD20"/>
+      <selection activeCell="G22" sqref="G22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="34.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -9552,8 +9557,7 @@
     </row>
     <row r="22" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="A22">
-        <f>A61</f>
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B22" t="s">
         <v>39</v>
@@ -9562,7 +9566,7 @@
         <v>33</v>
       </c>
       <c r="D22" t="s">
-        <v>68</v>
+        <v>215</v>
       </c>
       <c r="E22" s="2" t="s">
         <v>95</v>
@@ -9577,11 +9581,11 @@
         <v>70</v>
       </c>
       <c r="I22" s="1">
-        <f>VLOOKUP(F22,'Source lists'!$E$1:F20,2,FALSE)</f>
+        <f>VLOOKUP(F22,'Source lists'!$E$1:F23,2,FALSE)</f>
         <v>4</v>
       </c>
       <c r="J22" s="1">
-        <f>VLOOKUP(G22,'Source lists'!$H$1:I21,2,FALSE)</f>
+        <f>VLOOKUP(G22,'Source lists'!$H$1:I24,2,FALSE)</f>
         <v>7</v>
       </c>
       <c r="K22" s="1">
@@ -9589,47 +9593,52 @@
         <v>39.200000000000003</v>
       </c>
     </row>
-    <row r="23" spans="1:13" ht="136" x14ac:dyDescent="0.2">
-      <c r="A23">
-        <v>24</v>
-      </c>
-      <c r="B23" t="s">
-        <v>8</v>
-      </c>
-      <c r="C23" t="s">
-        <v>42</v>
-      </c>
-      <c r="D23" t="s">
-        <v>64</v>
-      </c>
-      <c r="E23" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="F23" t="s">
+    <row r="23" spans="1:13" ht="17" x14ac:dyDescent="0.2">
+      <c r="A23" s="3">
+        <f>A62</f>
+        <v>18</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="C23" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D23" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="E23" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="F23" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="G23" t="s">
+      <c r="G23" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="H23" t="s">
+      <c r="H23" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="I23" s="1">
-        <f>VLOOKUP(F23,'Source lists'!$E$1:F23,2,FALSE)</f>
+      <c r="I23" s="5">
+        <f>VLOOKUP(F23,'Source lists'!$E$1:F20,2,FALSE)</f>
         <v>4</v>
       </c>
-      <c r="J23" s="1">
-        <f>VLOOKUP(G23,'Source lists'!$H$1:I24,2,FALSE)</f>
+      <c r="J23" s="5">
+        <f>VLOOKUP(G23,'Source lists'!$H$1:I21,2,FALSE)</f>
         <v>7</v>
       </c>
-      <c r="K23" s="1">
+      <c r="K23" s="5">
         <f>VLOOKUP(F23,'Source lists'!$E$2:$F$6,2,FALSE)*(VLOOKUP(G23,'Source lists'!$H$2:$I$7,2,FALSE)^2)/VLOOKUP(H23,'Source lists'!$K$2:$L$9,2,FALSE)</f>
         <v>39.200000000000003</v>
       </c>
-    </row>
-    <row r="24" spans="1:13" ht="34" x14ac:dyDescent="0.2">
+      <c r="L23" s="3"/>
+      <c r="M23" s="3" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" ht="136" x14ac:dyDescent="0.2">
       <c r="A24">
-        <v>7</v>
+        <v>24</v>
       </c>
       <c r="B24" t="s">
         <v>8</v>
@@ -9637,34 +9646,37 @@
       <c r="C24" t="s">
         <v>42</v>
       </c>
+      <c r="D24" t="s">
+        <v>64</v>
+      </c>
       <c r="E24" s="2" t="s">
-        <v>43</v>
+        <v>72</v>
       </c>
       <c r="F24" t="s">
         <v>15</v>
       </c>
       <c r="G24" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="H24" t="s">
-        <v>23</v>
+        <v>70</v>
       </c>
       <c r="I24" s="1">
-        <f>VLOOKUP(F24,'Source lists'!$E$1:F24,2,FALSE)</f>
+        <f>VLOOKUP(F24,'Source lists'!$E$1:F23,2,FALSE)</f>
         <v>4</v>
       </c>
       <c r="J24" s="1">
-        <f>VLOOKUP(G24,'Source lists'!$H$1:I25,2,FALSE)</f>
-        <v>4</v>
+        <f>VLOOKUP(G24,'Source lists'!$H$1:I24,2,FALSE)</f>
+        <v>7</v>
       </c>
       <c r="K24" s="1">
         <f>VLOOKUP(F24,'Source lists'!$E$2:$F$6,2,FALSE)*(VLOOKUP(G24,'Source lists'!$H$2:$I$7,2,FALSE)^2)/VLOOKUP(H24,'Source lists'!$K$2:$L$9,2,FALSE)</f>
-        <v>32</v>
-      </c>
-    </row>
-    <row r="25" spans="1:13" ht="17" x14ac:dyDescent="0.2">
+        <v>39.200000000000003</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" ht="34" x14ac:dyDescent="0.2">
       <c r="A25">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B25" t="s">
         <v>8</v>
@@ -9672,11 +9684,8 @@
       <c r="C25" t="s">
         <v>42</v>
       </c>
-      <c r="D25" t="s">
-        <v>44</v>
-      </c>
       <c r="E25" s="2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="F25" t="s">
         <v>15</v>
@@ -9688,24 +9697,21 @@
         <v>23</v>
       </c>
       <c r="I25" s="1">
-        <f>VLOOKUP(F25,'Source lists'!$E$1:F25,2,FALSE)</f>
+        <f>VLOOKUP(F25,'Source lists'!$E$1:F24,2,FALSE)</f>
         <v>4</v>
       </c>
       <c r="J25" s="1">
-        <f>VLOOKUP(G25,'Source lists'!$H$1:I26,2,FALSE)</f>
+        <f>VLOOKUP(G25,'Source lists'!$H$1:I25,2,FALSE)</f>
         <v>4</v>
       </c>
       <c r="K25" s="1">
         <f>VLOOKUP(F25,'Source lists'!$E$2:$F$6,2,FALSE)*(VLOOKUP(G25,'Source lists'!$H$2:$I$7,2,FALSE)^2)/VLOOKUP(H25,'Source lists'!$K$2:$L$9,2,FALSE)</f>
         <v>32</v>
       </c>
-      <c r="L25">
-        <v>8</v>
-      </c>
     </row>
     <row r="26" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="A26">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B26" t="s">
         <v>8</v>
@@ -9717,7 +9723,7 @@
         <v>44</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="F26" t="s">
         <v>15</v>
@@ -9729,11 +9735,11 @@
         <v>23</v>
       </c>
       <c r="I26" s="1">
-        <f>VLOOKUP(F26,'Source lists'!$E$1:F26,2,FALSE)</f>
+        <f>VLOOKUP(F26,'Source lists'!$E$1:F25,2,FALSE)</f>
         <v>4</v>
       </c>
       <c r="J26" s="1">
-        <f>VLOOKUP(G26,'Source lists'!$H$1:I27,2,FALSE)</f>
+        <f>VLOOKUP(G26,'Source lists'!$H$1:I26,2,FALSE)</f>
         <v>4</v>
       </c>
       <c r="K26" s="1">
@@ -9746,7 +9752,7 @@
     </row>
     <row r="27" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="A27">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B27" t="s">
         <v>8</v>
@@ -9758,7 +9764,7 @@
         <v>44</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F27" t="s">
         <v>15</v>
@@ -9770,11 +9776,11 @@
         <v>23</v>
       </c>
       <c r="I27" s="1">
-        <f>VLOOKUP(F27,'Source lists'!$E$1:F27,2,FALSE)</f>
+        <f>VLOOKUP(F27,'Source lists'!$E$1:F26,2,FALSE)</f>
         <v>4</v>
       </c>
       <c r="J27" s="1">
-        <f>VLOOKUP(G27,'Source lists'!$H$1:I28,2,FALSE)</f>
+        <f>VLOOKUP(G27,'Source lists'!$H$1:I27,2,FALSE)</f>
         <v>4</v>
       </c>
       <c r="K27" s="1">
@@ -9787,7 +9793,7 @@
     </row>
     <row r="28" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="A28">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B28" t="s">
         <v>8</v>
@@ -9799,7 +9805,7 @@
         <v>44</v>
       </c>
       <c r="E28" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F28" t="s">
         <v>15</v>
@@ -9811,11 +9817,11 @@
         <v>23</v>
       </c>
       <c r="I28" s="1">
-        <f>VLOOKUP(F28,'Source lists'!$E$1:F28,2,FALSE)</f>
+        <f>VLOOKUP(F28,'Source lists'!$E$1:F27,2,FALSE)</f>
         <v>4</v>
       </c>
       <c r="J28" s="1">
-        <f>VLOOKUP(G28,'Source lists'!$H$1:I29,2,FALSE)</f>
+        <f>VLOOKUP(G28,'Source lists'!$H$1:I28,2,FALSE)</f>
         <v>4</v>
       </c>
       <c r="K28" s="1">
@@ -9828,19 +9834,19 @@
     </row>
     <row r="29" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="A29">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B29" t="s">
         <v>8</v>
       </c>
       <c r="C29" t="s">
-        <v>208</v>
+        <v>42</v>
       </c>
       <c r="D29" t="s">
-        <v>211</v>
+        <v>44</v>
       </c>
       <c r="E29" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F29" t="s">
         <v>15</v>
@@ -9852,11 +9858,11 @@
         <v>23</v>
       </c>
       <c r="I29" s="1">
-        <f>VLOOKUP(F29,'Source lists'!$E$1:F29,2,FALSE)</f>
+        <f>VLOOKUP(F29,'Source lists'!$E$1:F28,2,FALSE)</f>
         <v>4</v>
       </c>
       <c r="J29" s="1">
-        <f>VLOOKUP(G29,'Source lists'!$H$1:I30,2,FALSE)</f>
+        <f>VLOOKUP(G29,'Source lists'!$H$1:I29,2,FALSE)</f>
         <v>4</v>
       </c>
       <c r="K29" s="1">
@@ -9869,7 +9875,7 @@
     </row>
     <row r="30" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="A30">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B30" t="s">
         <v>8</v>
@@ -9881,7 +9887,7 @@
         <v>211</v>
       </c>
       <c r="E30" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F30" t="s">
         <v>15</v>
@@ -9893,11 +9899,11 @@
         <v>23</v>
       </c>
       <c r="I30" s="1">
-        <f>VLOOKUP(F30,'Source lists'!$E$1:F30,2,FALSE)</f>
+        <f>VLOOKUP(F30,'Source lists'!$E$1:F29,2,FALSE)</f>
         <v>4</v>
       </c>
       <c r="J30" s="1">
-        <f>VLOOKUP(G30,'Source lists'!$H$1:I31,2,FALSE)</f>
+        <f>VLOOKUP(G30,'Source lists'!$H$1:I30,2,FALSE)</f>
         <v>4</v>
       </c>
       <c r="K30" s="1">
@@ -9910,7 +9916,7 @@
     </row>
     <row r="31" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="A31">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B31" t="s">
         <v>8</v>
@@ -9922,7 +9928,7 @@
         <v>211</v>
       </c>
       <c r="E31" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F31" t="s">
         <v>15</v>
@@ -9934,11 +9940,11 @@
         <v>23</v>
       </c>
       <c r="I31" s="1">
-        <f>VLOOKUP(F31,'Source lists'!$E$1:F31,2,FALSE)</f>
+        <f>VLOOKUP(F31,'Source lists'!$E$1:F30,2,FALSE)</f>
         <v>4</v>
       </c>
       <c r="J31" s="1">
-        <f>VLOOKUP(G31,'Source lists'!$H$1:I32,2,FALSE)</f>
+        <f>VLOOKUP(G31,'Source lists'!$H$1:I31,2,FALSE)</f>
         <v>4</v>
       </c>
       <c r="K31" s="1">
@@ -9951,7 +9957,7 @@
     </row>
     <row r="32" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="A32">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B32" t="s">
         <v>8</v>
@@ -9963,7 +9969,7 @@
         <v>211</v>
       </c>
       <c r="E32" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F32" t="s">
         <v>15</v>
@@ -9975,11 +9981,11 @@
         <v>23</v>
       </c>
       <c r="I32" s="1">
-        <f>VLOOKUP(F32,'Source lists'!$E$1:F32,2,FALSE)</f>
+        <f>VLOOKUP(F32,'Source lists'!$E$1:F31,2,FALSE)</f>
         <v>4</v>
       </c>
       <c r="J32" s="1">
-        <f>VLOOKUP(G32,'Source lists'!$H$1:I33,2,FALSE)</f>
+        <f>VLOOKUP(G32,'Source lists'!$H$1:I32,2,FALSE)</f>
         <v>4</v>
       </c>
       <c r="K32" s="1">
@@ -9992,7 +9998,7 @@
     </row>
     <row r="33" spans="1:12" ht="17" x14ac:dyDescent="0.2">
       <c r="A33">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="B33" t="s">
         <v>8</v>
@@ -10000,8 +10006,11 @@
       <c r="C33" t="s">
         <v>208</v>
       </c>
+      <c r="D33" t="s">
+        <v>211</v>
+      </c>
       <c r="E33" s="2" t="s">
-        <v>63</v>
+        <v>53</v>
       </c>
       <c r="F33" t="s">
         <v>15</v>
@@ -10013,30 +10022,33 @@
         <v>23</v>
       </c>
       <c r="I33" s="1">
-        <f>VLOOKUP(F33,'Source lists'!$E$1:F33,2,FALSE)</f>
+        <f>VLOOKUP(F33,'Source lists'!$E$1:F32,2,FALSE)</f>
         <v>4</v>
       </c>
       <c r="J33" s="1">
-        <f>VLOOKUP(G33,'Source lists'!$H$1:I34,2,FALSE)</f>
+        <f>VLOOKUP(G33,'Source lists'!$H$1:I33,2,FALSE)</f>
         <v>4</v>
       </c>
       <c r="K33" s="1">
         <f>VLOOKUP(F33,'Source lists'!$E$2:$F$6,2,FALSE)*(VLOOKUP(G33,'Source lists'!$H$2:$I$7,2,FALSE)^2)/VLOOKUP(H33,'Source lists'!$K$2:$L$9,2,FALSE)</f>
         <v>32</v>
       </c>
-    </row>
-    <row r="34" spans="1:12" ht="34" x14ac:dyDescent="0.2">
+      <c r="L33">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="34" spans="1:12" ht="17" x14ac:dyDescent="0.2">
       <c r="A34">
-        <v>31</v>
+        <v>23</v>
       </c>
       <c r="B34" t="s">
-        <v>38</v>
+        <v>8</v>
       </c>
       <c r="C34" t="s">
-        <v>80</v>
+        <v>208</v>
       </c>
       <c r="E34" s="2" t="s">
-        <v>115</v>
+        <v>63</v>
       </c>
       <c r="F34" t="s">
         <v>15</v>
@@ -10048,11 +10060,11 @@
         <v>23</v>
       </c>
       <c r="I34" s="1">
-        <f>VLOOKUP(F34,'Source lists'!$E$1:F34,2,FALSE)</f>
+        <f>VLOOKUP(F34,'Source lists'!$E$1:F33,2,FALSE)</f>
         <v>4</v>
       </c>
       <c r="J34" s="1">
-        <f>VLOOKUP(G34,'Source lists'!$H$1:I35,2,FALSE)</f>
+        <f>VLOOKUP(G34,'Source lists'!$H$1:I34,2,FALSE)</f>
         <v>4</v>
       </c>
       <c r="K34" s="1">
@@ -10062,7 +10074,7 @@
     </row>
     <row r="35" spans="1:12" ht="34" x14ac:dyDescent="0.2">
       <c r="A35">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="B35" t="s">
         <v>38</v>
@@ -10070,11 +10082,8 @@
       <c r="C35" t="s">
         <v>80</v>
       </c>
-      <c r="D35" t="s">
-        <v>85</v>
-      </c>
       <c r="E35" s="2" t="s">
-        <v>83</v>
+        <v>115</v>
       </c>
       <c r="F35" t="s">
         <v>15</v>
@@ -10086,11 +10095,11 @@
         <v>23</v>
       </c>
       <c r="I35" s="1">
-        <f>VLOOKUP(F35,'Source lists'!$E$1:F35,2,FALSE)</f>
+        <f>VLOOKUP(F35,'Source lists'!$E$1:F34,2,FALSE)</f>
         <v>4</v>
       </c>
       <c r="J35" s="1">
-        <f>VLOOKUP(G35,'Source lists'!$H$1:I36,2,FALSE)</f>
+        <f>VLOOKUP(G35,'Source lists'!$H$1:I35,2,FALSE)</f>
         <v>4</v>
       </c>
       <c r="K35" s="1">
@@ -10100,16 +10109,19 @@
     </row>
     <row r="36" spans="1:12" ht="34" x14ac:dyDescent="0.2">
       <c r="A36">
-        <v>54</v>
+        <v>34</v>
       </c>
       <c r="B36" t="s">
-        <v>1</v>
+        <v>38</v>
       </c>
       <c r="C36" t="s">
-        <v>91</v>
+        <v>80</v>
+      </c>
+      <c r="D36" t="s">
+        <v>85</v>
       </c>
       <c r="E36" s="2" t="s">
-        <v>105</v>
+        <v>83</v>
       </c>
       <c r="F36" t="s">
         <v>15</v>
@@ -10121,11 +10133,11 @@
         <v>23</v>
       </c>
       <c r="I36" s="1">
-        <f>VLOOKUP(F36,'Source lists'!$E$1:F36,2,FALSE)</f>
+        <f>VLOOKUP(F36,'Source lists'!$E$1:F35,2,FALSE)</f>
         <v>4</v>
       </c>
       <c r="J36" s="1">
-        <f>VLOOKUP(G36,'Source lists'!$H$1:I37,2,FALSE)</f>
+        <f>VLOOKUP(G36,'Source lists'!$H$1:I36,2,FALSE)</f>
         <v>4</v>
       </c>
       <c r="K36" s="1">
@@ -10135,16 +10147,16 @@
     </row>
     <row r="37" spans="1:12" ht="34" x14ac:dyDescent="0.2">
       <c r="A37">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B37" t="s">
         <v>1</v>
       </c>
       <c r="C37" t="s">
-        <v>87</v>
+        <v>91</v>
       </c>
       <c r="E37" s="2" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="F37" t="s">
         <v>15</v>
@@ -10156,11 +10168,11 @@
         <v>23</v>
       </c>
       <c r="I37" s="1">
-        <f>VLOOKUP(F37,'Source lists'!$E$1:F37,2,FALSE)</f>
+        <f>VLOOKUP(F37,'Source lists'!$E$1:F36,2,FALSE)</f>
         <v>4</v>
       </c>
       <c r="J37" s="1">
-        <f>VLOOKUP(G37,'Source lists'!$H$1:I38,2,FALSE)</f>
+        <f>VLOOKUP(G37,'Source lists'!$H$1:I37,2,FALSE)</f>
         <v>4</v>
       </c>
       <c r="K37" s="1">
@@ -10168,18 +10180,18 @@
         <v>32</v>
       </c>
     </row>
-    <row r="38" spans="1:12" ht="68" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:12" ht="34" x14ac:dyDescent="0.2">
       <c r="A38">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="B38" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C38" t="s">
-        <v>106</v>
+        <v>87</v>
       </c>
       <c r="E38" s="2" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="F38" t="s">
         <v>15</v>
@@ -10191,11 +10203,11 @@
         <v>23</v>
       </c>
       <c r="I38" s="1">
-        <f>VLOOKUP(F38,'Source lists'!$E$1:F38,2,FALSE)</f>
+        <f>VLOOKUP(F38,'Source lists'!$E$1:F37,2,FALSE)</f>
         <v>4</v>
       </c>
       <c r="J38" s="1">
-        <f>VLOOKUP(G38,'Source lists'!$H$1:I39,2,FALSE)</f>
+        <f>VLOOKUP(G38,'Source lists'!$H$1:I38,2,FALSE)</f>
         <v>4</v>
       </c>
       <c r="K38" s="1">
@@ -10203,9 +10215,9 @@
         <v>32</v>
       </c>
     </row>
-    <row r="39" spans="1:12" ht="17" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:12" ht="68" x14ac:dyDescent="0.2">
       <c r="A39">
-        <v>67</v>
+        <v>58</v>
       </c>
       <c r="B39" t="s">
         <v>2</v>
@@ -10214,7 +10226,7 @@
         <v>106</v>
       </c>
       <c r="E39" s="2" t="s">
-        <v>130</v>
+        <v>108</v>
       </c>
       <c r="F39" t="s">
         <v>15</v>
@@ -10226,11 +10238,11 @@
         <v>23</v>
       </c>
       <c r="I39" s="1">
-        <f>VLOOKUP(F39,'Source lists'!$E$1:F39,2,FALSE)</f>
+        <f>VLOOKUP(F39,'Source lists'!$E$1:F38,2,FALSE)</f>
         <v>4</v>
       </c>
       <c r="J39" s="1">
-        <f>VLOOKUP(G39,'Source lists'!$H$1:I40,2,FALSE)</f>
+        <f>VLOOKUP(G39,'Source lists'!$H$1:I39,2,FALSE)</f>
         <v>4</v>
       </c>
       <c r="K39" s="1">
@@ -10238,18 +10250,18 @@
         <v>32</v>
       </c>
     </row>
-    <row r="40" spans="1:12" ht="34" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:12" ht="17" x14ac:dyDescent="0.2">
       <c r="A40">
-        <v>84</v>
+        <v>67</v>
       </c>
       <c r="B40" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="C40" t="s">
-        <v>150</v>
+        <v>106</v>
       </c>
       <c r="E40" s="2" t="s">
-        <v>151</v>
+        <v>130</v>
       </c>
       <c r="F40" t="s">
         <v>15</v>
@@ -10261,11 +10273,11 @@
         <v>23</v>
       </c>
       <c r="I40" s="1">
-        <f>VLOOKUP(F40,'Source lists'!$E$1:F40,2,FALSE)</f>
+        <f>VLOOKUP(F40,'Source lists'!$E$1:F39,2,FALSE)</f>
         <v>4</v>
       </c>
       <c r="J40" s="1">
-        <f>VLOOKUP(G40,'Source lists'!$H$1:I41,2,FALSE)</f>
+        <f>VLOOKUP(G40,'Source lists'!$H$1:I40,2,FALSE)</f>
         <v>4</v>
       </c>
       <c r="K40" s="1">
@@ -10273,9 +10285,9 @@
         <v>32</v>
       </c>
     </row>
-    <row r="41" spans="1:12" ht="17" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:12" ht="34" x14ac:dyDescent="0.2">
       <c r="A41">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="B41" t="s">
         <v>6</v>
@@ -10284,7 +10296,7 @@
         <v>150</v>
       </c>
       <c r="E41" s="2" t="s">
-        <v>157</v>
+        <v>151</v>
       </c>
       <c r="F41" t="s">
         <v>15</v>
@@ -10296,11 +10308,11 @@
         <v>23</v>
       </c>
       <c r="I41" s="1">
-        <f>VLOOKUP(F41,'Source lists'!$E$1:F41,2,FALSE)</f>
+        <f>VLOOKUP(F41,'Source lists'!$E$1:F40,2,FALSE)</f>
         <v>4</v>
       </c>
       <c r="J41" s="1">
-        <f>VLOOKUP(G41,'Source lists'!$H$1:I42,2,FALSE)</f>
+        <f>VLOOKUP(G41,'Source lists'!$H$1:I41,2,FALSE)</f>
         <v>4</v>
       </c>
       <c r="K41" s="1">
@@ -10308,18 +10320,18 @@
         <v>32</v>
       </c>
     </row>
-    <row r="42" spans="1:12" ht="34" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:12" ht="17" x14ac:dyDescent="0.2">
       <c r="A42">
-        <v>107</v>
+        <v>89</v>
       </c>
       <c r="B42" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="C42" t="s">
-        <v>140</v>
+        <v>150</v>
       </c>
       <c r="E42" s="2" t="s">
-        <v>186</v>
+        <v>157</v>
       </c>
       <c r="F42" t="s">
         <v>15</v>
@@ -10331,11 +10343,11 @@
         <v>23</v>
       </c>
       <c r="I42" s="1">
-        <f>VLOOKUP(F42,'Source lists'!$E$1:F42,2,FALSE)</f>
+        <f>VLOOKUP(F42,'Source lists'!$E$1:F41,2,FALSE)</f>
         <v>4</v>
       </c>
       <c r="J42" s="1">
-        <f>VLOOKUP(G42,'Source lists'!$H$1:I43,2,FALSE)</f>
+        <f>VLOOKUP(G42,'Source lists'!$H$1:I42,2,FALSE)</f>
         <v>4</v>
       </c>
       <c r="K42" s="1">
@@ -10345,16 +10357,16 @@
     </row>
     <row r="43" spans="1:12" ht="34" x14ac:dyDescent="0.2">
       <c r="A43">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B43" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="C43" t="s">
-        <v>150</v>
+        <v>140</v>
       </c>
       <c r="E43" s="2" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="F43" t="s">
         <v>15</v>
@@ -10366,11 +10378,11 @@
         <v>23</v>
       </c>
       <c r="I43" s="1">
-        <f>VLOOKUP(F43,'Source lists'!$E$1:F43,2,FALSE)</f>
+        <f>VLOOKUP(F43,'Source lists'!$E$1:F42,2,FALSE)</f>
         <v>4</v>
       </c>
       <c r="J43" s="1">
-        <f>VLOOKUP(G43,'Source lists'!$H$1:I44,2,FALSE)</f>
+        <f>VLOOKUP(G43,'Source lists'!$H$1:I43,2,FALSE)</f>
         <v>4</v>
       </c>
       <c r="K43" s="1">
@@ -10378,21 +10390,18 @@
         <v>32</v>
       </c>
     </row>
-    <row r="44" spans="1:12" ht="17" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:12" ht="34" x14ac:dyDescent="0.2">
       <c r="A44">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B44" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C44" t="s">
-        <v>42</v>
-      </c>
-      <c r="D44" t="s">
-        <v>44</v>
+        <v>150</v>
       </c>
       <c r="E44" s="2" t="s">
-        <v>180</v>
+        <v>187</v>
       </c>
       <c r="F44" t="s">
         <v>15</v>
@@ -10404,36 +10413,33 @@
         <v>23</v>
       </c>
       <c r="I44" s="1">
-        <f>VLOOKUP(F44,'Source lists'!$E$1:F44,2,FALSE)</f>
+        <f>VLOOKUP(F44,'Source lists'!$E$1:F43,2,FALSE)</f>
         <v>4</v>
       </c>
       <c r="J44" s="1">
-        <f>VLOOKUP(G44,'Source lists'!$H$1:I45,2,FALSE)</f>
+        <f>VLOOKUP(G44,'Source lists'!$H$1:I44,2,FALSE)</f>
         <v>4</v>
       </c>
       <c r="K44" s="1">
         <f>VLOOKUP(F44,'Source lists'!$E$2:$F$6,2,FALSE)*(VLOOKUP(G44,'Source lists'!$H$2:$I$7,2,FALSE)^2)/VLOOKUP(H44,'Source lists'!$K$2:$L$9,2,FALSE)</f>
         <v>32</v>
       </c>
-      <c r="L44">
-        <v>8</v>
-      </c>
     </row>
     <row r="45" spans="1:12" ht="17" x14ac:dyDescent="0.2">
       <c r="A45">
-        <v>115</v>
+        <v>109</v>
       </c>
       <c r="B45" t="s">
         <v>8</v>
       </c>
       <c r="C45" t="s">
-        <v>208</v>
+        <v>42</v>
       </c>
       <c r="D45" t="s">
-        <v>211</v>
+        <v>44</v>
       </c>
       <c r="E45" s="2" t="s">
-        <v>212</v>
+        <v>180</v>
       </c>
       <c r="F45" t="s">
         <v>15</v>
@@ -10445,11 +10451,11 @@
         <v>23</v>
       </c>
       <c r="I45" s="1">
-        <f>VLOOKUP(F45,'Source lists'!$E$1:F118,2,FALSE)</f>
+        <f>VLOOKUP(F45,'Source lists'!$E$1:F44,2,FALSE)</f>
         <v>4</v>
       </c>
       <c r="J45" s="1">
-        <f>VLOOKUP(G45,'Source lists'!$H$1:I119,2,FALSE)</f>
+        <f>VLOOKUP(G45,'Source lists'!$H$1:I45,2,FALSE)</f>
         <v>4</v>
       </c>
       <c r="K45" s="1">
@@ -10462,45 +10468,48 @@
     </row>
     <row r="46" spans="1:12" ht="17" x14ac:dyDescent="0.2">
       <c r="A46">
-        <v>8</v>
+        <v>115</v>
       </c>
       <c r="B46" t="s">
         <v>8</v>
       </c>
       <c r="C46" t="s">
-        <v>42</v>
+        <v>208</v>
       </c>
       <c r="D46" t="s">
-        <v>44</v>
+        <v>211</v>
       </c>
       <c r="E46" s="2" t="s">
-        <v>46</v>
+        <v>212</v>
       </c>
       <c r="F46" t="s">
         <v>15</v>
       </c>
       <c r="G46" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="H46" t="s">
-        <v>69</v>
+        <v>23</v>
       </c>
       <c r="I46" s="1">
-        <f>VLOOKUP(F46,'Source lists'!$E$1:F45,2,FALSE)</f>
+        <f>VLOOKUP(F46,'Source lists'!$E$1:F118,2,FALSE)</f>
         <v>4</v>
       </c>
       <c r="J46" s="1">
-        <f>VLOOKUP(G46,'Source lists'!$H$1:I46,2,FALSE)</f>
-        <v>7</v>
+        <f>VLOOKUP(G46,'Source lists'!$H$1:I119,2,FALSE)</f>
+        <v>4</v>
       </c>
       <c r="K46" s="1">
         <f>VLOOKUP(F46,'Source lists'!$E$2:$F$6,2,FALSE)*(VLOOKUP(G46,'Source lists'!$H$2:$I$7,2,FALSE)^2)/VLOOKUP(H46,'Source lists'!$K$2:$L$9,2,FALSE)</f>
-        <v>28</v>
-      </c>
-    </row>
-    <row r="47" spans="1:12" ht="34" x14ac:dyDescent="0.2">
+        <v>32</v>
+      </c>
+      <c r="L46">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="47" spans="1:12" ht="17" x14ac:dyDescent="0.2">
       <c r="A47">
-        <v>22</v>
+        <v>8</v>
       </c>
       <c r="B47" t="s">
         <v>8</v>
@@ -10508,69 +10517,72 @@
       <c r="C47" t="s">
         <v>42</v>
       </c>
+      <c r="D47" t="s">
+        <v>44</v>
+      </c>
       <c r="E47" s="2" t="s">
-        <v>61</v>
+        <v>46</v>
       </c>
       <c r="F47" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G47" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="H47" t="s">
-        <v>25</v>
+        <v>69</v>
       </c>
       <c r="I47" s="1">
-        <f>VLOOKUP(F47,'Source lists'!$E$1:F46,2,FALSE)</f>
-        <v>3</v>
+        <f>VLOOKUP(F47,'Source lists'!$E$1:F45,2,FALSE)</f>
+        <v>4</v>
       </c>
       <c r="J47" s="1">
-        <f>VLOOKUP(G47,'Source lists'!$H$1:I47,2,FALSE)</f>
-        <v>3</v>
+        <f>VLOOKUP(G47,'Source lists'!$H$1:I46,2,FALSE)</f>
+        <v>7</v>
       </c>
       <c r="K47" s="1">
         <f>VLOOKUP(F47,'Source lists'!$E$2:$F$6,2,FALSE)*(VLOOKUP(G47,'Source lists'!$H$2:$I$7,2,FALSE)^2)/VLOOKUP(H47,'Source lists'!$K$2:$L$9,2,FALSE)</f>
-        <v>27</v>
+        <v>28</v>
       </c>
     </row>
     <row r="48" spans="1:12" ht="34" x14ac:dyDescent="0.2">
       <c r="A48">
-        <v>43</v>
+        <v>22</v>
       </c>
       <c r="B48" t="s">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="C48" t="s">
-        <v>87</v>
+        <v>42</v>
       </c>
       <c r="E48" s="2" t="s">
-        <v>93</v>
+        <v>61</v>
       </c>
       <c r="F48" t="s">
         <v>16</v>
       </c>
       <c r="G48" t="s">
-        <v>159</v>
+        <v>29</v>
       </c>
       <c r="H48" t="s">
-        <v>67</v>
+        <v>25</v>
       </c>
       <c r="I48" s="1">
-        <f>VLOOKUP(F48,'Source lists'!$E$1:F47,2,FALSE)</f>
+        <f>VLOOKUP(F48,'Source lists'!$E$1:F46,2,FALSE)</f>
         <v>3</v>
       </c>
       <c r="J48" s="1">
-        <f>VLOOKUP(G48,'Source lists'!$H$1:I48,2,FALSE)</f>
-        <v>6</v>
+        <f>VLOOKUP(G48,'Source lists'!$H$1:I47,2,FALSE)</f>
+        <v>3</v>
       </c>
       <c r="K48" s="1">
         <f>VLOOKUP(F48,'Source lists'!$E$2:$F$6,2,FALSE)*(VLOOKUP(G48,'Source lists'!$H$2:$I$7,2,FALSE)^2)/VLOOKUP(H48,'Source lists'!$K$2:$L$9,2,FALSE)</f>
         <v>27</v>
       </c>
     </row>
-    <row r="49" spans="1:13" ht="68" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:13" ht="34" x14ac:dyDescent="0.2">
       <c r="A49">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B49" t="s">
         <v>1</v>
@@ -10579,7 +10591,7 @@
         <v>87</v>
       </c>
       <c r="E49" s="2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="F49" t="s">
         <v>16</v>
@@ -10591,11 +10603,11 @@
         <v>67</v>
       </c>
       <c r="I49" s="1">
-        <f>VLOOKUP(F49,'Source lists'!$E$1:F48,2,FALSE)</f>
+        <f>VLOOKUP(F49,'Source lists'!$E$1:F47,2,FALSE)</f>
         <v>3</v>
       </c>
       <c r="J49" s="1">
-        <f>VLOOKUP(G49,'Source lists'!$H$1:I49,2,FALSE)</f>
+        <f>VLOOKUP(G49,'Source lists'!$H$1:I48,2,FALSE)</f>
         <v>6</v>
       </c>
       <c r="K49" s="1">
@@ -10603,53 +10615,53 @@
         <v>27</v>
       </c>
     </row>
-    <row r="50" spans="1:13" ht="34" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:13" ht="68" x14ac:dyDescent="0.2">
       <c r="A50">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="B50" t="s">
         <v>1</v>
       </c>
       <c r="C50" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="E50" s="2" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="F50" t="s">
         <v>16</v>
       </c>
       <c r="G50" t="s">
-        <v>29</v>
+        <v>159</v>
       </c>
       <c r="H50" t="s">
-        <v>25</v>
+        <v>67</v>
       </c>
       <c r="I50" s="1">
-        <f>VLOOKUP(F50,'Source lists'!$E$1:F49,2,FALSE)</f>
+        <f>VLOOKUP(F50,'Source lists'!$E$1:F48,2,FALSE)</f>
         <v>3</v>
       </c>
       <c r="J50" s="1">
-        <f>VLOOKUP(G50,'Source lists'!$H$1:I50,2,FALSE)</f>
-        <v>3</v>
+        <f>VLOOKUP(G50,'Source lists'!$H$1:I49,2,FALSE)</f>
+        <v>6</v>
       </c>
       <c r="K50" s="1">
         <f>VLOOKUP(F50,'Source lists'!$E$2:$F$6,2,FALSE)*(VLOOKUP(G50,'Source lists'!$H$2:$I$7,2,FALSE)^2)/VLOOKUP(H50,'Source lists'!$K$2:$L$9,2,FALSE)</f>
         <v>27</v>
       </c>
     </row>
-    <row r="51" spans="1:13" ht="17" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:13" ht="34" x14ac:dyDescent="0.2">
       <c r="A51">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="B51" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C51" t="s">
-        <v>106</v>
+        <v>91</v>
       </c>
       <c r="E51" s="2" t="s">
-        <v>107</v>
+        <v>99</v>
       </c>
       <c r="F51" t="s">
         <v>16</v>
@@ -10661,11 +10673,11 @@
         <v>25</v>
       </c>
       <c r="I51" s="1">
-        <f>VLOOKUP(F51,'Source lists'!$E$1:F50,2,FALSE)</f>
+        <f>VLOOKUP(F51,'Source lists'!$E$1:F49,2,FALSE)</f>
         <v>3</v>
       </c>
       <c r="J51" s="1">
-        <f>VLOOKUP(G51,'Source lists'!$H$1:I51,2,FALSE)</f>
+        <f>VLOOKUP(G51,'Source lists'!$H$1:I50,2,FALSE)</f>
         <v>3</v>
       </c>
       <c r="K51" s="1">
@@ -10674,93 +10686,90 @@
       </c>
     </row>
     <row r="52" spans="1:13" ht="17" x14ac:dyDescent="0.2">
-      <c r="A52" s="3">
+      <c r="A52">
+        <v>57</v>
+      </c>
+      <c r="B52" t="s">
+        <v>2</v>
+      </c>
+      <c r="C52" t="s">
         <v>106</v>
       </c>
-      <c r="B52" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="C52" s="3"/>
-      <c r="D52" s="3"/>
-      <c r="E52" s="4" t="s">
-        <v>174</v>
-      </c>
-      <c r="F52" s="3" t="s">
+      <c r="E52" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="F52" t="s">
         <v>16</v>
       </c>
-      <c r="G52" s="3" t="s">
+      <c r="G52" t="s">
         <v>29</v>
       </c>
-      <c r="H52" s="3" t="s">
+      <c r="H52" t="s">
         <v>25</v>
       </c>
-      <c r="I52" s="5">
-        <f>VLOOKUP(F52,'Source lists'!$E$1:F51,2,FALSE)</f>
+      <c r="I52" s="1">
+        <f>VLOOKUP(F52,'Source lists'!$E$1:F50,2,FALSE)</f>
         <v>3</v>
       </c>
-      <c r="J52" s="5">
-        <f>VLOOKUP(G52,'Source lists'!$H$1:I52,2,FALSE)</f>
+      <c r="J52" s="1">
+        <f>VLOOKUP(G52,'Source lists'!$H$1:I51,2,FALSE)</f>
         <v>3</v>
       </c>
-      <c r="K52" s="5">
+      <c r="K52" s="1">
         <f>VLOOKUP(F52,'Source lists'!$E$2:$F$6,2,FALSE)*(VLOOKUP(G52,'Source lists'!$H$2:$I$7,2,FALSE)^2)/VLOOKUP(H52,'Source lists'!$K$2:$L$9,2,FALSE)</f>
         <v>27</v>
       </c>
-      <c r="L52" s="3"/>
-      <c r="M52" s="3" t="s">
+    </row>
+    <row r="53" spans="1:13" ht="17" x14ac:dyDescent="0.2">
+      <c r="A53" s="3">
+        <v>106</v>
+      </c>
+      <c r="B53" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="C53" s="3"/>
+      <c r="D53" s="3"/>
+      <c r="E53" s="4" t="s">
+        <v>174</v>
+      </c>
+      <c r="F53" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G53" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="H53" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="I53" s="5">
+        <f>VLOOKUP(F53,'Source lists'!$E$1:F51,2,FALSE)</f>
+        <v>3</v>
+      </c>
+      <c r="J53" s="5">
+        <f>VLOOKUP(G53,'Source lists'!$H$1:I52,2,FALSE)</f>
+        <v>3</v>
+      </c>
+      <c r="K53" s="5">
+        <f>VLOOKUP(F53,'Source lists'!$E$2:$F$6,2,FALSE)*(VLOOKUP(G53,'Source lists'!$H$2:$I$7,2,FALSE)^2)/VLOOKUP(H53,'Source lists'!$K$2:$L$9,2,FALSE)</f>
+        <v>27</v>
+      </c>
+      <c r="L53" s="3"/>
+      <c r="M53" s="3" t="s">
         <v>176</v>
-      </c>
-    </row>
-    <row r="53" spans="1:13" ht="34" x14ac:dyDescent="0.2">
-      <c r="A53">
-        <v>49</v>
-      </c>
-      <c r="B53" t="s">
-        <v>1</v>
-      </c>
-      <c r="C53" t="s">
-        <v>91</v>
-      </c>
-      <c r="E53" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="F53" t="s">
-        <v>15</v>
-      </c>
-      <c r="G53" t="s">
-        <v>28</v>
-      </c>
-      <c r="H53" t="s">
-        <v>24</v>
-      </c>
-      <c r="I53" s="1">
-        <f>VLOOKUP(F53,'Source lists'!$E$1:F52,2,FALSE)</f>
-        <v>4</v>
-      </c>
-      <c r="J53" s="1">
-        <f>VLOOKUP(G53,'Source lists'!$H$1:I53,2,FALSE)</f>
-        <v>4</v>
-      </c>
-      <c r="K53" s="1">
-        <f>VLOOKUP(F53,'Source lists'!$E$2:$F$6,2,FALSE)*(VLOOKUP(G53,'Source lists'!$H$2:$I$7,2,FALSE)^2)/VLOOKUP(H53,'Source lists'!$K$2:$L$9,2,FALSE)</f>
-        <v>21.333333333333332</v>
       </c>
     </row>
     <row r="54" spans="1:13" ht="34" x14ac:dyDescent="0.2">
       <c r="A54">
-        <v>74</v>
+        <v>49</v>
       </c>
       <c r="B54" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C54" t="s">
-        <v>133</v>
-      </c>
-      <c r="D54" t="s">
-        <v>188</v>
+        <v>91</v>
       </c>
       <c r="E54" s="2" t="s">
-        <v>137</v>
+        <v>100</v>
       </c>
       <c r="F54" t="s">
         <v>15</v>
@@ -10772,11 +10781,11 @@
         <v>24</v>
       </c>
       <c r="I54" s="1">
-        <f>VLOOKUP(F54,'Source lists'!$E$1:F53,2,FALSE)</f>
+        <f>VLOOKUP(F54,'Source lists'!$E$1:F52,2,FALSE)</f>
         <v>4</v>
       </c>
       <c r="J54" s="1">
-        <f>VLOOKUP(G54,'Source lists'!$H$1:I54,2,FALSE)</f>
+        <f>VLOOKUP(G54,'Source lists'!$H$1:I53,2,FALSE)</f>
         <v>4</v>
       </c>
       <c r="K54" s="1">
@@ -10784,18 +10793,21 @@
         <v>21.333333333333332</v>
       </c>
     </row>
-    <row r="55" spans="1:13" ht="51" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:13" ht="34" x14ac:dyDescent="0.2">
       <c r="A55">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="B55" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C55" t="s">
-        <v>142</v>
+        <v>133</v>
+      </c>
+      <c r="D55" t="s">
+        <v>188</v>
       </c>
       <c r="E55" s="2" t="s">
-        <v>155</v>
+        <v>137</v>
       </c>
       <c r="F55" t="s">
         <v>15</v>
@@ -10807,11 +10819,11 @@
         <v>24</v>
       </c>
       <c r="I55" s="1">
-        <f>VLOOKUP(F55,'Source lists'!$E$1:F54,2,FALSE)</f>
+        <f>VLOOKUP(F55,'Source lists'!$E$1:F53,2,FALSE)</f>
         <v>4</v>
       </c>
       <c r="J55" s="1">
-        <f>VLOOKUP(G55,'Source lists'!$H$1:I55,2,FALSE)</f>
+        <f>VLOOKUP(G55,'Source lists'!$H$1:I54,2,FALSE)</f>
         <v>4</v>
       </c>
       <c r="K55" s="1">
@@ -10821,16 +10833,16 @@
     </row>
     <row r="56" spans="1:13" ht="51" x14ac:dyDescent="0.2">
       <c r="A56">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B56" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C56" t="s">
-        <v>106</v>
+        <v>142</v>
       </c>
       <c r="E56" s="2" t="s">
-        <v>145</v>
+        <v>155</v>
       </c>
       <c r="F56" t="s">
         <v>15</v>
@@ -10842,11 +10854,11 @@
         <v>24</v>
       </c>
       <c r="I56" s="1">
-        <f>VLOOKUP(F56,'Source lists'!$E$1:F55,2,FALSE)</f>
+        <f>VLOOKUP(F56,'Source lists'!$E$1:F54,2,FALSE)</f>
         <v>4</v>
       </c>
       <c r="J56" s="1">
-        <f>VLOOKUP(G56,'Source lists'!$H$1:I56,2,FALSE)</f>
+        <f>VLOOKUP(G56,'Source lists'!$H$1:I55,2,FALSE)</f>
         <v>4</v>
       </c>
       <c r="K56" s="1">
@@ -10856,16 +10868,16 @@
     </row>
     <row r="57" spans="1:13" ht="51" x14ac:dyDescent="0.2">
       <c r="A57">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B57" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C57" t="s">
-        <v>142</v>
+        <v>106</v>
       </c>
       <c r="E57" s="2" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="F57" t="s">
         <v>15</v>
@@ -10877,11 +10889,11 @@
         <v>24</v>
       </c>
       <c r="I57" s="1">
-        <f>VLOOKUP(F57,'Source lists'!$E$1:F56,2,FALSE)</f>
+        <f>VLOOKUP(F57,'Source lists'!$E$1:F55,2,FALSE)</f>
         <v>4</v>
       </c>
       <c r="J57" s="1">
-        <f>VLOOKUP(G57,'Source lists'!$H$1:I57,2,FALSE)</f>
+        <f>VLOOKUP(G57,'Source lists'!$H$1:I56,2,FALSE)</f>
         <v>4</v>
       </c>
       <c r="K57" s="1">
@@ -10889,18 +10901,18 @@
         <v>21.333333333333332</v>
       </c>
     </row>
-    <row r="58" spans="1:13" ht="34" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:13" ht="51" x14ac:dyDescent="0.2">
       <c r="A58">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="B58" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="C58" t="s">
-        <v>154</v>
+        <v>142</v>
       </c>
       <c r="E58" s="2" t="s">
-        <v>189</v>
+        <v>146</v>
       </c>
       <c r="F58" t="s">
         <v>15</v>
@@ -10912,11 +10924,11 @@
         <v>24</v>
       </c>
       <c r="I58" s="1">
-        <f>VLOOKUP(F58,'Source lists'!$E$1:F57,2,FALSE)</f>
+        <f>VLOOKUP(F58,'Source lists'!$E$1:F56,2,FALSE)</f>
         <v>4</v>
       </c>
       <c r="J58" s="1">
-        <f>VLOOKUP(G58,'Source lists'!$H$1:I58,2,FALSE)</f>
+        <f>VLOOKUP(G58,'Source lists'!$H$1:I57,2,FALSE)</f>
         <v>4</v>
       </c>
       <c r="K58" s="1">
@@ -10926,7 +10938,7 @@
     </row>
     <row r="59" spans="1:13" ht="34" x14ac:dyDescent="0.2">
       <c r="A59">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B59" t="s">
         <v>6</v>
@@ -10935,7 +10947,7 @@
         <v>154</v>
       </c>
       <c r="E59" s="2" t="s">
-        <v>156</v>
+        <v>189</v>
       </c>
       <c r="F59" t="s">
         <v>15</v>
@@ -10947,11 +10959,11 @@
         <v>24</v>
       </c>
       <c r="I59" s="1">
-        <f>VLOOKUP(F59,'Source lists'!$E$1:F58,2,FALSE)</f>
+        <f>VLOOKUP(F59,'Source lists'!$E$1:F57,2,FALSE)</f>
         <v>4</v>
       </c>
       <c r="J59" s="1">
-        <f>VLOOKUP(G59,'Source lists'!$H$1:I59,2,FALSE)</f>
+        <f>VLOOKUP(G59,'Source lists'!$H$1:I58,2,FALSE)</f>
         <v>4</v>
       </c>
       <c r="K59" s="1">
@@ -10959,47 +10971,44 @@
         <v>21.333333333333332</v>
       </c>
     </row>
-    <row r="60" spans="1:13" ht="17" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:13" ht="34" x14ac:dyDescent="0.2">
       <c r="A60">
-        <v>17</v>
+        <v>88</v>
       </c>
       <c r="B60" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C60" t="s">
-        <v>42</v>
-      </c>
-      <c r="D60" t="s">
-        <v>54</v>
+        <v>154</v>
       </c>
       <c r="E60" s="2" t="s">
-        <v>55</v>
+        <v>156</v>
       </c>
       <c r="F60" t="s">
         <v>15</v>
       </c>
       <c r="G60" t="s">
-        <v>159</v>
+        <v>28</v>
       </c>
       <c r="H60" t="s">
-        <v>69</v>
+        <v>24</v>
       </c>
       <c r="I60" s="1">
-        <f>VLOOKUP(F60,'Source lists'!$E$1:F59,2,FALSE)</f>
+        <f>VLOOKUP(F60,'Source lists'!$E$1:F58,2,FALSE)</f>
         <v>4</v>
       </c>
       <c r="J60" s="1">
-        <f>VLOOKUP(G60,'Source lists'!$H$1:I60,2,FALSE)</f>
-        <v>6</v>
+        <f>VLOOKUP(G60,'Source lists'!$H$1:I59,2,FALSE)</f>
+        <v>4</v>
       </c>
       <c r="K60" s="1">
         <f>VLOOKUP(F60,'Source lists'!$E$2:$F$6,2,FALSE)*(VLOOKUP(G60,'Source lists'!$H$2:$I$7,2,FALSE)^2)/VLOOKUP(H60,'Source lists'!$K$2:$L$9,2,FALSE)</f>
-        <v>20.571428571428573</v>
+        <v>21.333333333333332</v>
       </c>
     </row>
     <row r="61" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="A61">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B61" t="s">
         <v>8</v>
@@ -11011,7 +11020,7 @@
         <v>54</v>
       </c>
       <c r="E61" s="2" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="F61" t="s">
         <v>15</v>
@@ -11023,11 +11032,11 @@
         <v>69</v>
       </c>
       <c r="I61" s="1">
-        <f>VLOOKUP(F61,'Source lists'!$E$1:F60,2,FALSE)</f>
+        <f>VLOOKUP(F61,'Source lists'!$E$1:F59,2,FALSE)</f>
         <v>4</v>
       </c>
       <c r="J61" s="1">
-        <f>VLOOKUP(G61,'Source lists'!$H$1:I61,2,FALSE)</f>
+        <f>VLOOKUP(G61,'Source lists'!$H$1:I60,2,FALSE)</f>
         <v>6</v>
       </c>
       <c r="K61" s="1">
@@ -11037,7 +11046,7 @@
     </row>
     <row r="62" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="A62">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B62" t="s">
         <v>8</v>
@@ -11049,7 +11058,7 @@
         <v>54</v>
       </c>
       <c r="E62" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="F62" t="s">
         <v>15</v>
@@ -11061,11 +11070,11 @@
         <v>69</v>
       </c>
       <c r="I62" s="1">
-        <f>VLOOKUP(F62,'Source lists'!$E$1:F61,2,FALSE)</f>
+        <f>VLOOKUP(F62,'Source lists'!$E$1:F60,2,FALSE)</f>
         <v>4</v>
       </c>
       <c r="J62" s="1">
-        <f>VLOOKUP(G62,'Source lists'!$H$1:I62,2,FALSE)</f>
+        <f>VLOOKUP(G62,'Source lists'!$H$1:I61,2,FALSE)</f>
         <v>6</v>
       </c>
       <c r="K62" s="1">
@@ -11075,7 +11084,7 @@
     </row>
     <row r="63" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="A63">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B63" t="s">
         <v>8</v>
@@ -11087,7 +11096,7 @@
         <v>54</v>
       </c>
       <c r="E63" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F63" t="s">
         <v>15</v>
@@ -11099,11 +11108,11 @@
         <v>69</v>
       </c>
       <c r="I63" s="1">
-        <f>VLOOKUP(F63,'Source lists'!$E$1:F62,2,FALSE)</f>
+        <f>VLOOKUP(F63,'Source lists'!$E$1:F61,2,FALSE)</f>
         <v>4</v>
       </c>
       <c r="J63" s="1">
-        <f>VLOOKUP(G63,'Source lists'!$H$1:I63,2,FALSE)</f>
+        <f>VLOOKUP(G63,'Source lists'!$H$1:I62,2,FALSE)</f>
         <v>6</v>
       </c>
       <c r="K63" s="1">
@@ -11113,7 +11122,7 @@
     </row>
     <row r="64" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="A64">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B64" t="s">
         <v>8</v>
@@ -11125,7 +11134,7 @@
         <v>54</v>
       </c>
       <c r="E64" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F64" t="s">
         <v>15</v>
@@ -11137,11 +11146,11 @@
         <v>69</v>
       </c>
       <c r="I64" s="1">
-        <f>VLOOKUP(F64,'Source lists'!$E$1:F63,2,FALSE)</f>
+        <f>VLOOKUP(F64,'Source lists'!$E$1:F62,2,FALSE)</f>
         <v>4</v>
       </c>
       <c r="J64" s="1">
-        <f>VLOOKUP(G64,'Source lists'!$H$1:I64,2,FALSE)</f>
+        <f>VLOOKUP(G64,'Source lists'!$H$1:I63,2,FALSE)</f>
         <v>6</v>
       </c>
       <c r="K64" s="1">
@@ -11149,53 +11158,56 @@
         <v>20.571428571428573</v>
       </c>
     </row>
-    <row r="65" spans="1:12" ht="34" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:12" ht="17" x14ac:dyDescent="0.2">
       <c r="A65">
-        <v>66</v>
+        <v>21</v>
       </c>
       <c r="B65" t="s">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="C65" t="s">
-        <v>106</v>
+        <v>42</v>
+      </c>
+      <c r="D65" t="s">
+        <v>54</v>
       </c>
       <c r="E65" s="2" t="s">
-        <v>190</v>
+        <v>60</v>
       </c>
       <c r="F65" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="G65" t="s">
         <v>159</v>
       </c>
       <c r="H65" t="s">
-        <v>23</v>
+        <v>69</v>
       </c>
       <c r="I65" s="1">
-        <f>VLOOKUP(F65,'Source lists'!$E$1:F64,2,FALSE)</f>
-        <v>1</v>
+        <f>VLOOKUP(F65,'Source lists'!$E$1:F63,2,FALSE)</f>
+        <v>4</v>
       </c>
       <c r="J65" s="1">
-        <f>VLOOKUP(G65,'Source lists'!$H$1:I65,2,FALSE)</f>
+        <f>VLOOKUP(G65,'Source lists'!$H$1:I64,2,FALSE)</f>
         <v>6</v>
       </c>
       <c r="K65" s="1">
         <f>VLOOKUP(F65,'Source lists'!$E$2:$F$6,2,FALSE)*(VLOOKUP(G65,'Source lists'!$H$2:$I$7,2,FALSE)^2)/VLOOKUP(H65,'Source lists'!$K$2:$L$9,2,FALSE)</f>
-        <v>18</v>
+        <v>20.571428571428573</v>
       </c>
     </row>
     <row r="66" spans="1:12" ht="34" x14ac:dyDescent="0.2">
       <c r="A66">
-        <v>76</v>
+        <v>66</v>
       </c>
       <c r="B66" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C66" t="s">
-        <v>139</v>
+        <v>106</v>
       </c>
       <c r="E66" s="2" t="s">
-        <v>141</v>
+        <v>190</v>
       </c>
       <c r="F66" t="s">
         <v>17</v>
@@ -11207,11 +11219,11 @@
         <v>23</v>
       </c>
       <c r="I66" s="1">
-        <f>VLOOKUP(F66,'Source lists'!$E$1:F65,2,FALSE)</f>
+        <f>VLOOKUP(F66,'Source lists'!$E$1:F64,2,FALSE)</f>
         <v>1</v>
       </c>
       <c r="J66" s="1">
-        <f>VLOOKUP(G66,'Source lists'!$H$1:I66,2,FALSE)</f>
+        <f>VLOOKUP(G66,'Source lists'!$H$1:I65,2,FALSE)</f>
         <v>6</v>
       </c>
       <c r="K66" s="1">
@@ -11221,89 +11233,86 @@
     </row>
     <row r="67" spans="1:12" ht="34" x14ac:dyDescent="0.2">
       <c r="A67">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="B67" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C67" t="s">
-        <v>133</v>
-      </c>
-      <c r="D67" t="s">
-        <v>188</v>
+        <v>139</v>
       </c>
       <c r="E67" s="2" t="s">
-        <v>136</v>
+        <v>141</v>
       </c>
       <c r="F67" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="G67" t="s">
-        <v>28</v>
+        <v>159</v>
       </c>
       <c r="H67" t="s">
-        <v>67</v>
+        <v>23</v>
       </c>
       <c r="I67" s="1">
-        <f>VLOOKUP(F67,'Source lists'!$E$1:F66,2,FALSE)</f>
-        <v>4</v>
+        <f>VLOOKUP(F67,'Source lists'!$E$1:F65,2,FALSE)</f>
+        <v>1</v>
       </c>
       <c r="J67" s="1">
-        <f>VLOOKUP(G67,'Source lists'!$H$1:I67,2,FALSE)</f>
-        <v>4</v>
+        <f>VLOOKUP(G67,'Source lists'!$H$1:I66,2,FALSE)</f>
+        <v>6</v>
       </c>
       <c r="K67" s="1">
         <f>VLOOKUP(F67,'Source lists'!$E$2:$F$6,2,FALSE)*(VLOOKUP(G67,'Source lists'!$H$2:$I$7,2,FALSE)^2)/VLOOKUP(H67,'Source lists'!$K$2:$L$9,2,FALSE)</f>
-        <v>16</v>
-      </c>
-    </row>
-    <row r="68" spans="1:12" ht="17" x14ac:dyDescent="0.2">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="68" spans="1:12" ht="34" x14ac:dyDescent="0.2">
       <c r="A68">
-        <v>91</v>
+        <v>73</v>
       </c>
       <c r="B68" t="s">
+        <v>2</v>
+      </c>
+      <c r="C68" t="s">
+        <v>133</v>
+      </c>
+      <c r="D68" t="s">
+        <v>188</v>
+      </c>
+      <c r="E68" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="F68" t="s">
+        <v>15</v>
+      </c>
+      <c r="G68" t="s">
+        <v>28</v>
+      </c>
+      <c r="H68" t="s">
+        <v>67</v>
+      </c>
+      <c r="I68" s="1">
+        <f>VLOOKUP(F68,'Source lists'!$E$1:F66,2,FALSE)</f>
         <v>4</v>
       </c>
-      <c r="C68" t="s">
-        <v>161</v>
-      </c>
-      <c r="E68" s="2" t="s">
-        <v>167</v>
-      </c>
-      <c r="F68" t="s">
-        <v>17</v>
-      </c>
-      <c r="G68" t="s">
-        <v>26</v>
-      </c>
-      <c r="H68" t="s">
-        <v>69</v>
-      </c>
-      <c r="I68" s="1">
-        <f>VLOOKUP(F68,'Source lists'!$E$1:F67,2,FALSE)</f>
-        <v>1</v>
-      </c>
       <c r="J68" s="1">
-        <f>VLOOKUP(G68,'Source lists'!$H$1:I68,2,FALSE)</f>
-        <v>10</v>
+        <f>VLOOKUP(G68,'Source lists'!$H$1:I67,2,FALSE)</f>
+        <v>4</v>
       </c>
       <c r="K68" s="1">
         <f>VLOOKUP(F68,'Source lists'!$E$2:$F$6,2,FALSE)*(VLOOKUP(G68,'Source lists'!$H$2:$I$7,2,FALSE)^2)/VLOOKUP(H68,'Source lists'!$K$2:$L$9,2,FALSE)</f>
-        <v>14.285714285714286</v>
-      </c>
-      <c r="L68">
-        <v>59</v>
+        <v>16</v>
       </c>
     </row>
     <row r="69" spans="1:12" ht="17" x14ac:dyDescent="0.2">
       <c r="A69">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B69" t="s">
         <v>4</v>
       </c>
       <c r="C69" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="E69" s="2" t="s">
         <v>167</v>
@@ -11318,11 +11327,11 @@
         <v>69</v>
       </c>
       <c r="I69" s="1">
-        <f>VLOOKUP(F69,'Source lists'!$E$1:F68,2,FALSE)</f>
+        <f>VLOOKUP(F69,'Source lists'!$E$1:F67,2,FALSE)</f>
         <v>1</v>
       </c>
       <c r="J69" s="1">
-        <f>VLOOKUP(G69,'Source lists'!$H$1:I69,2,FALSE)</f>
+        <f>VLOOKUP(G69,'Source lists'!$H$1:I68,2,FALSE)</f>
         <v>10</v>
       </c>
       <c r="K69" s="1">
@@ -11330,18 +11339,18 @@
         <v>14.285714285714286</v>
       </c>
       <c r="L69">
-        <v>64</v>
+        <v>59</v>
       </c>
     </row>
     <row r="70" spans="1:12" ht="17" x14ac:dyDescent="0.2">
       <c r="A70">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B70" t="s">
         <v>4</v>
       </c>
       <c r="C70" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="E70" s="2" t="s">
         <v>167</v>
@@ -11356,11 +11365,11 @@
         <v>69</v>
       </c>
       <c r="I70" s="1">
-        <f>VLOOKUP(F70,'Source lists'!$E$1:F69,2,FALSE)</f>
+        <f>VLOOKUP(F70,'Source lists'!$E$1:F68,2,FALSE)</f>
         <v>1</v>
       </c>
       <c r="J70" s="1">
-        <f>VLOOKUP(G70,'Source lists'!$H$1:I70,2,FALSE)</f>
+        <f>VLOOKUP(G70,'Source lists'!$H$1:I69,2,FALSE)</f>
         <v>10</v>
       </c>
       <c r="K70" s="1">
@@ -11368,18 +11377,18 @@
         <v>14.285714285714286</v>
       </c>
       <c r="L70">
-        <v>59</v>
+        <v>64</v>
       </c>
     </row>
     <row r="71" spans="1:12" ht="17" x14ac:dyDescent="0.2">
       <c r="A71">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B71" t="s">
         <v>4</v>
       </c>
       <c r="C71" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="E71" s="2" t="s">
         <v>167</v>
@@ -11394,11 +11403,11 @@
         <v>69</v>
       </c>
       <c r="I71" s="1">
-        <f>VLOOKUP(F71,'Source lists'!$E$1:F70,2,FALSE)</f>
+        <f>VLOOKUP(F71,'Source lists'!$E$1:F69,2,FALSE)</f>
         <v>1</v>
       </c>
       <c r="J71" s="1">
-        <f>VLOOKUP(G71,'Source lists'!$H$1:I71,2,FALSE)</f>
+        <f>VLOOKUP(G71,'Source lists'!$H$1:I70,2,FALSE)</f>
         <v>10</v>
       </c>
       <c r="K71" s="1">
@@ -11406,18 +11415,18 @@
         <v>14.285714285714286</v>
       </c>
       <c r="L71">
-        <v>64</v>
+        <v>59</v>
       </c>
     </row>
     <row r="72" spans="1:12" ht="17" x14ac:dyDescent="0.2">
       <c r="A72">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B72" t="s">
         <v>4</v>
       </c>
       <c r="C72" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="E72" s="2" t="s">
         <v>167</v>
@@ -11432,11 +11441,11 @@
         <v>69</v>
       </c>
       <c r="I72" s="1">
-        <f>VLOOKUP(F72,'Source lists'!$E$1:F71,2,FALSE)</f>
+        <f>VLOOKUP(F72,'Source lists'!$E$1:F70,2,FALSE)</f>
         <v>1</v>
       </c>
       <c r="J72" s="1">
-        <f>VLOOKUP(G72,'Source lists'!$H$1:I72,2,FALSE)</f>
+        <f>VLOOKUP(G72,'Source lists'!$H$1:I71,2,FALSE)</f>
         <v>10</v>
       </c>
       <c r="K72" s="1">
@@ -11444,18 +11453,18 @@
         <v>14.285714285714286</v>
       </c>
       <c r="L72">
-        <v>59</v>
+        <v>64</v>
       </c>
     </row>
     <row r="73" spans="1:12" ht="17" x14ac:dyDescent="0.2">
       <c r="A73">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B73" t="s">
         <v>4</v>
       </c>
       <c r="C73" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="E73" s="2" t="s">
         <v>167</v>
@@ -11470,11 +11479,11 @@
         <v>69</v>
       </c>
       <c r="I73" s="1">
-        <f>VLOOKUP(F73,'Source lists'!$E$1:F72,2,FALSE)</f>
+        <f>VLOOKUP(F73,'Source lists'!$E$1:F71,2,FALSE)</f>
         <v>1</v>
       </c>
       <c r="J73" s="1">
-        <f>VLOOKUP(G73,'Source lists'!$H$1:I73,2,FALSE)</f>
+        <f>VLOOKUP(G73,'Source lists'!$H$1:I72,2,FALSE)</f>
         <v>10</v>
       </c>
       <c r="K73" s="1">
@@ -11482,21 +11491,21 @@
         <v>14.285714285714286</v>
       </c>
       <c r="L73">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="74" spans="1:12" ht="34" x14ac:dyDescent="0.2">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="74" spans="1:12" ht="17" x14ac:dyDescent="0.2">
       <c r="A74">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B74" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C74" t="s">
-        <v>147</v>
+        <v>166</v>
       </c>
       <c r="E74" s="2" t="s">
-        <v>191</v>
+        <v>167</v>
       </c>
       <c r="F74" t="s">
         <v>17</v>
@@ -11508,11 +11517,11 @@
         <v>69</v>
       </c>
       <c r="I74" s="1">
-        <f>VLOOKUP(F74,'Source lists'!$E$1:F73,2,FALSE)</f>
+        <f>VLOOKUP(F74,'Source lists'!$E$1:F72,2,FALSE)</f>
         <v>1</v>
       </c>
       <c r="J74" s="1">
-        <f>VLOOKUP(G74,'Source lists'!$H$1:I74,2,FALSE)</f>
+        <f>VLOOKUP(G74,'Source lists'!$H$1:I73,2,FALSE)</f>
         <v>10</v>
       </c>
       <c r="K74" s="1">
@@ -11520,12 +11529,12 @@
         <v>14.285714285714286</v>
       </c>
       <c r="L74">
-        <v>59</v>
+        <v>64</v>
       </c>
     </row>
     <row r="75" spans="1:12" ht="34" x14ac:dyDescent="0.2">
       <c r="A75">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B75" t="s">
         <v>5</v>
@@ -11546,11 +11555,11 @@
         <v>69</v>
       </c>
       <c r="I75" s="1">
-        <f>VLOOKUP(F75,'Source lists'!$E$1:F74,2,FALSE)</f>
+        <f>VLOOKUP(F75,'Source lists'!$E$1:F73,2,FALSE)</f>
         <v>1</v>
       </c>
       <c r="J75" s="1">
-        <f>VLOOKUP(G75,'Source lists'!$H$1:I75,2,FALSE)</f>
+        <f>VLOOKUP(G75,'Source lists'!$H$1:I74,2,FALSE)</f>
         <v>10</v>
       </c>
       <c r="K75" s="1">
@@ -11558,21 +11567,21 @@
         <v>14.285714285714286</v>
       </c>
       <c r="L75">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="76" spans="1:12" ht="51" x14ac:dyDescent="0.2">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="76" spans="1:12" ht="34" x14ac:dyDescent="0.2">
       <c r="A76">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B76" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C76" t="s">
-        <v>169</v>
+        <v>147</v>
       </c>
       <c r="E76" s="2" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="F76" t="s">
         <v>17</v>
@@ -11584,11 +11593,11 @@
         <v>69</v>
       </c>
       <c r="I76" s="1">
-        <f>VLOOKUP(F76,'Source lists'!$E$1:F75,2,FALSE)</f>
+        <f>VLOOKUP(F76,'Source lists'!$E$1:F74,2,FALSE)</f>
         <v>1</v>
       </c>
       <c r="J76" s="1">
-        <f>VLOOKUP(G76,'Source lists'!$H$1:I76,2,FALSE)</f>
+        <f>VLOOKUP(G76,'Source lists'!$H$1:I75,2,FALSE)</f>
         <v>10</v>
       </c>
       <c r="K76" s="1">
@@ -11596,12 +11605,12 @@
         <v>14.285714285714286</v>
       </c>
       <c r="L76">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="77" spans="1:12" ht="34" x14ac:dyDescent="0.2">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="77" spans="1:12" ht="51" x14ac:dyDescent="0.2">
       <c r="A77">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B77" t="s">
         <v>6</v>
@@ -11610,7 +11619,7 @@
         <v>169</v>
       </c>
       <c r="E77" s="2" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="F77" t="s">
         <v>17</v>
@@ -11622,11 +11631,11 @@
         <v>69</v>
       </c>
       <c r="I77" s="1">
-        <f>VLOOKUP(F77,'Source lists'!$E$1:F76,2,FALSE)</f>
+        <f>VLOOKUP(F77,'Source lists'!$E$1:F75,2,FALSE)</f>
         <v>1</v>
       </c>
       <c r="J77" s="1">
-        <f>VLOOKUP(G77,'Source lists'!$H$1:I77,2,FALSE)</f>
+        <f>VLOOKUP(G77,'Source lists'!$H$1:I76,2,FALSE)</f>
         <v>10</v>
       </c>
       <c r="K77" s="1">
@@ -11634,21 +11643,21 @@
         <v>14.285714285714286</v>
       </c>
       <c r="L77">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="78" spans="1:12" ht="51" x14ac:dyDescent="0.2">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="78" spans="1:12" ht="34" x14ac:dyDescent="0.2">
       <c r="A78">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="B78" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C78" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="E78" s="2" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="F78" t="s">
         <v>17</v>
@@ -11660,11 +11669,11 @@
         <v>69</v>
       </c>
       <c r="I78" s="1">
-        <f>VLOOKUP(F78,'Source lists'!$E$1:F77,2,FALSE)</f>
+        <f>VLOOKUP(F78,'Source lists'!$E$1:F76,2,FALSE)</f>
         <v>1</v>
       </c>
       <c r="J78" s="1">
-        <f>VLOOKUP(G78,'Source lists'!$H$1:I78,2,FALSE)</f>
+        <f>VLOOKUP(G78,'Source lists'!$H$1:I77,2,FALSE)</f>
         <v>10</v>
       </c>
       <c r="K78" s="1">
@@ -11672,12 +11681,12 @@
         <v>14.285714285714286</v>
       </c>
       <c r="L78">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="79" spans="1:12" ht="34" x14ac:dyDescent="0.2">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="79" spans="1:12" ht="51" x14ac:dyDescent="0.2">
       <c r="A79">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B79" t="s">
         <v>5</v>
@@ -11686,7 +11695,7 @@
         <v>170</v>
       </c>
       <c r="E79" s="2" t="s">
-        <v>172</v>
+        <v>194</v>
       </c>
       <c r="F79" t="s">
         <v>17</v>
@@ -11698,11 +11707,11 @@
         <v>69</v>
       </c>
       <c r="I79" s="1">
-        <f>VLOOKUP(F79,'Source lists'!$E$1:F78,2,FALSE)</f>
+        <f>VLOOKUP(F79,'Source lists'!$E$1:F77,2,FALSE)</f>
         <v>1</v>
       </c>
       <c r="J79" s="1">
-        <f>VLOOKUP(G79,'Source lists'!$H$1:I79,2,FALSE)</f>
+        <f>VLOOKUP(G79,'Source lists'!$H$1:I78,2,FALSE)</f>
         <v>10</v>
       </c>
       <c r="K79" s="1">
@@ -11710,56 +11719,59 @@
         <v>14.285714285714286</v>
       </c>
       <c r="L79">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="80" spans="1:12" ht="34" x14ac:dyDescent="0.2">
       <c r="A80">
-        <v>35</v>
+        <v>104</v>
       </c>
       <c r="B80" t="s">
-        <v>38</v>
+        <v>5</v>
       </c>
       <c r="C80" t="s">
-        <v>80</v>
+        <v>170</v>
       </c>
       <c r="E80" s="2" t="s">
-        <v>84</v>
+        <v>172</v>
       </c>
       <c r="F80" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="G80" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="H80" t="s">
-        <v>23</v>
+        <v>69</v>
       </c>
       <c r="I80" s="1">
-        <f>VLOOKUP(F80,'Source lists'!$E$1:F79,2,FALSE)</f>
-        <v>3</v>
+        <f>VLOOKUP(F80,'Source lists'!$E$1:F78,2,FALSE)</f>
+        <v>1</v>
       </c>
       <c r="J80" s="1">
-        <f>VLOOKUP(G80,'Source lists'!$H$1:I80,2,FALSE)</f>
-        <v>3</v>
+        <f>VLOOKUP(G80,'Source lists'!$H$1:I79,2,FALSE)</f>
+        <v>10</v>
       </c>
       <c r="K80" s="1">
         <f>VLOOKUP(F80,'Source lists'!$E$2:$F$6,2,FALSE)*(VLOOKUP(G80,'Source lists'!$H$2:$I$7,2,FALSE)^2)/VLOOKUP(H80,'Source lists'!$K$2:$L$9,2,FALSE)</f>
-        <v>13.5</v>
+        <v>14.285714285714286</v>
+      </c>
+      <c r="L80">
+        <v>103</v>
       </c>
     </row>
     <row r="81" spans="1:11" ht="34" x14ac:dyDescent="0.2">
       <c r="A81">
+        <v>35</v>
+      </c>
+      <c r="B81" t="s">
         <v>38</v>
       </c>
-      <c r="B81" t="s">
-        <v>1</v>
-      </c>
       <c r="C81" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="E81" s="2" t="s">
-        <v>118</v>
+        <v>84</v>
       </c>
       <c r="F81" t="s">
         <v>16</v>
@@ -11771,11 +11783,11 @@
         <v>23</v>
       </c>
       <c r="I81" s="1">
-        <f>VLOOKUP(F81,'Source lists'!$E$1:F80,2,FALSE)</f>
+        <f>VLOOKUP(F81,'Source lists'!$E$1:F79,2,FALSE)</f>
         <v>3</v>
       </c>
       <c r="J81" s="1">
-        <f>VLOOKUP(G81,'Source lists'!$H$1:I81,2,FALSE)</f>
+        <f>VLOOKUP(G81,'Source lists'!$H$1:I80,2,FALSE)</f>
         <v>3</v>
       </c>
       <c r="K81" s="1">
@@ -11785,19 +11797,16 @@
     </row>
     <row r="82" spans="1:11" ht="34" x14ac:dyDescent="0.2">
       <c r="A82">
-        <v>71</v>
+        <v>38</v>
       </c>
       <c r="B82" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C82" t="s">
-        <v>133</v>
-      </c>
-      <c r="D82" t="s">
-        <v>188</v>
+        <v>87</v>
       </c>
       <c r="E82" s="2" t="s">
-        <v>135</v>
+        <v>118</v>
       </c>
       <c r="F82" t="s">
         <v>16</v>
@@ -11809,11 +11818,11 @@
         <v>23</v>
       </c>
       <c r="I82" s="1">
-        <f>VLOOKUP(F82,'Source lists'!$E$1:F81,2,FALSE)</f>
+        <f>VLOOKUP(F82,'Source lists'!$E$1:F80,2,FALSE)</f>
         <v>3</v>
       </c>
       <c r="J82" s="1">
-        <f>VLOOKUP(G82,'Source lists'!$H$1:I82,2,FALSE)</f>
+        <f>VLOOKUP(G82,'Source lists'!$H$1:I81,2,FALSE)</f>
         <v>3</v>
       </c>
       <c r="K82" s="1">
@@ -11823,7 +11832,7 @@
     </row>
     <row r="83" spans="1:11" ht="34" x14ac:dyDescent="0.2">
       <c r="A83">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B83" t="s">
         <v>2</v>
@@ -11835,7 +11844,7 @@
         <v>188</v>
       </c>
       <c r="E83" s="2" t="s">
-        <v>195</v>
+        <v>135</v>
       </c>
       <c r="F83" t="s">
         <v>16</v>
@@ -11847,11 +11856,11 @@
         <v>23</v>
       </c>
       <c r="I83" s="1">
-        <f>VLOOKUP(F83,'Source lists'!$E$1:F82,2,FALSE)</f>
+        <f>VLOOKUP(F83,'Source lists'!$E$1:F81,2,FALSE)</f>
         <v>3</v>
       </c>
       <c r="J83" s="1">
-        <f>VLOOKUP(G83,'Source lists'!$H$1:I83,2,FALSE)</f>
+        <f>VLOOKUP(G83,'Source lists'!$H$1:I82,2,FALSE)</f>
         <v>3</v>
       </c>
       <c r="K83" s="1">
@@ -11859,18 +11868,21 @@
         <v>13.5</v>
       </c>
     </row>
-    <row r="84" spans="1:11" ht="17" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:11" ht="34" x14ac:dyDescent="0.2">
       <c r="A84">
-        <v>85</v>
+        <v>72</v>
       </c>
       <c r="B84" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="C84" t="s">
-        <v>150</v>
+        <v>133</v>
+      </c>
+      <c r="D84" t="s">
+        <v>188</v>
       </c>
       <c r="E84" s="2" t="s">
-        <v>152</v>
+        <v>195</v>
       </c>
       <c r="F84" t="s">
         <v>16</v>
@@ -11882,11 +11894,11 @@
         <v>23</v>
       </c>
       <c r="I84" s="1">
-        <f>VLOOKUP(F84,'Source lists'!$E$1:F83,2,FALSE)</f>
+        <f>VLOOKUP(F84,'Source lists'!$E$1:F82,2,FALSE)</f>
         <v>3</v>
       </c>
       <c r="J84" s="1">
-        <f>VLOOKUP(G84,'Source lists'!$H$1:I84,2,FALSE)</f>
+        <f>VLOOKUP(G84,'Source lists'!$H$1:I83,2,FALSE)</f>
         <v>3</v>
       </c>
       <c r="K84" s="1">
@@ -11896,7 +11908,7 @@
     </row>
     <row r="85" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A85">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B85" t="s">
         <v>6</v>
@@ -11905,7 +11917,7 @@
         <v>150</v>
       </c>
       <c r="E85" s="2" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="F85" t="s">
         <v>16</v>
@@ -11917,11 +11929,11 @@
         <v>23</v>
       </c>
       <c r="I85" s="1">
-        <f>VLOOKUP(F85,'Source lists'!$E$1:F84,2,FALSE)</f>
+        <f>VLOOKUP(F85,'Source lists'!$E$1:F83,2,FALSE)</f>
         <v>3</v>
       </c>
       <c r="J85" s="1">
-        <f>VLOOKUP(G85,'Source lists'!$H$1:I85,2,FALSE)</f>
+        <f>VLOOKUP(G85,'Source lists'!$H$1:I84,2,FALSE)</f>
         <v>3</v>
       </c>
       <c r="K85" s="1">
@@ -11931,51 +11943,48 @@
     </row>
     <row r="86" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A86">
-        <v>36</v>
+        <v>86</v>
       </c>
       <c r="B86" t="s">
-        <v>66</v>
+        <v>6</v>
       </c>
       <c r="C86" t="s">
-        <v>73</v>
-      </c>
-      <c r="D86" t="s">
-        <v>85</v>
+        <v>150</v>
       </c>
       <c r="E86" s="2" t="s">
-        <v>86</v>
+        <v>153</v>
       </c>
       <c r="F86" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="G86" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="H86" t="s">
-        <v>70</v>
+        <v>23</v>
       </c>
       <c r="I86" s="1">
-        <f>VLOOKUP(F86,'Source lists'!$E$1:F85,2,FALSE)</f>
-        <v>4</v>
+        <f>VLOOKUP(F86,'Source lists'!$E$1:F84,2,FALSE)</f>
+        <v>3</v>
       </c>
       <c r="J86" s="1">
-        <f>VLOOKUP(G86,'Source lists'!$H$1:I86,2,FALSE)</f>
-        <v>4</v>
+        <f>VLOOKUP(G86,'Source lists'!$H$1:I85,2,FALSE)</f>
+        <v>3</v>
       </c>
       <c r="K86" s="1">
         <f>VLOOKUP(F86,'Source lists'!$E$2:$F$6,2,FALSE)*(VLOOKUP(G86,'Source lists'!$H$2:$I$7,2,FALSE)^2)/VLOOKUP(H86,'Source lists'!$K$2:$L$9,2,FALSE)</f>
-        <v>12.8</v>
+        <v>13.5</v>
       </c>
     </row>
     <row r="87" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A87">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B87" t="s">
-        <v>38</v>
+        <v>66</v>
       </c>
       <c r="C87" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
       <c r="D87" t="s">
         <v>85</v>
@@ -11993,11 +12002,11 @@
         <v>70</v>
       </c>
       <c r="I87" s="1">
-        <f>VLOOKUP(F87,'Source lists'!$E$1:F86,2,FALSE)</f>
+        <f>VLOOKUP(F87,'Source lists'!$E$1:F85,2,FALSE)</f>
         <v>4</v>
       </c>
       <c r="J87" s="1">
-        <f>VLOOKUP(G87,'Source lists'!$H$1:I87,2,FALSE)</f>
+        <f>VLOOKUP(G87,'Source lists'!$H$1:I86,2,FALSE)</f>
         <v>4</v>
       </c>
       <c r="K87" s="1">
@@ -12005,21 +12014,21 @@
         <v>12.8</v>
       </c>
     </row>
-    <row r="88" spans="1:11" ht="34" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A88">
-        <v>47</v>
+        <v>37</v>
       </c>
       <c r="B88" t="s">
-        <v>1</v>
+        <v>38</v>
       </c>
       <c r="C88" t="s">
-        <v>91</v>
+        <v>80</v>
       </c>
       <c r="D88" t="s">
-        <v>112</v>
+        <v>85</v>
       </c>
       <c r="E88" s="2" t="s">
-        <v>113</v>
+        <v>86</v>
       </c>
       <c r="F88" t="s">
         <v>15</v>
@@ -12031,11 +12040,11 @@
         <v>70</v>
       </c>
       <c r="I88" s="1">
-        <f>VLOOKUP(F88,'Source lists'!$E$1:F87,2,FALSE)</f>
+        <f>VLOOKUP(F88,'Source lists'!$E$1:F86,2,FALSE)</f>
         <v>4</v>
       </c>
       <c r="J88" s="1">
-        <f>VLOOKUP(G88,'Source lists'!$H$1:I88,2,FALSE)</f>
+        <f>VLOOKUP(G88,'Source lists'!$H$1:I87,2,FALSE)</f>
         <v>4</v>
       </c>
       <c r="K88" s="1">
@@ -12045,7 +12054,7 @@
     </row>
     <row r="89" spans="1:11" ht="34" x14ac:dyDescent="0.2">
       <c r="A89">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="B89" t="s">
         <v>1</v>
@@ -12057,7 +12066,7 @@
         <v>112</v>
       </c>
       <c r="E89" s="2" t="s">
-        <v>101</v>
+        <v>113</v>
       </c>
       <c r="F89" t="s">
         <v>15</v>
@@ -12069,11 +12078,11 @@
         <v>70</v>
       </c>
       <c r="I89" s="1">
-        <f>VLOOKUP(F89,'Source lists'!$E$1:F88,2,FALSE)</f>
+        <f>VLOOKUP(F89,'Source lists'!$E$1:F87,2,FALSE)</f>
         <v>4</v>
       </c>
       <c r="J89" s="1">
-        <f>VLOOKUP(G89,'Source lists'!$H$1:I89,2,FALSE)</f>
+        <f>VLOOKUP(G89,'Source lists'!$H$1:I88,2,FALSE)</f>
         <v>4</v>
       </c>
       <c r="K89" s="1">
@@ -12083,7 +12092,7 @@
     </row>
     <row r="90" spans="1:11" ht="34" x14ac:dyDescent="0.2">
       <c r="A90">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="B90" t="s">
         <v>1</v>
@@ -12091,8 +12100,11 @@
       <c r="C90" t="s">
         <v>91</v>
       </c>
+      <c r="D90" t="s">
+        <v>112</v>
+      </c>
       <c r="E90" s="2" t="s">
-        <v>110</v>
+        <v>101</v>
       </c>
       <c r="F90" t="s">
         <v>15</v>
@@ -12104,11 +12116,11 @@
         <v>70</v>
       </c>
       <c r="I90" s="1">
-        <f>VLOOKUP(F90,'Source lists'!$E$1:F89,2,FALSE)</f>
+        <f>VLOOKUP(F90,'Source lists'!$E$1:F88,2,FALSE)</f>
         <v>4</v>
       </c>
       <c r="J90" s="1">
-        <f>VLOOKUP(G90,'Source lists'!$H$1:I90,2,FALSE)</f>
+        <f>VLOOKUP(G90,'Source lists'!$H$1:I89,2,FALSE)</f>
         <v>4</v>
       </c>
       <c r="K90" s="1">
@@ -12116,56 +12128,56 @@
         <v>12.8</v>
       </c>
     </row>
-    <row r="91" spans="1:11" ht="119" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:11" ht="34" x14ac:dyDescent="0.2">
       <c r="A91">
-        <v>41</v>
+        <v>56</v>
       </c>
       <c r="B91" t="s">
         <v>1</v>
       </c>
       <c r="C91" t="s">
-        <v>87</v>
-      </c>
-      <c r="D91" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="E91" s="2" t="s">
-        <v>90</v>
+        <v>110</v>
       </c>
       <c r="F91" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="G91" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="H91" t="s">
-        <v>22</v>
+        <v>70</v>
       </c>
       <c r="I91" s="1">
-        <f>VLOOKUP(F91,'Source lists'!$E$1:F90,2,FALSE)</f>
-        <v>1</v>
+        <f>VLOOKUP(F91,'Source lists'!$E$1:F89,2,FALSE)</f>
+        <v>4</v>
       </c>
       <c r="J91" s="1">
-        <f>VLOOKUP(G91,'Source lists'!$H$1:I91,2,FALSE)</f>
-        <v>10</v>
+        <f>VLOOKUP(G91,'Source lists'!$H$1:I90,2,FALSE)</f>
+        <v>4</v>
       </c>
       <c r="K91" s="1">
         <f>VLOOKUP(F91,'Source lists'!$E$2:$F$6,2,FALSE)*(VLOOKUP(G91,'Source lists'!$H$2:$I$7,2,FALSE)^2)/VLOOKUP(H91,'Source lists'!$K$2:$L$9,2,FALSE)</f>
-        <v>12.5</v>
-      </c>
-    </row>
-    <row r="92" spans="1:11" ht="68" x14ac:dyDescent="0.2">
+        <v>12.8</v>
+      </c>
+    </row>
+    <row r="92" spans="1:11" ht="119" x14ac:dyDescent="0.2">
       <c r="A92">
-        <v>52</v>
+        <v>41</v>
       </c>
       <c r="B92" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C92" t="s">
-        <v>104</v>
+        <v>87</v>
+      </c>
+      <c r="D92" t="s">
+        <v>89</v>
       </c>
       <c r="E92" s="2" t="s">
-        <v>114</v>
+        <v>90</v>
       </c>
       <c r="F92" t="s">
         <v>17</v>
@@ -12177,11 +12189,11 @@
         <v>22</v>
       </c>
       <c r="I92" s="1">
-        <f>VLOOKUP(F92,'Source lists'!$E$1:F91,2,FALSE)</f>
+        <f>VLOOKUP(F92,'Source lists'!$E$1:F90,2,FALSE)</f>
         <v>1</v>
       </c>
       <c r="J92" s="1">
-        <f>VLOOKUP(G92,'Source lists'!$H$1:I92,2,FALSE)</f>
+        <f>VLOOKUP(G92,'Source lists'!$H$1:I91,2,FALSE)</f>
         <v>10</v>
       </c>
       <c r="K92" s="1">
@@ -12189,18 +12201,18 @@
         <v>12.5</v>
       </c>
     </row>
-    <row r="93" spans="1:11" ht="51" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:11" ht="68" x14ac:dyDescent="0.2">
       <c r="A93">
-        <v>65</v>
+        <v>52</v>
       </c>
       <c r="B93" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C93" t="s">
-        <v>128</v>
+        <v>104</v>
       </c>
       <c r="E93" s="2" t="s">
-        <v>129</v>
+        <v>114</v>
       </c>
       <c r="F93" t="s">
         <v>17</v>
@@ -12212,11 +12224,11 @@
         <v>22</v>
       </c>
       <c r="I93" s="1">
-        <f>VLOOKUP(F93,'Source lists'!$E$1:F92,2,FALSE)</f>
+        <f>VLOOKUP(F93,'Source lists'!$E$1:F91,2,FALSE)</f>
         <v>1</v>
       </c>
       <c r="J93" s="1">
-        <f>VLOOKUP(G93,'Source lists'!$H$1:I93,2,FALSE)</f>
+        <f>VLOOKUP(G93,'Source lists'!$H$1:I92,2,FALSE)</f>
         <v>10</v>
       </c>
       <c r="K93" s="1">
@@ -12224,18 +12236,18 @@
         <v>12.5</v>
       </c>
     </row>
-    <row r="94" spans="1:11" ht="34" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:11" ht="51" x14ac:dyDescent="0.2">
       <c r="A94">
-        <v>83</v>
+        <v>65</v>
       </c>
       <c r="B94" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C94" t="s">
-        <v>148</v>
+        <v>128</v>
       </c>
       <c r="E94" s="2" t="s">
-        <v>149</v>
+        <v>129</v>
       </c>
       <c r="F94" t="s">
         <v>17</v>
@@ -12247,11 +12259,11 @@
         <v>22</v>
       </c>
       <c r="I94" s="1">
-        <f>VLOOKUP(F94,'Source lists'!$E$1:F93,2,FALSE)</f>
+        <f>VLOOKUP(F94,'Source lists'!$E$1:F92,2,FALSE)</f>
         <v>1</v>
       </c>
       <c r="J94" s="1">
-        <f>VLOOKUP(G94,'Source lists'!$H$1:I94,2,FALSE)</f>
+        <f>VLOOKUP(G94,'Source lists'!$H$1:I93,2,FALSE)</f>
         <v>10</v>
       </c>
       <c r="K94" s="1">
@@ -12259,18 +12271,18 @@
         <v>12.5</v>
       </c>
     </row>
-    <row r="95" spans="1:11" ht="119" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:11" ht="34" x14ac:dyDescent="0.2">
       <c r="A95">
-        <v>102</v>
+        <v>83</v>
       </c>
       <c r="B95" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C95" t="s">
-        <v>170</v>
+        <v>148</v>
       </c>
       <c r="E95" s="2" t="s">
-        <v>171</v>
+        <v>149</v>
       </c>
       <c r="F95" t="s">
         <v>17</v>
@@ -12282,11 +12294,11 @@
         <v>22</v>
       </c>
       <c r="I95" s="1">
-        <f>VLOOKUP(F95,'Source lists'!$E$1:F94,2,FALSE)</f>
+        <f>VLOOKUP(F95,'Source lists'!$E$1:F93,2,FALSE)</f>
         <v>1</v>
       </c>
       <c r="J95" s="1">
-        <f>VLOOKUP(G95,'Source lists'!$H$1:I95,2,FALSE)</f>
+        <f>VLOOKUP(G95,'Source lists'!$H$1:I94,2,FALSE)</f>
         <v>10</v>
       </c>
       <c r="K95" s="1">
@@ -12294,18 +12306,18 @@
         <v>12.5</v>
       </c>
     </row>
-    <row r="96" spans="1:11" ht="68" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:11" ht="119" x14ac:dyDescent="0.2">
       <c r="A96">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="B96" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C96" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="E96" s="2" t="s">
-        <v>196</v>
+        <v>171</v>
       </c>
       <c r="F96" t="s">
         <v>17</v>
@@ -12317,11 +12329,11 @@
         <v>22</v>
       </c>
       <c r="I96" s="1">
-        <f>VLOOKUP(F96,'Source lists'!$E$1:F95,2,FALSE)</f>
+        <f>VLOOKUP(F96,'Source lists'!$E$1:F94,2,FALSE)</f>
         <v>1</v>
       </c>
       <c r="J96" s="1">
-        <f>VLOOKUP(G96,'Source lists'!$H$1:I96,2,FALSE)</f>
+        <f>VLOOKUP(G96,'Source lists'!$H$1:I95,2,FALSE)</f>
         <v>10</v>
       </c>
       <c r="K96" s="1">
@@ -12331,16 +12343,16 @@
     </row>
     <row r="97" spans="1:11" ht="68" x14ac:dyDescent="0.2">
       <c r="A97">
-        <v>33</v>
+        <v>105</v>
       </c>
       <c r="B97" t="s">
-        <v>66</v>
+        <v>8</v>
       </c>
       <c r="C97" t="s">
-        <v>82</v>
+        <v>173</v>
       </c>
       <c r="E97" s="2" t="s">
-        <v>117</v>
+        <v>196</v>
       </c>
       <c r="F97" t="s">
         <v>17</v>
@@ -12349,30 +12361,33 @@
         <v>26</v>
       </c>
       <c r="H97" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="I97" s="1">
-        <f>VLOOKUP(F97,'Source lists'!$E$1:F96,2,FALSE)</f>
+        <f>VLOOKUP(F97,'Source lists'!$E$1:F95,2,FALSE)</f>
         <v>1</v>
       </c>
       <c r="J97" s="1">
-        <f>VLOOKUP(G97,'Source lists'!$H$1:I97,2,FALSE)</f>
+        <f>VLOOKUP(G97,'Source lists'!$H$1:I96,2,FALSE)</f>
         <v>10</v>
       </c>
       <c r="K97" s="1">
         <f>VLOOKUP(F97,'Source lists'!$E$2:$F$6,2,FALSE)*(VLOOKUP(G97,'Source lists'!$H$2:$I$7,2,FALSE)^2)/VLOOKUP(H97,'Source lists'!$K$2:$L$9,2,FALSE)</f>
-        <v>10</v>
-      </c>
-    </row>
-    <row r="98" spans="1:11" ht="17" x14ac:dyDescent="0.2">
+        <v>12.5</v>
+      </c>
+    </row>
+    <row r="98" spans="1:11" ht="68" x14ac:dyDescent="0.2">
       <c r="A98">
-        <v>62</v>
+        <v>33</v>
       </c>
       <c r="B98" t="s">
-        <v>7</v>
+        <v>66</v>
+      </c>
+      <c r="C98" t="s">
+        <v>82</v>
       </c>
       <c r="E98" s="2" t="s">
-        <v>125</v>
+        <v>117</v>
       </c>
       <c r="F98" t="s">
         <v>17</v>
@@ -12384,11 +12399,11 @@
         <v>21</v>
       </c>
       <c r="I98" s="1">
-        <f>VLOOKUP(F98,'Source lists'!$E$1:F97,2,FALSE)</f>
+        <f>VLOOKUP(F98,'Source lists'!$E$1:F96,2,FALSE)</f>
         <v>1</v>
       </c>
       <c r="J98" s="1">
-        <f>VLOOKUP(G98,'Source lists'!$H$1:I98,2,FALSE)</f>
+        <f>VLOOKUP(G98,'Source lists'!$H$1:I97,2,FALSE)</f>
         <v>10</v>
       </c>
       <c r="K98" s="1">
@@ -12398,13 +12413,13 @@
     </row>
     <row r="99" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A99">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B99" t="s">
-        <v>123</v>
+        <v>7</v>
       </c>
       <c r="E99" s="2" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="F99" t="s">
         <v>17</v>
@@ -12416,11 +12431,11 @@
         <v>21</v>
       </c>
       <c r="I99" s="1">
-        <f>VLOOKUP(F99,'Source lists'!$E$1:F98,2,FALSE)</f>
+        <f>VLOOKUP(F99,'Source lists'!$E$1:F97,2,FALSE)</f>
         <v>1</v>
       </c>
       <c r="J99" s="1">
-        <f>VLOOKUP(G99,'Source lists'!$H$1:I99,2,FALSE)</f>
+        <f>VLOOKUP(G99,'Source lists'!$H$1:I98,2,FALSE)</f>
         <v>10</v>
       </c>
       <c r="K99" s="1">
@@ -12428,18 +12443,15 @@
         <v>10</v>
       </c>
     </row>
-    <row r="100" spans="1:11" ht="119" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A100">
-        <v>82</v>
+        <v>63</v>
       </c>
       <c r="B100" t="s">
-        <v>5</v>
-      </c>
-      <c r="C100" t="s">
-        <v>147</v>
+        <v>123</v>
       </c>
       <c r="E100" s="2" t="s">
-        <v>197</v>
+        <v>124</v>
       </c>
       <c r="F100" t="s">
         <v>17</v>
@@ -12451,11 +12463,11 @@
         <v>21</v>
       </c>
       <c r="I100" s="1">
-        <f>VLOOKUP(F100,'Source lists'!$E$1:F99,2,FALSE)</f>
+        <f>VLOOKUP(F100,'Source lists'!$E$1:F98,2,FALSE)</f>
         <v>1</v>
       </c>
       <c r="J100" s="1">
-        <f>VLOOKUP(G100,'Source lists'!$H$1:I100,2,FALSE)</f>
+        <f>VLOOKUP(G100,'Source lists'!$H$1:I99,2,FALSE)</f>
         <v>10</v>
       </c>
       <c r="K100" s="1">
@@ -12463,18 +12475,18 @@
         <v>10</v>
       </c>
     </row>
-    <row r="101" spans="1:11" ht="51" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:11" ht="119" x14ac:dyDescent="0.2">
       <c r="A101">
-        <v>99</v>
+        <v>82</v>
       </c>
       <c r="B101" t="s">
-        <v>168</v>
+        <v>5</v>
       </c>
       <c r="C101" t="s">
-        <v>169</v>
+        <v>147</v>
       </c>
       <c r="E101" s="2" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="F101" t="s">
         <v>17</v>
@@ -12486,11 +12498,11 @@
         <v>21</v>
       </c>
       <c r="I101" s="1">
-        <f>VLOOKUP(F101,'Source lists'!$E$1:F100,2,FALSE)</f>
+        <f>VLOOKUP(F101,'Source lists'!$E$1:F99,2,FALSE)</f>
         <v>1</v>
       </c>
       <c r="J101" s="1">
-        <f>VLOOKUP(G101,'Source lists'!$H$1:I101,2,FALSE)</f>
+        <f>VLOOKUP(G101,'Source lists'!$H$1:I100,2,FALSE)</f>
         <v>10</v>
       </c>
       <c r="K101" s="1">
@@ -12498,53 +12510,53 @@
         <v>10</v>
       </c>
     </row>
-    <row r="102" spans="1:11" ht="34" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:11" ht="51" x14ac:dyDescent="0.2">
       <c r="A102">
+        <v>99</v>
+      </c>
+      <c r="B102" t="s">
+        <v>168</v>
+      </c>
+      <c r="C102" t="s">
+        <v>169</v>
+      </c>
+      <c r="E102" s="2" t="s">
+        <v>198</v>
+      </c>
+      <c r="F102" t="s">
+        <v>17</v>
+      </c>
+      <c r="G102" t="s">
         <v>26</v>
       </c>
-      <c r="B102" t="s">
-        <v>66</v>
-      </c>
-      <c r="C102" t="s">
-        <v>73</v>
-      </c>
-      <c r="E102" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="F102" t="s">
-        <v>16</v>
-      </c>
-      <c r="G102" t="s">
-        <v>29</v>
-      </c>
       <c r="H102" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="I102" s="1">
-        <f>VLOOKUP(F102,'Source lists'!$E$1:F101,2,FALSE)</f>
-        <v>3</v>
+        <f>VLOOKUP(F102,'Source lists'!$E$1:F100,2,FALSE)</f>
+        <v>1</v>
       </c>
       <c r="J102" s="1">
-        <f>VLOOKUP(G102,'Source lists'!$H$1:I102,2,FALSE)</f>
-        <v>3</v>
+        <f>VLOOKUP(G102,'Source lists'!$H$1:I101,2,FALSE)</f>
+        <v>10</v>
       </c>
       <c r="K102" s="1">
         <f>VLOOKUP(F102,'Source lists'!$E$2:$F$6,2,FALSE)*(VLOOKUP(G102,'Source lists'!$H$2:$I$7,2,FALSE)^2)/VLOOKUP(H102,'Source lists'!$K$2:$L$9,2,FALSE)</f>
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="103" spans="1:11" ht="34" x14ac:dyDescent="0.2">
       <c r="A103">
-        <v>39</v>
+        <v>26</v>
       </c>
       <c r="B103" t="s">
-        <v>1</v>
+        <v>66</v>
       </c>
       <c r="C103" t="s">
-        <v>87</v>
+        <v>73</v>
       </c>
       <c r="E103" s="2" t="s">
-        <v>119</v>
+        <v>74</v>
       </c>
       <c r="F103" t="s">
         <v>16</v>
@@ -12556,11 +12568,11 @@
         <v>24</v>
       </c>
       <c r="I103" s="1">
-        <f>VLOOKUP(F103,'Source lists'!$E$1:F102,2,FALSE)</f>
+        <f>VLOOKUP(F103,'Source lists'!$E$1:F101,2,FALSE)</f>
         <v>3</v>
       </c>
       <c r="J103" s="1">
-        <f>VLOOKUP(G103,'Source lists'!$H$1:I103,2,FALSE)</f>
+        <f>VLOOKUP(G103,'Source lists'!$H$1:I102,2,FALSE)</f>
         <v>3</v>
       </c>
       <c r="K103" s="1">
@@ -12568,18 +12580,18 @@
         <v>9</v>
       </c>
     </row>
-    <row r="104" spans="1:11" ht="17" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:11" ht="34" x14ac:dyDescent="0.2">
       <c r="A104">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="B104" t="s">
         <v>1</v>
       </c>
       <c r="C104" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="E104" s="2" t="s">
-        <v>92</v>
+        <v>119</v>
       </c>
       <c r="F104" t="s">
         <v>16</v>
@@ -12591,11 +12603,11 @@
         <v>24</v>
       </c>
       <c r="I104" s="1">
-        <f>VLOOKUP(F104,'Source lists'!$E$1:F103,2,FALSE)</f>
+        <f>VLOOKUP(F104,'Source lists'!$E$1:F102,2,FALSE)</f>
         <v>3</v>
       </c>
       <c r="J104" s="1">
-        <f>VLOOKUP(G104,'Source lists'!$H$1:I104,2,FALSE)</f>
+        <f>VLOOKUP(G104,'Source lists'!$H$1:I103,2,FALSE)</f>
         <v>3</v>
       </c>
       <c r="K104" s="1">
@@ -12603,9 +12615,9 @@
         <v>9</v>
       </c>
     </row>
-    <row r="105" spans="1:11" ht="34" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A105">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="B105" t="s">
         <v>1</v>
@@ -12614,7 +12626,7 @@
         <v>91</v>
       </c>
       <c r="E105" s="2" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="F105" t="s">
         <v>16</v>
@@ -12626,11 +12638,11 @@
         <v>24</v>
       </c>
       <c r="I105" s="1">
-        <f>VLOOKUP(F105,'Source lists'!$E$1:F104,2,FALSE)</f>
+        <f>VLOOKUP(F105,'Source lists'!$E$1:F103,2,FALSE)</f>
         <v>3</v>
       </c>
       <c r="J105" s="1">
-        <f>VLOOKUP(G105,'Source lists'!$H$1:I105,2,FALSE)</f>
+        <f>VLOOKUP(G105,'Source lists'!$H$1:I104,2,FALSE)</f>
         <v>3</v>
       </c>
       <c r="K105" s="1">
@@ -12638,35 +12650,35 @@
         <v>9</v>
       </c>
     </row>
-    <row r="106" spans="1:11" ht="17" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:11" ht="34" x14ac:dyDescent="0.2">
       <c r="A106">
-        <v>68</v>
+        <v>46</v>
       </c>
       <c r="B106" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C106" t="s">
-        <v>131</v>
+        <v>91</v>
       </c>
       <c r="E106" s="2" t="s">
-        <v>199</v>
+        <v>98</v>
       </c>
       <c r="F106" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G106" t="s">
-        <v>159</v>
+        <v>29</v>
       </c>
       <c r="H106" t="s">
-        <v>67</v>
+        <v>24</v>
       </c>
       <c r="I106" s="1">
-        <f>VLOOKUP(F106,'Source lists'!$E$1:F105,2,FALSE)</f>
-        <v>1</v>
+        <f>VLOOKUP(F106,'Source lists'!$E$1:F104,2,FALSE)</f>
+        <v>3</v>
       </c>
       <c r="J106" s="1">
-        <f>VLOOKUP(G106,'Source lists'!$H$1:I106,2,FALSE)</f>
-        <v>6</v>
+        <f>VLOOKUP(G106,'Source lists'!$H$1:I105,2,FALSE)</f>
+        <v>3</v>
       </c>
       <c r="K106" s="1">
         <f>VLOOKUP(F106,'Source lists'!$E$2:$F$6,2,FALSE)*(VLOOKUP(G106,'Source lists'!$H$2:$I$7,2,FALSE)^2)/VLOOKUP(H106,'Source lists'!$K$2:$L$9,2,FALSE)</f>
@@ -12675,7 +12687,7 @@
     </row>
     <row r="107" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A107">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B107" t="s">
         <v>2</v>
@@ -12684,7 +12696,7 @@
         <v>131</v>
       </c>
       <c r="E107" s="2" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="F107" t="s">
         <v>17</v>
@@ -12696,11 +12708,11 @@
         <v>67</v>
       </c>
       <c r="I107" s="1">
-        <f>VLOOKUP(F107,'Source lists'!$E$1:F106,2,FALSE)</f>
+        <f>VLOOKUP(F107,'Source lists'!$E$1:F105,2,FALSE)</f>
         <v>1</v>
       </c>
       <c r="J107" s="1">
-        <f>VLOOKUP(G107,'Source lists'!$H$1:I107,2,FALSE)</f>
+        <f>VLOOKUP(G107,'Source lists'!$H$1:I106,2,FALSE)</f>
         <v>6</v>
       </c>
       <c r="K107" s="1">
@@ -12710,7 +12722,7 @@
     </row>
     <row r="108" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A108">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B108" t="s">
         <v>2</v>
@@ -12719,7 +12731,7 @@
         <v>131</v>
       </c>
       <c r="E108" s="2" t="s">
-        <v>132</v>
+        <v>200</v>
       </c>
       <c r="F108" t="s">
         <v>17</v>
@@ -12731,11 +12743,11 @@
         <v>67</v>
       </c>
       <c r="I108" s="1">
-        <f>VLOOKUP(F108,'Source lists'!$E$1:F107,2,FALSE)</f>
+        <f>VLOOKUP(F108,'Source lists'!$E$1:F106,2,FALSE)</f>
         <v>1</v>
       </c>
       <c r="J108" s="1">
-        <f>VLOOKUP(G108,'Source lists'!$H$1:I108,2,FALSE)</f>
+        <f>VLOOKUP(G108,'Source lists'!$H$1:I107,2,FALSE)</f>
         <v>6</v>
       </c>
       <c r="K108" s="1">
@@ -12743,21 +12755,18 @@
         <v>9</v>
       </c>
     </row>
-    <row r="109" spans="1:11" ht="119" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A109">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="B109" t="s">
         <v>2</v>
       </c>
       <c r="C109" t="s">
-        <v>133</v>
-      </c>
-      <c r="D109" t="s">
-        <v>138</v>
+        <v>131</v>
       </c>
       <c r="E109" s="2" t="s">
-        <v>201</v>
+        <v>132</v>
       </c>
       <c r="F109" t="s">
         <v>17</v>
@@ -12769,11 +12778,11 @@
         <v>67</v>
       </c>
       <c r="I109" s="1">
-        <f>VLOOKUP(F109,'Source lists'!$E$1:F108,2,FALSE)</f>
+        <f>VLOOKUP(F109,'Source lists'!$E$1:F107,2,FALSE)</f>
         <v>1</v>
       </c>
       <c r="J109" s="1">
-        <f>VLOOKUP(G109,'Source lists'!$H$1:I109,2,FALSE)</f>
+        <f>VLOOKUP(G109,'Source lists'!$H$1:I108,2,FALSE)</f>
         <v>6</v>
       </c>
       <c r="K109" s="1">
@@ -12781,18 +12790,21 @@
         <v>9</v>
       </c>
     </row>
-    <row r="110" spans="1:11" ht="17" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:11" ht="119" x14ac:dyDescent="0.2">
       <c r="A110">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B110" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C110" t="s">
-        <v>142</v>
+        <v>133</v>
+      </c>
+      <c r="D110" t="s">
+        <v>138</v>
       </c>
       <c r="E110" s="2" t="s">
-        <v>144</v>
+        <v>201</v>
       </c>
       <c r="F110" t="s">
         <v>17</v>
@@ -12804,11 +12816,11 @@
         <v>67</v>
       </c>
       <c r="I110" s="1">
-        <f>VLOOKUP(F110,'Source lists'!$E$1:F109,2,FALSE)</f>
+        <f>VLOOKUP(F110,'Source lists'!$E$1:F108,2,FALSE)</f>
         <v>1</v>
       </c>
       <c r="J110" s="1">
-        <f>VLOOKUP(G110,'Source lists'!$H$1:I110,2,FALSE)</f>
+        <f>VLOOKUP(G110,'Source lists'!$H$1:I109,2,FALSE)</f>
         <v>6</v>
       </c>
       <c r="K110" s="1">
@@ -12816,32 +12828,35 @@
         <v>9</v>
       </c>
     </row>
-    <row r="111" spans="1:11" ht="34" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A111">
-        <v>110</v>
+        <v>78</v>
       </c>
       <c r="B111" t="s">
-        <v>75</v>
+        <v>3</v>
+      </c>
+      <c r="C111" t="s">
+        <v>142</v>
       </c>
       <c r="E111" s="2" t="s">
-        <v>185</v>
+        <v>144</v>
       </c>
       <c r="F111" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="G111" t="s">
-        <v>29</v>
+        <v>159</v>
       </c>
       <c r="H111" t="s">
-        <v>24</v>
+        <v>67</v>
       </c>
       <c r="I111" s="1">
-        <f>VLOOKUP(F111,'Source lists'!$E$1:F45,2,FALSE)</f>
-        <v>3</v>
+        <f>VLOOKUP(F111,'Source lists'!$E$1:F109,2,FALSE)</f>
+        <v>1</v>
       </c>
       <c r="J111" s="1">
-        <f>VLOOKUP(G111,'Source lists'!$H$1:I46,2,FALSE)</f>
-        <v>3</v>
+        <f>VLOOKUP(G111,'Source lists'!$H$1:I110,2,FALSE)</f>
+        <v>6</v>
       </c>
       <c r="K111" s="1">
         <f>VLOOKUP(F111,'Source lists'!$E$2:$F$6,2,FALSE)*(VLOOKUP(G111,'Source lists'!$H$2:$I$7,2,FALSE)^2)/VLOOKUP(H111,'Source lists'!$K$2:$L$9,2,FALSE)</f>
@@ -12850,124 +12865,121 @@
     </row>
     <row r="112" spans="1:11" ht="34" x14ac:dyDescent="0.2">
       <c r="A112">
-        <v>51</v>
+        <v>110</v>
       </c>
       <c r="B112" t="s">
         <v>75</v>
       </c>
-      <c r="C112" t="s">
-        <v>102</v>
-      </c>
       <c r="E112" s="2" t="s">
-        <v>103</v>
+        <v>185</v>
       </c>
       <c r="F112" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G112" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="H112" t="s">
-        <v>69</v>
+        <v>24</v>
       </c>
       <c r="I112" s="1">
-        <f>VLOOKUP(F112,'Source lists'!$E$1:F110,2,FALSE)</f>
-        <v>1</v>
+        <f>VLOOKUP(F112,'Source lists'!$E$1:F45,2,FALSE)</f>
+        <v>3</v>
       </c>
       <c r="J112" s="1">
-        <f>VLOOKUP(G112,'Source lists'!$H$1:I111,2,FALSE)</f>
-        <v>7</v>
+        <f>VLOOKUP(G112,'Source lists'!$H$1:I46,2,FALSE)</f>
+        <v>3</v>
       </c>
       <c r="K112" s="1">
         <f>VLOOKUP(F112,'Source lists'!$E$2:$F$6,2,FALSE)*(VLOOKUP(G112,'Source lists'!$H$2:$I$7,2,FALSE)^2)/VLOOKUP(H112,'Source lists'!$K$2:$L$9,2,FALSE)</f>
-        <v>7</v>
+        <v>9</v>
       </c>
     </row>
     <row r="113" spans="1:13" ht="34" x14ac:dyDescent="0.2">
       <c r="A113">
-        <v>28</v>
+        <v>51</v>
       </c>
       <c r="B113" t="s">
-        <v>66</v>
+        <v>75</v>
       </c>
       <c r="C113" t="s">
-        <v>73</v>
+        <v>102</v>
       </c>
       <c r="E113" s="2" t="s">
-        <v>78</v>
+        <v>103</v>
       </c>
       <c r="F113" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="G113" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="H113" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="I113" s="1">
-        <f>VLOOKUP(F113,'Source lists'!$E$1:F111,2,FALSE)</f>
-        <v>3</v>
+        <f>VLOOKUP(F113,'Source lists'!$E$1:F110,2,FALSE)</f>
+        <v>1</v>
       </c>
       <c r="J113" s="1">
-        <f>VLOOKUP(G113,'Source lists'!$H$1:I112,2,FALSE)</f>
-        <v>3</v>
+        <f>VLOOKUP(G113,'Source lists'!$H$1:I111,2,FALSE)</f>
+        <v>7</v>
       </c>
       <c r="K113" s="1">
         <f>VLOOKUP(F113,'Source lists'!$E$2:$F$6,2,FALSE)*(VLOOKUP(G113,'Source lists'!$H$2:$I$7,2,FALSE)^2)/VLOOKUP(H113,'Source lists'!$K$2:$L$9,2,FALSE)</f>
-        <v>6.75</v>
+        <v>7</v>
       </c>
     </row>
     <row r="114" spans="1:13" ht="34" x14ac:dyDescent="0.2">
       <c r="A114">
-        <v>111</v>
+        <v>28</v>
       </c>
       <c r="B114" t="s">
-        <v>2</v>
+        <v>66</v>
       </c>
       <c r="C114" t="s">
-        <v>133</v>
+        <v>73</v>
       </c>
       <c r="E114" s="2" t="s">
-        <v>203</v>
+        <v>78</v>
       </c>
       <c r="F114" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="G114" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H114" t="s">
-        <v>23</v>
+        <v>67</v>
       </c>
       <c r="I114" s="1">
-        <f>VLOOKUP(F114,'Source lists'!$E$1:F46,2,FALSE)</f>
-        <v>4</v>
+        <f>VLOOKUP(F114,'Source lists'!$E$1:F111,2,FALSE)</f>
+        <v>3</v>
       </c>
       <c r="J114" s="1">
-        <f>VLOOKUP(G114,'Source lists'!$H$1:I47,2,FALSE)</f>
-        <v>1</v>
+        <f>VLOOKUP(G114,'Source lists'!$H$1:I112,2,FALSE)</f>
+        <v>3</v>
       </c>
       <c r="K114" s="1">
         <f>VLOOKUP(F114,'Source lists'!$E$2:$F$6,2,FALSE)*(VLOOKUP(G114,'Source lists'!$H$2:$I$7,2,FALSE)^2)/VLOOKUP(H114,'Source lists'!$K$2:$L$9,2,FALSE)</f>
-        <v>2</v>
+        <v>6.75</v>
       </c>
     </row>
     <row r="115" spans="1:13" ht="34" x14ac:dyDescent="0.2">
       <c r="A115">
-        <v>29</v>
+        <v>111</v>
       </c>
       <c r="B115" t="s">
-        <v>66</v>
+        <v>2</v>
       </c>
       <c r="C115" t="s">
-        <v>73</v>
+        <v>133</v>
       </c>
       <c r="E115" s="2" t="s">
-        <v>79</v>
+        <v>203</v>
       </c>
       <c r="F115" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G115" t="s">
         <v>30</v>
@@ -12976,27 +12988,27 @@
         <v>23</v>
       </c>
       <c r="I115" s="1">
-        <f>VLOOKUP(F115,'Source lists'!$E$1:F112,2,FALSE)</f>
-        <v>3</v>
+        <f>VLOOKUP(F115,'Source lists'!$E$1:F46,2,FALSE)</f>
+        <v>4</v>
       </c>
       <c r="J115" s="1">
-        <f>VLOOKUP(G115,'Source lists'!$H$1:I113,2,FALSE)</f>
+        <f>VLOOKUP(G115,'Source lists'!$H$1:I47,2,FALSE)</f>
         <v>1</v>
       </c>
       <c r="K115" s="1">
         <f>VLOOKUP(F115,'Source lists'!$E$2:$F$6,2,FALSE)*(VLOOKUP(G115,'Source lists'!$H$2:$I$7,2,FALSE)^2)/VLOOKUP(H115,'Source lists'!$K$2:$L$9,2,FALSE)</f>
-        <v>1.5</v>
-      </c>
-      <c r="L115">
-        <v>27</v>
+        <v>2</v>
       </c>
     </row>
     <row r="116" spans="1:13" ht="34" x14ac:dyDescent="0.2">
       <c r="A116">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B116" t="s">
-        <v>38</v>
+        <v>66</v>
+      </c>
+      <c r="C116" t="s">
+        <v>73</v>
       </c>
       <c r="E116" s="2" t="s">
         <v>79</v>
@@ -13011,11 +13023,11 @@
         <v>23</v>
       </c>
       <c r="I116" s="1">
-        <f>VLOOKUP(F116,'Source lists'!$E$1:F113,2,FALSE)</f>
+        <f>VLOOKUP(F116,'Source lists'!$E$1:F112,2,FALSE)</f>
         <v>3</v>
       </c>
       <c r="J116" s="1">
-        <f>VLOOKUP(G116,'Source lists'!$H$1:I114,2,FALSE)</f>
+        <f>VLOOKUP(G116,'Source lists'!$H$1:I113,2,FALSE)</f>
         <v>1</v>
       </c>
       <c r="K116" s="1">
@@ -13026,19 +13038,15 @@
         <v>27</v>
       </c>
     </row>
-    <row r="117" spans="1:13" s="3" customFormat="1" ht="34" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:13" ht="34" x14ac:dyDescent="0.2">
       <c r="A117">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="B117" t="s">
-        <v>75</v>
-      </c>
-      <c r="C117" t="s">
-        <v>76</v>
-      </c>
-      <c r="D117"/>
+        <v>38</v>
+      </c>
       <c r="E117" s="2" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="F117" t="s">
         <v>16</v>
@@ -13047,22 +13055,61 @@
         <v>30</v>
       </c>
       <c r="H117" t="s">
-        <v>69</v>
+        <v>23</v>
       </c>
       <c r="I117" s="1">
-        <f>VLOOKUP(F117,'Source lists'!$E$1:F114,2,FALSE)</f>
+        <f>VLOOKUP(F117,'Source lists'!$E$1:F113,2,FALSE)</f>
         <v>3</v>
       </c>
       <c r="J117" s="1">
-        <f>VLOOKUP(G117,'Source lists'!$H$1:I115,2,FALSE)</f>
+        <f>VLOOKUP(G117,'Source lists'!$H$1:I114,2,FALSE)</f>
         <v>1</v>
       </c>
       <c r="K117" s="1">
         <f>VLOOKUP(F117,'Source lists'!$E$2:$F$6,2,FALSE)*(VLOOKUP(G117,'Source lists'!$H$2:$I$7,2,FALSE)^2)/VLOOKUP(H117,'Source lists'!$K$2:$L$9,2,FALSE)</f>
+        <v>1.5</v>
+      </c>
+      <c r="L117">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="118" spans="1:13" s="3" customFormat="1" ht="34" x14ac:dyDescent="0.2">
+      <c r="A118">
+        <v>27</v>
+      </c>
+      <c r="B118" t="s">
+        <v>75</v>
+      </c>
+      <c r="C118" t="s">
+        <v>76</v>
+      </c>
+      <c r="D118"/>
+      <c r="E118" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="F118" t="s">
+        <v>16</v>
+      </c>
+      <c r="G118" t="s">
+        <v>30</v>
+      </c>
+      <c r="H118" t="s">
+        <v>69</v>
+      </c>
+      <c r="I118" s="1">
+        <f>VLOOKUP(F118,'Source lists'!$E$1:F114,2,FALSE)</f>
+        <v>3</v>
+      </c>
+      <c r="J118" s="1">
+        <f>VLOOKUP(G118,'Source lists'!$H$1:I115,2,FALSE)</f>
+        <v>1</v>
+      </c>
+      <c r="K118" s="1">
+        <f>VLOOKUP(F118,'Source lists'!$E$2:$F$6,2,FALSE)*(VLOOKUP(G118,'Source lists'!$H$2:$I$7,2,FALSE)^2)/VLOOKUP(H118,'Source lists'!$K$2:$L$9,2,FALSE)</f>
         <v>0.42857142857142855</v>
       </c>
-      <c r="L117"/>
-      <c r="M117"/>
+      <c r="L118"/>
+      <c r="M118"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:M1" xr:uid="{1EB57299-5CFD-7049-BDE4-6415040FFB14}">

</xml_diff>

<commit_message>
e-Questrian/libs/landing-page: Call to action seciton of landing page extracted to lib (Landing page lib componet now set up)
</commit_message>
<xml_diff>
--- a/apps/e-questrian/e-Questrian - To do list.xlsx
+++ b/apps/e-questrian/e-Questrian - To do list.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rferreira/sigmafox/apps/e-questrian/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A6B1278-B0D5-614F-BA21-F33C67100DDE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DFCE63B-F6F0-ED46-878E-F2114DAD0034}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="740" windowWidth="34560" windowHeight="21600" activeTab="2" xr2:uid="{DC2B379E-A936-2146-8C4F-53C43AECE05C}"/>
   </bookViews>
@@ -3652,7 +3652,7 @@
   <dimension ref="A1:XEX118"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="G22" sqref="G22"/>
+      <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="34.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
SigmaFox: Maintaince of repo
</commit_message>
<xml_diff>
--- a/apps/e-questrian/e-Questrian - To do list.xlsx
+++ b/apps/e-questrian/e-Questrian - To do list.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rferreira/sigmafox/apps/e-questrian/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DFCE63B-F6F0-ED46-878E-F2114DAD0034}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CAD30F0A-D96A-0042-80C6-359EF263DAF3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="740" windowWidth="34560" windowHeight="21600" activeTab="2" xr2:uid="{DC2B379E-A936-2146-8C4F-53C43AECE05C}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="19820" activeTab="2" xr2:uid="{DC2B379E-A936-2146-8C4F-53C43AECE05C}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary of completion" sheetId="3" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="869" uniqueCount="216">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="870" uniqueCount="216">
   <si>
     <t>Sections</t>
   </si>
@@ -260,14 +260,6 @@
   </si>
   <si>
     <t>Dependency #</t>
-  </si>
-  <si>
-    <t>After registering - User should be presented with a basis users detail form with:
-First name
-Last name
-Contact number
-User should also presented the option to skip
-Should be place on top of the main menu page (for now - will be replaced by dash board)</t>
   </si>
   <si>
     <t>Main menu</t>
@@ -726,6 +718,14 @@
   </si>
   <si>
     <t>Why us section</t>
+  </si>
+  <si>
+    <t>After registering - User should be presented with a basic users detail form with:
+First name
+Last name
+Contact number
+User should also presented the option to skip
+Should be place on top of the main menu page (for now - will be replaced by dash board)</t>
   </si>
 </sst>
 </file>
@@ -3111,23 +3111,23 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B1" s="6" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B2" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C2" t="s">
+        <v>177</v>
+      </c>
+      <c r="D2" t="s">
         <v>178</v>
-      </c>
-      <c r="D2" t="s">
-        <v>179</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B3">
         <v>1116.2</v>
@@ -3147,23 +3147,23 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B7" s="6" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B8" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C8" t="s">
+        <v>177</v>
+      </c>
+      <c r="D8" t="s">
         <v>178</v>
-      </c>
-      <c r="D8" t="s">
-        <v>179</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B9">
         <v>93</v>
@@ -3183,23 +3183,23 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B13" s="6" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B14" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C14" t="s">
+        <v>177</v>
+      </c>
+      <c r="D14" t="s">
         <v>178</v>
-      </c>
-      <c r="D14" t="s">
-        <v>179</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B15">
         <v>89</v>
@@ -3271,10 +3271,10 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E2" t="s">
         <v>13</v>
@@ -3300,7 +3300,7 @@
         <v>6</v>
       </c>
       <c r="B3" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C3" t="s">
         <v>35</v>
@@ -3329,10 +3329,10 @@
         <v>66</v>
       </c>
       <c r="B4" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C4" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="E4" t="s">
         <v>15</v>
@@ -3341,7 +3341,7 @@
         <v>4</v>
       </c>
       <c r="H4" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="I4">
         <v>6</v>
@@ -3358,7 +3358,7 @@
         <v>5</v>
       </c>
       <c r="B5" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C5" t="s">
         <v>40</v>
@@ -3387,7 +3387,7 @@
         <v>2</v>
       </c>
       <c r="B6" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C6" t="s">
         <v>54</v>
@@ -3416,10 +3416,10 @@
         <v>3</v>
       </c>
       <c r="B7" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C7" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="H7" t="s">
         <v>30</v>
@@ -3439,10 +3439,10 @@
         <v>4</v>
       </c>
       <c r="B8" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C8" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="K8" t="s">
         <v>23</v>
@@ -3453,10 +3453,10 @@
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B9" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C9" t="s">
         <v>37</v>
@@ -3470,13 +3470,13 @@
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B10" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C10" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.2">
@@ -3484,7 +3484,7 @@
         <v>39</v>
       </c>
       <c r="B11" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C11" t="s">
         <v>44</v>
@@ -3495,15 +3495,15 @@
         <v>38</v>
       </c>
       <c r="B12" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C12" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B13" t="s">
         <v>33</v>
@@ -3525,10 +3525,10 @@
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B15" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C15" t="s">
         <v>64</v>
@@ -3536,10 +3536,10 @@
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B16" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C16" t="s">
         <v>68</v>
@@ -3547,31 +3547,31 @@
     </row>
     <row r="17" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B17" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C17" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="18" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B18" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C18" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="19" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B19" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C19" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="20" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B20" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="21" spans="2:3" x14ac:dyDescent="0.2">
@@ -3581,62 +3581,62 @@
     </row>
     <row r="22" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B22" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="23" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B23" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="24" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B24" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="25" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B25" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="26" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B26" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="27" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B27" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="28" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B28" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="29" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B29" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="30" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B30" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="31" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B31" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="32" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B32" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="33" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B33" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
   </sheetData>
@@ -3652,7 +3652,7 @@
   <dimension ref="A1:XEX118"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="F22" sqref="F22"/>
+      <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="34.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3698,19 +3698,19 @@
         <v>20</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="L1" t="s">
         <v>71</v>
       </c>
       <c r="M1" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="2" spans="1:2046 2050:3066 3073:4093 4100:5120 5127:6141 6145:7168 7172:8188 8195:9215 9222:11263 11267:12283 12290:13310 13317:15358 15362:16378" s="3" customFormat="1" ht="34" x14ac:dyDescent="0.2">
@@ -3721,13 +3721,13 @@
         <v>1</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="F2" s="3" t="s">
         <v>14</v>
@@ -3754,7 +3754,7 @@
         <v>77</v>
       </c>
       <c r="M2" s="3" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="3" spans="1:2046 2050:3066 3073:4093 4100:5120 5127:6141 6145:7168 7172:8188 8195:9215 9222:11263 11267:12283 12290:13310 13317:15358 15362:16378" s="3" customFormat="1" ht="17" x14ac:dyDescent="0.2">
@@ -3768,7 +3768,7 @@
         <v>41</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="F3" s="3" t="s">
         <v>15</v>
@@ -3795,7 +3795,7 @@
         <v>1</v>
       </c>
       <c r="M3" s="3" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="4" spans="1:2046 2050:3066 3073:4093 4100:5120 5127:6141 6145:7168 7172:8188 8195:9215 9222:11263 11267:12283 12290:13310 13317:15358 15362:16378" ht="17" x14ac:dyDescent="0.2">
@@ -3806,17 +3806,17 @@
         <v>3</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="D4" s="3"/>
       <c r="E4" s="4" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="F4" s="3" t="s">
         <v>14</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="H4" s="3" t="s">
         <v>24</v>
@@ -3835,7 +3835,7 @@
       </c>
       <c r="L4" s="3"/>
       <c r="M4" s="3" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="5" spans="1:2046 2050:3066 3073:4093 4100:5120 5127:6141 6145:7168 7172:8188 8195:9215 9222:11263 11267:12283 12290:13310 13317:15358 15362:16378" ht="17" x14ac:dyDescent="0.2">
@@ -3846,17 +3846,17 @@
         <v>6</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="D5" s="3"/>
       <c r="E5" s="4" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="F5" s="3" t="s">
         <v>14</v>
       </c>
       <c r="G5" s="3" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="H5" s="3" t="s">
         <v>24</v>
@@ -3875,7 +3875,7 @@
       </c>
       <c r="L5" s="3"/>
       <c r="M5" s="3" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="6" spans="1:2046 2050:3066 3073:4093 4100:5120 5127:6141 6145:7168 7172:8188 8195:9215 9222:11263 11267:12283 12290:13310 13317:15358 15362:16378" ht="17" x14ac:dyDescent="0.2">
@@ -3886,17 +3886,17 @@
         <v>4</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="D6" s="3"/>
       <c r="E6" s="4" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="F6" s="3" t="s">
         <v>14</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="H6" s="3" t="s">
         <v>24</v>
@@ -3917,7 +3917,7 @@
         <v>53</v>
       </c>
       <c r="M6" s="3" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="7" spans="1:2046 2050:3066 3073:4093 4100:5120 5127:6141 6145:7168 7172:8188 8195:9215 9222:11263 11267:12283 12290:13310 13317:15358 15362:16378" ht="17" x14ac:dyDescent="0.2">
@@ -3928,17 +3928,17 @@
         <v>3</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="D7" s="3"/>
       <c r="E7" s="4" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="F7" s="3" t="s">
         <v>14</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="H7" s="3" t="s">
         <v>24</v>
@@ -3957,7 +3957,7 @@
       </c>
       <c r="L7" s="3"/>
       <c r="M7" s="3" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="8" spans="1:2046 2050:3066 3073:4093 4100:5120 5127:6141 6145:7168 7172:8188 8195:9215 9222:11263 11267:12283 12290:13310 13317:15358 15362:16378" ht="17" x14ac:dyDescent="0.2">
@@ -3968,19 +3968,19 @@
         <v>1</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="F8" s="3" t="s">
         <v>15</v>
       </c>
       <c r="G8" s="3" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="H8" s="3" t="s">
         <v>23</v>
@@ -3999,48 +3999,51 @@
       </c>
       <c r="L8" s="3"/>
       <c r="M8" s="3" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2046 2050:3066 3073:4093 4100:5120 5127:6141 6145:7168 7172:8188 8195:9215 9222:11263 11267:12283 12290:13310 13317:15358 15362:16378" ht="34" x14ac:dyDescent="0.2">
-      <c r="A9">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2046 2050:3066 3073:4093 4100:5120 5127:6141 6145:7168 7172:8188 8195:9215 9222:11263 11267:12283 12290:13310 13317:15358 15362:16378" ht="17" x14ac:dyDescent="0.2">
+      <c r="A9" s="3">
         <v>116</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C9" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="D9" t="s">
+      <c r="D9" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="E9" s="2" t="s">
-        <v>213</v>
-      </c>
-      <c r="F9" t="s">
+      <c r="E9" s="4" t="s">
+        <v>212</v>
+      </c>
+      <c r="F9" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="G9" t="s">
-        <v>159</v>
-      </c>
-      <c r="H9" t="s">
+      <c r="G9" s="3" t="s">
+        <v>158</v>
+      </c>
+      <c r="H9" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="I9" s="1">
+      <c r="I9" s="5">
         <f>VLOOKUP(F9,'Source lists'!$E$1:F133,2,FALSE)</f>
         <v>4</v>
       </c>
-      <c r="J9" s="1">
+      <c r="J9" s="5">
         <f>VLOOKUP(G9,'Source lists'!$H$1:I134,2,FALSE)</f>
         <v>6</v>
       </c>
-      <c r="K9" s="1">
+      <c r="K9" s="5">
         <f>VLOOKUP(F9,'Source lists'!$E$2:$F$6,2,FALSE)*(VLOOKUP(G9,'Source lists'!$H$2:$I$7,2,FALSE)^2)/VLOOKUP(H9,'Source lists'!$K$2:$L$9,2,FALSE)</f>
         <v>72</v>
       </c>
-      <c r="L9">
+      <c r="L9" s="3">
         <v>2</v>
+      </c>
+      <c r="M9" s="3" t="s">
+        <v>175</v>
       </c>
     </row>
     <row r="10" spans="1:2046 2050:3066 3073:4093 4100:5120 5127:6141 6145:7168 7172:8188 8195:9215 9222:11263 11267:12283 12290:13310 13317:15358 15362:16378" s="3" customFormat="1" ht="17" x14ac:dyDescent="0.2">
@@ -4051,10 +4054,10 @@
         <v>38</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="F10" s="3" t="s">
         <v>15</v>
@@ -4078,7 +4081,7 @@
         <v>64</v>
       </c>
       <c r="M10" s="3" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="R10" s="4"/>
       <c r="V10" s="5"/>
@@ -9122,20 +9125,20 @@
         <v>113</v>
       </c>
       <c r="B11" s="3" t="s">
+        <v>206</v>
+      </c>
+      <c r="C11" s="3" t="s">
         <v>207</v>
-      </c>
-      <c r="C11" s="3" t="s">
-        <v>208</v>
       </c>
       <c r="D11" s="3"/>
       <c r="E11" s="4" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="F11" s="3" t="s">
         <v>14</v>
       </c>
       <c r="G11" s="3" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="H11" s="3" t="s">
         <v>70</v>
@@ -9154,7 +9157,7 @@
       </c>
       <c r="L11" s="3"/>
       <c r="M11" s="3" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="12" spans="1:2046 2050:3066 3073:4093 4100:5120 5127:6141 6145:7168 7172:8188 8195:9215 9222:11263 11267:12283 12290:13310 13317:15358 15362:16378" ht="51" x14ac:dyDescent="0.2">
@@ -9194,7 +9197,7 @@
       </c>
       <c r="L12" s="3"/>
       <c r="M12" s="3" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="13" spans="1:2046 2050:3066 3073:4093 4100:5120 5127:6141 6145:7168 7172:8188 8195:9215 9222:11263 11267:12283 12290:13310 13317:15358 15362:16378" s="3" customFormat="1" ht="17" x14ac:dyDescent="0.2">
@@ -9205,11 +9208,11 @@
         <v>2</v>
       </c>
       <c r="C13" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D13"/>
       <c r="E13" s="2" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="F13" t="s">
         <v>17</v>
@@ -9245,10 +9248,10 @@
         <v>1</v>
       </c>
       <c r="C14" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="F14" t="s">
         <v>17</v>
@@ -9283,10 +9286,10 @@
         <v>1</v>
       </c>
       <c r="C15" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="F15" t="s">
         <v>17</v>
@@ -9321,10 +9324,10 @@
         <v>2</v>
       </c>
       <c r="C16" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="F16" t="s">
         <v>17</v>
@@ -9359,11 +9362,11 @@
         <v>1</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D17" s="3"/>
       <c r="E17" s="4" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="F17" s="3" t="s">
         <v>14</v>
@@ -9388,7 +9391,7 @@
       </c>
       <c r="L17" s="3"/>
       <c r="M17" s="3" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="18" spans="1:13" ht="34" x14ac:dyDescent="0.2">
@@ -9430,7 +9433,7 @@
       </c>
       <c r="L18" s="3"/>
       <c r="M18" s="3" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="19" spans="1:13" ht="17" x14ac:dyDescent="0.2">
@@ -9444,10 +9447,10 @@
         <v>33</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="E19" s="4" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F19" s="3" t="s">
         <v>15</v>
@@ -9472,7 +9475,7 @@
       </c>
       <c r="L19" s="3"/>
       <c r="M19" s="3" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="20" spans="1:13" ht="17" x14ac:dyDescent="0.2">
@@ -9489,7 +9492,7 @@
         <v>35</v>
       </c>
       <c r="E20" s="4" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F20" s="3" t="s">
         <v>15</v>
@@ -9514,62 +9517,67 @@
       </c>
       <c r="L20" s="3"/>
       <c r="M20" s="3" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="21" spans="1:13" ht="17" x14ac:dyDescent="0.2">
-      <c r="A21">
-        <v>5</v>
-      </c>
-      <c r="B21" t="s">
+      <c r="A21" s="3">
+        <f>A60</f>
+        <v>17</v>
+      </c>
+      <c r="B21" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="C21" t="s">
+      <c r="C21" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="D21" t="s">
-        <v>40</v>
-      </c>
-      <c r="E21" s="2" t="s">
-        <v>95</v>
-      </c>
-      <c r="F21" t="s">
+      <c r="D21" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="E21" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="F21" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="G21" t="s">
+      <c r="G21" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="H21" t="s">
+      <c r="H21" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="I21" s="1">
-        <f>VLOOKUP(F21,'Source lists'!$E$1:F22,2,FALSE)</f>
+      <c r="I21" s="5">
+        <f>VLOOKUP(F21,'Source lists'!$E$1:F20,2,FALSE)</f>
         <v>4</v>
       </c>
-      <c r="J21" s="1">
-        <f>VLOOKUP(G21,'Source lists'!$H$1:I23,2,FALSE)</f>
+      <c r="J21" s="5">
+        <f>VLOOKUP(G21,'Source lists'!$H$1:I21,2,FALSE)</f>
         <v>7</v>
       </c>
-      <c r="K21" s="1">
+      <c r="K21" s="5">
         <f>VLOOKUP(F21,'Source lists'!$E$2:$F$6,2,FALSE)*(VLOOKUP(G21,'Source lists'!$H$2:$I$7,2,FALSE)^2)/VLOOKUP(H21,'Source lists'!$K$2:$L$9,2,FALSE)</f>
         <v>39.200000000000003</v>
       </c>
-    </row>
-    <row r="22" spans="1:13" ht="17" x14ac:dyDescent="0.2">
+      <c r="L21" s="3"/>
+      <c r="M21" s="3" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" ht="136" x14ac:dyDescent="0.2">
       <c r="A22">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="B22" t="s">
-        <v>39</v>
+        <v>8</v>
       </c>
       <c r="C22" t="s">
-        <v>33</v>
+        <v>42</v>
       </c>
       <c r="D22" t="s">
+        <v>64</v>
+      </c>
+      <c r="E22" s="2" t="s">
         <v>215</v>
-      </c>
-      <c r="E22" s="2" t="s">
-        <v>95</v>
       </c>
       <c r="F22" t="s">
         <v>15</v>
@@ -9594,51 +9602,43 @@
       </c>
     </row>
     <row r="23" spans="1:13" ht="17" x14ac:dyDescent="0.2">
-      <c r="A23" s="3">
-        <f>A62</f>
-        <v>18</v>
-      </c>
-      <c r="B23" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="C23" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="D23" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="E23" s="4" t="s">
-        <v>95</v>
-      </c>
-      <c r="F23" s="3" t="s">
+      <c r="A23">
+        <v>7</v>
+      </c>
+      <c r="B23" t="s">
+        <v>8</v>
+      </c>
+      <c r="C23" t="s">
+        <v>42</v>
+      </c>
+      <c r="E23" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="F23" t="s">
         <v>15</v>
       </c>
-      <c r="G23" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="H23" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="I23" s="5">
-        <f>VLOOKUP(F23,'Source lists'!$E$1:F20,2,FALSE)</f>
+      <c r="G23" t="s">
+        <v>28</v>
+      </c>
+      <c r="H23" t="s">
+        <v>23</v>
+      </c>
+      <c r="I23" s="1">
+        <f>VLOOKUP(F23,'Source lists'!$E$1:F24,2,FALSE)</f>
         <v>4</v>
       </c>
-      <c r="J23" s="5">
-        <f>VLOOKUP(G23,'Source lists'!$H$1:I21,2,FALSE)</f>
-        <v>7</v>
-      </c>
-      <c r="K23" s="5">
+      <c r="J23" s="1">
+        <f>VLOOKUP(G23,'Source lists'!$H$1:I25,2,FALSE)</f>
+        <v>4</v>
+      </c>
+      <c r="K23" s="1">
         <f>VLOOKUP(F23,'Source lists'!$E$2:$F$6,2,FALSE)*(VLOOKUP(G23,'Source lists'!$H$2:$I$7,2,FALSE)^2)/VLOOKUP(H23,'Source lists'!$K$2:$L$9,2,FALSE)</f>
-        <v>39.200000000000003</v>
-      </c>
-      <c r="L23" s="3"/>
-      <c r="M23" s="3" t="s">
-        <v>176</v>
+        <v>32</v>
       </c>
     </row>
     <row r="24" spans="1:13" ht="136" x14ac:dyDescent="0.2">
       <c r="A24">
-        <v>24</v>
+        <v>9</v>
       </c>
       <c r="B24" t="s">
         <v>8</v>
@@ -9647,36 +9647,39 @@
         <v>42</v>
       </c>
       <c r="D24" t="s">
-        <v>64</v>
+        <v>44</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>72</v>
+        <v>45</v>
       </c>
       <c r="F24" t="s">
         <v>15</v>
       </c>
       <c r="G24" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="H24" t="s">
-        <v>70</v>
+        <v>23</v>
       </c>
       <c r="I24" s="1">
-        <f>VLOOKUP(F24,'Source lists'!$E$1:F23,2,FALSE)</f>
+        <f>VLOOKUP(F24,'Source lists'!$E$1:F25,2,FALSE)</f>
         <v>4</v>
       </c>
       <c r="J24" s="1">
-        <f>VLOOKUP(G24,'Source lists'!$H$1:I24,2,FALSE)</f>
-        <v>7</v>
+        <f>VLOOKUP(G24,'Source lists'!$H$1:I26,2,FALSE)</f>
+        <v>4</v>
       </c>
       <c r="K24" s="1">
         <f>VLOOKUP(F24,'Source lists'!$E$2:$F$6,2,FALSE)*(VLOOKUP(G24,'Source lists'!$H$2:$I$7,2,FALSE)^2)/VLOOKUP(H24,'Source lists'!$K$2:$L$9,2,FALSE)</f>
-        <v>39.200000000000003</v>
+        <v>32</v>
+      </c>
+      <c r="L24">
+        <v>8</v>
       </c>
     </row>
     <row r="25" spans="1:13" ht="34" x14ac:dyDescent="0.2">
       <c r="A25">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="B25" t="s">
         <v>8</v>
@@ -9684,8 +9687,11 @@
       <c r="C25" t="s">
         <v>42</v>
       </c>
+      <c r="D25" t="s">
+        <v>44</v>
+      </c>
       <c r="E25" s="2" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="F25" t="s">
         <v>15</v>
@@ -9697,21 +9703,24 @@
         <v>23</v>
       </c>
       <c r="I25" s="1">
-        <f>VLOOKUP(F25,'Source lists'!$E$1:F24,2,FALSE)</f>
+        <f>VLOOKUP(F25,'Source lists'!$E$1:F26,2,FALSE)</f>
         <v>4</v>
       </c>
       <c r="J25" s="1">
-        <f>VLOOKUP(G25,'Source lists'!$H$1:I25,2,FALSE)</f>
+        <f>VLOOKUP(G25,'Source lists'!$H$1:I27,2,FALSE)</f>
         <v>4</v>
       </c>
       <c r="K25" s="1">
         <f>VLOOKUP(F25,'Source lists'!$E$2:$F$6,2,FALSE)*(VLOOKUP(G25,'Source lists'!$H$2:$I$7,2,FALSE)^2)/VLOOKUP(H25,'Source lists'!$K$2:$L$9,2,FALSE)</f>
         <v>32</v>
       </c>
+      <c r="L25">
+        <v>8</v>
+      </c>
     </row>
     <row r="26" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="A26">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B26" t="s">
         <v>8</v>
@@ -9723,7 +9732,7 @@
         <v>44</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="F26" t="s">
         <v>15</v>
@@ -9735,11 +9744,11 @@
         <v>23</v>
       </c>
       <c r="I26" s="1">
-        <f>VLOOKUP(F26,'Source lists'!$E$1:F25,2,FALSE)</f>
+        <f>VLOOKUP(F26,'Source lists'!$E$1:F27,2,FALSE)</f>
         <v>4</v>
       </c>
       <c r="J26" s="1">
-        <f>VLOOKUP(G26,'Source lists'!$H$1:I26,2,FALSE)</f>
+        <f>VLOOKUP(G26,'Source lists'!$H$1:I28,2,FALSE)</f>
         <v>4</v>
       </c>
       <c r="K26" s="1">
@@ -9752,7 +9761,7 @@
     </row>
     <row r="27" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="A27">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B27" t="s">
         <v>8</v>
@@ -9764,7 +9773,7 @@
         <v>44</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="F27" t="s">
         <v>15</v>
@@ -9776,11 +9785,11 @@
         <v>23</v>
       </c>
       <c r="I27" s="1">
-        <f>VLOOKUP(F27,'Source lists'!$E$1:F26,2,FALSE)</f>
+        <f>VLOOKUP(F27,'Source lists'!$E$1:F28,2,FALSE)</f>
         <v>4</v>
       </c>
       <c r="J27" s="1">
-        <f>VLOOKUP(G27,'Source lists'!$H$1:I27,2,FALSE)</f>
+        <f>VLOOKUP(G27,'Source lists'!$H$1:I29,2,FALSE)</f>
         <v>4</v>
       </c>
       <c r="K27" s="1">
@@ -9793,19 +9802,19 @@
     </row>
     <row r="28" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="A28">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B28" t="s">
         <v>8</v>
       </c>
       <c r="C28" t="s">
-        <v>42</v>
+        <v>207</v>
       </c>
       <c r="D28" t="s">
-        <v>44</v>
+        <v>210</v>
       </c>
       <c r="E28" s="2" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="F28" t="s">
         <v>15</v>
@@ -9817,11 +9826,11 @@
         <v>23</v>
       </c>
       <c r="I28" s="1">
-        <f>VLOOKUP(F28,'Source lists'!$E$1:F27,2,FALSE)</f>
+        <f>VLOOKUP(F28,'Source lists'!$E$1:F29,2,FALSE)</f>
         <v>4</v>
       </c>
       <c r="J28" s="1">
-        <f>VLOOKUP(G28,'Source lists'!$H$1:I28,2,FALSE)</f>
+        <f>VLOOKUP(G28,'Source lists'!$H$1:I30,2,FALSE)</f>
         <v>4</v>
       </c>
       <c r="K28" s="1">
@@ -9834,19 +9843,19 @@
     </row>
     <row r="29" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="A29">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B29" t="s">
         <v>8</v>
       </c>
       <c r="C29" t="s">
-        <v>42</v>
+        <v>207</v>
       </c>
       <c r="D29" t="s">
-        <v>44</v>
+        <v>210</v>
       </c>
       <c r="E29" s="2" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="F29" t="s">
         <v>15</v>
@@ -9858,11 +9867,11 @@
         <v>23</v>
       </c>
       <c r="I29" s="1">
-        <f>VLOOKUP(F29,'Source lists'!$E$1:F28,2,FALSE)</f>
+        <f>VLOOKUP(F29,'Source lists'!$E$1:F30,2,FALSE)</f>
         <v>4</v>
       </c>
       <c r="J29" s="1">
-        <f>VLOOKUP(G29,'Source lists'!$H$1:I29,2,FALSE)</f>
+        <f>VLOOKUP(G29,'Source lists'!$H$1:I31,2,FALSE)</f>
         <v>4</v>
       </c>
       <c r="K29" s="1">
@@ -9875,19 +9884,19 @@
     </row>
     <row r="30" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="A30">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="B30" t="s">
         <v>8</v>
       </c>
       <c r="C30" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="D30" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="E30" s="2" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="F30" t="s">
         <v>15</v>
@@ -9899,11 +9908,11 @@
         <v>23</v>
       </c>
       <c r="I30" s="1">
-        <f>VLOOKUP(F30,'Source lists'!$E$1:F29,2,FALSE)</f>
+        <f>VLOOKUP(F30,'Source lists'!$E$1:F31,2,FALSE)</f>
         <v>4</v>
       </c>
       <c r="J30" s="1">
-        <f>VLOOKUP(G30,'Source lists'!$H$1:I30,2,FALSE)</f>
+        <f>VLOOKUP(G30,'Source lists'!$H$1:I32,2,FALSE)</f>
         <v>4</v>
       </c>
       <c r="K30" s="1">
@@ -9916,19 +9925,19 @@
     </row>
     <row r="31" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="A31">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="B31" t="s">
         <v>8</v>
       </c>
       <c r="C31" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="D31" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="E31" s="2" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="F31" t="s">
         <v>15</v>
@@ -9940,11 +9949,11 @@
         <v>23</v>
       </c>
       <c r="I31" s="1">
-        <f>VLOOKUP(F31,'Source lists'!$E$1:F30,2,FALSE)</f>
+        <f>VLOOKUP(F31,'Source lists'!$E$1:F32,2,FALSE)</f>
         <v>4</v>
       </c>
       <c r="J31" s="1">
-        <f>VLOOKUP(G31,'Source lists'!$H$1:I31,2,FALSE)</f>
+        <f>VLOOKUP(G31,'Source lists'!$H$1:I33,2,FALSE)</f>
         <v>4</v>
       </c>
       <c r="K31" s="1">
@@ -9957,19 +9966,16 @@
     </row>
     <row r="32" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="A32">
-        <v>15</v>
+        <v>23</v>
       </c>
       <c r="B32" t="s">
         <v>8</v>
       </c>
       <c r="C32" t="s">
-        <v>208</v>
-      </c>
-      <c r="D32" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="E32" s="2" t="s">
-        <v>52</v>
+        <v>63</v>
       </c>
       <c r="F32" t="s">
         <v>15</v>
@@ -9981,36 +9987,30 @@
         <v>23</v>
       </c>
       <c r="I32" s="1">
-        <f>VLOOKUP(F32,'Source lists'!$E$1:F31,2,FALSE)</f>
+        <f>VLOOKUP(F32,'Source lists'!$E$1:F33,2,FALSE)</f>
         <v>4</v>
       </c>
       <c r="J32" s="1">
-        <f>VLOOKUP(G32,'Source lists'!$H$1:I32,2,FALSE)</f>
+        <f>VLOOKUP(G32,'Source lists'!$H$1:I34,2,FALSE)</f>
         <v>4</v>
       </c>
       <c r="K32" s="1">
         <f>VLOOKUP(F32,'Source lists'!$E$2:$F$6,2,FALSE)*(VLOOKUP(G32,'Source lists'!$H$2:$I$7,2,FALSE)^2)/VLOOKUP(H32,'Source lists'!$K$2:$L$9,2,FALSE)</f>
         <v>32</v>
       </c>
-      <c r="L32">
-        <v>8</v>
-      </c>
     </row>
     <row r="33" spans="1:12" ht="17" x14ac:dyDescent="0.2">
       <c r="A33">
-        <v>16</v>
+        <v>31</v>
       </c>
       <c r="B33" t="s">
-        <v>8</v>
+        <v>38</v>
       </c>
       <c r="C33" t="s">
-        <v>208</v>
-      </c>
-      <c r="D33" t="s">
-        <v>211</v>
+        <v>79</v>
       </c>
       <c r="E33" s="2" t="s">
-        <v>53</v>
+        <v>114</v>
       </c>
       <c r="F33" t="s">
         <v>15</v>
@@ -10022,33 +10022,33 @@
         <v>23</v>
       </c>
       <c r="I33" s="1">
-        <f>VLOOKUP(F33,'Source lists'!$E$1:F32,2,FALSE)</f>
+        <f>VLOOKUP(F33,'Source lists'!$E$1:F34,2,FALSE)</f>
         <v>4</v>
       </c>
       <c r="J33" s="1">
-        <f>VLOOKUP(G33,'Source lists'!$H$1:I33,2,FALSE)</f>
+        <f>VLOOKUP(G33,'Source lists'!$H$1:I35,2,FALSE)</f>
         <v>4</v>
       </c>
       <c r="K33" s="1">
         <f>VLOOKUP(F33,'Source lists'!$E$2:$F$6,2,FALSE)*(VLOOKUP(G33,'Source lists'!$H$2:$I$7,2,FALSE)^2)/VLOOKUP(H33,'Source lists'!$K$2:$L$9,2,FALSE)</f>
         <v>32</v>
       </c>
-      <c r="L33">
-        <v>8</v>
-      </c>
     </row>
     <row r="34" spans="1:12" ht="17" x14ac:dyDescent="0.2">
       <c r="A34">
-        <v>23</v>
+        <v>34</v>
       </c>
       <c r="B34" t="s">
-        <v>8</v>
+        <v>38</v>
       </c>
       <c r="C34" t="s">
-        <v>208</v>
+        <v>79</v>
+      </c>
+      <c r="D34" t="s">
+        <v>84</v>
       </c>
       <c r="E34" s="2" t="s">
-        <v>63</v>
+        <v>82</v>
       </c>
       <c r="F34" t="s">
         <v>15</v>
@@ -10060,11 +10060,11 @@
         <v>23</v>
       </c>
       <c r="I34" s="1">
-        <f>VLOOKUP(F34,'Source lists'!$E$1:F33,2,FALSE)</f>
+        <f>VLOOKUP(F34,'Source lists'!$E$1:F35,2,FALSE)</f>
         <v>4</v>
       </c>
       <c r="J34" s="1">
-        <f>VLOOKUP(G34,'Source lists'!$H$1:I34,2,FALSE)</f>
+        <f>VLOOKUP(G34,'Source lists'!$H$1:I36,2,FALSE)</f>
         <v>4</v>
       </c>
       <c r="K34" s="1">
@@ -10074,16 +10074,16 @@
     </row>
     <row r="35" spans="1:12" ht="34" x14ac:dyDescent="0.2">
       <c r="A35">
-        <v>31</v>
+        <v>54</v>
       </c>
       <c r="B35" t="s">
-        <v>38</v>
+        <v>1</v>
       </c>
       <c r="C35" t="s">
-        <v>80</v>
+        <v>90</v>
       </c>
       <c r="E35" s="2" t="s">
-        <v>115</v>
+        <v>104</v>
       </c>
       <c r="F35" t="s">
         <v>15</v>
@@ -10095,11 +10095,11 @@
         <v>23</v>
       </c>
       <c r="I35" s="1">
-        <f>VLOOKUP(F35,'Source lists'!$E$1:F34,2,FALSE)</f>
+        <f>VLOOKUP(F35,'Source lists'!$E$1:F36,2,FALSE)</f>
         <v>4</v>
       </c>
       <c r="J35" s="1">
-        <f>VLOOKUP(G35,'Source lists'!$H$1:I35,2,FALSE)</f>
+        <f>VLOOKUP(G35,'Source lists'!$H$1:I37,2,FALSE)</f>
         <v>4</v>
       </c>
       <c r="K35" s="1">
@@ -10109,19 +10109,16 @@
     </row>
     <row r="36" spans="1:12" ht="34" x14ac:dyDescent="0.2">
       <c r="A36">
-        <v>34</v>
+        <v>55</v>
       </c>
       <c r="B36" t="s">
-        <v>38</v>
+        <v>1</v>
       </c>
       <c r="C36" t="s">
-        <v>80</v>
-      </c>
-      <c r="D36" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="E36" s="2" t="s">
-        <v>83</v>
+        <v>108</v>
       </c>
       <c r="F36" t="s">
         <v>15</v>
@@ -10133,11 +10130,11 @@
         <v>23</v>
       </c>
       <c r="I36" s="1">
-        <f>VLOOKUP(F36,'Source lists'!$E$1:F35,2,FALSE)</f>
+        <f>VLOOKUP(F36,'Source lists'!$E$1:F37,2,FALSE)</f>
         <v>4</v>
       </c>
       <c r="J36" s="1">
-        <f>VLOOKUP(G36,'Source lists'!$H$1:I36,2,FALSE)</f>
+        <f>VLOOKUP(G36,'Source lists'!$H$1:I38,2,FALSE)</f>
         <v>4</v>
       </c>
       <c r="K36" s="1">
@@ -10147,16 +10144,16 @@
     </row>
     <row r="37" spans="1:12" ht="34" x14ac:dyDescent="0.2">
       <c r="A37">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="B37" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C37" t="s">
-        <v>91</v>
+        <v>105</v>
       </c>
       <c r="E37" s="2" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="F37" t="s">
         <v>15</v>
@@ -10168,11 +10165,11 @@
         <v>23</v>
       </c>
       <c r="I37" s="1">
-        <f>VLOOKUP(F37,'Source lists'!$E$1:F36,2,FALSE)</f>
+        <f>VLOOKUP(F37,'Source lists'!$E$1:F38,2,FALSE)</f>
         <v>4</v>
       </c>
       <c r="J37" s="1">
-        <f>VLOOKUP(G37,'Source lists'!$H$1:I37,2,FALSE)</f>
+        <f>VLOOKUP(G37,'Source lists'!$H$1:I39,2,FALSE)</f>
         <v>4</v>
       </c>
       <c r="K37" s="1">
@@ -10182,16 +10179,16 @@
     </row>
     <row r="38" spans="1:12" ht="34" x14ac:dyDescent="0.2">
       <c r="A38">
-        <v>55</v>
+        <v>67</v>
       </c>
       <c r="B38" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C38" t="s">
-        <v>87</v>
+        <v>105</v>
       </c>
       <c r="E38" s="2" t="s">
-        <v>109</v>
+        <v>129</v>
       </c>
       <c r="F38" t="s">
         <v>15</v>
@@ -10203,11 +10200,11 @@
         <v>23</v>
       </c>
       <c r="I38" s="1">
-        <f>VLOOKUP(F38,'Source lists'!$E$1:F37,2,FALSE)</f>
+        <f>VLOOKUP(F38,'Source lists'!$E$1:F39,2,FALSE)</f>
         <v>4</v>
       </c>
       <c r="J38" s="1">
-        <f>VLOOKUP(G38,'Source lists'!$H$1:I38,2,FALSE)</f>
+        <f>VLOOKUP(G38,'Source lists'!$H$1:I40,2,FALSE)</f>
         <v>4</v>
       </c>
       <c r="K38" s="1">
@@ -10217,16 +10214,16 @@
     </row>
     <row r="39" spans="1:12" ht="68" x14ac:dyDescent="0.2">
       <c r="A39">
-        <v>58</v>
+        <v>84</v>
       </c>
       <c r="B39" t="s">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="C39" t="s">
-        <v>106</v>
+        <v>149</v>
       </c>
       <c r="E39" s="2" t="s">
-        <v>108</v>
+        <v>150</v>
       </c>
       <c r="F39" t="s">
         <v>15</v>
@@ -10238,11 +10235,11 @@
         <v>23</v>
       </c>
       <c r="I39" s="1">
-        <f>VLOOKUP(F39,'Source lists'!$E$1:F38,2,FALSE)</f>
+        <f>VLOOKUP(F39,'Source lists'!$E$1:F40,2,FALSE)</f>
         <v>4</v>
       </c>
       <c r="J39" s="1">
-        <f>VLOOKUP(G39,'Source lists'!$H$1:I39,2,FALSE)</f>
+        <f>VLOOKUP(G39,'Source lists'!$H$1:I41,2,FALSE)</f>
         <v>4</v>
       </c>
       <c r="K39" s="1">
@@ -10252,16 +10249,16 @@
     </row>
     <row r="40" spans="1:12" ht="17" x14ac:dyDescent="0.2">
       <c r="A40">
-        <v>67</v>
+        <v>89</v>
       </c>
       <c r="B40" t="s">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="C40" t="s">
-        <v>106</v>
+        <v>149</v>
       </c>
       <c r="E40" s="2" t="s">
-        <v>130</v>
+        <v>156</v>
       </c>
       <c r="F40" t="s">
         <v>15</v>
@@ -10273,11 +10270,11 @@
         <v>23</v>
       </c>
       <c r="I40" s="1">
-        <f>VLOOKUP(F40,'Source lists'!$E$1:F39,2,FALSE)</f>
+        <f>VLOOKUP(F40,'Source lists'!$E$1:F41,2,FALSE)</f>
         <v>4</v>
       </c>
       <c r="J40" s="1">
-        <f>VLOOKUP(G40,'Source lists'!$H$1:I40,2,FALSE)</f>
+        <f>VLOOKUP(G40,'Source lists'!$H$1:I42,2,FALSE)</f>
         <v>4</v>
       </c>
       <c r="K40" s="1">
@@ -10287,16 +10284,16 @@
     </row>
     <row r="41" spans="1:12" ht="34" x14ac:dyDescent="0.2">
       <c r="A41">
-        <v>84</v>
+        <v>107</v>
       </c>
       <c r="B41" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="C41" t="s">
-        <v>150</v>
+        <v>139</v>
       </c>
       <c r="E41" s="2" t="s">
-        <v>151</v>
+        <v>185</v>
       </c>
       <c r="F41" t="s">
         <v>15</v>
@@ -10308,11 +10305,11 @@
         <v>23</v>
       </c>
       <c r="I41" s="1">
-        <f>VLOOKUP(F41,'Source lists'!$E$1:F40,2,FALSE)</f>
+        <f>VLOOKUP(F41,'Source lists'!$E$1:F42,2,FALSE)</f>
         <v>4</v>
       </c>
       <c r="J41" s="1">
-        <f>VLOOKUP(G41,'Source lists'!$H$1:I41,2,FALSE)</f>
+        <f>VLOOKUP(G41,'Source lists'!$H$1:I43,2,FALSE)</f>
         <v>4</v>
       </c>
       <c r="K41" s="1">
@@ -10322,16 +10319,16 @@
     </row>
     <row r="42" spans="1:12" ht="17" x14ac:dyDescent="0.2">
       <c r="A42">
-        <v>89</v>
+        <v>108</v>
       </c>
       <c r="B42" t="s">
         <v>6</v>
       </c>
       <c r="C42" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="E42" s="2" t="s">
-        <v>157</v>
+        <v>186</v>
       </c>
       <c r="F42" t="s">
         <v>15</v>
@@ -10343,11 +10340,11 @@
         <v>23</v>
       </c>
       <c r="I42" s="1">
-        <f>VLOOKUP(F42,'Source lists'!$E$1:F41,2,FALSE)</f>
+        <f>VLOOKUP(F42,'Source lists'!$E$1:F43,2,FALSE)</f>
         <v>4</v>
       </c>
       <c r="J42" s="1">
-        <f>VLOOKUP(G42,'Source lists'!$H$1:I42,2,FALSE)</f>
+        <f>VLOOKUP(G42,'Source lists'!$H$1:I44,2,FALSE)</f>
         <v>4</v>
       </c>
       <c r="K42" s="1">
@@ -10357,16 +10354,19 @@
     </row>
     <row r="43" spans="1:12" ht="34" x14ac:dyDescent="0.2">
       <c r="A43">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="B43" t="s">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="C43" t="s">
-        <v>140</v>
+        <v>42</v>
+      </c>
+      <c r="D43" t="s">
+        <v>44</v>
       </c>
       <c r="E43" s="2" t="s">
-        <v>186</v>
+        <v>179</v>
       </c>
       <c r="F43" t="s">
         <v>15</v>
@@ -10378,30 +10378,36 @@
         <v>23</v>
       </c>
       <c r="I43" s="1">
-        <f>VLOOKUP(F43,'Source lists'!$E$1:F42,2,FALSE)</f>
+        <f>VLOOKUP(F43,'Source lists'!$E$1:F44,2,FALSE)</f>
         <v>4</v>
       </c>
       <c r="J43" s="1">
-        <f>VLOOKUP(G43,'Source lists'!$H$1:I43,2,FALSE)</f>
+        <f>VLOOKUP(G43,'Source lists'!$H$1:I45,2,FALSE)</f>
         <v>4</v>
       </c>
       <c r="K43" s="1">
         <f>VLOOKUP(F43,'Source lists'!$E$2:$F$6,2,FALSE)*(VLOOKUP(G43,'Source lists'!$H$2:$I$7,2,FALSE)^2)/VLOOKUP(H43,'Source lists'!$K$2:$L$9,2,FALSE)</f>
         <v>32</v>
       </c>
+      <c r="L43">
+        <v>8</v>
+      </c>
     </row>
     <row r="44" spans="1:12" ht="34" x14ac:dyDescent="0.2">
       <c r="A44">
-        <v>108</v>
+        <v>115</v>
       </c>
       <c r="B44" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C44" t="s">
-        <v>150</v>
+        <v>207</v>
+      </c>
+      <c r="D44" t="s">
+        <v>210</v>
       </c>
       <c r="E44" s="2" t="s">
-        <v>187</v>
+        <v>211</v>
       </c>
       <c r="F44" t="s">
         <v>15</v>
@@ -10413,103 +10419,100 @@
         <v>23</v>
       </c>
       <c r="I44" s="1">
-        <f>VLOOKUP(F44,'Source lists'!$E$1:F43,2,FALSE)</f>
+        <f>VLOOKUP(F44,'Source lists'!$E$1:F118,2,FALSE)</f>
         <v>4</v>
       </c>
       <c r="J44" s="1">
-        <f>VLOOKUP(G44,'Source lists'!$H$1:I44,2,FALSE)</f>
+        <f>VLOOKUP(G44,'Source lists'!$H$1:I119,2,FALSE)</f>
         <v>4</v>
       </c>
       <c r="K44" s="1">
         <f>VLOOKUP(F44,'Source lists'!$E$2:$F$6,2,FALSE)*(VLOOKUP(G44,'Source lists'!$H$2:$I$7,2,FALSE)^2)/VLOOKUP(H44,'Source lists'!$K$2:$L$9,2,FALSE)</f>
         <v>32</v>
       </c>
+      <c r="L44">
+        <v>8</v>
+      </c>
     </row>
     <row r="45" spans="1:12" ht="17" x14ac:dyDescent="0.2">
       <c r="A45">
-        <v>109</v>
+        <v>17</v>
       </c>
       <c r="B45" t="s">
-        <v>8</v>
+        <v>39</v>
       </c>
       <c r="C45" t="s">
-        <v>42</v>
+        <v>33</v>
       </c>
       <c r="D45" t="s">
-        <v>44</v>
+        <v>214</v>
       </c>
       <c r="E45" s="2" t="s">
-        <v>180</v>
+        <v>94</v>
       </c>
       <c r="F45" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="G45" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="H45" t="s">
-        <v>23</v>
+        <v>70</v>
       </c>
       <c r="I45" s="1">
-        <f>VLOOKUP(F45,'Source lists'!$E$1:F44,2,FALSE)</f>
-        <v>4</v>
+        <f>VLOOKUP(F45,'Source lists'!$E$1:F23,2,FALSE)</f>
+        <v>3</v>
       </c>
       <c r="J45" s="1">
-        <f>VLOOKUP(G45,'Source lists'!$H$1:I45,2,FALSE)</f>
-        <v>4</v>
+        <f>VLOOKUP(G45,'Source lists'!$H$1:I24,2,FALSE)</f>
+        <v>7</v>
       </c>
       <c r="K45" s="1">
         <f>VLOOKUP(F45,'Source lists'!$E$2:$F$6,2,FALSE)*(VLOOKUP(G45,'Source lists'!$H$2:$I$7,2,FALSE)^2)/VLOOKUP(H45,'Source lists'!$K$2:$L$9,2,FALSE)</f>
-        <v>32</v>
-      </c>
-      <c r="L45">
-        <v>8</v>
+        <v>29.4</v>
       </c>
     </row>
     <row r="46" spans="1:12" ht="17" x14ac:dyDescent="0.2">
       <c r="A46">
-        <v>115</v>
+        <v>8</v>
       </c>
       <c r="B46" t="s">
         <v>8</v>
       </c>
       <c r="C46" t="s">
-        <v>208</v>
+        <v>42</v>
       </c>
       <c r="D46" t="s">
-        <v>211</v>
+        <v>44</v>
       </c>
       <c r="E46" s="2" t="s">
-        <v>212</v>
+        <v>46</v>
       </c>
       <c r="F46" t="s">
         <v>15</v>
       </c>
       <c r="G46" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="H46" t="s">
-        <v>23</v>
+        <v>69</v>
       </c>
       <c r="I46" s="1">
-        <f>VLOOKUP(F46,'Source lists'!$E$1:F118,2,FALSE)</f>
+        <f>VLOOKUP(F46,'Source lists'!$E$1:F45,2,FALSE)</f>
         <v>4</v>
       </c>
       <c r="J46" s="1">
-        <f>VLOOKUP(G46,'Source lists'!$H$1:I119,2,FALSE)</f>
-        <v>4</v>
+        <f>VLOOKUP(G46,'Source lists'!$H$1:I46,2,FALSE)</f>
+        <v>7</v>
       </c>
       <c r="K46" s="1">
         <f>VLOOKUP(F46,'Source lists'!$E$2:$F$6,2,FALSE)*(VLOOKUP(G46,'Source lists'!$H$2:$I$7,2,FALSE)^2)/VLOOKUP(H46,'Source lists'!$K$2:$L$9,2,FALSE)</f>
-        <v>32</v>
-      </c>
-      <c r="L46">
-        <v>8</v>
+        <v>28</v>
       </c>
     </row>
     <row r="47" spans="1:12" ht="17" x14ac:dyDescent="0.2">
       <c r="A47">
-        <v>8</v>
+        <v>22</v>
       </c>
       <c r="B47" t="s">
         <v>8</v>
@@ -10517,63 +10520,60 @@
       <c r="C47" t="s">
         <v>42</v>
       </c>
-      <c r="D47" t="s">
-        <v>44</v>
-      </c>
       <c r="E47" s="2" t="s">
-        <v>46</v>
+        <v>61</v>
       </c>
       <c r="F47" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="G47" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="H47" t="s">
-        <v>69</v>
+        <v>25</v>
       </c>
       <c r="I47" s="1">
-        <f>VLOOKUP(F47,'Source lists'!$E$1:F45,2,FALSE)</f>
-        <v>4</v>
+        <f>VLOOKUP(F47,'Source lists'!$E$1:F46,2,FALSE)</f>
+        <v>3</v>
       </c>
       <c r="J47" s="1">
-        <f>VLOOKUP(G47,'Source lists'!$H$1:I46,2,FALSE)</f>
-        <v>7</v>
+        <f>VLOOKUP(G47,'Source lists'!$H$1:I47,2,FALSE)</f>
+        <v>3</v>
       </c>
       <c r="K47" s="1">
         <f>VLOOKUP(F47,'Source lists'!$E$2:$F$6,2,FALSE)*(VLOOKUP(G47,'Source lists'!$H$2:$I$7,2,FALSE)^2)/VLOOKUP(H47,'Source lists'!$K$2:$L$9,2,FALSE)</f>
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="48" spans="1:12" ht="34" x14ac:dyDescent="0.2">
       <c r="A48">
-        <v>22</v>
+        <v>43</v>
       </c>
       <c r="B48" t="s">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="C48" t="s">
-        <v>42</v>
+        <v>86</v>
       </c>
       <c r="E48" s="2" t="s">
-        <v>61</v>
+        <v>92</v>
       </c>
       <c r="F48" t="s">
         <v>16</v>
       </c>
       <c r="G48" t="s">
-        <v>29</v>
+        <v>158</v>
       </c>
       <c r="H48" t="s">
-        <v>25</v>
+        <v>67</v>
       </c>
       <c r="I48" s="1">
-        <f>VLOOKUP(F48,'Source lists'!$E$1:F46,2,FALSE)</f>
+        <f>VLOOKUP(F48,'Source lists'!$E$1:F47,2,FALSE)</f>
         <v>3</v>
       </c>
       <c r="J48" s="1">
-        <f>VLOOKUP(G48,'Source lists'!$H$1:I47,2,FALSE)</f>
-        <v>3</v>
+        <f>VLOOKUP(G48,'Source lists'!$H$1:I48,2,FALSE)</f>
+        <v>6</v>
       </c>
       <c r="K48" s="1">
         <f>VLOOKUP(F48,'Source lists'!$E$2:$F$6,2,FALSE)*(VLOOKUP(G48,'Source lists'!$H$2:$I$7,2,FALSE)^2)/VLOOKUP(H48,'Source lists'!$K$2:$L$9,2,FALSE)</f>
@@ -10582,13 +10582,13 @@
     </row>
     <row r="49" spans="1:13" ht="34" x14ac:dyDescent="0.2">
       <c r="A49">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B49" t="s">
         <v>1</v>
       </c>
       <c r="C49" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E49" s="2" t="s">
         <v>93</v>
@@ -10597,17 +10597,17 @@
         <v>16</v>
       </c>
       <c r="G49" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="H49" t="s">
         <v>67</v>
       </c>
       <c r="I49" s="1">
-        <f>VLOOKUP(F49,'Source lists'!$E$1:F47,2,FALSE)</f>
+        <f>VLOOKUP(F49,'Source lists'!$E$1:F48,2,FALSE)</f>
         <v>3</v>
       </c>
       <c r="J49" s="1">
-        <f>VLOOKUP(G49,'Source lists'!$H$1:I48,2,FALSE)</f>
+        <f>VLOOKUP(G49,'Source lists'!$H$1:I49,2,FALSE)</f>
         <v>6</v>
       </c>
       <c r="K49" s="1">
@@ -10617,33 +10617,33 @@
     </row>
     <row r="50" spans="1:13" ht="68" x14ac:dyDescent="0.2">
       <c r="A50">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="B50" t="s">
         <v>1</v>
       </c>
       <c r="C50" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
       <c r="E50" s="2" t="s">
-        <v>94</v>
+        <v>98</v>
       </c>
       <c r="F50" t="s">
         <v>16</v>
       </c>
       <c r="G50" t="s">
-        <v>159</v>
+        <v>29</v>
       </c>
       <c r="H50" t="s">
-        <v>67</v>
+        <v>25</v>
       </c>
       <c r="I50" s="1">
-        <f>VLOOKUP(F50,'Source lists'!$E$1:F48,2,FALSE)</f>
+        <f>VLOOKUP(F50,'Source lists'!$E$1:F49,2,FALSE)</f>
         <v>3</v>
       </c>
       <c r="J50" s="1">
-        <f>VLOOKUP(G50,'Source lists'!$H$1:I49,2,FALSE)</f>
-        <v>6</v>
+        <f>VLOOKUP(G50,'Source lists'!$H$1:I50,2,FALSE)</f>
+        <v>3</v>
       </c>
       <c r="K50" s="1">
         <f>VLOOKUP(F50,'Source lists'!$E$2:$F$6,2,FALSE)*(VLOOKUP(G50,'Source lists'!$H$2:$I$7,2,FALSE)^2)/VLOOKUP(H50,'Source lists'!$K$2:$L$9,2,FALSE)</f>
@@ -10652,16 +10652,16 @@
     </row>
     <row r="51" spans="1:13" ht="34" x14ac:dyDescent="0.2">
       <c r="A51">
-        <v>48</v>
+        <v>57</v>
       </c>
       <c r="B51" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C51" t="s">
-        <v>91</v>
+        <v>105</v>
       </c>
       <c r="E51" s="2" t="s">
-        <v>99</v>
+        <v>106</v>
       </c>
       <c r="F51" t="s">
         <v>16</v>
@@ -10673,11 +10673,11 @@
         <v>25</v>
       </c>
       <c r="I51" s="1">
-        <f>VLOOKUP(F51,'Source lists'!$E$1:F49,2,FALSE)</f>
+        <f>VLOOKUP(F51,'Source lists'!$E$1:F50,2,FALSE)</f>
         <v>3</v>
       </c>
       <c r="J51" s="1">
-        <f>VLOOKUP(G51,'Source lists'!$H$1:I50,2,FALSE)</f>
+        <f>VLOOKUP(G51,'Source lists'!$H$1:I51,2,FALSE)</f>
         <v>3</v>
       </c>
       <c r="K51" s="1">
@@ -10686,90 +10686,93 @@
       </c>
     </row>
     <row r="52" spans="1:13" ht="17" x14ac:dyDescent="0.2">
-      <c r="A52">
-        <v>57</v>
-      </c>
-      <c r="B52" t="s">
-        <v>2</v>
-      </c>
-      <c r="C52" t="s">
+      <c r="A52" s="3">
         <v>106</v>
       </c>
-      <c r="E52" s="2" t="s">
-        <v>107</v>
-      </c>
-      <c r="F52" t="s">
+      <c r="B52" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="C52" s="3"/>
+      <c r="D52" s="3"/>
+      <c r="E52" s="4" t="s">
+        <v>173</v>
+      </c>
+      <c r="F52" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="G52" t="s">
+      <c r="G52" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="H52" t="s">
+      <c r="H52" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="I52" s="1">
-        <f>VLOOKUP(F52,'Source lists'!$E$1:F50,2,FALSE)</f>
+      <c r="I52" s="5">
+        <f>VLOOKUP(F52,'Source lists'!$E$1:F51,2,FALSE)</f>
         <v>3</v>
       </c>
-      <c r="J52" s="1">
-        <f>VLOOKUP(G52,'Source lists'!$H$1:I51,2,FALSE)</f>
+      <c r="J52" s="5">
+        <f>VLOOKUP(G52,'Source lists'!$H$1:I52,2,FALSE)</f>
         <v>3</v>
       </c>
-      <c r="K52" s="1">
+      <c r="K52" s="5">
         <f>VLOOKUP(F52,'Source lists'!$E$2:$F$6,2,FALSE)*(VLOOKUP(G52,'Source lists'!$H$2:$I$7,2,FALSE)^2)/VLOOKUP(H52,'Source lists'!$K$2:$L$9,2,FALSE)</f>
         <v>27</v>
       </c>
+      <c r="L52" s="3"/>
+      <c r="M52" s="3" t="s">
+        <v>175</v>
+      </c>
     </row>
     <row r="53" spans="1:13" ht="17" x14ac:dyDescent="0.2">
-      <c r="A53" s="3">
-        <v>106</v>
-      </c>
-      <c r="B53" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="C53" s="3"/>
-      <c r="D53" s="3"/>
-      <c r="E53" s="4" t="s">
-        <v>174</v>
-      </c>
-      <c r="F53" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="G53" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="H53" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="I53" s="5">
-        <f>VLOOKUP(F53,'Source lists'!$E$1:F51,2,FALSE)</f>
-        <v>3</v>
-      </c>
-      <c r="J53" s="5">
-        <f>VLOOKUP(G53,'Source lists'!$H$1:I52,2,FALSE)</f>
-        <v>3</v>
-      </c>
-      <c r="K53" s="5">
+      <c r="A53">
+        <v>49</v>
+      </c>
+      <c r="B53" t="s">
+        <v>1</v>
+      </c>
+      <c r="C53" t="s">
+        <v>90</v>
+      </c>
+      <c r="E53" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="F53" t="s">
+        <v>15</v>
+      </c>
+      <c r="G53" t="s">
+        <v>28</v>
+      </c>
+      <c r="H53" t="s">
+        <v>24</v>
+      </c>
+      <c r="I53" s="1">
+        <f>VLOOKUP(F53,'Source lists'!$E$1:F52,2,FALSE)</f>
+        <v>4</v>
+      </c>
+      <c r="J53" s="1">
+        <f>VLOOKUP(G53,'Source lists'!$H$1:I53,2,FALSE)</f>
+        <v>4</v>
+      </c>
+      <c r="K53" s="1">
         <f>VLOOKUP(F53,'Source lists'!$E$2:$F$6,2,FALSE)*(VLOOKUP(G53,'Source lists'!$H$2:$I$7,2,FALSE)^2)/VLOOKUP(H53,'Source lists'!$K$2:$L$9,2,FALSE)</f>
-        <v>27</v>
-      </c>
-      <c r="L53" s="3"/>
-      <c r="M53" s="3" t="s">
-        <v>176</v>
+        <v>21.333333333333332</v>
       </c>
     </row>
     <row r="54" spans="1:13" ht="34" x14ac:dyDescent="0.2">
       <c r="A54">
-        <v>49</v>
+        <v>74</v>
       </c>
       <c r="B54" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C54" t="s">
-        <v>91</v>
+        <v>132</v>
+      </c>
+      <c r="D54" t="s">
+        <v>187</v>
       </c>
       <c r="E54" s="2" t="s">
-        <v>100</v>
+        <v>136</v>
       </c>
       <c r="F54" t="s">
         <v>15</v>
@@ -10781,11 +10784,11 @@
         <v>24</v>
       </c>
       <c r="I54" s="1">
-        <f>VLOOKUP(F54,'Source lists'!$E$1:F52,2,FALSE)</f>
+        <f>VLOOKUP(F54,'Source lists'!$E$1:F53,2,FALSE)</f>
         <v>4</v>
       </c>
       <c r="J54" s="1">
-        <f>VLOOKUP(G54,'Source lists'!$H$1:I53,2,FALSE)</f>
+        <f>VLOOKUP(G54,'Source lists'!$H$1:I54,2,FALSE)</f>
         <v>4</v>
       </c>
       <c r="K54" s="1">
@@ -10795,19 +10798,16 @@
     </row>
     <row r="55" spans="1:13" ht="34" x14ac:dyDescent="0.2">
       <c r="A55">
-        <v>74</v>
+        <v>79</v>
       </c>
       <c r="B55" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C55" t="s">
-        <v>133</v>
-      </c>
-      <c r="D55" t="s">
-        <v>188</v>
+        <v>141</v>
       </c>
       <c r="E55" s="2" t="s">
-        <v>137</v>
+        <v>154</v>
       </c>
       <c r="F55" t="s">
         <v>15</v>
@@ -10819,11 +10819,11 @@
         <v>24</v>
       </c>
       <c r="I55" s="1">
-        <f>VLOOKUP(F55,'Source lists'!$E$1:F53,2,FALSE)</f>
+        <f>VLOOKUP(F55,'Source lists'!$E$1:F54,2,FALSE)</f>
         <v>4</v>
       </c>
       <c r="J55" s="1">
-        <f>VLOOKUP(G55,'Source lists'!$H$1:I54,2,FALSE)</f>
+        <f>VLOOKUP(G55,'Source lists'!$H$1:I55,2,FALSE)</f>
         <v>4</v>
       </c>
       <c r="K55" s="1">
@@ -10833,16 +10833,16 @@
     </row>
     <row r="56" spans="1:13" ht="51" x14ac:dyDescent="0.2">
       <c r="A56">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="B56" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C56" t="s">
-        <v>142</v>
+        <v>105</v>
       </c>
       <c r="E56" s="2" t="s">
-        <v>155</v>
+        <v>144</v>
       </c>
       <c r="F56" t="s">
         <v>15</v>
@@ -10854,11 +10854,11 @@
         <v>24</v>
       </c>
       <c r="I56" s="1">
-        <f>VLOOKUP(F56,'Source lists'!$E$1:F54,2,FALSE)</f>
+        <f>VLOOKUP(F56,'Source lists'!$E$1:F55,2,FALSE)</f>
         <v>4</v>
       </c>
       <c r="J56" s="1">
-        <f>VLOOKUP(G56,'Source lists'!$H$1:I55,2,FALSE)</f>
+        <f>VLOOKUP(G56,'Source lists'!$H$1:I56,2,FALSE)</f>
         <v>4</v>
       </c>
       <c r="K56" s="1">
@@ -10868,13 +10868,13 @@
     </row>
     <row r="57" spans="1:13" ht="51" x14ac:dyDescent="0.2">
       <c r="A57">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="B57" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C57" t="s">
-        <v>106</v>
+        <v>141</v>
       </c>
       <c r="E57" s="2" t="s">
         <v>145</v>
@@ -10889,11 +10889,11 @@
         <v>24</v>
       </c>
       <c r="I57" s="1">
-        <f>VLOOKUP(F57,'Source lists'!$E$1:F55,2,FALSE)</f>
+        <f>VLOOKUP(F57,'Source lists'!$E$1:F56,2,FALSE)</f>
         <v>4</v>
       </c>
       <c r="J57" s="1">
-        <f>VLOOKUP(G57,'Source lists'!$H$1:I56,2,FALSE)</f>
+        <f>VLOOKUP(G57,'Source lists'!$H$1:I57,2,FALSE)</f>
         <v>4</v>
       </c>
       <c r="K57" s="1">
@@ -10903,16 +10903,16 @@
     </row>
     <row r="58" spans="1:13" ht="51" x14ac:dyDescent="0.2">
       <c r="A58">
-        <v>81</v>
+        <v>87</v>
       </c>
       <c r="B58" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="C58" t="s">
-        <v>142</v>
+        <v>153</v>
       </c>
       <c r="E58" s="2" t="s">
-        <v>146</v>
+        <v>188</v>
       </c>
       <c r="F58" t="s">
         <v>15</v>
@@ -10924,11 +10924,11 @@
         <v>24</v>
       </c>
       <c r="I58" s="1">
-        <f>VLOOKUP(F58,'Source lists'!$E$1:F56,2,FALSE)</f>
+        <f>VLOOKUP(F58,'Source lists'!$E$1:F57,2,FALSE)</f>
         <v>4</v>
       </c>
       <c r="J58" s="1">
-        <f>VLOOKUP(G58,'Source lists'!$H$1:I57,2,FALSE)</f>
+        <f>VLOOKUP(G58,'Source lists'!$H$1:I58,2,FALSE)</f>
         <v>4</v>
       </c>
       <c r="K58" s="1">
@@ -10938,16 +10938,16 @@
     </row>
     <row r="59" spans="1:13" ht="34" x14ac:dyDescent="0.2">
       <c r="A59">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="B59" t="s">
         <v>6</v>
       </c>
       <c r="C59" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="E59" s="2" t="s">
-        <v>189</v>
+        <v>155</v>
       </c>
       <c r="F59" t="s">
         <v>15</v>
@@ -10959,11 +10959,11 @@
         <v>24</v>
       </c>
       <c r="I59" s="1">
-        <f>VLOOKUP(F59,'Source lists'!$E$1:F57,2,FALSE)</f>
+        <f>VLOOKUP(F59,'Source lists'!$E$1:F58,2,FALSE)</f>
         <v>4</v>
       </c>
       <c r="J59" s="1">
-        <f>VLOOKUP(G59,'Source lists'!$H$1:I58,2,FALSE)</f>
+        <f>VLOOKUP(G59,'Source lists'!$H$1:I59,2,FALSE)</f>
         <v>4</v>
       </c>
       <c r="K59" s="1">
@@ -10973,42 +10973,45 @@
     </row>
     <row r="60" spans="1:13" ht="34" x14ac:dyDescent="0.2">
       <c r="A60">
-        <v>88</v>
+        <v>17</v>
       </c>
       <c r="B60" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C60" t="s">
-        <v>154</v>
+        <v>42</v>
+      </c>
+      <c r="D60" t="s">
+        <v>54</v>
       </c>
       <c r="E60" s="2" t="s">
-        <v>156</v>
+        <v>55</v>
       </c>
       <c r="F60" t="s">
         <v>15</v>
       </c>
       <c r="G60" t="s">
-        <v>28</v>
+        <v>158</v>
       </c>
       <c r="H60" t="s">
-        <v>24</v>
+        <v>69</v>
       </c>
       <c r="I60" s="1">
-        <f>VLOOKUP(F60,'Source lists'!$E$1:F58,2,FALSE)</f>
+        <f>VLOOKUP(F60,'Source lists'!$E$1:F59,2,FALSE)</f>
         <v>4</v>
       </c>
       <c r="J60" s="1">
-        <f>VLOOKUP(G60,'Source lists'!$H$1:I59,2,FALSE)</f>
-        <v>4</v>
+        <f>VLOOKUP(G60,'Source lists'!$H$1:I60,2,FALSE)</f>
+        <v>6</v>
       </c>
       <c r="K60" s="1">
         <f>VLOOKUP(F60,'Source lists'!$E$2:$F$6,2,FALSE)*(VLOOKUP(G60,'Source lists'!$H$2:$I$7,2,FALSE)^2)/VLOOKUP(H60,'Source lists'!$K$2:$L$9,2,FALSE)</f>
-        <v>21.333333333333332</v>
+        <v>20.571428571428573</v>
       </c>
     </row>
     <row r="61" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="A61">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B61" t="s">
         <v>8</v>
@@ -11020,23 +11023,23 @@
         <v>54</v>
       </c>
       <c r="E61" s="2" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="F61" t="s">
         <v>15</v>
       </c>
       <c r="G61" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="H61" t="s">
         <v>69</v>
       </c>
       <c r="I61" s="1">
-        <f>VLOOKUP(F61,'Source lists'!$E$1:F59,2,FALSE)</f>
+        <f>VLOOKUP(F61,'Source lists'!$E$1:F60,2,FALSE)</f>
         <v>4</v>
       </c>
       <c r="J61" s="1">
-        <f>VLOOKUP(G61,'Source lists'!$H$1:I60,2,FALSE)</f>
+        <f>VLOOKUP(G61,'Source lists'!$H$1:I61,2,FALSE)</f>
         <v>6</v>
       </c>
       <c r="K61" s="1">
@@ -11046,7 +11049,7 @@
     </row>
     <row r="62" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="A62">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B62" t="s">
         <v>8</v>
@@ -11058,23 +11061,23 @@
         <v>54</v>
       </c>
       <c r="E62" s="2" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="F62" t="s">
         <v>15</v>
       </c>
       <c r="G62" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="H62" t="s">
         <v>69</v>
       </c>
       <c r="I62" s="1">
-        <f>VLOOKUP(F62,'Source lists'!$E$1:F60,2,FALSE)</f>
+        <f>VLOOKUP(F62,'Source lists'!$E$1:F61,2,FALSE)</f>
         <v>4</v>
       </c>
       <c r="J62" s="1">
-        <f>VLOOKUP(G62,'Source lists'!$H$1:I61,2,FALSE)</f>
+        <f>VLOOKUP(G62,'Source lists'!$H$1:I62,2,FALSE)</f>
         <v>6</v>
       </c>
       <c r="K62" s="1">
@@ -11084,7 +11087,7 @@
     </row>
     <row r="63" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="A63">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B63" t="s">
         <v>8</v>
@@ -11096,23 +11099,23 @@
         <v>54</v>
       </c>
       <c r="E63" s="2" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="F63" t="s">
         <v>15</v>
       </c>
       <c r="G63" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="H63" t="s">
         <v>69</v>
       </c>
       <c r="I63" s="1">
-        <f>VLOOKUP(F63,'Source lists'!$E$1:F61,2,FALSE)</f>
+        <f>VLOOKUP(F63,'Source lists'!$E$1:F62,2,FALSE)</f>
         <v>4</v>
       </c>
       <c r="J63" s="1">
-        <f>VLOOKUP(G63,'Source lists'!$H$1:I62,2,FALSE)</f>
+        <f>VLOOKUP(G63,'Source lists'!$H$1:I63,2,FALSE)</f>
         <v>6</v>
       </c>
       <c r="K63" s="1">
@@ -11122,7 +11125,7 @@
     </row>
     <row r="64" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="A64">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B64" t="s">
         <v>8</v>
@@ -11134,23 +11137,23 @@
         <v>54</v>
       </c>
       <c r="E64" s="2" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="F64" t="s">
         <v>15</v>
       </c>
       <c r="G64" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="H64" t="s">
         <v>69</v>
       </c>
       <c r="I64" s="1">
-        <f>VLOOKUP(F64,'Source lists'!$E$1:F62,2,FALSE)</f>
+        <f>VLOOKUP(F64,'Source lists'!$E$1:F63,2,FALSE)</f>
         <v>4</v>
       </c>
       <c r="J64" s="1">
-        <f>VLOOKUP(G64,'Source lists'!$H$1:I63,2,FALSE)</f>
+        <f>VLOOKUP(G64,'Source lists'!$H$1:I64,2,FALSE)</f>
         <v>6</v>
       </c>
       <c r="K64" s="1">
@@ -11160,70 +11163,67 @@
     </row>
     <row r="65" spans="1:12" ht="17" x14ac:dyDescent="0.2">
       <c r="A65">
-        <v>21</v>
+        <v>66</v>
       </c>
       <c r="B65" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="C65" t="s">
-        <v>42</v>
-      </c>
-      <c r="D65" t="s">
-        <v>54</v>
+        <v>105</v>
       </c>
       <c r="E65" s="2" t="s">
-        <v>60</v>
+        <v>189</v>
       </c>
       <c r="F65" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="G65" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="H65" t="s">
-        <v>69</v>
+        <v>23</v>
       </c>
       <c r="I65" s="1">
-        <f>VLOOKUP(F65,'Source lists'!$E$1:F63,2,FALSE)</f>
-        <v>4</v>
+        <f>VLOOKUP(F65,'Source lists'!$E$1:F64,2,FALSE)</f>
+        <v>1</v>
       </c>
       <c r="J65" s="1">
-        <f>VLOOKUP(G65,'Source lists'!$H$1:I64,2,FALSE)</f>
+        <f>VLOOKUP(G65,'Source lists'!$H$1:I65,2,FALSE)</f>
         <v>6</v>
       </c>
       <c r="K65" s="1">
         <f>VLOOKUP(F65,'Source lists'!$E$2:$F$6,2,FALSE)*(VLOOKUP(G65,'Source lists'!$H$2:$I$7,2,FALSE)^2)/VLOOKUP(H65,'Source lists'!$K$2:$L$9,2,FALSE)</f>
-        <v>20.571428571428573</v>
+        <v>18</v>
       </c>
     </row>
     <row r="66" spans="1:12" ht="34" x14ac:dyDescent="0.2">
       <c r="A66">
-        <v>66</v>
+        <v>76</v>
       </c>
       <c r="B66" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C66" t="s">
-        <v>106</v>
+        <v>138</v>
       </c>
       <c r="E66" s="2" t="s">
-        <v>190</v>
+        <v>140</v>
       </c>
       <c r="F66" t="s">
         <v>17</v>
       </c>
       <c r="G66" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="H66" t="s">
         <v>23</v>
       </c>
       <c r="I66" s="1">
-        <f>VLOOKUP(F66,'Source lists'!$E$1:F64,2,FALSE)</f>
+        <f>VLOOKUP(F66,'Source lists'!$E$1:F65,2,FALSE)</f>
         <v>1</v>
       </c>
       <c r="J66" s="1">
-        <f>VLOOKUP(G66,'Source lists'!$H$1:I65,2,FALSE)</f>
+        <f>VLOOKUP(G66,'Source lists'!$H$1:I66,2,FALSE)</f>
         <v>6</v>
       </c>
       <c r="K66" s="1">
@@ -11233,80 +11233,83 @@
     </row>
     <row r="67" spans="1:12" ht="34" x14ac:dyDescent="0.2">
       <c r="A67">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="B67" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C67" t="s">
-        <v>139</v>
+        <v>132</v>
+      </c>
+      <c r="D67" t="s">
+        <v>187</v>
       </c>
       <c r="E67" s="2" t="s">
-        <v>141</v>
+        <v>135</v>
       </c>
       <c r="F67" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="G67" t="s">
-        <v>159</v>
+        <v>28</v>
       </c>
       <c r="H67" t="s">
-        <v>23</v>
+        <v>67</v>
       </c>
       <c r="I67" s="1">
-        <f>VLOOKUP(F67,'Source lists'!$E$1:F65,2,FALSE)</f>
-        <v>1</v>
+        <f>VLOOKUP(F67,'Source lists'!$E$1:F66,2,FALSE)</f>
+        <v>4</v>
       </c>
       <c r="J67" s="1">
-        <f>VLOOKUP(G67,'Source lists'!$H$1:I66,2,FALSE)</f>
-        <v>6</v>
+        <f>VLOOKUP(G67,'Source lists'!$H$1:I67,2,FALSE)</f>
+        <v>4</v>
       </c>
       <c r="K67" s="1">
         <f>VLOOKUP(F67,'Source lists'!$E$2:$F$6,2,FALSE)*(VLOOKUP(G67,'Source lists'!$H$2:$I$7,2,FALSE)^2)/VLOOKUP(H67,'Source lists'!$K$2:$L$9,2,FALSE)</f>
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="68" spans="1:12" ht="34" x14ac:dyDescent="0.2">
       <c r="A68">
-        <v>73</v>
+        <v>91</v>
       </c>
       <c r="B68" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C68" t="s">
-        <v>133</v>
-      </c>
-      <c r="D68" t="s">
-        <v>188</v>
+        <v>160</v>
       </c>
       <c r="E68" s="2" t="s">
-        <v>136</v>
+        <v>166</v>
       </c>
       <c r="F68" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="G68" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="H68" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="I68" s="1">
-        <f>VLOOKUP(F68,'Source lists'!$E$1:F66,2,FALSE)</f>
-        <v>4</v>
+        <f>VLOOKUP(F68,'Source lists'!$E$1:F67,2,FALSE)</f>
+        <v>1</v>
       </c>
       <c r="J68" s="1">
-        <f>VLOOKUP(G68,'Source lists'!$H$1:I67,2,FALSE)</f>
-        <v>4</v>
+        <f>VLOOKUP(G68,'Source lists'!$H$1:I68,2,FALSE)</f>
+        <v>10</v>
       </c>
       <c r="K68" s="1">
         <f>VLOOKUP(F68,'Source lists'!$E$2:$F$6,2,FALSE)*(VLOOKUP(G68,'Source lists'!$H$2:$I$7,2,FALSE)^2)/VLOOKUP(H68,'Source lists'!$K$2:$L$9,2,FALSE)</f>
-        <v>16</v>
+        <v>14.285714285714286</v>
+      </c>
+      <c r="L68">
+        <v>59</v>
       </c>
     </row>
     <row r="69" spans="1:12" ht="17" x14ac:dyDescent="0.2">
       <c r="A69">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="B69" t="s">
         <v>4</v>
@@ -11315,7 +11318,7 @@
         <v>161</v>
       </c>
       <c r="E69" s="2" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="F69" t="s">
         <v>17</v>
@@ -11327,11 +11330,11 @@
         <v>69</v>
       </c>
       <c r="I69" s="1">
-        <f>VLOOKUP(F69,'Source lists'!$E$1:F67,2,FALSE)</f>
+        <f>VLOOKUP(F69,'Source lists'!$E$1:F68,2,FALSE)</f>
         <v>1</v>
       </c>
       <c r="J69" s="1">
-        <f>VLOOKUP(G69,'Source lists'!$H$1:I68,2,FALSE)</f>
+        <f>VLOOKUP(G69,'Source lists'!$H$1:I69,2,FALSE)</f>
         <v>10</v>
       </c>
       <c r="K69" s="1">
@@ -11339,12 +11342,12 @@
         <v>14.285714285714286</v>
       </c>
       <c r="L69">
-        <v>59</v>
+        <v>64</v>
       </c>
     </row>
     <row r="70" spans="1:12" ht="17" x14ac:dyDescent="0.2">
       <c r="A70">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="B70" t="s">
         <v>4</v>
@@ -11353,7 +11356,7 @@
         <v>162</v>
       </c>
       <c r="E70" s="2" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="F70" t="s">
         <v>17</v>
@@ -11365,11 +11368,11 @@
         <v>69</v>
       </c>
       <c r="I70" s="1">
-        <f>VLOOKUP(F70,'Source lists'!$E$1:F68,2,FALSE)</f>
+        <f>VLOOKUP(F70,'Source lists'!$E$1:F69,2,FALSE)</f>
         <v>1</v>
       </c>
       <c r="J70" s="1">
-        <f>VLOOKUP(G70,'Source lists'!$H$1:I69,2,FALSE)</f>
+        <f>VLOOKUP(G70,'Source lists'!$H$1:I70,2,FALSE)</f>
         <v>10</v>
       </c>
       <c r="K70" s="1">
@@ -11377,12 +11380,12 @@
         <v>14.285714285714286</v>
       </c>
       <c r="L70">
-        <v>64</v>
+        <v>59</v>
       </c>
     </row>
     <row r="71" spans="1:12" ht="17" x14ac:dyDescent="0.2">
       <c r="A71">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="B71" t="s">
         <v>4</v>
@@ -11391,7 +11394,7 @@
         <v>163</v>
       </c>
       <c r="E71" s="2" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="F71" t="s">
         <v>17</v>
@@ -11403,11 +11406,11 @@
         <v>69</v>
       </c>
       <c r="I71" s="1">
-        <f>VLOOKUP(F71,'Source lists'!$E$1:F69,2,FALSE)</f>
+        <f>VLOOKUP(F71,'Source lists'!$E$1:F70,2,FALSE)</f>
         <v>1</v>
       </c>
       <c r="J71" s="1">
-        <f>VLOOKUP(G71,'Source lists'!$H$1:I70,2,FALSE)</f>
+        <f>VLOOKUP(G71,'Source lists'!$H$1:I71,2,FALSE)</f>
         <v>10</v>
       </c>
       <c r="K71" s="1">
@@ -11415,12 +11418,12 @@
         <v>14.285714285714286</v>
       </c>
       <c r="L71">
-        <v>59</v>
+        <v>64</v>
       </c>
     </row>
     <row r="72" spans="1:12" ht="17" x14ac:dyDescent="0.2">
       <c r="A72">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="B72" t="s">
         <v>4</v>
@@ -11429,7 +11432,7 @@
         <v>164</v>
       </c>
       <c r="E72" s="2" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="F72" t="s">
         <v>17</v>
@@ -11441,11 +11444,11 @@
         <v>69</v>
       </c>
       <c r="I72" s="1">
-        <f>VLOOKUP(F72,'Source lists'!$E$1:F70,2,FALSE)</f>
+        <f>VLOOKUP(F72,'Source lists'!$E$1:F71,2,FALSE)</f>
         <v>1</v>
       </c>
       <c r="J72" s="1">
-        <f>VLOOKUP(G72,'Source lists'!$H$1:I71,2,FALSE)</f>
+        <f>VLOOKUP(G72,'Source lists'!$H$1:I72,2,FALSE)</f>
         <v>10</v>
       </c>
       <c r="K72" s="1">
@@ -11453,12 +11456,12 @@
         <v>14.285714285714286</v>
       </c>
       <c r="L72">
-        <v>64</v>
+        <v>59</v>
       </c>
     </row>
     <row r="73" spans="1:12" ht="17" x14ac:dyDescent="0.2">
       <c r="A73">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="B73" t="s">
         <v>4</v>
@@ -11467,7 +11470,7 @@
         <v>165</v>
       </c>
       <c r="E73" s="2" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="F73" t="s">
         <v>17</v>
@@ -11479,11 +11482,11 @@
         <v>69</v>
       </c>
       <c r="I73" s="1">
-        <f>VLOOKUP(F73,'Source lists'!$E$1:F71,2,FALSE)</f>
+        <f>VLOOKUP(F73,'Source lists'!$E$1:F72,2,FALSE)</f>
         <v>1</v>
       </c>
       <c r="J73" s="1">
-        <f>VLOOKUP(G73,'Source lists'!$H$1:I72,2,FALSE)</f>
+        <f>VLOOKUP(G73,'Source lists'!$H$1:I73,2,FALSE)</f>
         <v>10</v>
       </c>
       <c r="K73" s="1">
@@ -11491,21 +11494,21 @@
         <v>14.285714285714286</v>
       </c>
       <c r="L73">
-        <v>59</v>
+        <v>64</v>
       </c>
     </row>
     <row r="74" spans="1:12" ht="17" x14ac:dyDescent="0.2">
       <c r="A74">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="B74" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C74" t="s">
-        <v>166</v>
+        <v>146</v>
       </c>
       <c r="E74" s="2" t="s">
-        <v>167</v>
+        <v>190</v>
       </c>
       <c r="F74" t="s">
         <v>17</v>
@@ -11517,11 +11520,11 @@
         <v>69</v>
       </c>
       <c r="I74" s="1">
-        <f>VLOOKUP(F74,'Source lists'!$E$1:F72,2,FALSE)</f>
+        <f>VLOOKUP(F74,'Source lists'!$E$1:F73,2,FALSE)</f>
         <v>1</v>
       </c>
       <c r="J74" s="1">
-        <f>VLOOKUP(G74,'Source lists'!$H$1:I73,2,FALSE)</f>
+        <f>VLOOKUP(G74,'Source lists'!$H$1:I74,2,FALSE)</f>
         <v>10</v>
       </c>
       <c r="K74" s="1">
@@ -11529,21 +11532,21 @@
         <v>14.285714285714286</v>
       </c>
       <c r="L74">
-        <v>64</v>
+        <v>59</v>
       </c>
     </row>
     <row r="75" spans="1:12" ht="34" x14ac:dyDescent="0.2">
       <c r="A75">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="B75" t="s">
         <v>5</v>
       </c>
       <c r="C75" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="E75" s="2" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="F75" t="s">
         <v>17</v>
@@ -11555,11 +11558,11 @@
         <v>69</v>
       </c>
       <c r="I75" s="1">
-        <f>VLOOKUP(F75,'Source lists'!$E$1:F73,2,FALSE)</f>
+        <f>VLOOKUP(F75,'Source lists'!$E$1:F74,2,FALSE)</f>
         <v>1</v>
       </c>
       <c r="J75" s="1">
-        <f>VLOOKUP(G75,'Source lists'!$H$1:I74,2,FALSE)</f>
+        <f>VLOOKUP(G75,'Source lists'!$H$1:I75,2,FALSE)</f>
         <v>10</v>
       </c>
       <c r="K75" s="1">
@@ -11567,18 +11570,18 @@
         <v>14.285714285714286</v>
       </c>
       <c r="L75">
-        <v>59</v>
+        <v>64</v>
       </c>
     </row>
     <row r="76" spans="1:12" ht="34" x14ac:dyDescent="0.2">
       <c r="A76">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="B76" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C76" t="s">
-        <v>147</v>
+        <v>168</v>
       </c>
       <c r="E76" s="2" t="s">
         <v>191</v>
@@ -11593,11 +11596,11 @@
         <v>69</v>
       </c>
       <c r="I76" s="1">
-        <f>VLOOKUP(F76,'Source lists'!$E$1:F74,2,FALSE)</f>
+        <f>VLOOKUP(F76,'Source lists'!$E$1:F75,2,FALSE)</f>
         <v>1</v>
       </c>
       <c r="J76" s="1">
-        <f>VLOOKUP(G76,'Source lists'!$H$1:I75,2,FALSE)</f>
+        <f>VLOOKUP(G76,'Source lists'!$H$1:I76,2,FALSE)</f>
         <v>10</v>
       </c>
       <c r="K76" s="1">
@@ -11605,18 +11608,18 @@
         <v>14.285714285714286</v>
       </c>
       <c r="L76">
-        <v>64</v>
+        <v>99</v>
       </c>
     </row>
     <row r="77" spans="1:12" ht="51" x14ac:dyDescent="0.2">
       <c r="A77">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="B77" t="s">
         <v>6</v>
       </c>
       <c r="C77" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="E77" s="2" t="s">
         <v>192</v>
@@ -11631,11 +11634,11 @@
         <v>69</v>
       </c>
       <c r="I77" s="1">
-        <f>VLOOKUP(F77,'Source lists'!$E$1:F75,2,FALSE)</f>
+        <f>VLOOKUP(F77,'Source lists'!$E$1:F76,2,FALSE)</f>
         <v>1</v>
       </c>
       <c r="J77" s="1">
-        <f>VLOOKUP(G77,'Source lists'!$H$1:I76,2,FALSE)</f>
+        <f>VLOOKUP(G77,'Source lists'!$H$1:I77,2,FALSE)</f>
         <v>10</v>
       </c>
       <c r="K77" s="1">
@@ -11643,15 +11646,15 @@
         <v>14.285714285714286</v>
       </c>
       <c r="L77">
-        <v>99</v>
+        <v>100</v>
       </c>
     </row>
     <row r="78" spans="1:12" ht="34" x14ac:dyDescent="0.2">
       <c r="A78">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="B78" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C78" t="s">
         <v>169</v>
@@ -11669,11 +11672,11 @@
         <v>69</v>
       </c>
       <c r="I78" s="1">
-        <f>VLOOKUP(F78,'Source lists'!$E$1:F76,2,FALSE)</f>
+        <f>VLOOKUP(F78,'Source lists'!$E$1:F77,2,FALSE)</f>
         <v>1</v>
       </c>
       <c r="J78" s="1">
-        <f>VLOOKUP(G78,'Source lists'!$H$1:I77,2,FALSE)</f>
+        <f>VLOOKUP(G78,'Source lists'!$H$1:I78,2,FALSE)</f>
         <v>10</v>
       </c>
       <c r="K78" s="1">
@@ -11681,21 +11684,21 @@
         <v>14.285714285714286</v>
       </c>
       <c r="L78">
-        <v>100</v>
+        <v>102</v>
       </c>
     </row>
     <row r="79" spans="1:12" ht="51" x14ac:dyDescent="0.2">
       <c r="A79">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="B79" t="s">
         <v>5</v>
       </c>
       <c r="C79" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="E79" s="2" t="s">
-        <v>194</v>
+        <v>171</v>
       </c>
       <c r="F79" t="s">
         <v>17</v>
@@ -11707,11 +11710,11 @@
         <v>69</v>
       </c>
       <c r="I79" s="1">
-        <f>VLOOKUP(F79,'Source lists'!$E$1:F77,2,FALSE)</f>
+        <f>VLOOKUP(F79,'Source lists'!$E$1:F78,2,FALSE)</f>
         <v>1</v>
       </c>
       <c r="J79" s="1">
-        <f>VLOOKUP(G79,'Source lists'!$H$1:I78,2,FALSE)</f>
+        <f>VLOOKUP(G79,'Source lists'!$H$1:I79,2,FALSE)</f>
         <v>10</v>
       </c>
       <c r="K79" s="1">
@@ -11719,59 +11722,56 @@
         <v>14.285714285714286</v>
       </c>
       <c r="L79">
-        <v>102</v>
+        <v>103</v>
       </c>
     </row>
     <row r="80" spans="1:12" ht="34" x14ac:dyDescent="0.2">
       <c r="A80">
-        <v>104</v>
+        <v>35</v>
       </c>
       <c r="B80" t="s">
-        <v>5</v>
+        <v>38</v>
       </c>
       <c r="C80" t="s">
-        <v>170</v>
+        <v>79</v>
       </c>
       <c r="E80" s="2" t="s">
-        <v>172</v>
+        <v>83</v>
       </c>
       <c r="F80" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G80" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="H80" t="s">
-        <v>69</v>
+        <v>23</v>
       </c>
       <c r="I80" s="1">
-        <f>VLOOKUP(F80,'Source lists'!$E$1:F78,2,FALSE)</f>
-        <v>1</v>
+        <f>VLOOKUP(F80,'Source lists'!$E$1:F79,2,FALSE)</f>
+        <v>3</v>
       </c>
       <c r="J80" s="1">
-        <f>VLOOKUP(G80,'Source lists'!$H$1:I79,2,FALSE)</f>
-        <v>10</v>
+        <f>VLOOKUP(G80,'Source lists'!$H$1:I80,2,FALSE)</f>
+        <v>3</v>
       </c>
       <c r="K80" s="1">
         <f>VLOOKUP(F80,'Source lists'!$E$2:$F$6,2,FALSE)*(VLOOKUP(G80,'Source lists'!$H$2:$I$7,2,FALSE)^2)/VLOOKUP(H80,'Source lists'!$K$2:$L$9,2,FALSE)</f>
-        <v>14.285714285714286</v>
-      </c>
-      <c r="L80">
-        <v>103</v>
+        <v>13.5</v>
       </c>
     </row>
     <row r="81" spans="1:11" ht="34" x14ac:dyDescent="0.2">
       <c r="A81">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="B81" t="s">
-        <v>38</v>
+        <v>1</v>
       </c>
       <c r="C81" t="s">
-        <v>80</v>
+        <v>86</v>
       </c>
       <c r="E81" s="2" t="s">
-        <v>84</v>
+        <v>117</v>
       </c>
       <c r="F81" t="s">
         <v>16</v>
@@ -11783,11 +11783,11 @@
         <v>23</v>
       </c>
       <c r="I81" s="1">
-        <f>VLOOKUP(F81,'Source lists'!$E$1:F79,2,FALSE)</f>
+        <f>VLOOKUP(F81,'Source lists'!$E$1:F80,2,FALSE)</f>
         <v>3</v>
       </c>
       <c r="J81" s="1">
-        <f>VLOOKUP(G81,'Source lists'!$H$1:I80,2,FALSE)</f>
+        <f>VLOOKUP(G81,'Source lists'!$H$1:I81,2,FALSE)</f>
         <v>3</v>
       </c>
       <c r="K81" s="1">
@@ -11797,16 +11797,19 @@
     </row>
     <row r="82" spans="1:11" ht="34" x14ac:dyDescent="0.2">
       <c r="A82">
-        <v>38</v>
+        <v>71</v>
       </c>
       <c r="B82" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C82" t="s">
-        <v>87</v>
+        <v>132</v>
+      </c>
+      <c r="D82" t="s">
+        <v>187</v>
       </c>
       <c r="E82" s="2" t="s">
-        <v>118</v>
+        <v>134</v>
       </c>
       <c r="F82" t="s">
         <v>16</v>
@@ -11818,11 +11821,11 @@
         <v>23</v>
       </c>
       <c r="I82" s="1">
-        <f>VLOOKUP(F82,'Source lists'!$E$1:F80,2,FALSE)</f>
+        <f>VLOOKUP(F82,'Source lists'!$E$1:F81,2,FALSE)</f>
         <v>3</v>
       </c>
       <c r="J82" s="1">
-        <f>VLOOKUP(G82,'Source lists'!$H$1:I81,2,FALSE)</f>
+        <f>VLOOKUP(G82,'Source lists'!$H$1:I82,2,FALSE)</f>
         <v>3</v>
       </c>
       <c r="K82" s="1">
@@ -11832,19 +11835,19 @@
     </row>
     <row r="83" spans="1:11" ht="34" x14ac:dyDescent="0.2">
       <c r="A83">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="B83" t="s">
         <v>2</v>
       </c>
       <c r="C83" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="D83" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="E83" s="2" t="s">
-        <v>135</v>
+        <v>194</v>
       </c>
       <c r="F83" t="s">
         <v>16</v>
@@ -11856,11 +11859,11 @@
         <v>23</v>
       </c>
       <c r="I83" s="1">
-        <f>VLOOKUP(F83,'Source lists'!$E$1:F81,2,FALSE)</f>
+        <f>VLOOKUP(F83,'Source lists'!$E$1:F82,2,FALSE)</f>
         <v>3</v>
       </c>
       <c r="J83" s="1">
-        <f>VLOOKUP(G83,'Source lists'!$H$1:I82,2,FALSE)</f>
+        <f>VLOOKUP(G83,'Source lists'!$H$1:I83,2,FALSE)</f>
         <v>3</v>
       </c>
       <c r="K83" s="1">
@@ -11870,19 +11873,16 @@
     </row>
     <row r="84" spans="1:11" ht="34" x14ac:dyDescent="0.2">
       <c r="A84">
-        <v>72</v>
+        <v>85</v>
       </c>
       <c r="B84" t="s">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="C84" t="s">
-        <v>133</v>
-      </c>
-      <c r="D84" t="s">
-        <v>188</v>
+        <v>149</v>
       </c>
       <c r="E84" s="2" t="s">
-        <v>195</v>
+        <v>151</v>
       </c>
       <c r="F84" t="s">
         <v>16</v>
@@ -11894,11 +11894,11 @@
         <v>23</v>
       </c>
       <c r="I84" s="1">
-        <f>VLOOKUP(F84,'Source lists'!$E$1:F82,2,FALSE)</f>
+        <f>VLOOKUP(F84,'Source lists'!$E$1:F83,2,FALSE)</f>
         <v>3</v>
       </c>
       <c r="J84" s="1">
-        <f>VLOOKUP(G84,'Source lists'!$H$1:I83,2,FALSE)</f>
+        <f>VLOOKUP(G84,'Source lists'!$H$1:I84,2,FALSE)</f>
         <v>3</v>
       </c>
       <c r="K84" s="1">
@@ -11908,13 +11908,13 @@
     </row>
     <row r="85" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A85">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="B85" t="s">
         <v>6</v>
       </c>
       <c r="C85" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="E85" s="2" t="s">
         <v>152</v>
@@ -11929,11 +11929,11 @@
         <v>23</v>
       </c>
       <c r="I85" s="1">
-        <f>VLOOKUP(F85,'Source lists'!$E$1:F83,2,FALSE)</f>
+        <f>VLOOKUP(F85,'Source lists'!$E$1:F84,2,FALSE)</f>
         <v>3</v>
       </c>
       <c r="J85" s="1">
-        <f>VLOOKUP(G85,'Source lists'!$H$1:I84,2,FALSE)</f>
+        <f>VLOOKUP(G85,'Source lists'!$H$1:I85,2,FALSE)</f>
         <v>3</v>
       </c>
       <c r="K85" s="1">
@@ -11943,54 +11943,57 @@
     </row>
     <row r="86" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A86">
-        <v>86</v>
+        <v>36</v>
       </c>
       <c r="B86" t="s">
-        <v>6</v>
+        <v>66</v>
       </c>
       <c r="C86" t="s">
-        <v>150</v>
+        <v>72</v>
+      </c>
+      <c r="D86" t="s">
+        <v>84</v>
       </c>
       <c r="E86" s="2" t="s">
-        <v>153</v>
+        <v>85</v>
       </c>
       <c r="F86" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G86" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="H86" t="s">
-        <v>23</v>
+        <v>70</v>
       </c>
       <c r="I86" s="1">
-        <f>VLOOKUP(F86,'Source lists'!$E$1:F84,2,FALSE)</f>
-        <v>3</v>
+        <f>VLOOKUP(F86,'Source lists'!$E$1:F85,2,FALSE)</f>
+        <v>4</v>
       </c>
       <c r="J86" s="1">
-        <f>VLOOKUP(G86,'Source lists'!$H$1:I85,2,FALSE)</f>
-        <v>3</v>
+        <f>VLOOKUP(G86,'Source lists'!$H$1:I86,2,FALSE)</f>
+        <v>4</v>
       </c>
       <c r="K86" s="1">
         <f>VLOOKUP(F86,'Source lists'!$E$2:$F$6,2,FALSE)*(VLOOKUP(G86,'Source lists'!$H$2:$I$7,2,FALSE)^2)/VLOOKUP(H86,'Source lists'!$K$2:$L$9,2,FALSE)</f>
-        <v>13.5</v>
+        <v>12.8</v>
       </c>
     </row>
     <row r="87" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A87">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B87" t="s">
-        <v>66</v>
+        <v>38</v>
       </c>
       <c r="C87" t="s">
-        <v>73</v>
+        <v>79</v>
       </c>
       <c r="D87" t="s">
+        <v>84</v>
+      </c>
+      <c r="E87" s="2" t="s">
         <v>85</v>
-      </c>
-      <c r="E87" s="2" t="s">
-        <v>86</v>
       </c>
       <c r="F87" t="s">
         <v>15</v>
@@ -12002,11 +12005,11 @@
         <v>70</v>
       </c>
       <c r="I87" s="1">
-        <f>VLOOKUP(F87,'Source lists'!$E$1:F85,2,FALSE)</f>
+        <f>VLOOKUP(F87,'Source lists'!$E$1:F86,2,FALSE)</f>
         <v>4</v>
       </c>
       <c r="J87" s="1">
-        <f>VLOOKUP(G87,'Source lists'!$H$1:I86,2,FALSE)</f>
+        <f>VLOOKUP(G87,'Source lists'!$H$1:I87,2,FALSE)</f>
         <v>4</v>
       </c>
       <c r="K87" s="1">
@@ -12016,19 +12019,19 @@
     </row>
     <row r="88" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A88">
-        <v>37</v>
+        <v>47</v>
       </c>
       <c r="B88" t="s">
-        <v>38</v>
+        <v>1</v>
       </c>
       <c r="C88" t="s">
-        <v>80</v>
+        <v>90</v>
       </c>
       <c r="D88" t="s">
-        <v>85</v>
+        <v>111</v>
       </c>
       <c r="E88" s="2" t="s">
-        <v>86</v>
+        <v>112</v>
       </c>
       <c r="F88" t="s">
         <v>15</v>
@@ -12040,11 +12043,11 @@
         <v>70</v>
       </c>
       <c r="I88" s="1">
-        <f>VLOOKUP(F88,'Source lists'!$E$1:F86,2,FALSE)</f>
+        <f>VLOOKUP(F88,'Source lists'!$E$1:F87,2,FALSE)</f>
         <v>4</v>
       </c>
       <c r="J88" s="1">
-        <f>VLOOKUP(G88,'Source lists'!$H$1:I87,2,FALSE)</f>
+        <f>VLOOKUP(G88,'Source lists'!$H$1:I88,2,FALSE)</f>
         <v>4</v>
       </c>
       <c r="K88" s="1">
@@ -12054,19 +12057,19 @@
     </row>
     <row r="89" spans="1:11" ht="34" x14ac:dyDescent="0.2">
       <c r="A89">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="B89" t="s">
         <v>1</v>
       </c>
       <c r="C89" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D89" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E89" s="2" t="s">
-        <v>113</v>
+        <v>100</v>
       </c>
       <c r="F89" t="s">
         <v>15</v>
@@ -12078,11 +12081,11 @@
         <v>70</v>
       </c>
       <c r="I89" s="1">
-        <f>VLOOKUP(F89,'Source lists'!$E$1:F87,2,FALSE)</f>
+        <f>VLOOKUP(F89,'Source lists'!$E$1:F88,2,FALSE)</f>
         <v>4</v>
       </c>
       <c r="J89" s="1">
-        <f>VLOOKUP(G89,'Source lists'!$H$1:I88,2,FALSE)</f>
+        <f>VLOOKUP(G89,'Source lists'!$H$1:I89,2,FALSE)</f>
         <v>4</v>
       </c>
       <c r="K89" s="1">
@@ -12092,19 +12095,16 @@
     </row>
     <row r="90" spans="1:11" ht="34" x14ac:dyDescent="0.2">
       <c r="A90">
-        <v>50</v>
+        <v>56</v>
       </c>
       <c r="B90" t="s">
         <v>1</v>
       </c>
       <c r="C90" t="s">
-        <v>91</v>
-      </c>
-      <c r="D90" t="s">
-        <v>112</v>
+        <v>90</v>
       </c>
       <c r="E90" s="2" t="s">
-        <v>101</v>
+        <v>109</v>
       </c>
       <c r="F90" t="s">
         <v>15</v>
@@ -12116,11 +12116,11 @@
         <v>70</v>
       </c>
       <c r="I90" s="1">
-        <f>VLOOKUP(F90,'Source lists'!$E$1:F88,2,FALSE)</f>
+        <f>VLOOKUP(F90,'Source lists'!$E$1:F89,2,FALSE)</f>
         <v>4</v>
       </c>
       <c r="J90" s="1">
-        <f>VLOOKUP(G90,'Source lists'!$H$1:I89,2,FALSE)</f>
+        <f>VLOOKUP(G90,'Source lists'!$H$1:I90,2,FALSE)</f>
         <v>4</v>
       </c>
       <c r="K90" s="1">
@@ -12130,54 +12130,54 @@
     </row>
     <row r="91" spans="1:11" ht="34" x14ac:dyDescent="0.2">
       <c r="A91">
-        <v>56</v>
+        <v>41</v>
       </c>
       <c r="B91" t="s">
         <v>1</v>
       </c>
       <c r="C91" t="s">
-        <v>91</v>
+        <v>86</v>
+      </c>
+      <c r="D91" t="s">
+        <v>88</v>
       </c>
       <c r="E91" s="2" t="s">
-        <v>110</v>
+        <v>89</v>
       </c>
       <c r="F91" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="G91" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="H91" t="s">
-        <v>70</v>
+        <v>22</v>
       </c>
       <c r="I91" s="1">
-        <f>VLOOKUP(F91,'Source lists'!$E$1:F89,2,FALSE)</f>
-        <v>4</v>
+        <f>VLOOKUP(F91,'Source lists'!$E$1:F90,2,FALSE)</f>
+        <v>1</v>
       </c>
       <c r="J91" s="1">
-        <f>VLOOKUP(G91,'Source lists'!$H$1:I90,2,FALSE)</f>
-        <v>4</v>
+        <f>VLOOKUP(G91,'Source lists'!$H$1:I91,2,FALSE)</f>
+        <v>10</v>
       </c>
       <c r="K91" s="1">
         <f>VLOOKUP(F91,'Source lists'!$E$2:$F$6,2,FALSE)*(VLOOKUP(G91,'Source lists'!$H$2:$I$7,2,FALSE)^2)/VLOOKUP(H91,'Source lists'!$K$2:$L$9,2,FALSE)</f>
-        <v>12.8</v>
+        <v>12.5</v>
       </c>
     </row>
     <row r="92" spans="1:11" ht="119" x14ac:dyDescent="0.2">
       <c r="A92">
-        <v>41</v>
+        <v>52</v>
       </c>
       <c r="B92" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C92" t="s">
-        <v>87</v>
-      </c>
-      <c r="D92" t="s">
-        <v>89</v>
+        <v>103</v>
       </c>
       <c r="E92" s="2" t="s">
-        <v>90</v>
+        <v>113</v>
       </c>
       <c r="F92" t="s">
         <v>17</v>
@@ -12189,11 +12189,11 @@
         <v>22</v>
       </c>
       <c r="I92" s="1">
-        <f>VLOOKUP(F92,'Source lists'!$E$1:F90,2,FALSE)</f>
+        <f>VLOOKUP(F92,'Source lists'!$E$1:F91,2,FALSE)</f>
         <v>1</v>
       </c>
       <c r="J92" s="1">
-        <f>VLOOKUP(G92,'Source lists'!$H$1:I91,2,FALSE)</f>
+        <f>VLOOKUP(G92,'Source lists'!$H$1:I92,2,FALSE)</f>
         <v>10</v>
       </c>
       <c r="K92" s="1">
@@ -12203,16 +12203,16 @@
     </row>
     <row r="93" spans="1:11" ht="68" x14ac:dyDescent="0.2">
       <c r="A93">
-        <v>52</v>
+        <v>65</v>
       </c>
       <c r="B93" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C93" t="s">
-        <v>104</v>
+        <v>127</v>
       </c>
       <c r="E93" s="2" t="s">
-        <v>114</v>
+        <v>128</v>
       </c>
       <c r="F93" t="s">
         <v>17</v>
@@ -12224,11 +12224,11 @@
         <v>22</v>
       </c>
       <c r="I93" s="1">
-        <f>VLOOKUP(F93,'Source lists'!$E$1:F91,2,FALSE)</f>
+        <f>VLOOKUP(F93,'Source lists'!$E$1:F92,2,FALSE)</f>
         <v>1</v>
       </c>
       <c r="J93" s="1">
-        <f>VLOOKUP(G93,'Source lists'!$H$1:I92,2,FALSE)</f>
+        <f>VLOOKUP(G93,'Source lists'!$H$1:I93,2,FALSE)</f>
         <v>10</v>
       </c>
       <c r="K93" s="1">
@@ -12238,16 +12238,16 @@
     </row>
     <row r="94" spans="1:11" ht="51" x14ac:dyDescent="0.2">
       <c r="A94">
-        <v>65</v>
+        <v>83</v>
       </c>
       <c r="B94" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C94" t="s">
-        <v>128</v>
+        <v>147</v>
       </c>
       <c r="E94" s="2" t="s">
-        <v>129</v>
+        <v>148</v>
       </c>
       <c r="F94" t="s">
         <v>17</v>
@@ -12259,11 +12259,11 @@
         <v>22</v>
       </c>
       <c r="I94" s="1">
-        <f>VLOOKUP(F94,'Source lists'!$E$1:F92,2,FALSE)</f>
+        <f>VLOOKUP(F94,'Source lists'!$E$1:F93,2,FALSE)</f>
         <v>1</v>
       </c>
       <c r="J94" s="1">
-        <f>VLOOKUP(G94,'Source lists'!$H$1:I93,2,FALSE)</f>
+        <f>VLOOKUP(G94,'Source lists'!$H$1:I94,2,FALSE)</f>
         <v>10</v>
       </c>
       <c r="K94" s="1">
@@ -12273,16 +12273,16 @@
     </row>
     <row r="95" spans="1:11" ht="34" x14ac:dyDescent="0.2">
       <c r="A95">
-        <v>83</v>
+        <v>102</v>
       </c>
       <c r="B95" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C95" t="s">
-        <v>148</v>
+        <v>169</v>
       </c>
       <c r="E95" s="2" t="s">
-        <v>149</v>
+        <v>170</v>
       </c>
       <c r="F95" t="s">
         <v>17</v>
@@ -12294,11 +12294,11 @@
         <v>22</v>
       </c>
       <c r="I95" s="1">
-        <f>VLOOKUP(F95,'Source lists'!$E$1:F93,2,FALSE)</f>
+        <f>VLOOKUP(F95,'Source lists'!$E$1:F94,2,FALSE)</f>
         <v>1</v>
       </c>
       <c r="J95" s="1">
-        <f>VLOOKUP(G95,'Source lists'!$H$1:I94,2,FALSE)</f>
+        <f>VLOOKUP(G95,'Source lists'!$H$1:I95,2,FALSE)</f>
         <v>10</v>
       </c>
       <c r="K95" s="1">
@@ -12308,16 +12308,16 @@
     </row>
     <row r="96" spans="1:11" ht="119" x14ac:dyDescent="0.2">
       <c r="A96">
-        <v>102</v>
+        <v>105</v>
       </c>
       <c r="B96" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="C96" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
       <c r="E96" s="2" t="s">
-        <v>171</v>
+        <v>195</v>
       </c>
       <c r="F96" t="s">
         <v>17</v>
@@ -12329,11 +12329,11 @@
         <v>22</v>
       </c>
       <c r="I96" s="1">
-        <f>VLOOKUP(F96,'Source lists'!$E$1:F94,2,FALSE)</f>
+        <f>VLOOKUP(F96,'Source lists'!$E$1:F95,2,FALSE)</f>
         <v>1</v>
       </c>
       <c r="J96" s="1">
-        <f>VLOOKUP(G96,'Source lists'!$H$1:I95,2,FALSE)</f>
+        <f>VLOOKUP(G96,'Source lists'!$H$1:I96,2,FALSE)</f>
         <v>10</v>
       </c>
       <c r="K96" s="1">
@@ -12343,16 +12343,16 @@
     </row>
     <row r="97" spans="1:11" ht="68" x14ac:dyDescent="0.2">
       <c r="A97">
-        <v>105</v>
+        <v>33</v>
       </c>
       <c r="B97" t="s">
-        <v>8</v>
+        <v>66</v>
       </c>
       <c r="C97" t="s">
-        <v>173</v>
+        <v>81</v>
       </c>
       <c r="E97" s="2" t="s">
-        <v>196</v>
+        <v>116</v>
       </c>
       <c r="F97" t="s">
         <v>17</v>
@@ -12361,33 +12361,30 @@
         <v>26</v>
       </c>
       <c r="H97" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="I97" s="1">
-        <f>VLOOKUP(F97,'Source lists'!$E$1:F95,2,FALSE)</f>
+        <f>VLOOKUP(F97,'Source lists'!$E$1:F96,2,FALSE)</f>
         <v>1</v>
       </c>
       <c r="J97" s="1">
-        <f>VLOOKUP(G97,'Source lists'!$H$1:I96,2,FALSE)</f>
+        <f>VLOOKUP(G97,'Source lists'!$H$1:I97,2,FALSE)</f>
         <v>10</v>
       </c>
       <c r="K97" s="1">
         <f>VLOOKUP(F97,'Source lists'!$E$2:$F$6,2,FALSE)*(VLOOKUP(G97,'Source lists'!$H$2:$I$7,2,FALSE)^2)/VLOOKUP(H97,'Source lists'!$K$2:$L$9,2,FALSE)</f>
-        <v>12.5</v>
+        <v>10</v>
       </c>
     </row>
     <row r="98" spans="1:11" ht="68" x14ac:dyDescent="0.2">
       <c r="A98">
-        <v>33</v>
+        <v>62</v>
       </c>
       <c r="B98" t="s">
-        <v>66</v>
-      </c>
-      <c r="C98" t="s">
-        <v>82</v>
+        <v>7</v>
       </c>
       <c r="E98" s="2" t="s">
-        <v>117</v>
+        <v>124</v>
       </c>
       <c r="F98" t="s">
         <v>17</v>
@@ -12399,11 +12396,11 @@
         <v>21</v>
       </c>
       <c r="I98" s="1">
-        <f>VLOOKUP(F98,'Source lists'!$E$1:F96,2,FALSE)</f>
+        <f>VLOOKUP(F98,'Source lists'!$E$1:F97,2,FALSE)</f>
         <v>1</v>
       </c>
       <c r="J98" s="1">
-        <f>VLOOKUP(G98,'Source lists'!$H$1:I97,2,FALSE)</f>
+        <f>VLOOKUP(G98,'Source lists'!$H$1:I98,2,FALSE)</f>
         <v>10</v>
       </c>
       <c r="K98" s="1">
@@ -12413,13 +12410,13 @@
     </row>
     <row r="99" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A99">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="B99" t="s">
-        <v>7</v>
+        <v>122</v>
       </c>
       <c r="E99" s="2" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="F99" t="s">
         <v>17</v>
@@ -12431,11 +12428,11 @@
         <v>21</v>
       </c>
       <c r="I99" s="1">
-        <f>VLOOKUP(F99,'Source lists'!$E$1:F97,2,FALSE)</f>
+        <f>VLOOKUP(F99,'Source lists'!$E$1:F98,2,FALSE)</f>
         <v>1</v>
       </c>
       <c r="J99" s="1">
-        <f>VLOOKUP(G99,'Source lists'!$H$1:I98,2,FALSE)</f>
+        <f>VLOOKUP(G99,'Source lists'!$H$1:I99,2,FALSE)</f>
         <v>10</v>
       </c>
       <c r="K99" s="1">
@@ -12445,13 +12442,16 @@
     </row>
     <row r="100" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A100">
-        <v>63</v>
+        <v>82</v>
       </c>
       <c r="B100" t="s">
-        <v>123</v>
+        <v>5</v>
+      </c>
+      <c r="C100" t="s">
+        <v>146</v>
       </c>
       <c r="E100" s="2" t="s">
-        <v>124</v>
+        <v>196</v>
       </c>
       <c r="F100" t="s">
         <v>17</v>
@@ -12463,11 +12463,11 @@
         <v>21</v>
       </c>
       <c r="I100" s="1">
-        <f>VLOOKUP(F100,'Source lists'!$E$1:F98,2,FALSE)</f>
+        <f>VLOOKUP(F100,'Source lists'!$E$1:F99,2,FALSE)</f>
         <v>1</v>
       </c>
       <c r="J100" s="1">
-        <f>VLOOKUP(G100,'Source lists'!$H$1:I99,2,FALSE)</f>
+        <f>VLOOKUP(G100,'Source lists'!$H$1:I100,2,FALSE)</f>
         <v>10</v>
       </c>
       <c r="K100" s="1">
@@ -12477,13 +12477,13 @@
     </row>
     <row r="101" spans="1:11" ht="119" x14ac:dyDescent="0.2">
       <c r="A101">
-        <v>82</v>
+        <v>99</v>
       </c>
       <c r="B101" t="s">
-        <v>5</v>
+        <v>167</v>
       </c>
       <c r="C101" t="s">
-        <v>147</v>
+        <v>168</v>
       </c>
       <c r="E101" s="2" t="s">
         <v>197</v>
@@ -12498,11 +12498,11 @@
         <v>21</v>
       </c>
       <c r="I101" s="1">
-        <f>VLOOKUP(F101,'Source lists'!$E$1:F99,2,FALSE)</f>
+        <f>VLOOKUP(F101,'Source lists'!$E$1:F100,2,FALSE)</f>
         <v>1</v>
       </c>
       <c r="J101" s="1">
-        <f>VLOOKUP(G101,'Source lists'!$H$1:I100,2,FALSE)</f>
+        <f>VLOOKUP(G101,'Source lists'!$H$1:I101,2,FALSE)</f>
         <v>10</v>
       </c>
       <c r="K101" s="1">
@@ -12512,37 +12512,40 @@
     </row>
     <row r="102" spans="1:11" ht="51" x14ac:dyDescent="0.2">
       <c r="A102">
-        <v>99</v>
+        <v>5</v>
       </c>
       <c r="B102" t="s">
-        <v>168</v>
+        <v>39</v>
       </c>
       <c r="C102" t="s">
-        <v>169</v>
+        <v>33</v>
+      </c>
+      <c r="D102" t="s">
+        <v>40</v>
       </c>
       <c r="E102" s="2" t="s">
-        <v>198</v>
+        <v>94</v>
       </c>
       <c r="F102" t="s">
         <v>17</v>
       </c>
       <c r="G102" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="H102" t="s">
-        <v>21</v>
+        <v>70</v>
       </c>
       <c r="I102" s="1">
-        <f>VLOOKUP(F102,'Source lists'!$E$1:F100,2,FALSE)</f>
+        <f>VLOOKUP(F102,'Source lists'!$E$1:F22,2,FALSE)</f>
         <v>1</v>
       </c>
       <c r="J102" s="1">
-        <f>VLOOKUP(G102,'Source lists'!$H$1:I101,2,FALSE)</f>
-        <v>10</v>
+        <f>VLOOKUP(G102,'Source lists'!$H$1:I23,2,FALSE)</f>
+        <v>7</v>
       </c>
       <c r="K102" s="1">
         <f>VLOOKUP(F102,'Source lists'!$E$2:$F$6,2,FALSE)*(VLOOKUP(G102,'Source lists'!$H$2:$I$7,2,FALSE)^2)/VLOOKUP(H102,'Source lists'!$K$2:$L$9,2,FALSE)</f>
-        <v>10</v>
+        <v>9.8000000000000007</v>
       </c>
     </row>
     <row r="103" spans="1:11" ht="34" x14ac:dyDescent="0.2">
@@ -12553,10 +12556,10 @@
         <v>66</v>
       </c>
       <c r="C103" t="s">
+        <v>72</v>
+      </c>
+      <c r="E103" s="2" t="s">
         <v>73</v>
-      </c>
-      <c r="E103" s="2" t="s">
-        <v>74</v>
       </c>
       <c r="F103" t="s">
         <v>16</v>
@@ -12588,10 +12591,10 @@
         <v>1</v>
       </c>
       <c r="C104" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E104" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="F104" t="s">
         <v>16</v>
@@ -12623,10 +12626,10 @@
         <v>1</v>
       </c>
       <c r="C105" t="s">
+        <v>90</v>
+      </c>
+      <c r="E105" s="2" t="s">
         <v>91</v>
-      </c>
-      <c r="E105" s="2" t="s">
-        <v>92</v>
       </c>
       <c r="F105" t="s">
         <v>16</v>
@@ -12658,10 +12661,10 @@
         <v>1</v>
       </c>
       <c r="C106" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E106" s="2" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="F106" t="s">
         <v>16</v>
@@ -12693,16 +12696,16 @@
         <v>2</v>
       </c>
       <c r="C107" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="E107" s="2" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="F107" t="s">
         <v>17</v>
       </c>
       <c r="G107" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="H107" t="s">
         <v>67</v>
@@ -12728,16 +12731,16 @@
         <v>2</v>
       </c>
       <c r="C108" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="E108" s="2" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="F108" t="s">
         <v>17</v>
       </c>
       <c r="G108" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="H108" t="s">
         <v>67</v>
@@ -12763,16 +12766,16 @@
         <v>2</v>
       </c>
       <c r="C109" t="s">
+        <v>130</v>
+      </c>
+      <c r="E109" s="2" t="s">
         <v>131</v>
-      </c>
-      <c r="E109" s="2" t="s">
-        <v>132</v>
       </c>
       <c r="F109" t="s">
         <v>17</v>
       </c>
       <c r="G109" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="H109" t="s">
         <v>67</v>
@@ -12798,19 +12801,19 @@
         <v>2</v>
       </c>
       <c r="C110" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="D110" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="E110" s="2" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="F110" t="s">
         <v>17</v>
       </c>
       <c r="G110" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="H110" t="s">
         <v>67</v>
@@ -12836,16 +12839,16 @@
         <v>3</v>
       </c>
       <c r="C111" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E111" s="2" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="F111" t="s">
         <v>17</v>
       </c>
       <c r="G111" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="H111" t="s">
         <v>67</v>
@@ -12868,10 +12871,10 @@
         <v>110</v>
       </c>
       <c r="B112" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E112" s="2" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="F112" t="s">
         <v>16</v>
@@ -12900,13 +12903,13 @@
         <v>51</v>
       </c>
       <c r="B113" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C113" t="s">
+        <v>101</v>
+      </c>
+      <c r="E113" s="2" t="s">
         <v>102</v>
-      </c>
-      <c r="E113" s="2" t="s">
-        <v>103</v>
       </c>
       <c r="F113" t="s">
         <v>17</v>
@@ -12938,10 +12941,10 @@
         <v>66</v>
       </c>
       <c r="C114" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E114" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="F114" t="s">
         <v>16</v>
@@ -12973,10 +12976,10 @@
         <v>2</v>
       </c>
       <c r="C115" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="E115" s="2" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="F115" t="s">
         <v>15</v>
@@ -13008,10 +13011,10 @@
         <v>66</v>
       </c>
       <c r="C116" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E116" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F116" t="s">
         <v>16</v>
@@ -13046,7 +13049,7 @@
         <v>38</v>
       </c>
       <c r="E117" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F117" t="s">
         <v>16</v>
@@ -13078,14 +13081,14 @@
         <v>27</v>
       </c>
       <c r="B118" t="s">
+        <v>74</v>
+      </c>
+      <c r="C118" t="s">
         <v>75</v>
-      </c>
-      <c r="C118" t="s">
-        <v>76</v>
       </c>
       <c r="D118"/>
       <c r="E118" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="F118" t="s">
         <v>16</v>
@@ -13113,8 +13116,8 @@
     </row>
   </sheetData>
   <autoFilter ref="A1:M1" xr:uid="{1EB57299-5CFD-7049-BDE4-6415040FFB14}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:M117">
-      <sortCondition descending="1" ref="K1:K117"/>
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:M118">
+      <sortCondition descending="1" ref="K1:K118"/>
     </sortState>
   </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
SigmaFox/modals/error: Created and utilised
</commit_message>
<xml_diff>
--- a/apps/e-questrian/e-Questrian - To do list.xlsx
+++ b/apps/e-questrian/e-Questrian - To do list.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rferreira/sigmafox/apps/e-questrian/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CAD30F0A-D96A-0042-80C6-359EF263DAF3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{403C0BF3-2CCA-9C4E-8AE8-6805EFED18EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="19820" activeTab="2" xr2:uid="{DC2B379E-A936-2146-8C4F-53C43AECE05C}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="19820" xr2:uid="{DC2B379E-A936-2146-8C4F-53C43AECE05C}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary of completion" sheetId="3" r:id="rId1"/>
@@ -22,7 +22,7 @@
   </definedNames>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="0" r:id="rId4"/>
+    <pivotCache cacheId="4" r:id="rId4"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="870" uniqueCount="216">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="874" uniqueCount="217">
   <si>
     <t>Sections</t>
   </si>
@@ -726,6 +726,9 @@
 Contact number
 User should also presented the option to skip
 Should be place on top of the main menu page (for now - will be replaced by dash board)</t>
+  </si>
+  <si>
+    <t>N/A</t>
   </si>
 </sst>
 </file>
@@ -781,7 +784,7 @@
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -794,6 +797,7 @@
     <xf numFmtId="43" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -814,7 +818,7 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Ruben Ferreira" refreshedDate="45310.2627931713" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="117" xr:uid="{AEB2BF63-68F2-404E-AE9B-E794DFB00774}">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Ruben Ferreira" refreshedDate="45319.716128009262" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="118" xr:uid="{AEB2BF63-68F2-404E-AE9B-E794DFB00774}">
   <cacheSource type="worksheet">
     <worksheetSource ref="A1:M1048576" sheet="Issues 3-1-24"/>
   </cacheSource>
@@ -856,9 +860,10 @@
       <sharedItems containsString="0" containsBlank="1" containsNumber="1" containsInteger="1" minValue="1" maxValue="103"/>
     </cacheField>
     <cacheField name="Status" numFmtId="0">
-      <sharedItems containsBlank="1" count="2">
+      <sharedItems containsBlank="1" count="3">
         <s v="Done"/>
         <m/>
+        <s v="N/A"/>
       </sharedItems>
     </cacheField>
   </cacheFields>
@@ -871,7 +876,7 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheRecords1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" count="117">
+<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" count="118">
   <r>
     <n v="53"/>
     <s v="Calendar/Appointments"/>
@@ -990,7 +995,7 @@
     <n v="6"/>
     <n v="72"/>
     <n v="2"/>
-    <x v="1"/>
+    <x v="0"/>
   </r>
   <r>
     <n v="32"/>
@@ -1158,22 +1163,7 @@
     <x v="0"/>
   </r>
   <r>
-    <n v="5"/>
-    <s v="Marketing"/>
-    <s v="Landing Page"/>
-    <s v="Footer bar"/>
-    <s v="Should be added to Landing page"/>
-    <s v="Poor UX"/>
-    <s v="New feature"/>
-    <s v="New component/service with simple integration"/>
-    <n v="4"/>
-    <n v="7"/>
-    <n v="39.200000000000003"/>
-    <m/>
-    <x v="1"/>
-  </r>
-  <r>
-    <n v="18"/>
+    <n v="17"/>
     <s v="Marketing"/>
     <s v="Landing Page"/>
     <s v="What's New Section"/>
@@ -1185,14 +1175,14 @@
     <n v="7"/>
     <n v="39.200000000000003"/>
     <m/>
-    <x v="1"/>
+    <x v="0"/>
   </r>
   <r>
     <n v="24"/>
     <s v="User Management"/>
     <s v="Sign in Modal"/>
     <s v="User details modal"/>
-    <s v="After registering - User should be presented with a basis users detail form with:_x000a_First name_x000a_Last name_x000a_Contact number_x000a_User should also presented the option to skip_x000a_Should be place on top of the main menu page (for now - will be replaced by dash board)"/>
+    <s v="After registering - User should be presented with a basic users detail form with:_x000a_First name_x000a_Last name_x000a_Contact number_x000a_User should also presented the option to skip_x000a_Should be place on top of the main menu page (for now - will be replaced by dash board)"/>
     <s v="Poor UX"/>
     <s v="New feature"/>
     <s v="New component/service with simple integration"/>
@@ -1200,7 +1190,7 @@
     <n v="7"/>
     <n v="39.200000000000003"/>
     <m/>
-    <x v="1"/>
+    <x v="2"/>
   </r>
   <r>
     <n v="7"/>
@@ -1533,6 +1523,21 @@
     <x v="1"/>
   </r>
   <r>
+    <n v="17"/>
+    <s v="Marketing"/>
+    <s v="Landing Page"/>
+    <s v="Why us section"/>
+    <s v="Should be added to Landing page"/>
+    <s v="Poor UI"/>
+    <s v="New feature"/>
+    <s v="New component/service with simple integration"/>
+    <n v="3"/>
+    <n v="7"/>
+    <n v="29.4"/>
+    <m/>
+    <x v="1"/>
+  </r>
+  <r>
     <n v="8"/>
     <s v="User Management"/>
     <s v="Sign in Modal"/>
@@ -2373,6 +2378,21 @@
     <x v="1"/>
   </r>
   <r>
+    <n v="5"/>
+    <s v="Marketing"/>
+    <s v="Landing Page"/>
+    <s v="Footer bar"/>
+    <s v="Should be added to Landing page"/>
+    <s v="Nice to have"/>
+    <s v="New feature"/>
+    <s v="New component/service with simple integration"/>
+    <n v="1"/>
+    <n v="7"/>
+    <n v="9.8000000000000007"/>
+    <m/>
+    <x v="1"/>
+  </r>
+  <r>
     <n v="26"/>
     <s v="Dashboard and Main Menu"/>
     <s v="Main menu"/>
@@ -2631,8 +2651,8 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{936C0618-B7B4-0144-93D9-409C5361BBD7}" name="PivotTable7" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
-  <location ref="A7:D9" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{936C0618-B7B4-0144-93D9-409C5361BBD7}" name="PivotTable7" cacheId="4" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="A7:E9" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="13">
     <pivotField showAll="0"/>
     <pivotField showAll="0"/>
@@ -2647,9 +2667,10 @@
     <pivotField showAll="0"/>
     <pivotField showAll="0"/>
     <pivotField axis="axisCol" showAll="0">
-      <items count="3">
+      <items count="4">
         <item x="0"/>
         <item x="1"/>
+        <item x="2"/>
         <item t="default"/>
       </items>
     </pivotField>
@@ -2660,12 +2681,15 @@
   <colFields count="1">
     <field x="12"/>
   </colFields>
-  <colItems count="3">
+  <colItems count="4">
     <i>
       <x/>
     </i>
     <i>
       <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
     </i>
     <i t="grand">
       <x/>
@@ -2687,8 +2711,8 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{4A183E6E-2837-3A40-90CB-E731BF47E9C0}" name="PivotTable6" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
-  <location ref="A1:D3" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{4A183E6E-2837-3A40-90CB-E731BF47E9C0}" name="PivotTable6" cacheId="4" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="A1:E3" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="13">
     <pivotField showAll="0"/>
     <pivotField showAll="0"/>
@@ -2703,9 +2727,10 @@
     <pivotField dataField="1" showAll="0"/>
     <pivotField showAll="0"/>
     <pivotField axis="axisCol" showAll="0">
-      <items count="3">
+      <items count="4">
         <item x="0"/>
         <item x="1"/>
+        <item x="2"/>
         <item t="default"/>
       </items>
     </pivotField>
@@ -2716,12 +2741,15 @@
   <colFields count="1">
     <field x="12"/>
   </colFields>
-  <colItems count="3">
+  <colItems count="4">
     <i>
       <x/>
     </i>
     <i>
       <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
     </i>
     <i t="grand">
       <x/>
@@ -2743,8 +2771,8 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{4DCC3165-0959-AA43-80CF-D9170B1DCB64}" name="PivotTable8" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
-  <location ref="A13:D15" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{4DCC3165-0959-AA43-80CF-D9170B1DCB64}" name="PivotTable8" cacheId="4" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="A13:E15" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="13">
     <pivotField showAll="0"/>
     <pivotField showAll="0"/>
@@ -2759,9 +2787,10 @@
     <pivotField showAll="0"/>
     <pivotField showAll="0"/>
     <pivotField axis="axisCol" showAll="0">
-      <items count="3">
+      <items count="4">
         <item x="0"/>
         <item x="1"/>
+        <item x="2"/>
         <item t="default"/>
       </items>
     </pivotField>
@@ -2772,12 +2801,15 @@
   <colFields count="1">
     <field x="12"/>
   </colFields>
-  <colItems count="3">
+  <colItems count="4">
     <i>
       <x/>
     </i>
     <i>
       <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
     </i>
     <i t="grand">
       <x/>
@@ -3095,10 +3127,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{37CCC35A-14FA-1E40-8319-0349AC17C33D}">
-  <dimension ref="A1:D17"/>
+  <dimension ref="A1:E17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3106,15 +3138,16 @@
     <col min="1" max="1" width="14.6640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="15.5" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="7" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B1" s="6" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B2" t="s">
         <v>175</v>
       </c>
@@ -3122,35 +3155,41 @@
         <v>177</v>
       </c>
       <c r="D2" t="s">
+        <v>216</v>
+      </c>
+      <c r="E2" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>205</v>
       </c>
-      <c r="B3">
-        <v>1116.2</v>
-      </c>
-      <c r="C3">
-        <v>2111.3976190476178</v>
-      </c>
-      <c r="D3">
-        <v>3227.5976190476176</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="D5" s="7">
+      <c r="B3" s="8">
+        <v>1227.4000000000003</v>
+      </c>
+      <c r="C3" s="8">
+        <v>1960.9976190476179</v>
+      </c>
+      <c r="D3" s="8">
+        <v>39.200000000000003</v>
+      </c>
+      <c r="E3" s="8">
+        <v>3227.5976190476181</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E5" s="7">
         <f>GETPIVOTDATA("Priority S",$A$1,"Status","Done")/GETPIVOTDATA("Priority S",$A$1)</f>
-        <v>0.34582997379002978</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+        <v>0.38028284342401231</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B7" s="6" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B8" t="s">
         <v>175</v>
       </c>
@@ -3158,35 +3197,41 @@
         <v>177</v>
       </c>
       <c r="D8" t="s">
+        <v>216</v>
+      </c>
+      <c r="E8" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>182</v>
       </c>
-      <c r="B9">
-        <v>93</v>
-      </c>
-      <c r="C9">
-        <v>279</v>
-      </c>
-      <c r="D9">
+      <c r="B9" s="8">
+        <v>101</v>
+      </c>
+      <c r="C9" s="8">
+        <v>267</v>
+      </c>
+      <c r="D9" s="8">
+        <v>4</v>
+      </c>
+      <c r="E9" s="8">
         <v>372</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="D11" s="7">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E11" s="7">
         <f>GETPIVOTDATA("Importance S",$A$7,"Status","Done")/GETPIVOTDATA("Importance S",$A$7)</f>
-        <v>0.25</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+        <v>0.271505376344086</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B13" s="6" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B14" t="s">
         <v>175</v>
       </c>
@@ -3194,27 +3239,33 @@
         <v>177</v>
       </c>
       <c r="D14" t="s">
+        <v>216</v>
+      </c>
+      <c r="E14" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>183</v>
       </c>
-      <c r="B15">
-        <v>89</v>
-      </c>
-      <c r="C15">
-        <v>584</v>
-      </c>
-      <c r="D15">
-        <v>673</v>
-      </c>
-    </row>
-    <row r="17" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D17" s="7">
+      <c r="B15" s="8">
+        <v>102</v>
+      </c>
+      <c r="C15" s="8">
+        <v>571</v>
+      </c>
+      <c r="D15" s="8">
+        <v>7</v>
+      </c>
+      <c r="E15" s="8">
+        <v>680</v>
+      </c>
+    </row>
+    <row r="17" spans="5:5" x14ac:dyDescent="0.2">
+      <c r="E17" s="7">
         <f>GETPIVOTDATA("Impact S",$A$13,"Status","Done")/GETPIVOTDATA("Impact S",$A$13)</f>
-        <v>0.13224368499257058</v>
+        <v>0.15</v>
       </c>
     </row>
   </sheetData>
@@ -3651,8 +3702,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1EB57299-5CFD-7049-BDE4-6415040FFB14}">
   <dimension ref="A1:XEX118"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
+    <sheetView topLeftCell="A11" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="34.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -9563,42 +9614,46 @@
         <v>175</v>
       </c>
     </row>
-    <row r="22" spans="1:13" ht="136" x14ac:dyDescent="0.2">
-      <c r="A22">
+    <row r="22" spans="1:13" ht="17" x14ac:dyDescent="0.2">
+      <c r="A22" s="3">
         <v>24</v>
       </c>
-      <c r="B22" t="s">
+      <c r="B22" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C22" t="s">
+      <c r="C22" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="D22" t="s">
+      <c r="D22" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="E22" s="2" t="s">
+      <c r="E22" s="4" t="s">
         <v>215</v>
       </c>
-      <c r="F22" t="s">
+      <c r="F22" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="G22" t="s">
+      <c r="G22" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="H22" t="s">
+      <c r="H22" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="I22" s="1">
+      <c r="I22" s="5">
         <f>VLOOKUP(F22,'Source lists'!$E$1:F23,2,FALSE)</f>
         <v>4</v>
       </c>
-      <c r="J22" s="1">
+      <c r="J22" s="5">
         <f>VLOOKUP(G22,'Source lists'!$H$1:I24,2,FALSE)</f>
         <v>7</v>
       </c>
-      <c r="K22" s="1">
+      <c r="K22" s="5">
         <f>VLOOKUP(F22,'Source lists'!$E$2:$F$6,2,FALSE)*(VLOOKUP(G22,'Source lists'!$H$2:$I$7,2,FALSE)^2)/VLOOKUP(H22,'Source lists'!$K$2:$L$9,2,FALSE)</f>
         <v>39.200000000000003</v>
+      </c>
+      <c r="L22" s="3"/>
+      <c r="M22" s="3" t="s">
+        <v>216</v>
       </c>
     </row>
     <row r="23" spans="1:13" ht="17" x14ac:dyDescent="0.2">
@@ -10142,7 +10197,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="37" spans="1:12" ht="34" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:12" ht="68" x14ac:dyDescent="0.2">
       <c r="A37">
         <v>58</v>
       </c>
@@ -10177,7 +10232,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="38" spans="1:12" ht="34" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:12" ht="17" x14ac:dyDescent="0.2">
       <c r="A38">
         <v>67</v>
       </c>
@@ -10212,7 +10267,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="39" spans="1:12" ht="68" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:12" ht="34" x14ac:dyDescent="0.2">
       <c r="A39">
         <v>84</v>
       </c>
@@ -10317,7 +10372,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="42" spans="1:12" ht="17" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:12" ht="34" x14ac:dyDescent="0.2">
       <c r="A42">
         <v>108</v>
       </c>
@@ -10352,7 +10407,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="43" spans="1:12" ht="34" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:12" ht="17" x14ac:dyDescent="0.2">
       <c r="A43">
         <v>109</v>
       </c>
@@ -10393,7 +10448,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="44" spans="1:12" ht="34" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:12" ht="17" x14ac:dyDescent="0.2">
       <c r="A44">
         <v>115</v>
       </c>
@@ -10510,7 +10565,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="47" spans="1:12" ht="17" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:12" ht="34" x14ac:dyDescent="0.2">
       <c r="A47">
         <v>22</v>
       </c>
@@ -10580,7 +10635,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="49" spans="1:13" ht="34" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:13" ht="68" x14ac:dyDescent="0.2">
       <c r="A49">
         <v>44</v>
       </c>
@@ -10615,7 +10670,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="50" spans="1:13" ht="68" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:13" ht="34" x14ac:dyDescent="0.2">
       <c r="A50">
         <v>48</v>
       </c>
@@ -10650,7 +10705,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="51" spans="1:13" ht="34" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="A51">
         <v>57</v>
       </c>
@@ -10723,7 +10778,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="53" spans="1:13" ht="17" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:13" ht="34" x14ac:dyDescent="0.2">
       <c r="A53">
         <v>49</v>
       </c>
@@ -10796,7 +10851,7 @@
         <v>21.333333333333332</v>
       </c>
     </row>
-    <row r="55" spans="1:13" ht="34" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:13" ht="51" x14ac:dyDescent="0.2">
       <c r="A55">
         <v>79</v>
       </c>
@@ -10901,7 +10956,7 @@
         <v>21.333333333333332</v>
       </c>
     </row>
-    <row r="58" spans="1:13" ht="51" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:13" ht="34" x14ac:dyDescent="0.2">
       <c r="A58">
         <v>87</v>
       </c>
@@ -10971,7 +11026,7 @@
         <v>21.333333333333332</v>
       </c>
     </row>
-    <row r="60" spans="1:13" ht="34" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="A60">
         <v>17</v>
       </c>
@@ -11161,7 +11216,7 @@
         <v>20.571428571428573</v>
       </c>
     </row>
-    <row r="65" spans="1:12" ht="17" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:12" ht="34" x14ac:dyDescent="0.2">
       <c r="A65">
         <v>66</v>
       </c>
@@ -11269,7 +11324,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="68" spans="1:12" ht="34" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:12" ht="17" x14ac:dyDescent="0.2">
       <c r="A68">
         <v>91</v>
       </c>
@@ -11497,7 +11552,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="74" spans="1:12" ht="17" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:12" ht="34" x14ac:dyDescent="0.2">
       <c r="A74">
         <v>97</v>
       </c>
@@ -11573,7 +11628,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="76" spans="1:12" ht="34" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:12" ht="51" x14ac:dyDescent="0.2">
       <c r="A76">
         <v>100</v>
       </c>
@@ -11611,7 +11666,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="77" spans="1:12" ht="51" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:12" ht="34" x14ac:dyDescent="0.2">
       <c r="A77">
         <v>101</v>
       </c>
@@ -11649,7 +11704,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="78" spans="1:12" ht="34" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:12" ht="51" x14ac:dyDescent="0.2">
       <c r="A78">
         <v>103</v>
       </c>
@@ -11687,7 +11742,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="79" spans="1:12" ht="51" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:12" ht="34" x14ac:dyDescent="0.2">
       <c r="A79">
         <v>104</v>
       </c>
@@ -11871,7 +11926,7 @@
         <v>13.5</v>
       </c>
     </row>
-    <row r="84" spans="1:11" ht="34" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A84">
         <v>85</v>
       </c>
@@ -12017,7 +12072,7 @@
         <v>12.8</v>
       </c>
     </row>
-    <row r="88" spans="1:11" ht="17" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:11" ht="34" x14ac:dyDescent="0.2">
       <c r="A88">
         <v>47</v>
       </c>
@@ -12128,7 +12183,7 @@
         <v>12.8</v>
       </c>
     </row>
-    <row r="91" spans="1:11" ht="34" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:11" ht="119" x14ac:dyDescent="0.2">
       <c r="A91">
         <v>41</v>
       </c>
@@ -12166,7 +12221,7 @@
         <v>12.5</v>
       </c>
     </row>
-    <row r="92" spans="1:11" ht="119" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:11" ht="68" x14ac:dyDescent="0.2">
       <c r="A92">
         <v>52</v>
       </c>
@@ -12201,7 +12256,7 @@
         <v>12.5</v>
       </c>
     </row>
-    <row r="93" spans="1:11" ht="68" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:11" ht="51" x14ac:dyDescent="0.2">
       <c r="A93">
         <v>65</v>
       </c>
@@ -12236,7 +12291,7 @@
         <v>12.5</v>
       </c>
     </row>
-    <row r="94" spans="1:11" ht="51" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:11" ht="34" x14ac:dyDescent="0.2">
       <c r="A94">
         <v>83</v>
       </c>
@@ -12271,7 +12326,7 @@
         <v>12.5</v>
       </c>
     </row>
-    <row r="95" spans="1:11" ht="34" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:11" ht="119" x14ac:dyDescent="0.2">
       <c r="A95">
         <v>102</v>
       </c>
@@ -12306,7 +12361,7 @@
         <v>12.5</v>
       </c>
     </row>
-    <row r="96" spans="1:11" ht="119" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:11" ht="68" x14ac:dyDescent="0.2">
       <c r="A96">
         <v>105</v>
       </c>
@@ -12376,7 +12431,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="98" spans="1:11" ht="68" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A98">
         <v>62</v>
       </c>
@@ -12440,7 +12495,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="100" spans="1:11" ht="17" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:11" ht="119" x14ac:dyDescent="0.2">
       <c r="A100">
         <v>82</v>
       </c>
@@ -12475,7 +12530,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="101" spans="1:11" ht="119" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:11" ht="51" x14ac:dyDescent="0.2">
       <c r="A101">
         <v>99</v>
       </c>
@@ -12510,7 +12565,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="102" spans="1:11" ht="51" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A102">
         <v>5</v>
       </c>

</xml_diff>

<commit_message>
SigmaFox/modals/sign-in: Inputs now present error on bluring
</commit_message>
<xml_diff>
--- a/apps/e-questrian/e-Questrian - To do list.xlsx
+++ b/apps/e-questrian/e-Questrian - To do list.xlsx
@@ -2,15 +2,15 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10114"/>
-  <workbookPr defaultThemeVersion="166925"/>
+  <workbookPr hidePivotFieldList="1" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rferreira/sigmafox/apps/e-questrian/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{403C0BF3-2CCA-9C4E-8AE8-6805EFED18EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD32AEA6-13FE-1440-906C-461E01E8F476}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="19820" xr2:uid="{DC2B379E-A936-2146-8C4F-53C43AECE05C}"/>
+    <workbookView xWindow="0" yWindow="740" windowWidth="34560" windowHeight="21600" activeTab="2" xr2:uid="{DC2B379E-A936-2146-8C4F-53C43AECE05C}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary of completion" sheetId="3" r:id="rId1"/>
@@ -22,7 +22,7 @@
   </definedNames>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="4" r:id="rId4"/>
+    <pivotCache cacheId="7" r:id="rId4"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="874" uniqueCount="217">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="876" uniqueCount="217">
   <si>
     <t>Sections</t>
   </si>
@@ -848,13 +848,52 @@
       <sharedItems containsBlank="1"/>
     </cacheField>
     <cacheField name="Importance S" numFmtId="43">
-      <sharedItems containsString="0" containsBlank="1" containsNumber="1" containsInteger="1" minValue="1" maxValue="10"/>
+      <sharedItems containsString="0" containsBlank="1" containsNumber="1" containsInteger="1" minValue="1" maxValue="10" count="6">
+        <n v="8"/>
+        <n v="4"/>
+        <n v="10"/>
+        <n v="1"/>
+        <n v="3"/>
+        <m/>
+      </sharedItems>
     </cacheField>
     <cacheField name="Impact S" numFmtId="43">
       <sharedItems containsString="0" containsBlank="1" containsNumber="1" containsInteger="1" minValue="1" maxValue="10"/>
     </cacheField>
     <cacheField name="Priority S" numFmtId="43">
-      <sharedItems containsString="0" containsBlank="1" containsNumber="1" minValue="0.42857142857142855" maxValue="200"/>
+      <sharedItems containsString="0" containsBlank="1" containsNumber="1" minValue="0.42857142857142855" maxValue="200" count="31">
+        <n v="200"/>
+        <n v="98"/>
+        <n v="96"/>
+        <n v="72"/>
+        <n v="64"/>
+        <n v="57.6"/>
+        <n v="53.333333333333336"/>
+        <n v="50"/>
+        <n v="42.666666666666664"/>
+        <n v="39.200000000000003"/>
+        <n v="32"/>
+        <n v="29.4"/>
+        <n v="28"/>
+        <n v="27"/>
+        <n v="21.333333333333332"/>
+        <n v="20.571428571428573"/>
+        <n v="18"/>
+        <n v="16"/>
+        <n v="14.285714285714286"/>
+        <n v="13.5"/>
+        <n v="12.8"/>
+        <n v="12.5"/>
+        <n v="10"/>
+        <n v="9.8000000000000007"/>
+        <n v="9"/>
+        <n v="7"/>
+        <n v="6.75"/>
+        <n v="2"/>
+        <n v="1.5"/>
+        <n v="0.42857142857142855"/>
+        <m/>
+      </sharedItems>
     </cacheField>
     <cacheField name="Dependency #" numFmtId="0">
       <sharedItems containsString="0" containsBlank="1" containsNumber="1" containsInteger="1" minValue="1" maxValue="103"/>
@@ -886,9 +925,9 @@
     <s v="Does not function as expected"/>
     <s v="USP"/>
     <s v="Major change to current component"/>
-    <n v="8"/>
+    <x v="0"/>
     <n v="10"/>
-    <n v="200"/>
+    <x v="0"/>
     <n v="77"/>
     <x v="0"/>
   </r>
@@ -901,9 +940,9 @@
     <s v="Poor UX"/>
     <s v="New feature"/>
     <s v="Minor change to current component"/>
-    <n v="4"/>
+    <x v="1"/>
     <n v="7"/>
-    <n v="98"/>
+    <x v="1"/>
     <n v="1"/>
     <x v="0"/>
   </r>
@@ -916,9 +955,9 @@
     <s v="Does not function as expected"/>
     <s v="Feature enhancement/fix"/>
     <s v="Investigation and change"/>
-    <n v="8"/>
+    <x v="0"/>
     <n v="6"/>
-    <n v="96"/>
+    <x v="2"/>
     <m/>
     <x v="0"/>
   </r>
@@ -931,9 +970,9 @@
     <s v="Does not function as expected"/>
     <s v="Feature enhancement/fix"/>
     <s v="Investigation and change"/>
-    <n v="8"/>
+    <x v="0"/>
     <n v="6"/>
-    <n v="96"/>
+    <x v="2"/>
     <m/>
     <x v="0"/>
   </r>
@@ -946,9 +985,9 @@
     <s v="Does not function as expected"/>
     <s v="Feature enhancement/fix"/>
     <s v="Investigation and change"/>
-    <n v="8"/>
+    <x v="0"/>
     <n v="6"/>
-    <n v="96"/>
+    <x v="2"/>
     <n v="53"/>
     <x v="0"/>
   </r>
@@ -961,9 +1000,9 @@
     <s v="Does not function as expected"/>
     <s v="Feature enhancement/fix"/>
     <s v="Investigation and change"/>
-    <n v="8"/>
+    <x v="0"/>
     <n v="6"/>
-    <n v="96"/>
+    <x v="2"/>
     <m/>
     <x v="0"/>
   </r>
@@ -976,9 +1015,9 @@
     <s v="Poor UX"/>
     <s v="Feature enhancement/fix"/>
     <s v="Minor change to current component"/>
-    <n v="4"/>
+    <x v="1"/>
     <n v="6"/>
-    <n v="72"/>
+    <x v="3"/>
     <m/>
     <x v="0"/>
   </r>
@@ -991,9 +1030,9 @@
     <s v="Poor UX"/>
     <s v="Feature enhancement/fix"/>
     <s v="Minor change to current component"/>
-    <n v="4"/>
+    <x v="1"/>
     <n v="6"/>
-    <n v="72"/>
+    <x v="3"/>
     <n v="2"/>
     <x v="0"/>
   </r>
@@ -1006,9 +1045,9 @@
     <s v="Poor UX"/>
     <s v="Improved UX"/>
     <s v="Minor tweak"/>
+    <x v="1"/>
     <n v="4"/>
-    <n v="4"/>
-    <n v="64"/>
+    <x v="4"/>
     <m/>
     <x v="0"/>
   </r>
@@ -1021,9 +1060,9 @@
     <s v="Does not function as expected"/>
     <s v="Feature enhancement/fix"/>
     <s v="New component/service with simple integration"/>
-    <n v="8"/>
+    <x v="0"/>
     <n v="6"/>
-    <n v="57.6"/>
+    <x v="5"/>
     <m/>
     <x v="0"/>
   </r>
@@ -1036,9 +1075,9 @@
     <s v="Breaks App"/>
     <s v="Improved UX"/>
     <s v="Investigation and change"/>
-    <n v="10"/>
+    <x v="2"/>
     <n v="4"/>
-    <n v="53.333333333333336"/>
+    <x v="6"/>
     <m/>
     <x v="0"/>
   </r>
@@ -1051,9 +1090,9 @@
     <s v="Nice to have"/>
     <s v="USP"/>
     <s v="Minor change to current component"/>
-    <n v="1"/>
+    <x v="3"/>
     <n v="10"/>
-    <n v="50"/>
+    <x v="7"/>
     <n v="60"/>
     <x v="1"/>
   </r>
@@ -1066,9 +1105,9 @@
     <s v="Nice to have"/>
     <s v="USP"/>
     <s v="Minor change to current component"/>
-    <n v="1"/>
+    <x v="3"/>
     <n v="10"/>
-    <n v="50"/>
+    <x v="7"/>
     <n v="62"/>
     <x v="1"/>
   </r>
@@ -1081,9 +1120,9 @@
     <s v="Nice to have"/>
     <s v="USP"/>
     <s v="Minor change to current component"/>
-    <n v="1"/>
+    <x v="3"/>
     <n v="10"/>
-    <n v="50"/>
+    <x v="7"/>
     <n v="63"/>
     <x v="1"/>
   </r>
@@ -1096,9 +1135,9 @@
     <s v="Nice to have"/>
     <s v="USP"/>
     <s v="Minor change to current component"/>
-    <n v="1"/>
+    <x v="3"/>
     <n v="10"/>
-    <n v="50"/>
+    <x v="7"/>
     <n v="61"/>
     <x v="1"/>
   </r>
@@ -1111,9 +1150,9 @@
     <s v="Does not function as expected"/>
     <s v="Improved UX"/>
     <s v="Investigation and change"/>
-    <n v="8"/>
+    <x v="0"/>
     <n v="4"/>
-    <n v="42.666666666666664"/>
+    <x v="8"/>
     <m/>
     <x v="0"/>
   </r>
@@ -1126,9 +1165,9 @@
     <s v="Poor UX"/>
     <s v="New feature"/>
     <s v="New component/service with simple integration"/>
-    <n v="4"/>
+    <x v="1"/>
     <n v="7"/>
-    <n v="39.200000000000003"/>
+    <x v="9"/>
     <m/>
     <x v="0"/>
   </r>
@@ -1141,9 +1180,9 @@
     <s v="Poor UX"/>
     <s v="New feature"/>
     <s v="New component/service with simple integration"/>
-    <n v="4"/>
+    <x v="1"/>
     <n v="7"/>
-    <n v="39.200000000000003"/>
+    <x v="9"/>
     <m/>
     <x v="0"/>
   </r>
@@ -1156,9 +1195,9 @@
     <s v="Poor UX"/>
     <s v="New feature"/>
     <s v="New component/service with simple integration"/>
-    <n v="4"/>
+    <x v="1"/>
     <n v="7"/>
-    <n v="39.200000000000003"/>
+    <x v="9"/>
     <m/>
     <x v="0"/>
   </r>
@@ -1171,9 +1210,9 @@
     <s v="Poor UX"/>
     <s v="New feature"/>
     <s v="New component/service with simple integration"/>
-    <n v="4"/>
+    <x v="1"/>
     <n v="7"/>
-    <n v="39.200000000000003"/>
+    <x v="9"/>
     <m/>
     <x v="0"/>
   </r>
@@ -1186,9 +1225,9 @@
     <s v="Poor UX"/>
     <s v="New feature"/>
     <s v="New component/service with simple integration"/>
-    <n v="4"/>
+    <x v="1"/>
     <n v="7"/>
-    <n v="39.200000000000003"/>
+    <x v="9"/>
     <m/>
     <x v="2"/>
   </r>
@@ -1201,9 +1240,9 @@
     <s v="Poor UX"/>
     <s v="Improved UX"/>
     <s v="Minor change to current component"/>
+    <x v="1"/>
     <n v="4"/>
-    <n v="4"/>
-    <n v="32"/>
+    <x v="10"/>
     <m/>
     <x v="1"/>
   </r>
@@ -1216,9 +1255,9 @@
     <s v="Poor UX"/>
     <s v="Improved UX"/>
     <s v="Minor change to current component"/>
+    <x v="1"/>
     <n v="4"/>
-    <n v="4"/>
-    <n v="32"/>
+    <x v="10"/>
     <n v="8"/>
     <x v="1"/>
   </r>
@@ -1231,9 +1270,9 @@
     <s v="Poor UX"/>
     <s v="Improved UX"/>
     <s v="Minor change to current component"/>
+    <x v="1"/>
     <n v="4"/>
-    <n v="4"/>
-    <n v="32"/>
+    <x v="10"/>
     <n v="8"/>
     <x v="1"/>
   </r>
@@ -1246,9 +1285,9 @@
     <s v="Poor UX"/>
     <s v="Improved UX"/>
     <s v="Minor change to current component"/>
+    <x v="1"/>
     <n v="4"/>
-    <n v="4"/>
-    <n v="32"/>
+    <x v="10"/>
     <n v="8"/>
     <x v="1"/>
   </r>
@@ -1261,9 +1300,9 @@
     <s v="Poor UX"/>
     <s v="Improved UX"/>
     <s v="Minor change to current component"/>
+    <x v="1"/>
     <n v="4"/>
-    <n v="4"/>
-    <n v="32"/>
+    <x v="10"/>
     <n v="8"/>
     <x v="1"/>
   </r>
@@ -1276,9 +1315,9 @@
     <s v="Poor UX"/>
     <s v="Improved UX"/>
     <s v="Minor change to current component"/>
+    <x v="1"/>
     <n v="4"/>
-    <n v="4"/>
-    <n v="32"/>
+    <x v="10"/>
     <n v="8"/>
     <x v="1"/>
   </r>
@@ -1291,9 +1330,9 @@
     <s v="Poor UX"/>
     <s v="Improved UX"/>
     <s v="Minor change to current component"/>
+    <x v="1"/>
     <n v="4"/>
-    <n v="4"/>
-    <n v="32"/>
+    <x v="10"/>
     <n v="8"/>
     <x v="1"/>
   </r>
@@ -1306,9 +1345,9 @@
     <s v="Poor UX"/>
     <s v="Improved UX"/>
     <s v="Minor change to current component"/>
+    <x v="1"/>
     <n v="4"/>
-    <n v="4"/>
-    <n v="32"/>
+    <x v="10"/>
     <n v="8"/>
     <x v="1"/>
   </r>
@@ -1321,9 +1360,9 @@
     <s v="Poor UX"/>
     <s v="Improved UX"/>
     <s v="Minor change to current component"/>
+    <x v="1"/>
     <n v="4"/>
-    <n v="4"/>
-    <n v="32"/>
+    <x v="10"/>
     <n v="8"/>
     <x v="1"/>
   </r>
@@ -1336,9 +1375,9 @@
     <s v="Poor UX"/>
     <s v="Improved UX"/>
     <s v="Minor change to current component"/>
+    <x v="1"/>
     <n v="4"/>
-    <n v="4"/>
-    <n v="32"/>
+    <x v="10"/>
     <m/>
     <x v="1"/>
   </r>
@@ -1351,9 +1390,9 @@
     <s v="Poor UX"/>
     <s v="Improved UX"/>
     <s v="Minor change to current component"/>
+    <x v="1"/>
     <n v="4"/>
-    <n v="4"/>
-    <n v="32"/>
+    <x v="10"/>
     <m/>
     <x v="1"/>
   </r>
@@ -1366,9 +1405,9 @@
     <s v="Poor UX"/>
     <s v="Improved UX"/>
     <s v="Minor change to current component"/>
+    <x v="1"/>
     <n v="4"/>
-    <n v="4"/>
-    <n v="32"/>
+    <x v="10"/>
     <m/>
     <x v="1"/>
   </r>
@@ -1381,9 +1420,9 @@
     <s v="Poor UX"/>
     <s v="Improved UX"/>
     <s v="Minor change to current component"/>
+    <x v="1"/>
     <n v="4"/>
-    <n v="4"/>
-    <n v="32"/>
+    <x v="10"/>
     <m/>
     <x v="1"/>
   </r>
@@ -1396,9 +1435,9 @@
     <s v="Poor UX"/>
     <s v="Improved UX"/>
     <s v="Minor change to current component"/>
+    <x v="1"/>
     <n v="4"/>
-    <n v="4"/>
-    <n v="32"/>
+    <x v="10"/>
     <m/>
     <x v="1"/>
   </r>
@@ -1411,9 +1450,9 @@
     <s v="Poor UX"/>
     <s v="Improved UX"/>
     <s v="Minor change to current component"/>
+    <x v="1"/>
     <n v="4"/>
-    <n v="4"/>
-    <n v="32"/>
+    <x v="10"/>
     <m/>
     <x v="1"/>
   </r>
@@ -1426,9 +1465,9 @@
     <s v="Poor UX"/>
     <s v="Improved UX"/>
     <s v="Minor change to current component"/>
+    <x v="1"/>
     <n v="4"/>
-    <n v="4"/>
-    <n v="32"/>
+    <x v="10"/>
     <m/>
     <x v="1"/>
   </r>
@@ -1441,9 +1480,9 @@
     <s v="Poor UX"/>
     <s v="Improved UX"/>
     <s v="Minor change to current component"/>
+    <x v="1"/>
     <n v="4"/>
-    <n v="4"/>
-    <n v="32"/>
+    <x v="10"/>
     <m/>
     <x v="1"/>
   </r>
@@ -1456,9 +1495,9 @@
     <s v="Poor UX"/>
     <s v="Improved UX"/>
     <s v="Minor change to current component"/>
+    <x v="1"/>
     <n v="4"/>
-    <n v="4"/>
-    <n v="32"/>
+    <x v="10"/>
     <m/>
     <x v="1"/>
   </r>
@@ -1471,9 +1510,9 @@
     <s v="Poor UX"/>
     <s v="Improved UX"/>
     <s v="Minor change to current component"/>
+    <x v="1"/>
     <n v="4"/>
-    <n v="4"/>
-    <n v="32"/>
+    <x v="10"/>
     <m/>
     <x v="1"/>
   </r>
@@ -1486,9 +1525,9 @@
     <s v="Poor UX"/>
     <s v="Improved UX"/>
     <s v="Minor change to current component"/>
+    <x v="1"/>
     <n v="4"/>
-    <n v="4"/>
-    <n v="32"/>
+    <x v="10"/>
     <m/>
     <x v="1"/>
   </r>
@@ -1501,9 +1540,9 @@
     <s v="Poor UX"/>
     <s v="Improved UX"/>
     <s v="Minor change to current component"/>
+    <x v="1"/>
     <n v="4"/>
-    <n v="4"/>
-    <n v="32"/>
+    <x v="10"/>
     <n v="8"/>
     <x v="1"/>
   </r>
@@ -1516,9 +1555,9 @@
     <s v="Poor UX"/>
     <s v="Improved UX"/>
     <s v="Minor change to current component"/>
+    <x v="1"/>
     <n v="4"/>
-    <n v="4"/>
-    <n v="32"/>
+    <x v="10"/>
     <n v="8"/>
     <x v="1"/>
   </r>
@@ -1531,9 +1570,9 @@
     <s v="Poor UI"/>
     <s v="New feature"/>
     <s v="New component/service with simple integration"/>
-    <n v="3"/>
+    <x v="4"/>
     <n v="7"/>
-    <n v="29.4"/>
+    <x v="11"/>
     <m/>
     <x v="1"/>
   </r>
@@ -1546,9 +1585,9 @@
     <s v="Poor UX"/>
     <s v="New feature"/>
     <s v="New component/service with complex integration"/>
-    <n v="4"/>
+    <x v="1"/>
     <n v="7"/>
-    <n v="28"/>
+    <x v="12"/>
     <m/>
     <x v="1"/>
   </r>
@@ -1561,9 +1600,9 @@
     <s v="Poor UI"/>
     <s v="Improved UI"/>
     <s v="Minor tweak"/>
+    <x v="4"/>
     <n v="3"/>
-    <n v="3"/>
-    <n v="27"/>
+    <x v="13"/>
     <m/>
     <x v="1"/>
   </r>
@@ -1576,9 +1615,9 @@
     <s v="Poor UI"/>
     <s v="Feature enhancement/fix"/>
     <s v="Major change to current component"/>
-    <n v="3"/>
+    <x v="4"/>
     <n v="6"/>
-    <n v="27"/>
+    <x v="13"/>
     <m/>
     <x v="1"/>
   </r>
@@ -1591,9 +1630,9 @@
     <s v="Poor UI"/>
     <s v="Feature enhancement/fix"/>
     <s v="Major change to current component"/>
-    <n v="3"/>
+    <x v="4"/>
     <n v="6"/>
-    <n v="27"/>
+    <x v="13"/>
     <m/>
     <x v="1"/>
   </r>
@@ -1606,9 +1645,9 @@
     <s v="Poor UI"/>
     <s v="Improved UI"/>
     <s v="Minor tweak"/>
+    <x v="4"/>
     <n v="3"/>
-    <n v="3"/>
-    <n v="27"/>
+    <x v="13"/>
     <m/>
     <x v="1"/>
   </r>
@@ -1621,9 +1660,9 @@
     <s v="Poor UI"/>
     <s v="Improved UI"/>
     <s v="Minor tweak"/>
+    <x v="4"/>
     <n v="3"/>
-    <n v="3"/>
-    <n v="27"/>
+    <x v="13"/>
     <m/>
     <x v="1"/>
   </r>
@@ -1636,9 +1675,9 @@
     <s v="Poor UI"/>
     <s v="Improved UI"/>
     <s v="Minor tweak"/>
+    <x v="4"/>
     <n v="3"/>
-    <n v="3"/>
-    <n v="27"/>
+    <x v="13"/>
     <m/>
     <x v="0"/>
   </r>
@@ -1651,9 +1690,9 @@
     <s v="Poor UX"/>
     <s v="Improved UX"/>
     <s v="Investigation and change"/>
+    <x v="1"/>
     <n v="4"/>
-    <n v="4"/>
-    <n v="21.333333333333332"/>
+    <x v="14"/>
     <m/>
     <x v="1"/>
   </r>
@@ -1666,9 +1705,9 @@
     <s v="Poor UX"/>
     <s v="Improved UX"/>
     <s v="Investigation and change"/>
+    <x v="1"/>
     <n v="4"/>
-    <n v="4"/>
-    <n v="21.333333333333332"/>
+    <x v="14"/>
     <m/>
     <x v="1"/>
   </r>
@@ -1681,9 +1720,9 @@
     <s v="Poor UX"/>
     <s v="Improved UX"/>
     <s v="Investigation and change"/>
+    <x v="1"/>
     <n v="4"/>
-    <n v="4"/>
-    <n v="21.333333333333332"/>
+    <x v="14"/>
     <m/>
     <x v="1"/>
   </r>
@@ -1696,9 +1735,9 @@
     <s v="Poor UX"/>
     <s v="Improved UX"/>
     <s v="Investigation and change"/>
+    <x v="1"/>
     <n v="4"/>
-    <n v="4"/>
-    <n v="21.333333333333332"/>
+    <x v="14"/>
     <m/>
     <x v="1"/>
   </r>
@@ -1711,9 +1750,9 @@
     <s v="Poor UX"/>
     <s v="Improved UX"/>
     <s v="Investigation and change"/>
+    <x v="1"/>
     <n v="4"/>
-    <n v="4"/>
-    <n v="21.333333333333332"/>
+    <x v="14"/>
     <m/>
     <x v="1"/>
   </r>
@@ -1726,9 +1765,9 @@
     <s v="Poor UX"/>
     <s v="Improved UX"/>
     <s v="Investigation and change"/>
+    <x v="1"/>
     <n v="4"/>
-    <n v="4"/>
-    <n v="21.333333333333332"/>
+    <x v="14"/>
     <m/>
     <x v="1"/>
   </r>
@@ -1741,9 +1780,9 @@
     <s v="Poor UX"/>
     <s v="Improved UX"/>
     <s v="Investigation and change"/>
+    <x v="1"/>
     <n v="4"/>
-    <n v="4"/>
-    <n v="21.333333333333332"/>
+    <x v="14"/>
     <m/>
     <x v="1"/>
   </r>
@@ -1756,9 +1795,9 @@
     <s v="Poor UX"/>
     <s v="Feature enhancement/fix"/>
     <s v="New component/service with complex integration"/>
-    <n v="4"/>
+    <x v="1"/>
     <n v="6"/>
-    <n v="20.571428571428573"/>
+    <x v="15"/>
     <m/>
     <x v="1"/>
   </r>
@@ -1771,9 +1810,9 @@
     <s v="Poor UX"/>
     <s v="Feature enhancement/fix"/>
     <s v="New component/service with complex integration"/>
-    <n v="4"/>
+    <x v="1"/>
     <n v="6"/>
-    <n v="20.571428571428573"/>
+    <x v="15"/>
     <m/>
     <x v="1"/>
   </r>
@@ -1786,9 +1825,9 @@
     <s v="Poor UX"/>
     <s v="Feature enhancement/fix"/>
     <s v="New component/service with complex integration"/>
-    <n v="4"/>
+    <x v="1"/>
     <n v="6"/>
-    <n v="20.571428571428573"/>
+    <x v="15"/>
     <m/>
     <x v="1"/>
   </r>
@@ -1801,9 +1840,9 @@
     <s v="Poor UX"/>
     <s v="Feature enhancement/fix"/>
     <s v="New component/service with complex integration"/>
-    <n v="4"/>
+    <x v="1"/>
     <n v="6"/>
-    <n v="20.571428571428573"/>
+    <x v="15"/>
     <m/>
     <x v="1"/>
   </r>
@@ -1816,9 +1855,9 @@
     <s v="Poor UX"/>
     <s v="Feature enhancement/fix"/>
     <s v="New component/service with complex integration"/>
-    <n v="4"/>
+    <x v="1"/>
     <n v="6"/>
-    <n v="20.571428571428573"/>
+    <x v="15"/>
     <m/>
     <x v="1"/>
   </r>
@@ -1831,9 +1870,9 @@
     <s v="Nice to have"/>
     <s v="Feature enhancement/fix"/>
     <s v="Minor change to current component"/>
-    <n v="1"/>
+    <x v="3"/>
     <n v="6"/>
-    <n v="18"/>
+    <x v="16"/>
     <m/>
     <x v="1"/>
   </r>
@@ -1846,9 +1885,9 @@
     <s v="Nice to have"/>
     <s v="Feature enhancement/fix"/>
     <s v="Minor change to current component"/>
-    <n v="1"/>
+    <x v="3"/>
     <n v="6"/>
-    <n v="18"/>
+    <x v="16"/>
     <m/>
     <x v="1"/>
   </r>
@@ -1861,9 +1900,9 @@
     <s v="Poor UX"/>
     <s v="Improved UX"/>
     <s v="Major change to current component"/>
+    <x v="1"/>
     <n v="4"/>
-    <n v="4"/>
-    <n v="16"/>
+    <x v="17"/>
     <m/>
     <x v="1"/>
   </r>
@@ -1876,9 +1915,9 @@
     <s v="Nice to have"/>
     <s v="USP"/>
     <s v="New component/service with complex integration"/>
-    <n v="1"/>
+    <x v="3"/>
     <n v="10"/>
-    <n v="14.285714285714286"/>
+    <x v="18"/>
     <n v="59"/>
     <x v="1"/>
   </r>
@@ -1891,9 +1930,9 @@
     <s v="Nice to have"/>
     <s v="USP"/>
     <s v="New component/service with complex integration"/>
-    <n v="1"/>
+    <x v="3"/>
     <n v="10"/>
-    <n v="14.285714285714286"/>
+    <x v="18"/>
     <n v="64"/>
     <x v="1"/>
   </r>
@@ -1906,9 +1945,9 @@
     <s v="Nice to have"/>
     <s v="USP"/>
     <s v="New component/service with complex integration"/>
-    <n v="1"/>
+    <x v="3"/>
     <n v="10"/>
-    <n v="14.285714285714286"/>
+    <x v="18"/>
     <n v="59"/>
     <x v="1"/>
   </r>
@@ -1921,9 +1960,9 @@
     <s v="Nice to have"/>
     <s v="USP"/>
     <s v="New component/service with complex integration"/>
-    <n v="1"/>
+    <x v="3"/>
     <n v="10"/>
-    <n v="14.285714285714286"/>
+    <x v="18"/>
     <n v="64"/>
     <x v="1"/>
   </r>
@@ -1936,9 +1975,9 @@
     <s v="Nice to have"/>
     <s v="USP"/>
     <s v="New component/service with complex integration"/>
-    <n v="1"/>
+    <x v="3"/>
     <n v="10"/>
-    <n v="14.285714285714286"/>
+    <x v="18"/>
     <n v="59"/>
     <x v="1"/>
   </r>
@@ -1951,9 +1990,9 @@
     <s v="Nice to have"/>
     <s v="USP"/>
     <s v="New component/service with complex integration"/>
-    <n v="1"/>
+    <x v="3"/>
     <n v="10"/>
-    <n v="14.285714285714286"/>
+    <x v="18"/>
     <n v="64"/>
     <x v="1"/>
   </r>
@@ -1966,9 +2005,9 @@
     <s v="Nice to have"/>
     <s v="USP"/>
     <s v="New component/service with complex integration"/>
-    <n v="1"/>
+    <x v="3"/>
     <n v="10"/>
-    <n v="14.285714285714286"/>
+    <x v="18"/>
     <n v="59"/>
     <x v="1"/>
   </r>
@@ -1981,9 +2020,9 @@
     <s v="Nice to have"/>
     <s v="USP"/>
     <s v="New component/service with complex integration"/>
-    <n v="1"/>
+    <x v="3"/>
     <n v="10"/>
-    <n v="14.285714285714286"/>
+    <x v="18"/>
     <n v="64"/>
     <x v="1"/>
   </r>
@@ -1996,9 +2035,9 @@
     <s v="Nice to have"/>
     <s v="USP"/>
     <s v="New component/service with complex integration"/>
-    <n v="1"/>
+    <x v="3"/>
     <n v="10"/>
-    <n v="14.285714285714286"/>
+    <x v="18"/>
     <n v="99"/>
     <x v="1"/>
   </r>
@@ -2011,9 +2050,9 @@
     <s v="Nice to have"/>
     <s v="USP"/>
     <s v="New component/service with complex integration"/>
-    <n v="1"/>
+    <x v="3"/>
     <n v="10"/>
-    <n v="14.285714285714286"/>
+    <x v="18"/>
     <n v="100"/>
     <x v="1"/>
   </r>
@@ -2026,9 +2065,9 @@
     <s v="Nice to have"/>
     <s v="USP"/>
     <s v="New component/service with complex integration"/>
-    <n v="1"/>
+    <x v="3"/>
     <n v="10"/>
-    <n v="14.285714285714286"/>
+    <x v="18"/>
     <n v="102"/>
     <x v="1"/>
   </r>
@@ -2041,9 +2080,9 @@
     <s v="Nice to have"/>
     <s v="USP"/>
     <s v="New component/service with complex integration"/>
-    <n v="1"/>
+    <x v="3"/>
     <n v="10"/>
-    <n v="14.285714285714286"/>
+    <x v="18"/>
     <n v="103"/>
     <x v="1"/>
   </r>
@@ -2056,9 +2095,9 @@
     <s v="Poor UI"/>
     <s v="Improved UI"/>
     <s v="Minor change to current component"/>
+    <x v="4"/>
     <n v="3"/>
-    <n v="3"/>
-    <n v="13.5"/>
+    <x v="19"/>
     <m/>
     <x v="1"/>
   </r>
@@ -2071,9 +2110,9 @@
     <s v="Poor UI"/>
     <s v="Improved UI"/>
     <s v="Minor change to current component"/>
+    <x v="4"/>
     <n v="3"/>
-    <n v="3"/>
-    <n v="13.5"/>
+    <x v="19"/>
     <m/>
     <x v="1"/>
   </r>
@@ -2086,9 +2125,9 @@
     <s v="Poor UI"/>
     <s v="Improved UI"/>
     <s v="Minor change to current component"/>
+    <x v="4"/>
     <n v="3"/>
-    <n v="3"/>
-    <n v="13.5"/>
+    <x v="19"/>
     <m/>
     <x v="1"/>
   </r>
@@ -2101,9 +2140,9 @@
     <s v="Poor UI"/>
     <s v="Improved UI"/>
     <s v="Minor change to current component"/>
+    <x v="4"/>
     <n v="3"/>
-    <n v="3"/>
-    <n v="13.5"/>
+    <x v="19"/>
     <m/>
     <x v="1"/>
   </r>
@@ -2116,9 +2155,9 @@
     <s v="Poor UI"/>
     <s v="Improved UI"/>
     <s v="Minor change to current component"/>
+    <x v="4"/>
     <n v="3"/>
-    <n v="3"/>
-    <n v="13.5"/>
+    <x v="19"/>
     <m/>
     <x v="1"/>
   </r>
@@ -2131,9 +2170,9 @@
     <s v="Poor UI"/>
     <s v="Improved UI"/>
     <s v="Minor change to current component"/>
+    <x v="4"/>
     <n v="3"/>
-    <n v="3"/>
-    <n v="13.5"/>
+    <x v="19"/>
     <m/>
     <x v="1"/>
   </r>
@@ -2146,9 +2185,9 @@
     <s v="Poor UX"/>
     <s v="Improved UX"/>
     <s v="New component/service with simple integration"/>
+    <x v="1"/>
     <n v="4"/>
-    <n v="4"/>
-    <n v="12.8"/>
+    <x v="20"/>
     <m/>
     <x v="1"/>
   </r>
@@ -2161,9 +2200,9 @@
     <s v="Poor UX"/>
     <s v="Improved UX"/>
     <s v="New component/service with simple integration"/>
+    <x v="1"/>
     <n v="4"/>
-    <n v="4"/>
-    <n v="12.8"/>
+    <x v="20"/>
     <m/>
     <x v="1"/>
   </r>
@@ -2176,9 +2215,9 @@
     <s v="Poor UX"/>
     <s v="Improved UX"/>
     <s v="New component/service with simple integration"/>
+    <x v="1"/>
     <n v="4"/>
-    <n v="4"/>
-    <n v="12.8"/>
+    <x v="20"/>
     <m/>
     <x v="1"/>
   </r>
@@ -2191,9 +2230,9 @@
     <s v="Poor UX"/>
     <s v="Improved UX"/>
     <s v="New component/service with simple integration"/>
+    <x v="1"/>
     <n v="4"/>
-    <n v="4"/>
-    <n v="12.8"/>
+    <x v="20"/>
     <m/>
     <x v="1"/>
   </r>
@@ -2206,9 +2245,9 @@
     <s v="Poor UX"/>
     <s v="Improved UX"/>
     <s v="New component/service with simple integration"/>
+    <x v="1"/>
     <n v="4"/>
-    <n v="4"/>
-    <n v="12.8"/>
+    <x v="20"/>
     <m/>
     <x v="1"/>
   </r>
@@ -2221,9 +2260,9 @@
     <s v="Nice to have"/>
     <s v="USP"/>
     <s v="Whole new feature"/>
-    <n v="1"/>
+    <x v="3"/>
     <n v="10"/>
-    <n v="12.5"/>
+    <x v="21"/>
     <m/>
     <x v="1"/>
   </r>
@@ -2236,9 +2275,9 @@
     <s v="Nice to have"/>
     <s v="USP"/>
     <s v="Whole new feature"/>
-    <n v="1"/>
+    <x v="3"/>
     <n v="10"/>
-    <n v="12.5"/>
+    <x v="21"/>
     <m/>
     <x v="1"/>
   </r>
@@ -2251,9 +2290,9 @@
     <s v="Nice to have"/>
     <s v="USP"/>
     <s v="Whole new feature"/>
-    <n v="1"/>
+    <x v="3"/>
     <n v="10"/>
-    <n v="12.5"/>
+    <x v="21"/>
     <m/>
     <x v="1"/>
   </r>
@@ -2266,9 +2305,9 @@
     <s v="Nice to have"/>
     <s v="USP"/>
     <s v="Whole new feature"/>
-    <n v="1"/>
+    <x v="3"/>
     <n v="10"/>
-    <n v="12.5"/>
+    <x v="21"/>
     <m/>
     <x v="1"/>
   </r>
@@ -2281,9 +2320,9 @@
     <s v="Nice to have"/>
     <s v="USP"/>
     <s v="Whole new feature"/>
-    <n v="1"/>
+    <x v="3"/>
     <n v="10"/>
-    <n v="12.5"/>
+    <x v="21"/>
     <m/>
     <x v="1"/>
   </r>
@@ -2296,9 +2335,9 @@
     <s v="Nice to have"/>
     <s v="USP"/>
     <s v="Whole new feature"/>
-    <n v="1"/>
+    <x v="3"/>
     <n v="10"/>
-    <n v="12.5"/>
+    <x v="21"/>
     <m/>
     <x v="1"/>
   </r>
@@ -2311,9 +2350,9 @@
     <s v="Nice to have"/>
     <s v="USP"/>
     <s v="Whole new section"/>
-    <n v="1"/>
+    <x v="3"/>
     <n v="10"/>
-    <n v="10"/>
+    <x v="22"/>
     <m/>
     <x v="1"/>
   </r>
@@ -2326,9 +2365,9 @@
     <s v="Nice to have"/>
     <s v="USP"/>
     <s v="Whole new section"/>
-    <n v="1"/>
+    <x v="3"/>
     <n v="10"/>
-    <n v="10"/>
+    <x v="22"/>
     <m/>
     <x v="1"/>
   </r>
@@ -2341,9 +2380,9 @@
     <s v="Nice to have"/>
     <s v="USP"/>
     <s v="Whole new section"/>
-    <n v="1"/>
+    <x v="3"/>
     <n v="10"/>
-    <n v="10"/>
+    <x v="22"/>
     <m/>
     <x v="1"/>
   </r>
@@ -2356,9 +2395,9 @@
     <s v="Nice to have"/>
     <s v="USP"/>
     <s v="Whole new section"/>
-    <n v="1"/>
+    <x v="3"/>
     <n v="10"/>
-    <n v="10"/>
+    <x v="22"/>
     <m/>
     <x v="1"/>
   </r>
@@ -2371,9 +2410,9 @@
     <s v="Nice to have"/>
     <s v="USP"/>
     <s v="Whole new section"/>
-    <n v="1"/>
+    <x v="3"/>
     <n v="10"/>
-    <n v="10"/>
+    <x v="22"/>
     <m/>
     <x v="1"/>
   </r>
@@ -2386,9 +2425,9 @@
     <s v="Nice to have"/>
     <s v="New feature"/>
     <s v="New component/service with simple integration"/>
-    <n v="1"/>
+    <x v="3"/>
     <n v="7"/>
-    <n v="9.8000000000000007"/>
+    <x v="23"/>
     <m/>
     <x v="1"/>
   </r>
@@ -2401,9 +2440,9 @@
     <s v="Poor UI"/>
     <s v="Improved UI"/>
     <s v="Investigation and change"/>
+    <x v="4"/>
     <n v="3"/>
-    <n v="3"/>
-    <n v="9"/>
+    <x v="24"/>
     <m/>
     <x v="1"/>
   </r>
@@ -2416,9 +2455,9 @@
     <s v="Poor UI"/>
     <s v="Improved UI"/>
     <s v="Investigation and change"/>
+    <x v="4"/>
     <n v="3"/>
-    <n v="3"/>
-    <n v="9"/>
+    <x v="24"/>
     <m/>
     <x v="1"/>
   </r>
@@ -2431,9 +2470,9 @@
     <s v="Poor UI"/>
     <s v="Improved UI"/>
     <s v="Investigation and change"/>
+    <x v="4"/>
     <n v="3"/>
-    <n v="3"/>
-    <n v="9"/>
+    <x v="24"/>
     <m/>
     <x v="1"/>
   </r>
@@ -2446,9 +2485,9 @@
     <s v="Poor UI"/>
     <s v="Improved UI"/>
     <s v="Investigation and change"/>
+    <x v="4"/>
     <n v="3"/>
-    <n v="3"/>
-    <n v="9"/>
+    <x v="24"/>
     <m/>
     <x v="1"/>
   </r>
@@ -2461,9 +2500,9 @@
     <s v="Nice to have"/>
     <s v="Feature enhancement/fix"/>
     <s v="Major change to current component"/>
-    <n v="1"/>
+    <x v="3"/>
     <n v="6"/>
-    <n v="9"/>
+    <x v="24"/>
     <m/>
     <x v="1"/>
   </r>
@@ -2476,9 +2515,9 @@
     <s v="Nice to have"/>
     <s v="Feature enhancement/fix"/>
     <s v="Major change to current component"/>
-    <n v="1"/>
+    <x v="3"/>
     <n v="6"/>
-    <n v="9"/>
+    <x v="24"/>
     <m/>
     <x v="1"/>
   </r>
@@ -2491,9 +2530,9 @@
     <s v="Nice to have"/>
     <s v="Feature enhancement/fix"/>
     <s v="Major change to current component"/>
-    <n v="1"/>
+    <x v="3"/>
     <n v="6"/>
-    <n v="9"/>
+    <x v="24"/>
     <m/>
     <x v="1"/>
   </r>
@@ -2506,9 +2545,9 @@
     <s v="Nice to have"/>
     <s v="Feature enhancement/fix"/>
     <s v="Major change to current component"/>
-    <n v="1"/>
+    <x v="3"/>
     <n v="6"/>
-    <n v="9"/>
+    <x v="24"/>
     <m/>
     <x v="1"/>
   </r>
@@ -2521,9 +2560,9 @@
     <s v="Nice to have"/>
     <s v="Feature enhancement/fix"/>
     <s v="Major change to current component"/>
-    <n v="1"/>
+    <x v="3"/>
     <n v="6"/>
-    <n v="9"/>
+    <x v="24"/>
     <m/>
     <x v="1"/>
   </r>
@@ -2536,9 +2575,9 @@
     <s v="Poor UI"/>
     <s v="Improved UI"/>
     <s v="Investigation and change"/>
+    <x v="4"/>
     <n v="3"/>
-    <n v="3"/>
-    <n v="9"/>
+    <x v="24"/>
     <m/>
     <x v="1"/>
   </r>
@@ -2551,9 +2590,9 @@
     <s v="Nice to have"/>
     <s v="New feature"/>
     <s v="New component/service with complex integration"/>
-    <n v="1"/>
+    <x v="3"/>
     <n v="7"/>
-    <n v="7"/>
+    <x v="25"/>
     <m/>
     <x v="1"/>
   </r>
@@ -2566,9 +2605,9 @@
     <s v="Poor UI"/>
     <s v="Improved UI"/>
     <s v="Major change to current component"/>
+    <x v="4"/>
     <n v="3"/>
-    <n v="3"/>
-    <n v="6.75"/>
+    <x v="26"/>
     <m/>
     <x v="1"/>
   </r>
@@ -2581,9 +2620,9 @@
     <s v="Poor UX"/>
     <s v="Refactor/Tech debt"/>
     <s v="Minor change to current component"/>
-    <n v="4"/>
+    <x v="1"/>
     <n v="1"/>
-    <n v="2"/>
+    <x v="27"/>
     <m/>
     <x v="1"/>
   </r>
@@ -2596,9 +2635,9 @@
     <s v="Poor UI"/>
     <s v="Refactor/Tech debt"/>
     <s v="Minor change to current component"/>
-    <n v="3"/>
+    <x v="4"/>
     <n v="1"/>
-    <n v="1.5"/>
+    <x v="28"/>
     <n v="27"/>
     <x v="1"/>
   </r>
@@ -2611,9 +2650,9 @@
     <s v="Poor UI"/>
     <s v="Refactor/Tech debt"/>
     <s v="Minor change to current component"/>
-    <n v="3"/>
+    <x v="4"/>
     <n v="1"/>
-    <n v="1.5"/>
+    <x v="28"/>
     <n v="27"/>
     <x v="1"/>
   </r>
@@ -2626,9 +2665,9 @@
     <s v="Poor UI"/>
     <s v="Refactor/Tech debt"/>
     <s v="New component/service with complex integration"/>
-    <n v="3"/>
+    <x v="4"/>
     <n v="1"/>
-    <n v="0.42857142857142855"/>
+    <x v="29"/>
     <m/>
     <x v="1"/>
   </r>
@@ -2641,9 +2680,9 @@
     <m/>
     <m/>
     <m/>
-    <m/>
-    <m/>
-    <m/>
+    <x v="5"/>
+    <m/>
+    <x v="30"/>
     <m/>
     <x v="1"/>
   </r>
@@ -2651,7 +2690,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{936C0618-B7B4-0144-93D9-409C5361BBD7}" name="PivotTable7" cacheId="4" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{936C0618-B7B4-0144-93D9-409C5361BBD7}" name="PivotTable7" cacheId="7" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A7:E9" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="13">
     <pivotField showAll="0"/>
@@ -2666,11 +2705,11 @@
     <pivotField showAll="0"/>
     <pivotField showAll="0"/>
     <pivotField showAll="0"/>
-    <pivotField axis="axisCol" showAll="0">
+    <pivotField axis="axisCol" showAll="0" sortType="ascending">
       <items count="4">
         <item x="0"/>
+        <item x="2"/>
         <item x="1"/>
-        <item x="2"/>
         <item t="default"/>
       </items>
     </pivotField>
@@ -2711,7 +2750,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{4A183E6E-2837-3A40-90CB-E731BF47E9C0}" name="PivotTable6" cacheId="4" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{4A183E6E-2837-3A40-90CB-E731BF47E9C0}" name="PivotTable6" cacheId="7" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A1:E3" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="13">
     <pivotField showAll="0"/>
@@ -2726,11 +2765,11 @@
     <pivotField showAll="0"/>
     <pivotField dataField="1" showAll="0"/>
     <pivotField showAll="0"/>
-    <pivotField axis="axisCol" showAll="0">
+    <pivotField axis="axisCol" showAll="0" sortType="ascending">
       <items count="4">
         <item x="0"/>
+        <item x="2"/>
         <item x="1"/>
-        <item x="2"/>
         <item t="default"/>
       </items>
     </pivotField>
@@ -2771,7 +2810,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{4DCC3165-0959-AA43-80CF-D9170B1DCB64}" name="PivotTable8" cacheId="4" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{4DCC3165-0959-AA43-80CF-D9170B1DCB64}" name="PivotTable8" cacheId="7" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A13:E15" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="13">
     <pivotField showAll="0"/>
@@ -2786,11 +2825,11 @@
     <pivotField dataField="1" showAll="0"/>
     <pivotField showAll="0"/>
     <pivotField showAll="0"/>
-    <pivotField axis="axisCol" showAll="0">
+    <pivotField axis="axisCol" showAll="0" sortType="ascending">
       <items count="4">
         <item x="0"/>
+        <item x="2"/>
         <item x="1"/>
-        <item x="2"/>
         <item t="default"/>
       </items>
     </pivotField>
@@ -3129,16 +3168,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{37CCC35A-14FA-1E40-8319-0349AC17C33D}">
   <dimension ref="A1:E17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="14.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="4.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="10.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -3146,16 +3185,18 @@
       <c r="B1" s="6" t="s">
         <v>176</v>
       </c>
+      <c r="C1"/>
+      <c r="D1"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B2" t="s">
         <v>175</v>
       </c>
       <c r="C2" t="s">
+        <v>216</v>
+      </c>
+      <c r="D2" t="s">
         <v>177</v>
-      </c>
-      <c r="D2" t="s">
-        <v>216</v>
       </c>
       <c r="E2" t="s">
         <v>178</v>
@@ -3169,35 +3210,37 @@
         <v>1227.4000000000003</v>
       </c>
       <c r="C3" s="8">
+        <v>39.200000000000003</v>
+      </c>
+      <c r="D3" s="8">
         <v>1960.9976190476179</v>
       </c>
-      <c r="D3" s="8">
-        <v>39.200000000000003</v>
-      </c>
       <c r="E3" s="8">
-        <v>3227.5976190476181</v>
+        <v>3227.5976190476185</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="E5" s="7">
-        <f>GETPIVOTDATA("Priority S",$A$1,"Status","Done")/GETPIVOTDATA("Priority S",$A$1)</f>
-        <v>0.38028284342401231</v>
+        <f>SUM(B3:C3)/GETPIVOTDATA("Priority S",$A$1)</f>
+        <v>0.39242809962591979</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B7" s="6" t="s">
         <v>176</v>
       </c>
+      <c r="C7"/>
+      <c r="D7"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B8" t="s">
         <v>175</v>
       </c>
       <c r="C8" t="s">
+        <v>216</v>
+      </c>
+      <c r="D8" t="s">
         <v>177</v>
-      </c>
-      <c r="D8" t="s">
-        <v>216</v>
       </c>
       <c r="E8" t="s">
         <v>178</v>
@@ -3211,10 +3254,10 @@
         <v>101</v>
       </c>
       <c r="C9" s="8">
+        <v>4</v>
+      </c>
+      <c r="D9" s="8">
         <v>267</v>
-      </c>
-      <c r="D9" s="8">
-        <v>4</v>
       </c>
       <c r="E9" s="8">
         <v>372</v>
@@ -3222,24 +3265,26 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="E11" s="7">
-        <f>GETPIVOTDATA("Importance S",$A$7,"Status","Done")/GETPIVOTDATA("Importance S",$A$7)</f>
-        <v>0.271505376344086</v>
+        <f>SUM(B9:C9)/GETPIVOTDATA("Importance S",$A$7)</f>
+        <v>0.28225806451612906</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B13" s="6" t="s">
         <v>176</v>
       </c>
+      <c r="C13"/>
+      <c r="D13"/>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B14" t="s">
         <v>175</v>
       </c>
       <c r="C14" t="s">
+        <v>216</v>
+      </c>
+      <c r="D14" t="s">
         <v>177</v>
-      </c>
-      <c r="D14" t="s">
-        <v>216</v>
       </c>
       <c r="E14" t="s">
         <v>178</v>
@@ -3253,10 +3298,10 @@
         <v>102</v>
       </c>
       <c r="C15" s="8">
+        <v>7</v>
+      </c>
+      <c r="D15" s="8">
         <v>571</v>
-      </c>
-      <c r="D15" s="8">
-        <v>7</v>
       </c>
       <c r="E15" s="8">
         <v>680</v>
@@ -3264,8 +3309,8 @@
     </row>
     <row r="17" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E17" s="7">
-        <f>GETPIVOTDATA("Impact S",$A$13,"Status","Done")/GETPIVOTDATA("Impact S",$A$13)</f>
-        <v>0.15</v>
+        <f>SUM(B15:C15)/GETPIVOTDATA("Impact S",$A$13)</f>
+        <v>0.16029411764705884</v>
       </c>
     </row>
   </sheetData>
@@ -3702,8 +3747,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1EB57299-5CFD-7049-BDE4-6415040FFB14}">
   <dimension ref="A1:XEX118"/>
   <sheetViews>
-    <sheetView topLeftCell="A11" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+    <sheetView tabSelected="1" topLeftCell="A12" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="E25" sqref="E25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="34.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4053,7 +4098,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="9" spans="1:2046 2050:3066 3073:4093 4100:5120 5127:6141 6145:7168 7172:8188 8195:9215 9222:11263 11267:12283 12290:13310 13317:15358 15362:16378" ht="17" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:2046 2050:3066 3073:4093 4100:5120 5127:6141 6145:7168 7172:8188 8195:9215 9222:11263 11267:12283 12290:13310 13317:15358 15362:16378" ht="34" x14ac:dyDescent="0.2">
       <c r="A9" s="3">
         <v>116</v>
       </c>
@@ -9614,7 +9659,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="22" spans="1:13" ht="17" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:13" ht="136" x14ac:dyDescent="0.2">
       <c r="A22" s="3">
         <v>24</v>
       </c>
@@ -9656,83 +9701,91 @@
         <v>216</v>
       </c>
     </row>
-    <row r="23" spans="1:13" ht="17" x14ac:dyDescent="0.2">
-      <c r="A23">
+    <row r="23" spans="1:13" ht="34" x14ac:dyDescent="0.2">
+      <c r="A23" s="3">
         <v>7</v>
       </c>
-      <c r="B23" t="s">
+      <c r="B23" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C23" t="s">
+      <c r="C23" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="E23" s="2" t="s">
+      <c r="D23" s="3"/>
+      <c r="E23" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="F23" t="s">
+      <c r="F23" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="G23" t="s">
+      <c r="G23" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="H23" t="s">
+      <c r="H23" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="I23" s="1">
+      <c r="I23" s="5">
         <f>VLOOKUP(F23,'Source lists'!$E$1:F24,2,FALSE)</f>
         <v>4</v>
       </c>
-      <c r="J23" s="1">
+      <c r="J23" s="5">
         <f>VLOOKUP(G23,'Source lists'!$H$1:I25,2,FALSE)</f>
         <v>4</v>
       </c>
-      <c r="K23" s="1">
+      <c r="K23" s="5">
         <f>VLOOKUP(F23,'Source lists'!$E$2:$F$6,2,FALSE)*(VLOOKUP(G23,'Source lists'!$H$2:$I$7,2,FALSE)^2)/VLOOKUP(H23,'Source lists'!$K$2:$L$9,2,FALSE)</f>
         <v>32</v>
       </c>
-    </row>
-    <row r="24" spans="1:13" ht="136" x14ac:dyDescent="0.2">
-      <c r="A24">
+      <c r="L23" s="3"/>
+      <c r="M23" s="3" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" ht="17" x14ac:dyDescent="0.2">
+      <c r="A24" s="3">
         <v>9</v>
       </c>
-      <c r="B24" t="s">
+      <c r="B24" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C24" t="s">
+      <c r="C24" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="D24" t="s">
+      <c r="D24" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="E24" s="2" t="s">
+      <c r="E24" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="F24" t="s">
+      <c r="F24" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="G24" t="s">
+      <c r="G24" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="H24" t="s">
+      <c r="H24" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="I24" s="1">
+      <c r="I24" s="5">
         <f>VLOOKUP(F24,'Source lists'!$E$1:F25,2,FALSE)</f>
         <v>4</v>
       </c>
-      <c r="J24" s="1">
+      <c r="J24" s="5">
         <f>VLOOKUP(G24,'Source lists'!$H$1:I26,2,FALSE)</f>
         <v>4</v>
       </c>
-      <c r="K24" s="1">
+      <c r="K24" s="5">
         <f>VLOOKUP(F24,'Source lists'!$E$2:$F$6,2,FALSE)*(VLOOKUP(G24,'Source lists'!$H$2:$I$7,2,FALSE)^2)/VLOOKUP(H24,'Source lists'!$K$2:$L$9,2,FALSE)</f>
         <v>32</v>
       </c>
-      <c r="L24">
+      <c r="L24" s="3">
         <v>8</v>
       </c>
-    </row>
-    <row r="25" spans="1:13" ht="34" x14ac:dyDescent="0.2">
+      <c r="M24" s="3" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>10</v>
       </c>
@@ -10054,7 +10107,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="33" spans="1:12" ht="17" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:12" ht="34" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>31</v>
       </c>

</xml_diff>

<commit_message>
SigmaFireFox/modals/dynamic: DynamicModal now built and SignInModal now built using it
</commit_message>
<xml_diff>
--- a/apps/e-questrian/e-Questrian - To do list.xlsx
+++ b/apps/e-questrian/e-Questrian - To do list.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rferreira/sigmafox/apps/e-questrian/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD32AEA6-13FE-1440-906C-461E01E8F476}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD40BD0B-D06A-F04D-AB96-0A1A9BD8C790}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="740" windowWidth="34560" windowHeight="21600" activeTab="2" xr2:uid="{DC2B379E-A936-2146-8C4F-53C43AECE05C}"/>
   </bookViews>
@@ -22,7 +22,7 @@
   </definedNames>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="7" r:id="rId4"/>
+    <pivotCache cacheId="0" r:id="rId4"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="876" uniqueCount="217">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="879" uniqueCount="217">
   <si>
     <t>Sections</t>
   </si>
@@ -784,7 +784,7 @@
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -797,7 +797,6 @@
     <xf numFmtId="43" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -2690,7 +2689,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{936C0618-B7B4-0144-93D9-409C5361BBD7}" name="PivotTable7" cacheId="7" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{936C0618-B7B4-0144-93D9-409C5361BBD7}" name="PivotTable7" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A7:E9" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="13">
     <pivotField showAll="0"/>
@@ -2750,7 +2749,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{4A183E6E-2837-3A40-90CB-E731BF47E9C0}" name="PivotTable6" cacheId="7" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{4A183E6E-2837-3A40-90CB-E731BF47E9C0}" name="PivotTable6" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A1:E3" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="13">
     <pivotField showAll="0"/>
@@ -2810,7 +2809,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{4DCC3165-0959-AA43-80CF-D9170B1DCB64}" name="PivotTable8" cacheId="7" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{4DCC3165-0959-AA43-80CF-D9170B1DCB64}" name="PivotTable8" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A13:E15" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="13">
     <pivotField showAll="0"/>
@@ -3206,16 +3205,16 @@
       <c r="A3" t="s">
         <v>205</v>
       </c>
-      <c r="B3" s="8">
+      <c r="B3">
         <v>1227.4000000000003</v>
       </c>
-      <c r="C3" s="8">
+      <c r="C3">
         <v>39.200000000000003</v>
       </c>
-      <c r="D3" s="8">
+      <c r="D3">
         <v>1960.9976190476179</v>
       </c>
-      <c r="E3" s="8">
+      <c r="E3">
         <v>3227.5976190476185</v>
       </c>
     </row>
@@ -3250,16 +3249,16 @@
       <c r="A9" t="s">
         <v>182</v>
       </c>
-      <c r="B9" s="8">
+      <c r="B9">
         <v>101</v>
       </c>
-      <c r="C9" s="8">
+      <c r="C9">
         <v>4</v>
       </c>
-      <c r="D9" s="8">
+      <c r="D9">
         <v>267</v>
       </c>
-      <c r="E9" s="8">
+      <c r="E9">
         <v>372</v>
       </c>
     </row>
@@ -3294,16 +3293,16 @@
       <c r="A15" t="s">
         <v>183</v>
       </c>
-      <c r="B15" s="8">
+      <c r="B15">
         <v>102</v>
       </c>
-      <c r="C15" s="8">
+      <c r="C15">
         <v>7</v>
       </c>
-      <c r="D15" s="8">
+      <c r="D15">
         <v>571</v>
       </c>
-      <c r="E15" s="8">
+      <c r="E15">
         <v>680</v>
       </c>
     </row>
@@ -3747,8 +3746,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1EB57299-5CFD-7049-BDE4-6415040FFB14}">
   <dimension ref="A1:XEX118"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="E25" sqref="E25"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="M27" sqref="M27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="34.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -9786,126 +9785,135 @@
       </c>
     </row>
     <row r="25" spans="1:13" ht="17" x14ac:dyDescent="0.2">
-      <c r="A25">
+      <c r="A25" s="3">
         <v>10</v>
       </c>
-      <c r="B25" t="s">
+      <c r="B25" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C25" t="s">
+      <c r="C25" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="D25" t="s">
+      <c r="D25" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="E25" s="2" t="s">
+      <c r="E25" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="F25" t="s">
+      <c r="F25" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="G25" t="s">
+      <c r="G25" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="H25" t="s">
+      <c r="H25" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="I25" s="1">
+      <c r="I25" s="5">
         <f>VLOOKUP(F25,'Source lists'!$E$1:F26,2,FALSE)</f>
         <v>4</v>
       </c>
-      <c r="J25" s="1">
+      <c r="J25" s="5">
         <f>VLOOKUP(G25,'Source lists'!$H$1:I27,2,FALSE)</f>
         <v>4</v>
       </c>
-      <c r="K25" s="1">
+      <c r="K25" s="5">
         <f>VLOOKUP(F25,'Source lists'!$E$2:$F$6,2,FALSE)*(VLOOKUP(G25,'Source lists'!$H$2:$I$7,2,FALSE)^2)/VLOOKUP(H25,'Source lists'!$K$2:$L$9,2,FALSE)</f>
         <v>32</v>
       </c>
-      <c r="L25">
+      <c r="L25" s="3">
         <v>8</v>
       </c>
+      <c r="M25" s="3" t="s">
+        <v>175</v>
+      </c>
     </row>
     <row r="26" spans="1:13" ht="17" x14ac:dyDescent="0.2">
-      <c r="A26">
+      <c r="A26" s="3">
         <v>11</v>
       </c>
-      <c r="B26" t="s">
+      <c r="B26" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C26" t="s">
+      <c r="C26" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="D26" t="s">
+      <c r="D26" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="E26" s="2" t="s">
+      <c r="E26" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="F26" t="s">
+      <c r="F26" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="G26" t="s">
+      <c r="G26" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="H26" t="s">
+      <c r="H26" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="I26" s="1">
+      <c r="I26" s="5">
         <f>VLOOKUP(F26,'Source lists'!$E$1:F27,2,FALSE)</f>
         <v>4</v>
       </c>
-      <c r="J26" s="1">
+      <c r="J26" s="5">
         <f>VLOOKUP(G26,'Source lists'!$H$1:I28,2,FALSE)</f>
         <v>4</v>
       </c>
-      <c r="K26" s="1">
+      <c r="K26" s="5">
         <f>VLOOKUP(F26,'Source lists'!$E$2:$F$6,2,FALSE)*(VLOOKUP(G26,'Source lists'!$H$2:$I$7,2,FALSE)^2)/VLOOKUP(H26,'Source lists'!$K$2:$L$9,2,FALSE)</f>
         <v>32</v>
       </c>
-      <c r="L26">
+      <c r="L26" s="3">
         <v>8</v>
       </c>
+      <c r="M26" s="3" t="s">
+        <v>175</v>
+      </c>
     </row>
     <row r="27" spans="1:13" ht="17" x14ac:dyDescent="0.2">
-      <c r="A27">
+      <c r="A27" s="3">
         <v>12</v>
       </c>
-      <c r="B27" t="s">
+      <c r="B27" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C27" t="s">
+      <c r="C27" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="D27" t="s">
+      <c r="D27" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="E27" s="2" t="s">
+      <c r="E27" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="F27" t="s">
+      <c r="F27" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="G27" t="s">
+      <c r="G27" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="H27" t="s">
+      <c r="H27" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="I27" s="1">
+      <c r="I27" s="5">
         <f>VLOOKUP(F27,'Source lists'!$E$1:F28,2,FALSE)</f>
         <v>4</v>
       </c>
-      <c r="J27" s="1">
+      <c r="J27" s="5">
         <f>VLOOKUP(G27,'Source lists'!$H$1:I29,2,FALSE)</f>
         <v>4</v>
       </c>
-      <c r="K27" s="1">
+      <c r="K27" s="5">
         <f>VLOOKUP(F27,'Source lists'!$E$2:$F$6,2,FALSE)*(VLOOKUP(G27,'Source lists'!$H$2:$I$7,2,FALSE)^2)/VLOOKUP(H27,'Source lists'!$K$2:$L$9,2,FALSE)</f>
         <v>32</v>
       </c>
-      <c r="L27">
+      <c r="L27" s="3">
         <v>8</v>
+      </c>
+      <c r="M27" s="3" t="s">
+        <v>175</v>
       </c>
     </row>
     <row r="28" spans="1:13" ht="17" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
e-Questrain/pages/calendar: Invoiced lessons now marked with asterisk
</commit_message>
<xml_diff>
--- a/apps/e-questrian/e-Questrian - To do list.xlsx
+++ b/apps/e-questrian/e-Questrian - To do list.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rferreira/sigmafox/apps/e-questrian/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC46D784-33C7-1E44-86CC-0F2BE5FD6019}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE023CAE-9D22-F241-9DB3-E628F3A796BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="19820" activeTab="2" xr2:uid="{DC2B379E-A936-2146-8C4F-53C43AECE05C}"/>
   </bookViews>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="974" uniqueCount="219">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="974" uniqueCount="218">
   <si>
     <t>Sections</t>
   </si>
@@ -361,9 +361,6 @@
     <t>Bulk uploads</t>
   </si>
   <si>
-    <t>Invoices appointments should display the invoice number when the details are views - not to be edited</t>
-  </si>
-  <si>
     <t>Invoice view</t>
   </si>
   <si>
@@ -591,9 +588,6 @@
   </si>
   <si>
     <t>Column Labels</t>
-  </si>
-  <si>
-    <t>(blank)</t>
   </si>
   <si>
     <t>Grand Total</t>
@@ -735,6 +729,9 @@
   </si>
   <si>
     <t>To do</t>
+  </si>
+  <si>
+    <t>Invoiced appointments should display the invoice number when the details are viewed - not to be editable</t>
   </si>
 </sst>
 </file>
@@ -824,11 +821,11 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Ruben Ferreira" refreshedDate="45320.705912962963" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="118" xr:uid="{AEB2BF63-68F2-404E-AE9B-E794DFB00774}">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Ruben Ferreira" refreshedDate="45321.401953703702" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="119" xr:uid="{AEB2BF63-68F2-404E-AE9B-E794DFB00774}">
   <cacheSource type="worksheet">
     <worksheetSource ref="A1:N1048576" sheet="Issues 3-1-24"/>
   </cacheSource>
-  <cacheFields count="13">
+  <cacheFields count="14">
     <cacheField name="#" numFmtId="0">
       <sharedItems containsString="0" containsBlank="1" containsNumber="1" containsInteger="1" minValue="1" maxValue="116"/>
     </cacheField>
@@ -865,11 +862,15 @@
     <cacheField name="Dependency #" numFmtId="0">
       <sharedItems containsString="0" containsBlank="1" containsNumber="1" containsInteger="1" minValue="1" maxValue="103"/>
     </cacheField>
-    <cacheField name="Status" numFmtId="0">
-      <sharedItems containsBlank="1" count="3">
+    <cacheField name="Dep status" numFmtId="43">
+      <sharedItems containsBlank="1"/>
+    </cacheField>
+    <cacheField name="Status" numFmtId="43">
+      <sharedItems containsBlank="1" count="4">
         <s v="Done"/>
+        <s v="To do"/>
+        <s v="N/A"/>
         <m/>
-        <s v="N/A"/>
       </sharedItems>
     </cacheField>
   </cacheFields>
@@ -882,7 +883,7 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheRecords1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" count="118">
+<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" count="119">
   <r>
     <n v="53"/>
     <s v="Calendar/Appointments"/>
@@ -896,6 +897,7 @@
     <n v="10"/>
     <n v="200"/>
     <n v="77"/>
+    <s v="Done"/>
     <x v="0"/>
   </r>
   <r>
@@ -911,6 +913,7 @@
     <n v="7"/>
     <n v="98"/>
     <n v="1"/>
+    <s v="Done"/>
     <x v="0"/>
   </r>
   <r>
@@ -926,6 +929,7 @@
     <n v="6"/>
     <n v="96"/>
     <m/>
+    <s v=""/>
     <x v="0"/>
   </r>
   <r>
@@ -941,6 +945,7 @@
     <n v="6"/>
     <n v="96"/>
     <m/>
+    <s v=""/>
     <x v="0"/>
   </r>
   <r>
@@ -956,6 +961,7 @@
     <n v="6"/>
     <n v="96"/>
     <n v="53"/>
+    <s v="Done"/>
     <x v="0"/>
   </r>
   <r>
@@ -971,6 +977,7 @@
     <n v="6"/>
     <n v="96"/>
     <m/>
+    <s v=""/>
     <x v="0"/>
   </r>
   <r>
@@ -986,6 +993,7 @@
     <n v="6"/>
     <n v="72"/>
     <m/>
+    <s v=""/>
     <x v="0"/>
   </r>
   <r>
@@ -1001,6 +1009,7 @@
     <n v="6"/>
     <n v="72"/>
     <n v="2"/>
+    <s v="Done"/>
     <x v="0"/>
   </r>
   <r>
@@ -1016,6 +1025,7 @@
     <n v="4"/>
     <n v="64"/>
     <m/>
+    <s v=""/>
     <x v="0"/>
   </r>
   <r>
@@ -1031,6 +1041,7 @@
     <n v="6"/>
     <n v="57.6"/>
     <m/>
+    <s v=""/>
     <x v="0"/>
   </r>
   <r>
@@ -1046,6 +1057,7 @@
     <n v="4"/>
     <n v="53.333333333333336"/>
     <m/>
+    <s v=""/>
     <x v="0"/>
   </r>
   <r>
@@ -1061,6 +1073,7 @@
     <n v="10"/>
     <n v="50"/>
     <n v="60"/>
+    <s v="To do"/>
     <x v="1"/>
   </r>
   <r>
@@ -1076,6 +1089,7 @@
     <n v="10"/>
     <n v="50"/>
     <n v="62"/>
+    <s v="To do"/>
     <x v="1"/>
   </r>
   <r>
@@ -1091,6 +1105,7 @@
     <n v="10"/>
     <n v="50"/>
     <n v="63"/>
+    <s v="To do"/>
     <x v="1"/>
   </r>
   <r>
@@ -1106,6 +1121,7 @@
     <n v="10"/>
     <n v="50"/>
     <n v="61"/>
+    <s v="To do"/>
     <x v="1"/>
   </r>
   <r>
@@ -1121,6 +1137,7 @@
     <n v="4"/>
     <n v="42.666666666666664"/>
     <m/>
+    <s v=""/>
     <x v="0"/>
   </r>
   <r>
@@ -1136,6 +1153,7 @@
     <n v="7"/>
     <n v="39.200000000000003"/>
     <m/>
+    <s v=""/>
     <x v="0"/>
   </r>
   <r>
@@ -1151,6 +1169,7 @@
     <n v="7"/>
     <n v="39.200000000000003"/>
     <m/>
+    <s v=""/>
     <x v="0"/>
   </r>
   <r>
@@ -1166,6 +1185,7 @@
     <n v="7"/>
     <n v="39.200000000000003"/>
     <m/>
+    <s v=""/>
     <x v="0"/>
   </r>
   <r>
@@ -1181,6 +1201,7 @@
     <n v="7"/>
     <n v="39.200000000000003"/>
     <m/>
+    <s v=""/>
     <x v="0"/>
   </r>
   <r>
@@ -1196,21 +1217,7 @@
     <n v="7"/>
     <n v="39.200000000000003"/>
     <m/>
-    <x v="2"/>
-  </r>
-  <r>
-    <n v="7"/>
-    <s v="User Management"/>
-    <s v="Sign in Modal"/>
-    <m/>
-    <s v="Needs to be above the landing page with a sheath background"/>
-    <s v="Poor UX"/>
-    <s v="Improved UX"/>
-    <s v="Minor change to current component"/>
-    <n v="4"/>
-    <n v="4"/>
-    <n v="32"/>
-    <m/>
+    <s v=""/>
     <x v="2"/>
   </r>
   <r>
@@ -1226,6 +1233,7 @@
     <n v="4"/>
     <n v="32"/>
     <n v="8"/>
+    <s v="Done"/>
     <x v="0"/>
   </r>
   <r>
@@ -1241,6 +1249,7 @@
     <n v="4"/>
     <n v="32"/>
     <n v="8"/>
+    <s v="Done"/>
     <x v="0"/>
   </r>
   <r>
@@ -1256,6 +1265,7 @@
     <n v="4"/>
     <n v="32"/>
     <n v="8"/>
+    <s v="Done"/>
     <x v="0"/>
   </r>
   <r>
@@ -1271,6 +1281,7 @@
     <n v="4"/>
     <n v="32"/>
     <n v="8"/>
+    <s v="Done"/>
     <x v="0"/>
   </r>
   <r>
@@ -1286,6 +1297,7 @@
     <n v="4"/>
     <n v="32"/>
     <n v="8"/>
+    <s v="Done"/>
     <x v="0"/>
   </r>
   <r>
@@ -1301,6 +1313,7 @@
     <n v="4"/>
     <n v="32"/>
     <n v="8"/>
+    <s v="Done"/>
     <x v="0"/>
   </r>
   <r>
@@ -1316,6 +1329,7 @@
     <n v="4"/>
     <n v="32"/>
     <n v="8"/>
+    <s v="Done"/>
     <x v="0"/>
   </r>
   <r>
@@ -1331,6 +1345,7 @@
     <n v="4"/>
     <n v="32"/>
     <n v="8"/>
+    <s v="Done"/>
     <x v="0"/>
   </r>
   <r>
@@ -1346,22 +1361,40 @@
     <n v="4"/>
     <n v="32"/>
     <m/>
+    <s v=""/>
     <x v="0"/>
   </r>
   <r>
-    <n v="31"/>
-    <s v="Navbar"/>
-    <s v="Drop down menu"/>
-    <m/>
-    <s v="The menu hamburger should not be available if on the main menu (make no sense)"/>
+    <n v="115"/>
+    <s v="User Management"/>
+    <s v="Register modal"/>
+    <s v="Register error warnings"/>
+    <s v="Passwords don't match"/>
     <s v="Poor UX"/>
     <s v="Improved UX"/>
     <s v="Minor change to current component"/>
     <n v="4"/>
     <n v="4"/>
     <n v="32"/>
-    <m/>
-    <x v="1"/>
+    <n v="8"/>
+    <s v="Done"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <n v="7"/>
+    <s v="User Management"/>
+    <s v="Sign in Modal"/>
+    <m/>
+    <s v="Needs to be above the landing page with a sheath background"/>
+    <s v="Poor UX"/>
+    <s v="Improved UX"/>
+    <s v="Minor change to current component"/>
+    <n v="4"/>
+    <n v="4"/>
+    <n v="32"/>
+    <m/>
+    <s v=""/>
+    <x v="2"/>
   </r>
   <r>
     <n v="34"/>
@@ -1376,7 +1409,8 @@
     <n v="4"/>
     <n v="32"/>
     <m/>
-    <x v="1"/>
+    <s v=""/>
+    <x v="0"/>
   </r>
   <r>
     <n v="54"/>
@@ -1391,6 +1425,7 @@
     <n v="4"/>
     <n v="32"/>
     <m/>
+    <s v=""/>
     <x v="1"/>
   </r>
   <r>
@@ -1406,6 +1441,7 @@
     <n v="4"/>
     <n v="32"/>
     <m/>
+    <s v=""/>
     <x v="1"/>
   </r>
   <r>
@@ -1421,6 +1457,7 @@
     <n v="4"/>
     <n v="32"/>
     <m/>
+    <s v=""/>
     <x v="1"/>
   </r>
   <r>
@@ -1436,6 +1473,7 @@
     <n v="4"/>
     <n v="32"/>
     <m/>
+    <s v=""/>
     <x v="1"/>
   </r>
   <r>
@@ -1451,6 +1489,7 @@
     <n v="4"/>
     <n v="32"/>
     <m/>
+    <s v=""/>
     <x v="1"/>
   </r>
   <r>
@@ -1466,6 +1505,7 @@
     <n v="4"/>
     <n v="32"/>
     <m/>
+    <s v=""/>
     <x v="1"/>
   </r>
   <r>
@@ -1481,6 +1521,7 @@
     <n v="4"/>
     <n v="32"/>
     <m/>
+    <s v=""/>
     <x v="1"/>
   </r>
   <r>
@@ -1496,6 +1537,7 @@
     <n v="4"/>
     <n v="32"/>
     <m/>
+    <s v=""/>
     <x v="1"/>
   </r>
   <r>
@@ -1511,22 +1553,24 @@
     <n v="4"/>
     <n v="32"/>
     <n v="8"/>
+    <s v="Done"/>
     <x v="1"/>
   </r>
   <r>
-    <n v="115"/>
-    <s v="User Management"/>
-    <s v="Register modal"/>
-    <s v="Register error warnings"/>
-    <s v="Passwords don't match"/>
+    <n v="31"/>
+    <s v="Navbar"/>
+    <s v="Drop down menu"/>
+    <m/>
+    <s v="The menu hamburger should not be available if on the main menu (make no sense)"/>
     <s v="Poor UX"/>
     <s v="Improved UX"/>
     <s v="Minor change to current component"/>
     <n v="4"/>
     <n v="4"/>
     <n v="32"/>
-    <n v="8"/>
-    <x v="0"/>
+    <m/>
+    <s v=""/>
+    <x v="2"/>
   </r>
   <r>
     <n v="17"/>
@@ -1541,6 +1585,7 @@
     <n v="7"/>
     <n v="29.4"/>
     <m/>
+    <s v=""/>
     <x v="1"/>
   </r>
   <r>
@@ -1556,6 +1601,23 @@
     <n v="7"/>
     <n v="28"/>
     <m/>
+    <s v=""/>
+    <x v="0"/>
+  </r>
+  <r>
+    <n v="106"/>
+    <s v="General"/>
+    <m/>
+    <m/>
+    <s v="Update favicon with new logo"/>
+    <s v="Poor UI"/>
+    <s v="Improved UI"/>
+    <s v="Minor tweak"/>
+    <n v="3"/>
+    <n v="3"/>
+    <n v="27"/>
+    <m/>
+    <s v=""/>
     <x v="0"/>
   </r>
   <r>
@@ -1571,6 +1633,7 @@
     <n v="3"/>
     <n v="27"/>
     <m/>
+    <s v=""/>
     <x v="1"/>
   </r>
   <r>
@@ -1586,6 +1649,7 @@
     <n v="6"/>
     <n v="27"/>
     <m/>
+    <s v=""/>
     <x v="1"/>
   </r>
   <r>
@@ -1601,6 +1665,7 @@
     <n v="6"/>
     <n v="27"/>
     <m/>
+    <s v=""/>
     <x v="1"/>
   </r>
   <r>
@@ -1616,6 +1681,7 @@
     <n v="3"/>
     <n v="27"/>
     <m/>
+    <s v=""/>
     <x v="1"/>
   </r>
   <r>
@@ -1631,22 +1697,8 @@
     <n v="3"/>
     <n v="27"/>
     <m/>
+    <s v=""/>
     <x v="1"/>
-  </r>
-  <r>
-    <n v="106"/>
-    <s v="General"/>
-    <m/>
-    <m/>
-    <s v="Update favicon with new logo"/>
-    <s v="Poor UI"/>
-    <s v="Improved UI"/>
-    <s v="Minor tweak"/>
-    <n v="3"/>
-    <n v="3"/>
-    <n v="27"/>
-    <m/>
-    <x v="0"/>
   </r>
   <r>
     <n v="49"/>
@@ -1661,6 +1713,7 @@
     <n v="4"/>
     <n v="21.333333333333332"/>
     <m/>
+    <s v=""/>
     <x v="1"/>
   </r>
   <r>
@@ -1676,6 +1729,7 @@
     <n v="4"/>
     <n v="21.333333333333332"/>
     <m/>
+    <s v=""/>
     <x v="1"/>
   </r>
   <r>
@@ -1691,6 +1745,7 @@
     <n v="4"/>
     <n v="21.333333333333332"/>
     <m/>
+    <s v=""/>
     <x v="1"/>
   </r>
   <r>
@@ -1706,6 +1761,7 @@
     <n v="4"/>
     <n v="21.333333333333332"/>
     <m/>
+    <s v=""/>
     <x v="1"/>
   </r>
   <r>
@@ -1721,6 +1777,7 @@
     <n v="4"/>
     <n v="21.333333333333332"/>
     <m/>
+    <s v=""/>
     <x v="1"/>
   </r>
   <r>
@@ -1736,6 +1793,7 @@
     <n v="4"/>
     <n v="21.333333333333332"/>
     <m/>
+    <s v=""/>
     <x v="1"/>
   </r>
   <r>
@@ -1751,6 +1809,7 @@
     <n v="4"/>
     <n v="21.333333333333332"/>
     <m/>
+    <s v=""/>
     <x v="1"/>
   </r>
   <r>
@@ -1766,6 +1825,7 @@
     <n v="6"/>
     <n v="20.571428571428573"/>
     <m/>
+    <s v=""/>
     <x v="1"/>
   </r>
   <r>
@@ -1781,6 +1841,7 @@
     <n v="6"/>
     <n v="20.571428571428573"/>
     <m/>
+    <s v=""/>
     <x v="1"/>
   </r>
   <r>
@@ -1796,6 +1857,7 @@
     <n v="6"/>
     <n v="20.571428571428573"/>
     <m/>
+    <s v=""/>
     <x v="1"/>
   </r>
   <r>
@@ -1811,6 +1873,7 @@
     <n v="6"/>
     <n v="20.571428571428573"/>
     <m/>
+    <s v=""/>
     <x v="1"/>
   </r>
   <r>
@@ -1826,6 +1889,7 @@
     <n v="6"/>
     <n v="20.571428571428573"/>
     <m/>
+    <s v=""/>
     <x v="1"/>
   </r>
   <r>
@@ -1841,6 +1905,7 @@
     <n v="6"/>
     <n v="18"/>
     <m/>
+    <s v=""/>
     <x v="1"/>
   </r>
   <r>
@@ -1856,6 +1921,7 @@
     <n v="6"/>
     <n v="18"/>
     <m/>
+    <s v=""/>
     <x v="1"/>
   </r>
   <r>
@@ -1871,6 +1937,7 @@
     <n v="4"/>
     <n v="16"/>
     <m/>
+    <s v=""/>
     <x v="1"/>
   </r>
   <r>
@@ -1886,6 +1953,7 @@
     <n v="10"/>
     <n v="14.285714285714286"/>
     <n v="59"/>
+    <s v="To do"/>
     <x v="1"/>
   </r>
   <r>
@@ -1901,6 +1969,7 @@
     <n v="10"/>
     <n v="14.285714285714286"/>
     <n v="64"/>
+    <s v="To do"/>
     <x v="1"/>
   </r>
   <r>
@@ -1916,6 +1985,7 @@
     <n v="10"/>
     <n v="14.285714285714286"/>
     <n v="59"/>
+    <s v="To do"/>
     <x v="1"/>
   </r>
   <r>
@@ -1931,6 +2001,7 @@
     <n v="10"/>
     <n v="14.285714285714286"/>
     <n v="64"/>
+    <s v="To do"/>
     <x v="1"/>
   </r>
   <r>
@@ -1946,6 +2017,7 @@
     <n v="10"/>
     <n v="14.285714285714286"/>
     <n v="59"/>
+    <s v="To do"/>
     <x v="1"/>
   </r>
   <r>
@@ -1961,6 +2033,7 @@
     <n v="10"/>
     <n v="14.285714285714286"/>
     <n v="64"/>
+    <s v="To do"/>
     <x v="1"/>
   </r>
   <r>
@@ -1976,6 +2049,7 @@
     <n v="10"/>
     <n v="14.285714285714286"/>
     <n v="59"/>
+    <s v="To do"/>
     <x v="1"/>
   </r>
   <r>
@@ -1991,6 +2065,7 @@
     <n v="10"/>
     <n v="14.285714285714286"/>
     <n v="64"/>
+    <s v="To do"/>
     <x v="1"/>
   </r>
   <r>
@@ -2006,6 +2081,7 @@
     <n v="10"/>
     <n v="14.285714285714286"/>
     <n v="99"/>
+    <s v="To do"/>
     <x v="1"/>
   </r>
   <r>
@@ -2021,6 +2097,7 @@
     <n v="10"/>
     <n v="14.285714285714286"/>
     <n v="100"/>
+    <s v="To do"/>
     <x v="1"/>
   </r>
   <r>
@@ -2036,6 +2113,7 @@
     <n v="10"/>
     <n v="14.285714285714286"/>
     <n v="102"/>
+    <s v="To do"/>
     <x v="1"/>
   </r>
   <r>
@@ -2051,6 +2129,7 @@
     <n v="10"/>
     <n v="14.285714285714286"/>
     <n v="103"/>
+    <s v="To do"/>
     <x v="1"/>
   </r>
   <r>
@@ -2066,6 +2145,7 @@
     <n v="3"/>
     <n v="13.5"/>
     <m/>
+    <s v=""/>
     <x v="1"/>
   </r>
   <r>
@@ -2081,6 +2161,7 @@
     <n v="3"/>
     <n v="13.5"/>
     <m/>
+    <s v=""/>
     <x v="1"/>
   </r>
   <r>
@@ -2096,6 +2177,7 @@
     <n v="3"/>
     <n v="13.5"/>
     <m/>
+    <s v=""/>
     <x v="1"/>
   </r>
   <r>
@@ -2111,6 +2193,7 @@
     <n v="3"/>
     <n v="13.5"/>
     <m/>
+    <s v=""/>
     <x v="1"/>
   </r>
   <r>
@@ -2126,6 +2209,7 @@
     <n v="3"/>
     <n v="13.5"/>
     <m/>
+    <s v=""/>
     <x v="1"/>
   </r>
   <r>
@@ -2141,6 +2225,7 @@
     <n v="3"/>
     <n v="13.5"/>
     <m/>
+    <s v=""/>
     <x v="1"/>
   </r>
   <r>
@@ -2156,6 +2241,7 @@
     <n v="4"/>
     <n v="12.8"/>
     <m/>
+    <s v=""/>
     <x v="1"/>
   </r>
   <r>
@@ -2171,6 +2257,7 @@
     <n v="4"/>
     <n v="12.8"/>
     <m/>
+    <s v=""/>
     <x v="1"/>
   </r>
   <r>
@@ -2186,6 +2273,7 @@
     <n v="4"/>
     <n v="12.8"/>
     <m/>
+    <s v=""/>
     <x v="1"/>
   </r>
   <r>
@@ -2201,6 +2289,7 @@
     <n v="4"/>
     <n v="12.8"/>
     <m/>
+    <s v=""/>
     <x v="1"/>
   </r>
   <r>
@@ -2216,6 +2305,7 @@
     <n v="4"/>
     <n v="12.8"/>
     <m/>
+    <s v=""/>
     <x v="1"/>
   </r>
   <r>
@@ -2231,6 +2321,7 @@
     <n v="10"/>
     <n v="12.5"/>
     <m/>
+    <s v=""/>
     <x v="1"/>
   </r>
   <r>
@@ -2246,6 +2337,7 @@
     <n v="10"/>
     <n v="12.5"/>
     <m/>
+    <s v=""/>
     <x v="1"/>
   </r>
   <r>
@@ -2261,6 +2353,7 @@
     <n v="10"/>
     <n v="12.5"/>
     <m/>
+    <s v=""/>
     <x v="1"/>
   </r>
   <r>
@@ -2276,6 +2369,7 @@
     <n v="10"/>
     <n v="12.5"/>
     <m/>
+    <s v=""/>
     <x v="1"/>
   </r>
   <r>
@@ -2291,6 +2385,7 @@
     <n v="10"/>
     <n v="12.5"/>
     <m/>
+    <s v=""/>
     <x v="1"/>
   </r>
   <r>
@@ -2306,6 +2401,7 @@
     <n v="10"/>
     <n v="12.5"/>
     <m/>
+    <s v=""/>
     <x v="1"/>
   </r>
   <r>
@@ -2321,6 +2417,7 @@
     <n v="10"/>
     <n v="10"/>
     <m/>
+    <s v=""/>
     <x v="1"/>
   </r>
   <r>
@@ -2336,6 +2433,7 @@
     <n v="10"/>
     <n v="10"/>
     <m/>
+    <s v=""/>
     <x v="1"/>
   </r>
   <r>
@@ -2351,6 +2449,7 @@
     <n v="10"/>
     <n v="10"/>
     <m/>
+    <s v=""/>
     <x v="1"/>
   </r>
   <r>
@@ -2366,6 +2465,7 @@
     <n v="10"/>
     <n v="10"/>
     <m/>
+    <s v=""/>
     <x v="1"/>
   </r>
   <r>
@@ -2381,6 +2481,7 @@
     <n v="10"/>
     <n v="10"/>
     <m/>
+    <s v=""/>
     <x v="1"/>
   </r>
   <r>
@@ -2396,6 +2497,7 @@
     <n v="7"/>
     <n v="9.8000000000000007"/>
     <m/>
+    <s v=""/>
     <x v="1"/>
   </r>
   <r>
@@ -2411,6 +2513,7 @@
     <n v="3"/>
     <n v="9"/>
     <m/>
+    <s v=""/>
     <x v="1"/>
   </r>
   <r>
@@ -2426,6 +2529,7 @@
     <n v="3"/>
     <n v="9"/>
     <m/>
+    <s v=""/>
     <x v="1"/>
   </r>
   <r>
@@ -2441,6 +2545,7 @@
     <n v="3"/>
     <n v="9"/>
     <m/>
+    <s v=""/>
     <x v="1"/>
   </r>
   <r>
@@ -2456,6 +2561,7 @@
     <n v="3"/>
     <n v="9"/>
     <m/>
+    <s v=""/>
     <x v="1"/>
   </r>
   <r>
@@ -2471,6 +2577,7 @@
     <n v="6"/>
     <n v="9"/>
     <m/>
+    <s v=""/>
     <x v="1"/>
   </r>
   <r>
@@ -2486,6 +2593,7 @@
     <n v="6"/>
     <n v="9"/>
     <m/>
+    <s v=""/>
     <x v="1"/>
   </r>
   <r>
@@ -2501,6 +2609,7 @@
     <n v="6"/>
     <n v="9"/>
     <m/>
+    <s v=""/>
     <x v="1"/>
   </r>
   <r>
@@ -2516,6 +2625,7 @@
     <n v="6"/>
     <n v="9"/>
     <m/>
+    <s v=""/>
     <x v="1"/>
   </r>
   <r>
@@ -2531,6 +2641,7 @@
     <n v="6"/>
     <n v="9"/>
     <m/>
+    <s v=""/>
     <x v="1"/>
   </r>
   <r>
@@ -2546,6 +2657,7 @@
     <n v="3"/>
     <n v="9"/>
     <m/>
+    <s v=""/>
     <x v="1"/>
   </r>
   <r>
@@ -2561,6 +2673,7 @@
     <n v="7"/>
     <n v="7"/>
     <m/>
+    <s v=""/>
     <x v="1"/>
   </r>
   <r>
@@ -2576,6 +2689,7 @@
     <n v="3"/>
     <n v="6.75"/>
     <m/>
+    <s v=""/>
     <x v="1"/>
   </r>
   <r>
@@ -2591,6 +2705,7 @@
     <n v="1"/>
     <n v="2"/>
     <m/>
+    <s v=""/>
     <x v="1"/>
   </r>
   <r>
@@ -2606,6 +2721,7 @@
     <n v="1"/>
     <n v="1.5"/>
     <n v="27"/>
+    <s v="To do"/>
     <x v="1"/>
   </r>
   <r>
@@ -2621,6 +2737,7 @@
     <n v="1"/>
     <n v="1.5"/>
     <n v="27"/>
+    <s v="To do"/>
     <x v="1"/>
   </r>
   <r>
@@ -2636,6 +2753,7 @@
     <n v="1"/>
     <n v="0.42857142857142855"/>
     <m/>
+    <s v=""/>
     <x v="1"/>
   </r>
   <r>
@@ -2651,7 +2769,24 @@
     <m/>
     <m/>
     <m/>
-    <x v="1"/>
+    <m/>
+    <x v="3"/>
+  </r>
+  <r>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <x v="3"/>
   </r>
 </pivotCacheRecords>
 </file>
@@ -2659,7 +2794,7 @@
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{936C0618-B7B4-0144-93D9-409C5361BBD7}" name="PivotTable7" cacheId="4" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A7:E9" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
-  <pivotFields count="13">
+  <pivotFields count="14">
     <pivotField showAll="0"/>
     <pivotField showAll="0"/>
     <pivotField showAll="0"/>
@@ -2672,11 +2807,13 @@
     <pivotField showAll="0"/>
     <pivotField showAll="0"/>
     <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
     <pivotField axis="axisCol" showAll="0" sortType="ascending">
-      <items count="4">
+      <items count="5">
         <item x="0"/>
         <item x="2"/>
         <item x="1"/>
+        <item h="1" x="3"/>
         <item t="default"/>
       </items>
     </pivotField>
@@ -2685,7 +2822,7 @@
     <i/>
   </rowItems>
   <colFields count="1">
-    <field x="12"/>
+    <field x="13"/>
   </colFields>
   <colItems count="4">
     <i>
@@ -2719,7 +2856,7 @@
 <file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{4A183E6E-2837-3A40-90CB-E731BF47E9C0}" name="PivotTable6" cacheId="4" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A1:E3" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
-  <pivotFields count="13">
+  <pivotFields count="14">
     <pivotField showAll="0"/>
     <pivotField showAll="0"/>
     <pivotField showAll="0"/>
@@ -2732,11 +2869,13 @@
     <pivotField showAll="0"/>
     <pivotField dataField="1" showAll="0"/>
     <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
     <pivotField axis="axisCol" showAll="0" sortType="ascending">
-      <items count="4">
+      <items count="5">
         <item x="0"/>
         <item x="2"/>
         <item x="1"/>
+        <item h="1" x="3"/>
         <item t="default"/>
       </items>
     </pivotField>
@@ -2745,7 +2884,7 @@
     <i/>
   </rowItems>
   <colFields count="1">
-    <field x="12"/>
+    <field x="13"/>
   </colFields>
   <colItems count="4">
     <i>
@@ -2779,7 +2918,7 @@
 <file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{4DCC3165-0959-AA43-80CF-D9170B1DCB64}" name="PivotTable8" cacheId="4" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A13:E15" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
-  <pivotFields count="13">
+  <pivotFields count="14">
     <pivotField showAll="0"/>
     <pivotField showAll="0"/>
     <pivotField showAll="0"/>
@@ -2792,11 +2931,13 @@
     <pivotField dataField="1" showAll="0"/>
     <pivotField showAll="0"/>
     <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
     <pivotField axis="axisCol" showAll="0" sortType="ascending">
-      <items count="4">
+      <items count="5">
         <item x="0"/>
         <item x="2"/>
         <item x="1"/>
+        <item h="1" x="3"/>
         <item t="default"/>
       </items>
     </pivotField>
@@ -2805,7 +2946,7 @@
     <i/>
   </rowItems>
   <colFields count="1">
-    <field x="12"/>
+    <field x="13"/>
   </colFields>
   <colItems count="4">
     <i>
@@ -3136,7 +3277,7 @@
   <dimension ref="A1:E17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3144,87 +3285,87 @@
     <col min="1" max="1" width="14.6640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="15.5" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="4.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="5.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="10.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B1" s="6" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C1"/>
       <c r="D1"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B2" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C2" t="s">
+        <v>214</v>
+      </c>
+      <c r="D2" t="s">
         <v>216</v>
       </c>
-      <c r="D2" t="s">
-        <v>177</v>
-      </c>
       <c r="E2" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="B3" s="8">
-        <v>1575.4000000000003</v>
+        <v>1607.4000000000003</v>
       </c>
       <c r="C3" s="8">
-        <v>71.2</v>
+        <v>103.2</v>
       </c>
       <c r="D3" s="8">
-        <v>1580.9976190476182</v>
+        <v>1516.9976190476186</v>
       </c>
       <c r="E3" s="8">
-        <v>3227.5976190476185</v>
+        <v>3227.597619047619</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="E5" s="7">
         <f>SUM(B3:C3)/GETPIVOTDATA("Priority S",$A$1)</f>
-        <v>0.51016272607298241</v>
+        <v>0.52999171579038229</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B7" s="6" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C7"/>
       <c r="D7"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B8" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C8" t="s">
+        <v>214</v>
+      </c>
+      <c r="D8" t="s">
         <v>216</v>
       </c>
-      <c r="D8" t="s">
-        <v>177</v>
-      </c>
       <c r="E8" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="B9" s="8">
-        <v>145</v>
+        <v>149</v>
       </c>
       <c r="C9" s="8">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="D9" s="8">
-        <v>219</v>
+        <v>211</v>
       </c>
       <c r="E9" s="8">
         <v>372</v>
@@ -3233,42 +3374,42 @@
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="E11" s="7">
         <f>SUM(B9:C9)/GETPIVOTDATA("Importance S",$A$7)</f>
-        <v>0.41129032258064518</v>
+        <v>0.43279569892473119</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B13" s="6" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C13"/>
       <c r="D13"/>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B14" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C14" t="s">
+        <v>214</v>
+      </c>
+      <c r="D14" t="s">
         <v>216</v>
       </c>
-      <c r="D14" t="s">
-        <v>177</v>
-      </c>
       <c r="E14" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="B15" s="8">
-        <v>149</v>
+        <v>153</v>
       </c>
       <c r="C15" s="8">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="D15" s="8">
-        <v>520</v>
+        <v>512</v>
       </c>
       <c r="E15" s="8">
         <v>680</v>
@@ -3277,7 +3418,7 @@
     <row r="17" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E17" s="7">
         <f>SUM(B15:C15)/GETPIVOTDATA("Impact S",$A$13)</f>
-        <v>0.23529411764705882</v>
+        <v>0.24705882352941178</v>
       </c>
     </row>
   </sheetData>
@@ -3337,7 +3478,7 @@
         <v>90</v>
       </c>
       <c r="C2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E2" t="s">
         <v>13</v>
@@ -3363,7 +3504,7 @@
         <v>6</v>
       </c>
       <c r="B3" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C3" t="s">
         <v>35</v>
@@ -3404,7 +3545,7 @@
         <v>4</v>
       </c>
       <c r="H4" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="I4">
         <v>6</v>
@@ -3450,7 +3591,7 @@
         <v>2</v>
       </c>
       <c r="B6" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C6" t="s">
         <v>54</v>
@@ -3479,10 +3620,10 @@
         <v>3</v>
       </c>
       <c r="B7" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C7" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="H7" t="s">
         <v>30</v>
@@ -3505,7 +3646,7 @@
         <v>81</v>
       </c>
       <c r="C8" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="K8" t="s">
         <v>23</v>
@@ -3533,10 +3674,10 @@
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B10" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C10" t="s">
         <v>84</v>
@@ -3547,7 +3688,7 @@
         <v>39</v>
       </c>
       <c r="B11" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C11" t="s">
         <v>44</v>
@@ -3558,15 +3699,15 @@
         <v>38</v>
       </c>
       <c r="B12" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C12" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B13" t="s">
         <v>33</v>
@@ -3588,7 +3729,7 @@
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B15" t="s">
         <v>80</v>
@@ -3599,7 +3740,7 @@
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="B16" t="s">
         <v>72</v>
@@ -3610,7 +3751,7 @@
     </row>
     <row r="17" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B17" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C17" t="s">
         <v>88</v>
@@ -3618,23 +3759,23 @@
     </row>
     <row r="18" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B18" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C18" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
     </row>
     <row r="19" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B19" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C19" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
     </row>
     <row r="20" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B20" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="21" spans="2:3" x14ac:dyDescent="0.2">
@@ -3654,52 +3795,52 @@
     </row>
     <row r="24" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B24" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="25" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B25" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="26" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B26" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="27" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B27" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="28" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B28" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="29" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B29" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="30" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B30" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="31" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B31" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="32" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B32" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="33" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B33" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
     </row>
   </sheetData>
@@ -3716,7 +3857,7 @@
   <dimension ref="A1:XEY118"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="F36" sqref="F36"/>
+      <selection activeCell="D37" sqref="D37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="34.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3762,22 +3903,22 @@
         <v>20</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="L1" t="s">
         <v>71</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="2" spans="1:2047 2051:3067 3074:4094 4101:6142 6146:7162 7169:8189 8196:9216 9223:10237 10241:11264 11268:12284 12291:13311 13318:15359 15363:16379" s="3" customFormat="1" ht="34" hidden="1" x14ac:dyDescent="0.2">
@@ -3791,10 +3932,10 @@
         <v>90</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="F2" s="3" t="s">
         <v>14</v>
@@ -3821,11 +3962,11 @@
         <v>77</v>
       </c>
       <c r="M2" s="5" t="str">
-        <f>IF(ISBLANK(L2),"",VLOOKUP(L2,A:N,14,FALSE))</f>
+        <f t="shared" ref="M2:M12" si="0">IF(ISBLANK(L2),"",VLOOKUP(L2,A:N,14,FALSE))</f>
         <v>Done</v>
       </c>
       <c r="N2" s="5" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="3" spans="1:2047 2051:3067 3074:4094 4101:6142 6146:7162 7169:8189 8196:9216 9223:10237 10241:11264 11268:12284 12291:13311 13318:15359 15363:16379" s="3" customFormat="1" ht="17" hidden="1" x14ac:dyDescent="0.2">
@@ -3866,11 +4007,11 @@
         <v>1</v>
       </c>
       <c r="M3" s="5" t="str">
-        <f>IF(ISBLANK(L3),"",VLOOKUP(L3,A:N,14,FALSE))</f>
+        <f t="shared" si="0"/>
         <v>Done</v>
       </c>
       <c r="N3" s="5" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="4" spans="1:2047 2051:3067 3074:4094 4101:6142 6146:7162 7169:8189 8196:9216 9223:10237 10241:11264 11268:12284 12291:13311 13318:15359 15363:16379" ht="17" hidden="1" x14ac:dyDescent="0.2">
@@ -3881,17 +4022,17 @@
         <v>3</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D4" s="3"/>
       <c r="E4" s="4" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="F4" s="3" t="s">
         <v>14</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="H4" s="3" t="s">
         <v>24</v>
@@ -3910,11 +4051,11 @@
       </c>
       <c r="L4" s="3"/>
       <c r="M4" s="5" t="str">
-        <f>IF(ISBLANK(L4),"",VLOOKUP(L4,A:N,14,FALSE))</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="N4" s="5" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="5" spans="1:2047 2051:3067 3074:4094 4101:6142 6146:7162 7169:8189 8196:9216 9223:10237 10241:11264 11268:12284 12291:13311 13318:15359 15363:16379" ht="17" hidden="1" x14ac:dyDescent="0.2">
@@ -3925,17 +4066,17 @@
         <v>6</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="D5" s="3"/>
       <c r="E5" s="4" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="F5" s="3" t="s">
         <v>14</v>
       </c>
       <c r="G5" s="3" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="H5" s="3" t="s">
         <v>24</v>
@@ -3954,11 +4095,11 @@
       </c>
       <c r="L5" s="3"/>
       <c r="M5" s="5" t="str">
-        <f>IF(ISBLANK(L5),"",VLOOKUP(L5,A:N,14,FALSE))</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="N5" s="5" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="6" spans="1:2047 2051:3067 3074:4094 4101:6142 6146:7162 7169:8189 8196:9216 9223:10237 10241:11264 11268:12284 12291:13311 13318:15359 15363:16379" ht="17" hidden="1" x14ac:dyDescent="0.2">
@@ -3969,17 +4110,17 @@
         <v>4</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="D6" s="3"/>
       <c r="E6" s="4" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="F6" s="3" t="s">
         <v>14</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="H6" s="3" t="s">
         <v>24</v>
@@ -4000,11 +4141,11 @@
         <v>53</v>
       </c>
       <c r="M6" s="5" t="str">
-        <f>IF(ISBLANK(L6),"",VLOOKUP(L6,A:N,14,FALSE))</f>
+        <f t="shared" si="0"/>
         <v>Done</v>
       </c>
       <c r="N6" s="5" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="7" spans="1:2047 2051:3067 3074:4094 4101:6142 6146:7162 7169:8189 8196:9216 9223:10237 10241:11264 11268:12284 12291:13311 13318:15359 15363:16379" ht="17" hidden="1" x14ac:dyDescent="0.2">
@@ -4015,17 +4156,17 @@
         <v>3</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D7" s="3"/>
       <c r="E7" s="4" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="F7" s="3" t="s">
         <v>14</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="H7" s="3" t="s">
         <v>24</v>
@@ -4044,11 +4185,11 @@
       </c>
       <c r="L7" s="3"/>
       <c r="M7" s="5" t="str">
-        <f>IF(ISBLANK(L7),"",VLOOKUP(L7,A:N,14,FALSE))</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="N7" s="5" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="8" spans="1:2047 2051:3067 3074:4094 4101:6142 6146:7162 7169:8189 8196:9216 9223:10237 10241:11264 11268:12284 12291:13311 13318:15359 15363:16379" ht="17" hidden="1" x14ac:dyDescent="0.2">
@@ -4065,13 +4206,13 @@
         <v>96</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="F8" s="3" t="s">
         <v>15</v>
       </c>
       <c r="G8" s="3" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="H8" s="3" t="s">
         <v>23</v>
@@ -4090,11 +4231,11 @@
       </c>
       <c r="L8" s="3"/>
       <c r="M8" s="5" t="str">
-        <f>IF(ISBLANK(L8),"",VLOOKUP(L8,A:N,14,FALSE))</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="N8" s="5" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="9" spans="1:2047 2051:3067 3074:4094 4101:6142 6146:7162 7169:8189 8196:9216 9223:10237 10241:11264 11268:12284 12291:13311 13318:15359 15363:16379" ht="34" hidden="1" x14ac:dyDescent="0.2">
@@ -4111,13 +4252,13 @@
         <v>34</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="F9" s="3" t="s">
         <v>15</v>
       </c>
       <c r="G9" s="3" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="H9" s="3" t="s">
         <v>23</v>
@@ -4138,11 +4279,11 @@
         <v>2</v>
       </c>
       <c r="M9" s="5" t="str">
-        <f>IF(ISBLANK(L9),"",VLOOKUP(L9,A:N,14,FALSE))</f>
+        <f t="shared" si="0"/>
         <v>Done</v>
       </c>
       <c r="N9" s="5" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="10" spans="1:2047 2051:3067 3074:4094 4101:6142 6146:7162 7169:8189 8196:9216 9223:10237 10241:11264 11268:12284 12291:13311 13318:15359 15363:16379" s="3" customFormat="1" ht="17" hidden="1" x14ac:dyDescent="0.2">
@@ -4156,7 +4297,7 @@
         <v>80</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="F10" s="3" t="s">
         <v>15</v>
@@ -4180,11 +4321,11 @@
         <v>64</v>
       </c>
       <c r="M10" s="5" t="str">
-        <f>IF(ISBLANK(L10),"",VLOOKUP(L10,A:N,14,FALSE))</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="N10" s="5" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="S10" s="4"/>
       <c r="W10" s="5"/>
@@ -9228,20 +9369,20 @@
         <v>113</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="D11" s="3"/>
       <c r="E11" s="4" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="F11" s="3" t="s">
         <v>14</v>
       </c>
       <c r="G11" s="3" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="H11" s="3" t="s">
         <v>70</v>
@@ -9260,11 +9401,11 @@
       </c>
       <c r="L11" s="3"/>
       <c r="M11" s="5" t="str">
-        <f>IF(ISBLANK(L11),"",VLOOKUP(L11,A:N,14,FALSE))</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="N11" s="5" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="12" spans="1:2047 2051:3067 3074:4094 4101:6142 6146:7162 7169:8189 8196:9216 9223:10237 10241:11264 11268:12284 12291:13311 13318:15359 15363:16379" ht="51" hidden="1" x14ac:dyDescent="0.2">
@@ -9304,14 +9445,14 @@
       </c>
       <c r="L12" s="3"/>
       <c r="M12" s="5" t="str">
-        <f>IF(ISBLANK(L12),"",VLOOKUP(L12,A:N,14,FALSE))</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="N12" s="5" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2047 2051:3067 3074:4094 4101:6142 6146:7162 7169:8189 8196:9216 9223:10237 10241:11264 11268:12284 12291:13311 13318:15359 15363:16379" s="3" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2047 2051:3067 3074:4094 4101:6142 6146:7162 7169:8189 8196:9216 9223:10237 10241:11264 11268:12284 12291:13311 13318:15359 15363:16379" s="3" customFormat="1" ht="17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>59</v>
       </c>
@@ -9319,11 +9460,11 @@
         <v>2</v>
       </c>
       <c r="C13" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D13"/>
       <c r="E13" s="2" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="F13" t="s">
         <v>17</v>
@@ -9354,10 +9495,10 @@
         <v>To do</v>
       </c>
       <c r="N13" s="1" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2047 2051:3067 3074:4094 4101:6142 6146:7162 7169:8189 8196:9216 9223:10237 10241:11264 11268:12284 12291:13311 13318:15359 15363:16379" ht="17" x14ac:dyDescent="0.2">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2047 2051:3067 3074:4094 4101:6142 6146:7162 7169:8189 8196:9216 9223:10237 10241:11264 11268:12284 12291:13311 13318:15359 15363:16379" ht="17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>60</v>
       </c>
@@ -9368,7 +9509,7 @@
         <v>90</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="F14" t="s">
         <v>17</v>
@@ -9395,14 +9536,14 @@
         <v>62</v>
       </c>
       <c r="M14" s="1" t="str">
-        <f>IF(ISBLANK(L14),"",VLOOKUP(L14,A:N,14,FALSE))</f>
+        <f t="shared" ref="M14:M45" si="1">IF(ISBLANK(L14),"",VLOOKUP(L14,A:N,14,FALSE))</f>
         <v>To do</v>
       </c>
       <c r="N14" s="1" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2047 2051:3067 3074:4094 4101:6142 6146:7162 7169:8189 8196:9216 9223:10237 10241:11264 11268:12284 12291:13311 13318:15359 15363:16379" ht="17" x14ac:dyDescent="0.2">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2047 2051:3067 3074:4094 4101:6142 6146:7162 7169:8189 8196:9216 9223:10237 10241:11264 11268:12284 12291:13311 13318:15359 15363:16379" ht="17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>61</v>
       </c>
@@ -9413,7 +9554,7 @@
         <v>90</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="F15" t="s">
         <v>17</v>
@@ -9440,14 +9581,14 @@
         <v>63</v>
       </c>
       <c r="M15" s="1" t="str">
-        <f>IF(ISBLANK(L15),"",VLOOKUP(L15,A:N,14,FALSE))</f>
+        <f t="shared" si="1"/>
         <v>To do</v>
       </c>
       <c r="N15" s="1" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2047 2051:3067 3074:4094 4101:6142 6146:7162 7169:8189 8196:9216 9223:10237 10241:11264 11268:12284 12291:13311 13318:15359 15363:16379" ht="17" x14ac:dyDescent="0.2">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2047 2051:3067 3074:4094 4101:6142 6146:7162 7169:8189 8196:9216 9223:10237 10241:11264 11268:12284 12291:13311 13318:15359 15363:16379" ht="17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>64</v>
       </c>
@@ -9455,10 +9596,10 @@
         <v>2</v>
       </c>
       <c r="C16" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="F16" t="s">
         <v>17</v>
@@ -9485,11 +9626,11 @@
         <v>61</v>
       </c>
       <c r="M16" s="1" t="str">
-        <f>IF(ISBLANK(L16),"",VLOOKUP(L16,A:N,14,FALSE))</f>
+        <f t="shared" si="1"/>
         <v>To do</v>
       </c>
       <c r="N16" s="1" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
     </row>
     <row r="17" spans="1:14" ht="17" hidden="1" x14ac:dyDescent="0.2">
@@ -9529,11 +9670,11 @@
       </c>
       <c r="L17" s="3"/>
       <c r="M17" s="5" t="str">
-        <f>IF(ISBLANK(L17),"",VLOOKUP(L17,A:N,14,FALSE))</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="N17" s="5" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="18" spans="1:14" ht="34" hidden="1" x14ac:dyDescent="0.2">
@@ -9575,11 +9716,11 @@
       </c>
       <c r="L18" s="3"/>
       <c r="M18" s="5" t="str">
-        <f>IF(ISBLANK(L18),"",VLOOKUP(L18,A:N,14,FALSE))</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="N18" s="5" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="19" spans="1:14" ht="17" hidden="1" x14ac:dyDescent="0.2">
@@ -9593,7 +9734,7 @@
         <v>33</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="E19" s="4" t="s">
         <v>94</v>
@@ -9621,11 +9762,11 @@
       </c>
       <c r="L19" s="3"/>
       <c r="M19" s="5" t="str">
-        <f>IF(ISBLANK(L19),"",VLOOKUP(L19,A:N,14,FALSE))</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="N19" s="5" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="20" spans="1:14" ht="17" hidden="1" x14ac:dyDescent="0.2">
@@ -9667,11 +9808,11 @@
       </c>
       <c r="L20" s="3"/>
       <c r="M20" s="5" t="str">
-        <f>IF(ISBLANK(L20),"",VLOOKUP(L20,A:N,14,FALSE))</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="N20" s="5" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="21" spans="1:14" ht="17" hidden="1" x14ac:dyDescent="0.2">
@@ -9714,11 +9855,11 @@
       </c>
       <c r="L21" s="3"/>
       <c r="M21" s="5" t="str">
-        <f>IF(ISBLANK(L21),"",VLOOKUP(L21,A:N,14,FALSE))</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="N21" s="5" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="22" spans="1:14" ht="136" hidden="1" x14ac:dyDescent="0.2">
@@ -9735,7 +9876,7 @@
         <v>64</v>
       </c>
       <c r="E22" s="4" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="F22" s="3" t="s">
         <v>15</v>
@@ -9760,11 +9901,11 @@
       </c>
       <c r="L22" s="3"/>
       <c r="M22" s="5" t="str">
-        <f>IF(ISBLANK(L22),"",VLOOKUP(L22,A:N,14,FALSE))</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="N22" s="5" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
     </row>
     <row r="23" spans="1:14" ht="17" hidden="1" x14ac:dyDescent="0.2">
@@ -9808,11 +9949,11 @@
         <v>8</v>
       </c>
       <c r="M23" s="5" t="str">
-        <f>IF(ISBLANK(L23),"",VLOOKUP(L23,A:N,14,FALSE))</f>
+        <f t="shared" si="1"/>
         <v>Done</v>
       </c>
       <c r="N23" s="5" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="24" spans="1:14" ht="17" hidden="1" x14ac:dyDescent="0.2">
@@ -9856,11 +9997,11 @@
         <v>8</v>
       </c>
       <c r="M24" s="5" t="str">
-        <f>IF(ISBLANK(L24),"",VLOOKUP(L24,A:N,14,FALSE))</f>
+        <f t="shared" si="1"/>
         <v>Done</v>
       </c>
       <c r="N24" s="5" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="25" spans="1:14" ht="17" hidden="1" x14ac:dyDescent="0.2">
@@ -9904,11 +10045,11 @@
         <v>8</v>
       </c>
       <c r="M25" s="5" t="str">
-        <f>IF(ISBLANK(L25),"",VLOOKUP(L25,A:N,14,FALSE))</f>
+        <f t="shared" si="1"/>
         <v>Done</v>
       </c>
       <c r="N25" s="5" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="26" spans="1:14" ht="17" hidden="1" x14ac:dyDescent="0.2">
@@ -9952,11 +10093,11 @@
         <v>8</v>
       </c>
       <c r="M26" s="5" t="str">
-        <f>IF(ISBLANK(L26),"",VLOOKUP(L26,A:N,14,FALSE))</f>
+        <f t="shared" si="1"/>
         <v>Done</v>
       </c>
       <c r="N26" s="5" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="27" spans="1:14" ht="17" hidden="1" x14ac:dyDescent="0.2">
@@ -9967,10 +10108,10 @@
         <v>8</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="D27" s="3" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="E27" s="4" t="s">
         <v>50</v>
@@ -10000,11 +10141,11 @@
         <v>8</v>
       </c>
       <c r="M27" s="5" t="str">
-        <f>IF(ISBLANK(L27),"",VLOOKUP(L27,A:N,14,FALSE))</f>
+        <f t="shared" si="1"/>
         <v>Done</v>
       </c>
       <c r="N27" s="5" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="28" spans="1:14" ht="17" hidden="1" x14ac:dyDescent="0.2">
@@ -10015,10 +10156,10 @@
         <v>8</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="D28" s="3" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="E28" s="4" t="s">
         <v>51</v>
@@ -10048,11 +10189,11 @@
         <v>8</v>
       </c>
       <c r="M28" s="5" t="str">
-        <f>IF(ISBLANK(L28),"",VLOOKUP(L28,A:N,14,FALSE))</f>
+        <f t="shared" si="1"/>
         <v>Done</v>
       </c>
       <c r="N28" s="5" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="29" spans="1:14" ht="17" hidden="1" x14ac:dyDescent="0.2">
@@ -10063,10 +10204,10 @@
         <v>8</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="D29" s="3" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="E29" s="4" t="s">
         <v>52</v>
@@ -10096,11 +10237,11 @@
         <v>8</v>
       </c>
       <c r="M29" s="5" t="str">
-        <f>IF(ISBLANK(L29),"",VLOOKUP(L29,A:N,14,FALSE))</f>
+        <f t="shared" si="1"/>
         <v>Done</v>
       </c>
       <c r="N29" s="5" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="30" spans="1:14" ht="17" hidden="1" x14ac:dyDescent="0.2">
@@ -10111,10 +10252,10 @@
         <v>8</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="D30" s="3" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="E30" s="4" t="s">
         <v>53</v>
@@ -10144,11 +10285,11 @@
         <v>8</v>
       </c>
       <c r="M30" s="5" t="str">
-        <f>IF(ISBLANK(L30),"",VLOOKUP(L30,A:N,14,FALSE))</f>
+        <f t="shared" si="1"/>
         <v>Done</v>
       </c>
       <c r="N30" s="5" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="31" spans="1:14" ht="17" hidden="1" x14ac:dyDescent="0.2">
@@ -10159,7 +10300,7 @@
         <v>8</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="D31" s="3"/>
       <c r="E31" s="4" t="s">
@@ -10188,11 +10329,11 @@
       </c>
       <c r="L31" s="3"/>
       <c r="M31" s="5" t="str">
-        <f>IF(ISBLANK(L31),"",VLOOKUP(L31,A:N,14,FALSE))</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="N31" s="5" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="32" spans="1:14" ht="17" hidden="1" x14ac:dyDescent="0.2">
@@ -10203,13 +10344,13 @@
         <v>8</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="D32" s="3" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="E32" s="4" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="F32" s="3" t="s">
         <v>15</v>
@@ -10236,11 +10377,11 @@
         <v>8</v>
       </c>
       <c r="M32" s="5" t="str">
-        <f>IF(ISBLANK(L32),"",VLOOKUP(L32,A:N,14,FALSE))</f>
+        <f t="shared" si="1"/>
         <v>Done</v>
       </c>
       <c r="N32" s="5" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="33" spans="1:14" ht="34" hidden="1" x14ac:dyDescent="0.2">
@@ -10280,112 +10421,112 @@
       </c>
       <c r="L33" s="3"/>
       <c r="M33" s="5" t="str">
-        <f>IF(ISBLANK(L33),"",VLOOKUP(L33,A:N,14,FALSE))</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="N33" s="5" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="34" spans="1:14" ht="34" x14ac:dyDescent="0.2">
-      <c r="A34">
-        <v>31</v>
-      </c>
-      <c r="B34" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="34" spans="1:14" s="3" customFormat="1" ht="17" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A34" s="3">
+        <v>34</v>
+      </c>
+      <c r="B34" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="C34" t="s">
+      <c r="C34" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="E34" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="F34" t="s">
+      <c r="D34" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="E34" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="F34" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="G34" t="s">
+      <c r="G34" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="H34" t="s">
+      <c r="H34" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="I34" s="1">
-        <f>VLOOKUP(F34,'Source lists'!$E$1:F34,2,FALSE)</f>
+      <c r="I34" s="5">
+        <f>VLOOKUP(F34,'Source lists'!$E$1:F35,2,FALSE)</f>
         <v>4</v>
       </c>
-      <c r="J34" s="1">
-        <f>VLOOKUP(G34,'Source lists'!$H$1:I35,2,FALSE)</f>
+      <c r="J34" s="5">
+        <f>VLOOKUP(G34,'Source lists'!$H$1:I36,2,FALSE)</f>
         <v>4</v>
       </c>
-      <c r="K34" s="1">
+      <c r="K34" s="5">
         <f>VLOOKUP(F34,'Source lists'!$E$2:$F$6,2,FALSE)*(VLOOKUP(G34,'Source lists'!$H$2:$I$7,2,FALSE)^2)/VLOOKUP(H34,'Source lists'!$K$2:$L$9,2,FALSE)</f>
         <v>32</v>
       </c>
-      <c r="M34" s="1" t="str">
+      <c r="M34" s="5" t="str">
         <f>IF(ISBLANK(L34),"",VLOOKUP(L34,A:N,14,FALSE))</f>
         <v/>
       </c>
-      <c r="N34" s="1" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="35" spans="1:14" ht="17" x14ac:dyDescent="0.2">
-      <c r="A35">
-        <v>34</v>
-      </c>
-      <c r="B35" t="s">
-        <v>38</v>
-      </c>
-      <c r="C35" t="s">
-        <v>79</v>
-      </c>
-      <c r="D35" t="s">
-        <v>84</v>
-      </c>
-      <c r="E35" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="F35" t="s">
+      <c r="N34" s="5" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="35" spans="1:14" s="3" customFormat="1" ht="34" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A35" s="3">
+        <v>54</v>
+      </c>
+      <c r="B35" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C35" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="E35" s="4" t="s">
+        <v>217</v>
+      </c>
+      <c r="F35" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="G35" t="s">
+      <c r="G35" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="H35" t="s">
+      <c r="H35" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="I35" s="1">
-        <f>VLOOKUP(F35,'Source lists'!$E$1:F35,2,FALSE)</f>
+      <c r="I35" s="5">
+        <f>VLOOKUP(F35,'Source lists'!$E$1:F36,2,FALSE)</f>
         <v>4</v>
       </c>
-      <c r="J35" s="1">
-        <f>VLOOKUP(G35,'Source lists'!$H$1:I36,2,FALSE)</f>
+      <c r="J35" s="5">
+        <f>VLOOKUP(G35,'Source lists'!$H$1:I37,2,FALSE)</f>
         <v>4</v>
       </c>
-      <c r="K35" s="1">
+      <c r="K35" s="5">
         <f>VLOOKUP(F35,'Source lists'!$E$2:$F$6,2,FALSE)*(VLOOKUP(G35,'Source lists'!$H$2:$I$7,2,FALSE)^2)/VLOOKUP(H35,'Source lists'!$K$2:$L$9,2,FALSE)</f>
         <v>32</v>
       </c>
-      <c r="M35" s="1" t="str">
+      <c r="M35" s="5" t="str">
         <f>IF(ISBLANK(L35),"",VLOOKUP(L35,A:N,14,FALSE))</f>
         <v/>
       </c>
-      <c r="N35" s="1" t="s">
-        <v>218</v>
+      <c r="N35" s="5" t="s">
+        <v>174</v>
       </c>
     </row>
     <row r="36" spans="1:14" ht="34" x14ac:dyDescent="0.2">
       <c r="A36">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B36" t="s">
         <v>1</v>
       </c>
       <c r="C36" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="E36" s="2" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="F36" t="s">
         <v>15</v>
@@ -10397,11 +10538,11 @@
         <v>23</v>
       </c>
       <c r="I36" s="1">
-        <f>VLOOKUP(F36,'Source lists'!$E$1:F36,2,FALSE)</f>
+        <f>VLOOKUP(F36,'Source lists'!$E$1:F37,2,FALSE)</f>
         <v>4</v>
       </c>
       <c r="J36" s="1">
-        <f>VLOOKUP(G36,'Source lists'!$H$1:I37,2,FALSE)</f>
+        <f>VLOOKUP(G36,'Source lists'!$H$1:I38,2,FALSE)</f>
         <v>4</v>
       </c>
       <c r="K36" s="1">
@@ -10413,21 +10554,21 @@
         <v/>
       </c>
       <c r="N36" s="1" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
     </row>
     <row r="37" spans="1:14" ht="34" x14ac:dyDescent="0.2">
       <c r="A37">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="B37" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C37" t="s">
-        <v>86</v>
+        <v>104</v>
       </c>
       <c r="E37" s="2" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="F37" t="s">
         <v>15</v>
@@ -10439,11 +10580,11 @@
         <v>23</v>
       </c>
       <c r="I37" s="1">
-        <f>VLOOKUP(F37,'Source lists'!$E$1:F37,2,FALSE)</f>
+        <f>VLOOKUP(F37,'Source lists'!$E$1:F38,2,FALSE)</f>
         <v>4</v>
       </c>
       <c r="J37" s="1">
-        <f>VLOOKUP(G37,'Source lists'!$H$1:I38,2,FALSE)</f>
+        <f>VLOOKUP(G37,'Source lists'!$H$1:I39,2,FALSE)</f>
         <v>4</v>
       </c>
       <c r="K37" s="1">
@@ -10455,21 +10596,21 @@
         <v/>
       </c>
       <c r="N37" s="1" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
     </row>
     <row r="38" spans="1:14" ht="68" x14ac:dyDescent="0.2">
       <c r="A38">
-        <v>58</v>
+        <v>67</v>
       </c>
       <c r="B38" t="s">
         <v>2</v>
       </c>
       <c r="C38" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E38" s="2" t="s">
-        <v>107</v>
+        <v>128</v>
       </c>
       <c r="F38" t="s">
         <v>15</v>
@@ -10481,11 +10622,11 @@
         <v>23</v>
       </c>
       <c r="I38" s="1">
-        <f>VLOOKUP(F38,'Source lists'!$E$1:F38,2,FALSE)</f>
+        <f>VLOOKUP(F38,'Source lists'!$E$1:F39,2,FALSE)</f>
         <v>4</v>
       </c>
       <c r="J38" s="1">
-        <f>VLOOKUP(G38,'Source lists'!$H$1:I39,2,FALSE)</f>
+        <f>VLOOKUP(G38,'Source lists'!$H$1:I40,2,FALSE)</f>
         <v>4</v>
       </c>
       <c r="K38" s="1">
@@ -10497,21 +10638,21 @@
         <v/>
       </c>
       <c r="N38" s="1" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
     </row>
     <row r="39" spans="1:14" ht="17" x14ac:dyDescent="0.2">
       <c r="A39">
-        <v>67</v>
+        <v>84</v>
       </c>
       <c r="B39" t="s">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="C39" t="s">
-        <v>105</v>
+        <v>148</v>
       </c>
       <c r="E39" s="2" t="s">
-        <v>129</v>
+        <v>149</v>
       </c>
       <c r="F39" t="s">
         <v>15</v>
@@ -10523,11 +10664,11 @@
         <v>23</v>
       </c>
       <c r="I39" s="1">
-        <f>VLOOKUP(F39,'Source lists'!$E$1:F39,2,FALSE)</f>
+        <f>VLOOKUP(F39,'Source lists'!$E$1:F40,2,FALSE)</f>
         <v>4</v>
       </c>
       <c r="J39" s="1">
-        <f>VLOOKUP(G39,'Source lists'!$H$1:I40,2,FALSE)</f>
+        <f>VLOOKUP(G39,'Source lists'!$H$1:I41,2,FALSE)</f>
         <v>4</v>
       </c>
       <c r="K39" s="1">
@@ -10539,21 +10680,21 @@
         <v/>
       </c>
       <c r="N39" s="1" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
     </row>
     <row r="40" spans="1:14" ht="34" x14ac:dyDescent="0.2">
       <c r="A40">
-        <v>84</v>
+        <v>89</v>
       </c>
       <c r="B40" t="s">
         <v>6</v>
       </c>
       <c r="C40" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="E40" s="2" t="s">
-        <v>150</v>
+        <v>155</v>
       </c>
       <c r="F40" t="s">
         <v>15</v>
@@ -10565,11 +10706,11 @@
         <v>23</v>
       </c>
       <c r="I40" s="1">
-        <f>VLOOKUP(F40,'Source lists'!$E$1:F40,2,FALSE)</f>
+        <f>VLOOKUP(F40,'Source lists'!$E$1:F41,2,FALSE)</f>
         <v>4</v>
       </c>
       <c r="J40" s="1">
-        <f>VLOOKUP(G40,'Source lists'!$H$1:I41,2,FALSE)</f>
+        <f>VLOOKUP(G40,'Source lists'!$H$1:I42,2,FALSE)</f>
         <v>4</v>
       </c>
       <c r="K40" s="1">
@@ -10581,21 +10722,21 @@
         <v/>
       </c>
       <c r="N40" s="1" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
     </row>
     <row r="41" spans="1:14" ht="17" x14ac:dyDescent="0.2">
       <c r="A41">
-        <v>89</v>
+        <v>107</v>
       </c>
       <c r="B41" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="C41" t="s">
-        <v>149</v>
+        <v>138</v>
       </c>
       <c r="E41" s="2" t="s">
-        <v>156</v>
+        <v>183</v>
       </c>
       <c r="F41" t="s">
         <v>15</v>
@@ -10607,11 +10748,11 @@
         <v>23</v>
       </c>
       <c r="I41" s="1">
-        <f>VLOOKUP(F41,'Source lists'!$E$1:F41,2,FALSE)</f>
+        <f>VLOOKUP(F41,'Source lists'!$E$1:F42,2,FALSE)</f>
         <v>4</v>
       </c>
       <c r="J41" s="1">
-        <f>VLOOKUP(G41,'Source lists'!$H$1:I42,2,FALSE)</f>
+        <f>VLOOKUP(G41,'Source lists'!$H$1:I43,2,FALSE)</f>
         <v>4</v>
       </c>
       <c r="K41" s="1">
@@ -10623,21 +10764,21 @@
         <v/>
       </c>
       <c r="N41" s="1" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
     </row>
     <row r="42" spans="1:14" ht="34" x14ac:dyDescent="0.2">
       <c r="A42">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="B42" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="C42" t="s">
-        <v>139</v>
+        <v>148</v>
       </c>
       <c r="E42" s="2" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="F42" t="s">
         <v>15</v>
@@ -10649,11 +10790,11 @@
         <v>23</v>
       </c>
       <c r="I42" s="1">
-        <f>VLOOKUP(F42,'Source lists'!$E$1:F42,2,FALSE)</f>
+        <f>VLOOKUP(F42,'Source lists'!$E$1:F43,2,FALSE)</f>
         <v>4</v>
       </c>
       <c r="J42" s="1">
-        <f>VLOOKUP(G42,'Source lists'!$H$1:I43,2,FALSE)</f>
+        <f>VLOOKUP(G42,'Source lists'!$H$1:I44,2,FALSE)</f>
         <v>4</v>
       </c>
       <c r="K42" s="1">
@@ -10665,21 +10806,24 @@
         <v/>
       </c>
       <c r="N42" s="1" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
     </row>
     <row r="43" spans="1:14" ht="34" x14ac:dyDescent="0.2">
       <c r="A43">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="B43" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C43" t="s">
-        <v>149</v>
+        <v>42</v>
+      </c>
+      <c r="D43" t="s">
+        <v>44</v>
       </c>
       <c r="E43" s="2" t="s">
-        <v>186</v>
+        <v>177</v>
       </c>
       <c r="F43" t="s">
         <v>15</v>
@@ -10691,71 +10835,70 @@
         <v>23</v>
       </c>
       <c r="I43" s="1">
-        <f>VLOOKUP(F43,'Source lists'!$E$1:F43,2,FALSE)</f>
+        <f>VLOOKUP(F43,'Source lists'!$E$1:F44,2,FALSE)</f>
         <v>4</v>
       </c>
       <c r="J43" s="1">
-        <f>VLOOKUP(G43,'Source lists'!$H$1:I44,2,FALSE)</f>
+        <f>VLOOKUP(G43,'Source lists'!$H$1:I45,2,FALSE)</f>
         <v>4</v>
       </c>
       <c r="K43" s="1">
         <f>VLOOKUP(F43,'Source lists'!$E$2:$F$6,2,FALSE)*(VLOOKUP(G43,'Source lists'!$H$2:$I$7,2,FALSE)^2)/VLOOKUP(H43,'Source lists'!$K$2:$L$9,2,FALSE)</f>
         <v>32</v>
       </c>
+      <c r="L43">
+        <v>8</v>
+      </c>
       <c r="M43" s="1" t="str">
         <f>IF(ISBLANK(L43),"",VLOOKUP(L43,A:N,14,FALSE))</f>
-        <v/>
+        <v>Done</v>
       </c>
       <c r="N43" s="1" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="44" spans="1:14" ht="17" x14ac:dyDescent="0.2">
-      <c r="A44">
-        <v>109</v>
-      </c>
-      <c r="B44" t="s">
-        <v>8</v>
-      </c>
-      <c r="C44" t="s">
-        <v>42</v>
-      </c>
-      <c r="D44" t="s">
-        <v>44</v>
-      </c>
-      <c r="E44" s="2" t="s">
-        <v>179</v>
-      </c>
-      <c r="F44" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="44" spans="1:14" ht="17" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A44" s="3">
+        <v>31</v>
+      </c>
+      <c r="B44" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C44" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="D44" s="3"/>
+      <c r="E44" s="4" t="s">
+        <v>113</v>
+      </c>
+      <c r="F44" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="G44" t="s">
+      <c r="G44" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="H44" t="s">
+      <c r="H44" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="I44" s="1">
-        <f>VLOOKUP(F44,'Source lists'!$E$1:F44,2,FALSE)</f>
+      <c r="I44" s="5">
+        <f>VLOOKUP(F44,'Source lists'!$E$1:F34,2,FALSE)</f>
         <v>4</v>
       </c>
-      <c r="J44" s="1">
-        <f>VLOOKUP(G44,'Source lists'!$H$1:I45,2,FALSE)</f>
+      <c r="J44" s="5">
+        <f>VLOOKUP(G44,'Source lists'!$H$1:I35,2,FALSE)</f>
         <v>4</v>
       </c>
-      <c r="K44" s="1">
+      <c r="K44" s="5">
         <f>VLOOKUP(F44,'Source lists'!$E$2:$F$6,2,FALSE)*(VLOOKUP(G44,'Source lists'!$H$2:$I$7,2,FALSE)^2)/VLOOKUP(H44,'Source lists'!$K$2:$L$9,2,FALSE)</f>
         <v>32</v>
       </c>
-      <c r="L44">
-        <v>8</v>
-      </c>
-      <c r="M44" s="1" t="str">
+      <c r="L44" s="3"/>
+      <c r="M44" s="5" t="str">
         <f>IF(ISBLANK(L44),"",VLOOKUP(L44,A:N,14,FALSE))</f>
-        <v>Done</v>
-      </c>
-      <c r="N44" s="1" t="s">
-        <v>218</v>
+        <v/>
+      </c>
+      <c r="N44" s="5" t="s">
+        <v>214</v>
       </c>
     </row>
     <row r="45" spans="1:14" ht="17" x14ac:dyDescent="0.2">
@@ -10769,7 +10912,7 @@
         <v>33</v>
       </c>
       <c r="D45" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="E45" s="2" t="s">
         <v>94</v>
@@ -10800,7 +10943,7 @@
         <v/>
       </c>
       <c r="N45" s="1" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
     </row>
     <row r="46" spans="1:14" ht="17" hidden="1" x14ac:dyDescent="0.2">
@@ -10846,7 +10989,7 @@
         <v/>
       </c>
       <c r="N46" s="5" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="47" spans="1:14" ht="17" hidden="1" x14ac:dyDescent="0.2">
@@ -10859,7 +11002,7 @@
       <c r="C47" s="3"/>
       <c r="D47" s="3"/>
       <c r="E47" s="4" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="F47" s="3" t="s">
         <v>16</v>
@@ -10888,7 +11031,7 @@
         <v/>
       </c>
       <c r="N47" s="5" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="48" spans="1:14" ht="34" x14ac:dyDescent="0.2">
@@ -10930,7 +11073,7 @@
         <v/>
       </c>
       <c r="N48" s="1" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
     </row>
     <row r="49" spans="1:14" ht="34" x14ac:dyDescent="0.2">
@@ -10950,7 +11093,7 @@
         <v>16</v>
       </c>
       <c r="G49" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="H49" t="s">
         <v>67</v>
@@ -10972,7 +11115,7 @@
         <v/>
       </c>
       <c r="N49" s="1" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
     </row>
     <row r="50" spans="1:14" ht="68" x14ac:dyDescent="0.2">
@@ -10992,7 +11135,7 @@
         <v>16</v>
       </c>
       <c r="G50" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="H50" t="s">
         <v>67</v>
@@ -11014,7 +11157,7 @@
         <v/>
       </c>
       <c r="N50" s="1" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
     </row>
     <row r="51" spans="1:14" ht="34" x14ac:dyDescent="0.2">
@@ -11056,7 +11199,7 @@
         <v/>
       </c>
       <c r="N51" s="1" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
     </row>
     <row r="52" spans="1:14" ht="17" x14ac:dyDescent="0.2">
@@ -11067,10 +11210,10 @@
         <v>2</v>
       </c>
       <c r="C52" t="s">
+        <v>104</v>
+      </c>
+      <c r="E52" s="2" t="s">
         <v>105</v>
-      </c>
-      <c r="E52" s="2" t="s">
-        <v>106</v>
       </c>
       <c r="F52" t="s">
         <v>16</v>
@@ -11098,7 +11241,7 @@
         <v/>
       </c>
       <c r="N52" s="1" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
     </row>
     <row r="53" spans="1:14" ht="34" x14ac:dyDescent="0.2">
@@ -11140,7 +11283,7 @@
         <v/>
       </c>
       <c r="N53" s="1" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
     </row>
     <row r="54" spans="1:14" ht="34" x14ac:dyDescent="0.2">
@@ -11151,13 +11294,13 @@
         <v>2</v>
       </c>
       <c r="C54" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="D54" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="E54" s="2" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="F54" t="s">
         <v>15</v>
@@ -11185,7 +11328,7 @@
         <v/>
       </c>
       <c r="N54" s="1" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
     </row>
     <row r="55" spans="1:14" ht="51" x14ac:dyDescent="0.2">
@@ -11196,10 +11339,10 @@
         <v>3</v>
       </c>
       <c r="C55" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="E55" s="2" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="F55" t="s">
         <v>15</v>
@@ -11227,7 +11370,7 @@
         <v/>
       </c>
       <c r="N55" s="1" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
     </row>
     <row r="56" spans="1:14" ht="51" x14ac:dyDescent="0.2">
@@ -11238,10 +11381,10 @@
         <v>2</v>
       </c>
       <c r="C56" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E56" s="2" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="F56" t="s">
         <v>15</v>
@@ -11269,7 +11412,7 @@
         <v/>
       </c>
       <c r="N56" s="1" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
     </row>
     <row r="57" spans="1:14" ht="51" x14ac:dyDescent="0.2">
@@ -11280,10 +11423,10 @@
         <v>3</v>
       </c>
       <c r="C57" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="E57" s="2" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="F57" t="s">
         <v>15</v>
@@ -11311,7 +11454,7 @@
         <v/>
       </c>
       <c r="N57" s="1" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
     </row>
     <row r="58" spans="1:14" ht="34" x14ac:dyDescent="0.2">
@@ -11322,10 +11465,10 @@
         <v>6</v>
       </c>
       <c r="C58" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="E58" s="2" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="F58" t="s">
         <v>15</v>
@@ -11353,7 +11496,7 @@
         <v/>
       </c>
       <c r="N58" s="1" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
     </row>
     <row r="59" spans="1:14" ht="34" x14ac:dyDescent="0.2">
@@ -11364,10 +11507,10 @@
         <v>6</v>
       </c>
       <c r="C59" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="E59" s="2" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="F59" t="s">
         <v>15</v>
@@ -11395,7 +11538,7 @@
         <v/>
       </c>
       <c r="N59" s="1" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
     </row>
     <row r="60" spans="1:14" ht="17" x14ac:dyDescent="0.2">
@@ -11418,7 +11561,7 @@
         <v>15</v>
       </c>
       <c r="G60" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="H60" t="s">
         <v>69</v>
@@ -11440,7 +11583,7 @@
         <v/>
       </c>
       <c r="N60" s="1" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
     </row>
     <row r="61" spans="1:14" ht="17" x14ac:dyDescent="0.2">
@@ -11463,7 +11606,7 @@
         <v>15</v>
       </c>
       <c r="G61" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="H61" t="s">
         <v>69</v>
@@ -11485,7 +11628,7 @@
         <v/>
       </c>
       <c r="N61" s="1" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
     </row>
     <row r="62" spans="1:14" ht="17" x14ac:dyDescent="0.2">
@@ -11508,7 +11651,7 @@
         <v>15</v>
       </c>
       <c r="G62" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="H62" t="s">
         <v>69</v>
@@ -11530,7 +11673,7 @@
         <v/>
       </c>
       <c r="N62" s="1" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
     </row>
     <row r="63" spans="1:14" ht="17" x14ac:dyDescent="0.2">
@@ -11553,7 +11696,7 @@
         <v>15</v>
       </c>
       <c r="G63" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="H63" t="s">
         <v>69</v>
@@ -11575,7 +11718,7 @@
         <v/>
       </c>
       <c r="N63" s="1" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
     </row>
     <row r="64" spans="1:14" ht="17" x14ac:dyDescent="0.2">
@@ -11598,7 +11741,7 @@
         <v>15</v>
       </c>
       <c r="G64" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="H64" t="s">
         <v>69</v>
@@ -11620,7 +11763,7 @@
         <v/>
       </c>
       <c r="N64" s="1" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
     </row>
     <row r="65" spans="1:14" ht="34" x14ac:dyDescent="0.2">
@@ -11631,16 +11774,16 @@
         <v>2</v>
       </c>
       <c r="C65" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E65" s="2" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="F65" t="s">
         <v>17</v>
       </c>
       <c r="G65" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="H65" t="s">
         <v>23</v>
@@ -11662,7 +11805,7 @@
         <v/>
       </c>
       <c r="N65" s="1" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
     </row>
     <row r="66" spans="1:14" ht="34" x14ac:dyDescent="0.2">
@@ -11673,16 +11816,16 @@
         <v>3</v>
       </c>
       <c r="C66" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="E66" s="2" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="F66" t="s">
         <v>17</v>
       </c>
       <c r="G66" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="H66" t="s">
         <v>23</v>
@@ -11704,7 +11847,7 @@
         <v/>
       </c>
       <c r="N66" s="1" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
     </row>
     <row r="67" spans="1:14" ht="34" x14ac:dyDescent="0.2">
@@ -11715,13 +11858,13 @@
         <v>2</v>
       </c>
       <c r="C67" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="D67" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="E67" s="2" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="F67" t="s">
         <v>15</v>
@@ -11749,10 +11892,10 @@
         <v/>
       </c>
       <c r="N67" s="1" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="68" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="68" spans="1:14" ht="17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A68">
         <v>91</v>
       </c>
@@ -11760,10 +11903,10 @@
         <v>4</v>
       </c>
       <c r="C68" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="E68" s="2" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="F68" t="s">
         <v>17</v>
@@ -11794,10 +11937,10 @@
         <v>To do</v>
       </c>
       <c r="N68" s="1" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="69" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="69" spans="1:14" ht="17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A69">
         <v>92</v>
       </c>
@@ -11805,10 +11948,10 @@
         <v>4</v>
       </c>
       <c r="C69" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="E69" s="2" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="F69" t="s">
         <v>17</v>
@@ -11839,10 +11982,10 @@
         <v>To do</v>
       </c>
       <c r="N69" s="1" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="70" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="70" spans="1:14" ht="17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A70">
         <v>93</v>
       </c>
@@ -11850,10 +11993,10 @@
         <v>4</v>
       </c>
       <c r="C70" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="E70" s="2" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="F70" t="s">
         <v>17</v>
@@ -11884,10 +12027,10 @@
         <v>To do</v>
       </c>
       <c r="N70" s="1" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="71" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="71" spans="1:14" ht="17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A71">
         <v>94</v>
       </c>
@@ -11895,10 +12038,10 @@
         <v>4</v>
       </c>
       <c r="C71" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="E71" s="2" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="F71" t="s">
         <v>17</v>
@@ -11929,10 +12072,10 @@
         <v>To do</v>
       </c>
       <c r="N71" s="1" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="72" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="72" spans="1:14" ht="17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A72">
         <v>95</v>
       </c>
@@ -11940,10 +12083,10 @@
         <v>4</v>
       </c>
       <c r="C72" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="E72" s="2" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="F72" t="s">
         <v>17</v>
@@ -11974,10 +12117,10 @@
         <v>To do</v>
       </c>
       <c r="N72" s="1" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="73" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="73" spans="1:14" ht="17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A73">
         <v>96</v>
       </c>
@@ -11985,10 +12128,10 @@
         <v>4</v>
       </c>
       <c r="C73" t="s">
+        <v>164</v>
+      </c>
+      <c r="E73" s="2" t="s">
         <v>165</v>
-      </c>
-      <c r="E73" s="2" t="s">
-        <v>166</v>
       </c>
       <c r="F73" t="s">
         <v>17</v>
@@ -12019,10 +12162,10 @@
         <v>To do</v>
       </c>
       <c r="N73" s="1" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="74" spans="1:14" ht="34" x14ac:dyDescent="0.2">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="74" spans="1:14" ht="34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A74">
         <v>97</v>
       </c>
@@ -12030,10 +12173,10 @@
         <v>5</v>
       </c>
       <c r="C74" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="E74" s="2" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="F74" t="s">
         <v>17</v>
@@ -12064,10 +12207,10 @@
         <v>To do</v>
       </c>
       <c r="N74" s="1" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="75" spans="1:14" ht="34" x14ac:dyDescent="0.2">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="75" spans="1:14" ht="34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A75">
         <v>98</v>
       </c>
@@ -12075,10 +12218,10 @@
         <v>5</v>
       </c>
       <c r="C75" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="E75" s="2" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="F75" t="s">
         <v>17</v>
@@ -12109,10 +12252,10 @@
         <v>To do</v>
       </c>
       <c r="N75" s="1" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="76" spans="1:14" ht="51" x14ac:dyDescent="0.2">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="76" spans="1:14" ht="51" hidden="1" x14ac:dyDescent="0.2">
       <c r="A76">
         <v>100</v>
       </c>
@@ -12120,10 +12263,10 @@
         <v>6</v>
       </c>
       <c r="C76" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="E76" s="2" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="F76" t="s">
         <v>17</v>
@@ -12154,10 +12297,10 @@
         <v>To do</v>
       </c>
       <c r="N76" s="1" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="77" spans="1:14" ht="34" x14ac:dyDescent="0.2">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="77" spans="1:14" ht="34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A77">
         <v>101</v>
       </c>
@@ -12165,10 +12308,10 @@
         <v>6</v>
       </c>
       <c r="C77" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="E77" s="2" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="F77" t="s">
         <v>17</v>
@@ -12199,10 +12342,10 @@
         <v>To do</v>
       </c>
       <c r="N77" s="1" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="78" spans="1:14" ht="51" x14ac:dyDescent="0.2">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="78" spans="1:14" ht="51" hidden="1" x14ac:dyDescent="0.2">
       <c r="A78">
         <v>103</v>
       </c>
@@ -12210,10 +12353,10 @@
         <v>5</v>
       </c>
       <c r="C78" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="E78" s="2" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="F78" t="s">
         <v>17</v>
@@ -12244,10 +12387,10 @@
         <v>To do</v>
       </c>
       <c r="N78" s="1" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="79" spans="1:14" ht="34" x14ac:dyDescent="0.2">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="79" spans="1:14" ht="34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A79">
         <v>104</v>
       </c>
@@ -12255,10 +12398,10 @@
         <v>5</v>
       </c>
       <c r="C79" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="E79" s="2" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="F79" t="s">
         <v>17</v>
@@ -12289,7 +12432,7 @@
         <v>To do</v>
       </c>
       <c r="N79" s="1" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
     </row>
     <row r="80" spans="1:14" ht="34" x14ac:dyDescent="0.2">
@@ -12331,7 +12474,7 @@
         <v/>
       </c>
       <c r="N80" s="1" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
     </row>
     <row r="81" spans="1:14" ht="34" x14ac:dyDescent="0.2">
@@ -12345,7 +12488,7 @@
         <v>86</v>
       </c>
       <c r="E81" s="2" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="F81" t="s">
         <v>16</v>
@@ -12373,7 +12516,7 @@
         <v/>
       </c>
       <c r="N81" s="1" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
     </row>
     <row r="82" spans="1:14" ht="34" x14ac:dyDescent="0.2">
@@ -12384,13 +12527,13 @@
         <v>2</v>
       </c>
       <c r="C82" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="D82" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="E82" s="2" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="F82" t="s">
         <v>16</v>
@@ -12418,7 +12561,7 @@
         <v/>
       </c>
       <c r="N82" s="1" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
     </row>
     <row r="83" spans="1:14" ht="34" x14ac:dyDescent="0.2">
@@ -12429,13 +12572,13 @@
         <v>2</v>
       </c>
       <c r="C83" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="D83" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="E83" s="2" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="F83" t="s">
         <v>16</v>
@@ -12463,7 +12606,7 @@
         <v/>
       </c>
       <c r="N83" s="1" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
     </row>
     <row r="84" spans="1:14" ht="17" x14ac:dyDescent="0.2">
@@ -12474,10 +12617,10 @@
         <v>6</v>
       </c>
       <c r="C84" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="E84" s="2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="F84" t="s">
         <v>16</v>
@@ -12505,7 +12648,7 @@
         <v/>
       </c>
       <c r="N84" s="1" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
     </row>
     <row r="85" spans="1:14" ht="17" x14ac:dyDescent="0.2">
@@ -12516,10 +12659,10 @@
         <v>6</v>
       </c>
       <c r="C85" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="E85" s="2" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="F85" t="s">
         <v>16</v>
@@ -12547,7 +12690,7 @@
         <v/>
       </c>
       <c r="N85" s="1" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
     </row>
     <row r="86" spans="1:14" ht="17" x14ac:dyDescent="0.2">
@@ -12592,7 +12735,7 @@
         <v/>
       </c>
       <c r="N86" s="1" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
     </row>
     <row r="87" spans="1:14" ht="17" x14ac:dyDescent="0.2">
@@ -12637,7 +12780,7 @@
         <v/>
       </c>
       <c r="N87" s="1" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
     </row>
     <row r="88" spans="1:14" ht="34" x14ac:dyDescent="0.2">
@@ -12651,10 +12794,10 @@
         <v>90</v>
       </c>
       <c r="D88" t="s">
+        <v>110</v>
+      </c>
+      <c r="E88" s="2" t="s">
         <v>111</v>
-      </c>
-      <c r="E88" s="2" t="s">
-        <v>112</v>
       </c>
       <c r="F88" t="s">
         <v>15</v>
@@ -12682,7 +12825,7 @@
         <v/>
       </c>
       <c r="N88" s="1" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
     </row>
     <row r="89" spans="1:14" ht="34" x14ac:dyDescent="0.2">
@@ -12696,7 +12839,7 @@
         <v>90</v>
       </c>
       <c r="D89" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E89" s="2" t="s">
         <v>100</v>
@@ -12727,7 +12870,7 @@
         <v/>
       </c>
       <c r="N89" s="1" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
     </row>
     <row r="90" spans="1:14" ht="34" x14ac:dyDescent="0.2">
@@ -12741,7 +12884,7 @@
         <v>90</v>
       </c>
       <c r="E90" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="F90" t="s">
         <v>15</v>
@@ -12769,7 +12912,7 @@
         <v/>
       </c>
       <c r="N90" s="1" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
     </row>
     <row r="91" spans="1:14" ht="119" x14ac:dyDescent="0.2">
@@ -12814,7 +12957,7 @@
         <v/>
       </c>
       <c r="N91" s="1" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
     </row>
     <row r="92" spans="1:14" ht="68" x14ac:dyDescent="0.2">
@@ -12828,7 +12971,7 @@
         <v>103</v>
       </c>
       <c r="E92" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="F92" t="s">
         <v>17</v>
@@ -12856,7 +12999,7 @@
         <v/>
       </c>
       <c r="N92" s="1" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
     </row>
     <row r="93" spans="1:14" ht="51" x14ac:dyDescent="0.2">
@@ -12867,10 +13010,10 @@
         <v>2</v>
       </c>
       <c r="C93" t="s">
+        <v>126</v>
+      </c>
+      <c r="E93" s="2" t="s">
         <v>127</v>
-      </c>
-      <c r="E93" s="2" t="s">
-        <v>128</v>
       </c>
       <c r="F93" t="s">
         <v>17</v>
@@ -12898,7 +13041,7 @@
         <v/>
       </c>
       <c r="N93" s="1" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
     </row>
     <row r="94" spans="1:14" ht="34" x14ac:dyDescent="0.2">
@@ -12909,10 +13052,10 @@
         <v>4</v>
       </c>
       <c r="C94" t="s">
+        <v>146</v>
+      </c>
+      <c r="E94" s="2" t="s">
         <v>147</v>
-      </c>
-      <c r="E94" s="2" t="s">
-        <v>148</v>
       </c>
       <c r="F94" t="s">
         <v>17</v>
@@ -12940,7 +13083,7 @@
         <v/>
       </c>
       <c r="N94" s="1" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
     </row>
     <row r="95" spans="1:14" ht="119" x14ac:dyDescent="0.2">
@@ -12951,10 +13094,10 @@
         <v>5</v>
       </c>
       <c r="C95" t="s">
+        <v>168</v>
+      </c>
+      <c r="E95" s="2" t="s">
         <v>169</v>
-      </c>
-      <c r="E95" s="2" t="s">
-        <v>170</v>
       </c>
       <c r="F95" t="s">
         <v>17</v>
@@ -12982,7 +13125,7 @@
         <v/>
       </c>
       <c r="N95" s="1" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
     </row>
     <row r="96" spans="1:14" ht="68" x14ac:dyDescent="0.2">
@@ -12993,10 +13136,10 @@
         <v>8</v>
       </c>
       <c r="C96" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="E96" s="2" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="F96" t="s">
         <v>17</v>
@@ -13024,7 +13167,7 @@
         <v/>
       </c>
       <c r="N96" s="1" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
     </row>
     <row r="97" spans="1:14" ht="68" x14ac:dyDescent="0.2">
@@ -13038,7 +13181,7 @@
         <v>81</v>
       </c>
       <c r="E97" s="2" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="F97" t="s">
         <v>17</v>
@@ -13066,7 +13209,7 @@
         <v/>
       </c>
       <c r="N97" s="1" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
     </row>
     <row r="98" spans="1:14" ht="17" x14ac:dyDescent="0.2">
@@ -13077,7 +13220,7 @@
         <v>7</v>
       </c>
       <c r="E98" s="2" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="F98" t="s">
         <v>17</v>
@@ -13105,7 +13248,7 @@
         <v/>
       </c>
       <c r="N98" s="1" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
     </row>
     <row r="99" spans="1:14" ht="17" x14ac:dyDescent="0.2">
@@ -13113,10 +13256,10 @@
         <v>63</v>
       </c>
       <c r="B99" t="s">
+        <v>121</v>
+      </c>
+      <c r="E99" s="2" t="s">
         <v>122</v>
-      </c>
-      <c r="E99" s="2" t="s">
-        <v>123</v>
       </c>
       <c r="F99" t="s">
         <v>17</v>
@@ -13144,7 +13287,7 @@
         <v/>
       </c>
       <c r="N99" s="1" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
     </row>
     <row r="100" spans="1:14" ht="119" x14ac:dyDescent="0.2">
@@ -13155,10 +13298,10 @@
         <v>5</v>
       </c>
       <c r="C100" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="E100" s="2" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="F100" t="s">
         <v>17</v>
@@ -13186,7 +13329,7 @@
         <v/>
       </c>
       <c r="N100" s="1" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
     </row>
     <row r="101" spans="1:14" ht="51" x14ac:dyDescent="0.2">
@@ -13194,13 +13337,13 @@
         <v>99</v>
       </c>
       <c r="B101" t="s">
+        <v>166</v>
+      </c>
+      <c r="C101" t="s">
         <v>167</v>
       </c>
-      <c r="C101" t="s">
-        <v>168</v>
-      </c>
       <c r="E101" s="2" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="F101" t="s">
         <v>17</v>
@@ -13228,7 +13371,7 @@
         <v/>
       </c>
       <c r="N101" s="1" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
     </row>
     <row r="102" spans="1:14" ht="17" x14ac:dyDescent="0.2">
@@ -13273,7 +13416,7 @@
         <v/>
       </c>
       <c r="N102" s="1" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
     </row>
     <row r="103" spans="1:14" ht="34" x14ac:dyDescent="0.2">
@@ -13315,7 +13458,7 @@
         <v/>
       </c>
       <c r="N103" s="1" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
     </row>
     <row r="104" spans="1:14" ht="34" x14ac:dyDescent="0.2">
@@ -13329,7 +13472,7 @@
         <v>86</v>
       </c>
       <c r="E104" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="F104" t="s">
         <v>16</v>
@@ -13357,7 +13500,7 @@
         <v/>
       </c>
       <c r="N104" s="1" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
     </row>
     <row r="105" spans="1:14" ht="17" x14ac:dyDescent="0.2">
@@ -13399,7 +13542,7 @@
         <v/>
       </c>
       <c r="N105" s="1" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
     </row>
     <row r="106" spans="1:14" ht="34" x14ac:dyDescent="0.2">
@@ -13441,7 +13584,7 @@
         <v/>
       </c>
       <c r="N106" s="1" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
     </row>
     <row r="107" spans="1:14" ht="17" x14ac:dyDescent="0.2">
@@ -13452,16 +13595,16 @@
         <v>2</v>
       </c>
       <c r="C107" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="E107" s="2" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="F107" t="s">
         <v>17</v>
       </c>
       <c r="G107" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="H107" t="s">
         <v>67</v>
@@ -13483,7 +13626,7 @@
         <v/>
       </c>
       <c r="N107" s="1" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
     </row>
     <row r="108" spans="1:14" ht="17" x14ac:dyDescent="0.2">
@@ -13494,16 +13637,16 @@
         <v>2</v>
       </c>
       <c r="C108" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="E108" s="2" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="F108" t="s">
         <v>17</v>
       </c>
       <c r="G108" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="H108" t="s">
         <v>67</v>
@@ -13525,7 +13668,7 @@
         <v/>
       </c>
       <c r="N108" s="1" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
     </row>
     <row r="109" spans="1:14" ht="17" x14ac:dyDescent="0.2">
@@ -13536,16 +13679,16 @@
         <v>2</v>
       </c>
       <c r="C109" t="s">
+        <v>129</v>
+      </c>
+      <c r="E109" s="2" t="s">
         <v>130</v>
-      </c>
-      <c r="E109" s="2" t="s">
-        <v>131</v>
       </c>
       <c r="F109" t="s">
         <v>17</v>
       </c>
       <c r="G109" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="H109" t="s">
         <v>67</v>
@@ -13567,7 +13710,7 @@
         <v/>
       </c>
       <c r="N109" s="1" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
     </row>
     <row r="110" spans="1:14" ht="119" x14ac:dyDescent="0.2">
@@ -13578,19 +13721,19 @@
         <v>2</v>
       </c>
       <c r="C110" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="D110" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="E110" s="2" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="F110" t="s">
         <v>17</v>
       </c>
       <c r="G110" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="H110" t="s">
         <v>67</v>
@@ -13612,7 +13755,7 @@
         <v/>
       </c>
       <c r="N110" s="1" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
     </row>
     <row r="111" spans="1:14" ht="17" x14ac:dyDescent="0.2">
@@ -13623,16 +13766,16 @@
         <v>3</v>
       </c>
       <c r="C111" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="E111" s="2" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="F111" t="s">
         <v>17</v>
       </c>
       <c r="G111" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="H111" t="s">
         <v>67</v>
@@ -13654,7 +13797,7 @@
         <v/>
       </c>
       <c r="N111" s="1" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
     </row>
     <row r="112" spans="1:14" ht="34" x14ac:dyDescent="0.2">
@@ -13665,7 +13808,7 @@
         <v>74</v>
       </c>
       <c r="E112" s="2" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="F112" t="s">
         <v>16</v>
@@ -13693,7 +13836,7 @@
         <v/>
       </c>
       <c r="N112" s="1" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
     </row>
     <row r="113" spans="1:14" ht="34" x14ac:dyDescent="0.2">
@@ -13735,7 +13878,7 @@
         <v/>
       </c>
       <c r="N113" s="1" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
     </row>
     <row r="114" spans="1:14" ht="34" x14ac:dyDescent="0.2">
@@ -13777,7 +13920,7 @@
         <v/>
       </c>
       <c r="N114" s="1" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
     </row>
     <row r="115" spans="1:14" ht="34" x14ac:dyDescent="0.2">
@@ -13788,10 +13931,10 @@
         <v>2</v>
       </c>
       <c r="C115" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="E115" s="2" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="F115" t="s">
         <v>15</v>
@@ -13819,10 +13962,10 @@
         <v/>
       </c>
       <c r="N115" s="1" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="116" spans="1:14" ht="34" x14ac:dyDescent="0.2">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="116" spans="1:14" ht="34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A116">
         <v>29</v>
       </c>
@@ -13864,10 +14007,10 @@
         <v>To do</v>
       </c>
       <c r="N116" s="1" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="117" spans="1:14" ht="34" x14ac:dyDescent="0.2">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="117" spans="1:14" ht="34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A117">
         <v>30</v>
       </c>
@@ -13906,7 +14049,7 @@
         <v>To do</v>
       </c>
       <c r="N117" s="1" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
     </row>
     <row r="118" spans="1:14" s="3" customFormat="1" ht="34" x14ac:dyDescent="0.2">
@@ -13950,17 +14093,22 @@
         <v/>
       </c>
       <c r="N118" s="1" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:N118" xr:uid="{1EB57299-5CFD-7049-BDE4-6415040FFB14}">
+    <filterColumn colId="12">
+      <filters blank="1">
+        <filter val="Done"/>
+      </filters>
+    </filterColumn>
     <filterColumn colId="13">
       <filters>
         <filter val="To do"/>
       </filters>
     </filterColumn>
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:N118">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A34:N118">
       <sortCondition descending="1" ref="K1:K118"/>
     </sortState>
   </autoFilter>

</xml_diff>

<commit_message>
e-Questrain/finance/invoice-detail: Invoice details now has a summary section with a sub-total, VAT and Total. Also took to restructure finance page as its own module with its own routing
</commit_message>
<xml_diff>
--- a/apps/e-questrian/e-Questrian - To do list.xlsx
+++ b/apps/e-questrian/e-Questrian - To do list.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rferreira/sigmafox/apps/e-questrian/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE023CAE-9D22-F241-9DB3-E628F3A796BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7DED31E2-BBD4-1F44-BBD3-2D88DB278BB3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="19820" activeTab="2" xr2:uid="{DC2B379E-A936-2146-8C4F-53C43AECE05C}"/>
   </bookViews>
@@ -22,7 +22,7 @@
   </definedNames>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="4" r:id="rId4"/>
+    <pivotCache cacheId="13" r:id="rId4"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -821,7 +821,7 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Ruben Ferreira" refreshedDate="45321.401953703702" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="119" xr:uid="{AEB2BF63-68F2-404E-AE9B-E794DFB00774}">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Ruben Ferreira" refreshedDate="45321.408745949077" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="118" xr:uid="{AEB2BF63-68F2-404E-AE9B-E794DFB00774}">
   <cacheSource type="worksheet">
     <worksheetSource ref="A1:N1048576" sheet="Issues 3-1-24"/>
   </cacheSource>
@@ -883,7 +883,7 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheRecords1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" count="119">
+<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" count="118">
   <r>
     <n v="53"/>
     <s v="Calendar/Appointments"/>
@@ -1417,7 +1417,7 @@
     <s v="Calendar/Appointments"/>
     <s v="Appointments modal"/>
     <m/>
-    <s v="Invoices appointments should display the invoice number when the details are views - not to be edited"/>
+    <s v="Invoiced appointments should display the invoice number when the details are viewed - not to be editable"/>
     <s v="Poor UX"/>
     <s v="Improved UX"/>
     <s v="Minor change to current component"/>
@@ -1426,7 +1426,7 @@
     <n v="32"/>
     <m/>
     <s v=""/>
-    <x v="1"/>
+    <x v="0"/>
   </r>
   <r>
     <n v="55"/>
@@ -1442,7 +1442,7 @@
     <n v="32"/>
     <m/>
     <s v=""/>
-    <x v="1"/>
+    <x v="0"/>
   </r>
   <r>
     <n v="58"/>
@@ -2772,27 +2772,11 @@
     <m/>
     <x v="3"/>
   </r>
-  <r>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <x v="3"/>
-  </r>
 </pivotCacheRecords>
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{936C0618-B7B4-0144-93D9-409C5361BBD7}" name="PivotTable7" cacheId="4" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{936C0618-B7B4-0144-93D9-409C5361BBD7}" name="PivotTable7" cacheId="13" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A7:E9" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="14">
     <pivotField showAll="0"/>
@@ -2854,7 +2838,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{4A183E6E-2837-3A40-90CB-E731BF47E9C0}" name="PivotTable6" cacheId="4" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{4A183E6E-2837-3A40-90CB-E731BF47E9C0}" name="PivotTable6" cacheId="13" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A1:E3" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="14">
     <pivotField showAll="0"/>
@@ -2916,7 +2900,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{4DCC3165-0959-AA43-80CF-D9170B1DCB64}" name="PivotTable8" cacheId="4" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{4DCC3165-0959-AA43-80CF-D9170B1DCB64}" name="PivotTable8" cacheId="13" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A13:E15" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="14">
     <pivotField showAll="0"/>
@@ -3277,7 +3261,7 @@
   <dimension ref="A1:E17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3315,22 +3299,22 @@
         <v>203</v>
       </c>
       <c r="B3" s="8">
-        <v>1607.4000000000003</v>
+        <v>1671.4000000000003</v>
       </c>
       <c r="C3" s="8">
         <v>103.2</v>
       </c>
       <c r="D3" s="8">
-        <v>1516.9976190476186</v>
+        <v>1452.9976190476191</v>
       </c>
       <c r="E3" s="8">
-        <v>3227.597619047619</v>
+        <v>3227.5976190476194</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="E5" s="7">
         <f>SUM(B3:C3)/GETPIVOTDATA("Priority S",$A$1)</f>
-        <v>0.52999171579038229</v>
+        <v>0.54982070550778228</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
@@ -3359,13 +3343,13 @@
         <v>180</v>
       </c>
       <c r="B9" s="8">
-        <v>149</v>
+        <v>157</v>
       </c>
       <c r="C9" s="8">
         <v>12</v>
       </c>
       <c r="D9" s="8">
-        <v>211</v>
+        <v>203</v>
       </c>
       <c r="E9" s="8">
         <v>372</v>
@@ -3374,7 +3358,7 @@
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="E11" s="7">
         <f>SUM(B9:C9)/GETPIVOTDATA("Importance S",$A$7)</f>
-        <v>0.43279569892473119</v>
+        <v>0.45430107526881719</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
@@ -3403,13 +3387,13 @@
         <v>181</v>
       </c>
       <c r="B15" s="8">
-        <v>153</v>
+        <v>161</v>
       </c>
       <c r="C15" s="8">
         <v>15</v>
       </c>
       <c r="D15" s="8">
-        <v>512</v>
+        <v>504</v>
       </c>
       <c r="E15" s="8">
         <v>680</v>
@@ -3418,7 +3402,7 @@
     <row r="17" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E17" s="7">
         <f>SUM(B15:C15)/GETPIVOTDATA("Impact S",$A$13)</f>
-        <v>0.24705882352941178</v>
+        <v>0.25882352941176473</v>
       </c>
     </row>
   </sheetData>
@@ -3857,7 +3841,7 @@
   <dimension ref="A1:XEY118"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="D37" sqref="D37"/>
+      <selection activeCell="E37" sqref="E37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="34.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -9536,7 +9520,7 @@
         <v>62</v>
       </c>
       <c r="M14" s="1" t="str">
-        <f t="shared" ref="M14:M45" si="1">IF(ISBLANK(L14),"",VLOOKUP(L14,A:N,14,FALSE))</f>
+        <f t="shared" ref="M14:M33" si="1">IF(ISBLANK(L14),"",VLOOKUP(L14,A:N,14,FALSE))</f>
         <v>To do</v>
       </c>
       <c r="N14" s="1" t="s">
@@ -10466,7 +10450,7 @@
         <v>32</v>
       </c>
       <c r="M34" s="5" t="str">
-        <f>IF(ISBLANK(L34),"",VLOOKUP(L34,A:N,14,FALSE))</f>
+        <f t="shared" ref="M34:M65" si="2">IF(ISBLANK(L34),"",VLOOKUP(L34,A:N,14,FALSE))</f>
         <v/>
       </c>
       <c r="N34" s="5" t="s">
@@ -10508,56 +10492,56 @@
         <v>32</v>
       </c>
       <c r="M35" s="5" t="str">
-        <f>IF(ISBLANK(L35),"",VLOOKUP(L35,A:N,14,FALSE))</f>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="N35" s="5" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="36" spans="1:14" ht="34" x14ac:dyDescent="0.2">
-      <c r="A36">
+    <row r="36" spans="1:14" s="3" customFormat="1" ht="34" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A36" s="3">
         <v>55</v>
       </c>
-      <c r="B36" t="s">
+      <c r="B36" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C36" t="s">
+      <c r="C36" s="3" t="s">
         <v>86</v>
       </c>
-      <c r="E36" s="2" t="s">
+      <c r="E36" s="4" t="s">
         <v>107</v>
       </c>
-      <c r="F36" t="s">
+      <c r="F36" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="G36" t="s">
+      <c r="G36" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="H36" t="s">
+      <c r="H36" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="I36" s="1">
+      <c r="I36" s="5">
         <f>VLOOKUP(F36,'Source lists'!$E$1:F37,2,FALSE)</f>
         <v>4</v>
       </c>
-      <c r="J36" s="1">
+      <c r="J36" s="5">
         <f>VLOOKUP(G36,'Source lists'!$H$1:I38,2,FALSE)</f>
         <v>4</v>
       </c>
-      <c r="K36" s="1">
+      <c r="K36" s="5">
         <f>VLOOKUP(F36,'Source lists'!$E$2:$F$6,2,FALSE)*(VLOOKUP(G36,'Source lists'!$H$2:$I$7,2,FALSE)^2)/VLOOKUP(H36,'Source lists'!$K$2:$L$9,2,FALSE)</f>
         <v>32</v>
       </c>
-      <c r="M36" s="1" t="str">
-        <f>IF(ISBLANK(L36),"",VLOOKUP(L36,A:N,14,FALSE))</f>
+      <c r="M36" s="5" t="str">
+        <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="N36" s="1" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="37" spans="1:14" ht="34" x14ac:dyDescent="0.2">
+      <c r="N36" s="5" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="37" spans="1:14" ht="68" x14ac:dyDescent="0.2">
       <c r="A37">
         <v>58</v>
       </c>
@@ -10592,7 +10576,7 @@
         <v>32</v>
       </c>
       <c r="M37" s="1" t="str">
-        <f>IF(ISBLANK(L37),"",VLOOKUP(L37,A:N,14,FALSE))</f>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="N37" s="1" t="s">
@@ -10634,7 +10618,7 @@
         <v>32</v>
       </c>
       <c r="M38" s="1" t="str">
-        <f>IF(ISBLANK(L38),"",VLOOKUP(L38,A:N,14,FALSE))</f>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="N38" s="1" t="s">
@@ -10676,7 +10660,7 @@
         <v>32</v>
       </c>
       <c r="M39" s="1" t="str">
-        <f>IF(ISBLANK(L39),"",VLOOKUP(L39,A:N,14,FALSE))</f>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="N39" s="1" t="s">
@@ -10718,7 +10702,7 @@
         <v>32</v>
       </c>
       <c r="M40" s="1" t="str">
-        <f>IF(ISBLANK(L40),"",VLOOKUP(L40,A:N,14,FALSE))</f>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="N40" s="1" t="s">
@@ -10760,7 +10744,7 @@
         <v>32</v>
       </c>
       <c r="M41" s="1" t="str">
-        <f>IF(ISBLANK(L41),"",VLOOKUP(L41,A:N,14,FALSE))</f>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="N41" s="1" t="s">
@@ -10802,7 +10786,7 @@
         <v>32</v>
       </c>
       <c r="M42" s="1" t="str">
-        <f>IF(ISBLANK(L42),"",VLOOKUP(L42,A:N,14,FALSE))</f>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="N42" s="1" t="s">
@@ -10850,7 +10834,7 @@
         <v>8</v>
       </c>
       <c r="M43" s="1" t="str">
-        <f>IF(ISBLANK(L43),"",VLOOKUP(L43,A:N,14,FALSE))</f>
+        <f t="shared" si="2"/>
         <v>Done</v>
       </c>
       <c r="N43" s="1" t="s">
@@ -10894,7 +10878,7 @@
       </c>
       <c r="L44" s="3"/>
       <c r="M44" s="5" t="str">
-        <f>IF(ISBLANK(L44),"",VLOOKUP(L44,A:N,14,FALSE))</f>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="N44" s="5" t="s">
@@ -10939,7 +10923,7 @@
         <v>29.4</v>
       </c>
       <c r="M45" s="1" t="str">
-        <f>IF(ISBLANK(L45),"",VLOOKUP(L45,A:N,14,FALSE))</f>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="N45" s="1" t="s">
@@ -10985,7 +10969,7 @@
       </c>
       <c r="L46" s="3"/>
       <c r="M46" s="5" t="str">
-        <f>IF(ISBLANK(L46),"",VLOOKUP(L46,A:N,14,FALSE))</f>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="N46" s="5" t="s">
@@ -11027,7 +11011,7 @@
       </c>
       <c r="L47" s="3"/>
       <c r="M47" s="5" t="str">
-        <f>IF(ISBLANK(L47),"",VLOOKUP(L47,A:N,14,FALSE))</f>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="N47" s="5" t="s">
@@ -11069,7 +11053,7 @@
         <v>27</v>
       </c>
       <c r="M48" s="1" t="str">
-        <f>IF(ISBLANK(L48),"",VLOOKUP(L48,A:N,14,FALSE))</f>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="N48" s="1" t="s">
@@ -11111,7 +11095,7 @@
         <v>27</v>
       </c>
       <c r="M49" s="1" t="str">
-        <f>IF(ISBLANK(L49),"",VLOOKUP(L49,A:N,14,FALSE))</f>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="N49" s="1" t="s">
@@ -11153,7 +11137,7 @@
         <v>27</v>
       </c>
       <c r="M50" s="1" t="str">
-        <f>IF(ISBLANK(L50),"",VLOOKUP(L50,A:N,14,FALSE))</f>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="N50" s="1" t="s">
@@ -11195,7 +11179,7 @@
         <v>27</v>
       </c>
       <c r="M51" s="1" t="str">
-        <f>IF(ISBLANK(L51),"",VLOOKUP(L51,A:N,14,FALSE))</f>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="N51" s="1" t="s">
@@ -11237,7 +11221,7 @@
         <v>27</v>
       </c>
       <c r="M52" s="1" t="str">
-        <f>IF(ISBLANK(L52),"",VLOOKUP(L52,A:N,14,FALSE))</f>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="N52" s="1" t="s">
@@ -11279,7 +11263,7 @@
         <v>21.333333333333332</v>
       </c>
       <c r="M53" s="1" t="str">
-        <f>IF(ISBLANK(L53),"",VLOOKUP(L53,A:N,14,FALSE))</f>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="N53" s="1" t="s">
@@ -11324,7 +11308,7 @@
         <v>21.333333333333332</v>
       </c>
       <c r="M54" s="1" t="str">
-        <f>IF(ISBLANK(L54),"",VLOOKUP(L54,A:N,14,FALSE))</f>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="N54" s="1" t="s">
@@ -11366,7 +11350,7 @@
         <v>21.333333333333332</v>
       </c>
       <c r="M55" s="1" t="str">
-        <f>IF(ISBLANK(L55),"",VLOOKUP(L55,A:N,14,FALSE))</f>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="N55" s="1" t="s">
@@ -11408,7 +11392,7 @@
         <v>21.333333333333332</v>
       </c>
       <c r="M56" s="1" t="str">
-        <f>IF(ISBLANK(L56),"",VLOOKUP(L56,A:N,14,FALSE))</f>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="N56" s="1" t="s">
@@ -11450,7 +11434,7 @@
         <v>21.333333333333332</v>
       </c>
       <c r="M57" s="1" t="str">
-        <f>IF(ISBLANK(L57),"",VLOOKUP(L57,A:N,14,FALSE))</f>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="N57" s="1" t="s">
@@ -11492,7 +11476,7 @@
         <v>21.333333333333332</v>
       </c>
       <c r="M58" s="1" t="str">
-        <f>IF(ISBLANK(L58),"",VLOOKUP(L58,A:N,14,FALSE))</f>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="N58" s="1" t="s">
@@ -11534,7 +11518,7 @@
         <v>21.333333333333332</v>
       </c>
       <c r="M59" s="1" t="str">
-        <f>IF(ISBLANK(L59),"",VLOOKUP(L59,A:N,14,FALSE))</f>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="N59" s="1" t="s">
@@ -11579,7 +11563,7 @@
         <v>20.571428571428573</v>
       </c>
       <c r="M60" s="1" t="str">
-        <f>IF(ISBLANK(L60),"",VLOOKUP(L60,A:N,14,FALSE))</f>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="N60" s="1" t="s">
@@ -11624,7 +11608,7 @@
         <v>20.571428571428573</v>
       </c>
       <c r="M61" s="1" t="str">
-        <f>IF(ISBLANK(L61),"",VLOOKUP(L61,A:N,14,FALSE))</f>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="N61" s="1" t="s">
@@ -11669,7 +11653,7 @@
         <v>20.571428571428573</v>
       </c>
       <c r="M62" s="1" t="str">
-        <f>IF(ISBLANK(L62),"",VLOOKUP(L62,A:N,14,FALSE))</f>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="N62" s="1" t="s">
@@ -11714,7 +11698,7 @@
         <v>20.571428571428573</v>
       </c>
       <c r="M63" s="1" t="str">
-        <f>IF(ISBLANK(L63),"",VLOOKUP(L63,A:N,14,FALSE))</f>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="N63" s="1" t="s">
@@ -11759,7 +11743,7 @@
         <v>20.571428571428573</v>
       </c>
       <c r="M64" s="1" t="str">
-        <f>IF(ISBLANK(L64),"",VLOOKUP(L64,A:N,14,FALSE))</f>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="N64" s="1" t="s">
@@ -11801,7 +11785,7 @@
         <v>18</v>
       </c>
       <c r="M65" s="1" t="str">
-        <f>IF(ISBLANK(L65),"",VLOOKUP(L65,A:N,14,FALSE))</f>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="N65" s="1" t="s">
@@ -11843,7 +11827,7 @@
         <v>18</v>
       </c>
       <c r="M66" s="1" t="str">
-        <f>IF(ISBLANK(L66),"",VLOOKUP(L66,A:N,14,FALSE))</f>
+        <f t="shared" ref="M66:M97" si="3">IF(ISBLANK(L66),"",VLOOKUP(L66,A:N,14,FALSE))</f>
         <v/>
       </c>
       <c r="N66" s="1" t="s">
@@ -11888,7 +11872,7 @@
         <v>16</v>
       </c>
       <c r="M67" s="1" t="str">
-        <f>IF(ISBLANK(L67),"",VLOOKUP(L67,A:N,14,FALSE))</f>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="N67" s="1" t="s">
@@ -11933,7 +11917,7 @@
         <v>59</v>
       </c>
       <c r="M68" s="1" t="str">
-        <f>IF(ISBLANK(L68),"",VLOOKUP(L68,A:N,14,FALSE))</f>
+        <f t="shared" si="3"/>
         <v>To do</v>
       </c>
       <c r="N68" s="1" t="s">
@@ -11978,7 +11962,7 @@
         <v>64</v>
       </c>
       <c r="M69" s="1" t="str">
-        <f>IF(ISBLANK(L69),"",VLOOKUP(L69,A:N,14,FALSE))</f>
+        <f t="shared" si="3"/>
         <v>To do</v>
       </c>
       <c r="N69" s="1" t="s">
@@ -12023,7 +12007,7 @@
         <v>59</v>
       </c>
       <c r="M70" s="1" t="str">
-        <f>IF(ISBLANK(L70),"",VLOOKUP(L70,A:N,14,FALSE))</f>
+        <f t="shared" si="3"/>
         <v>To do</v>
       </c>
       <c r="N70" s="1" t="s">
@@ -12068,7 +12052,7 @@
         <v>64</v>
       </c>
       <c r="M71" s="1" t="str">
-        <f>IF(ISBLANK(L71),"",VLOOKUP(L71,A:N,14,FALSE))</f>
+        <f t="shared" si="3"/>
         <v>To do</v>
       </c>
       <c r="N71" s="1" t="s">
@@ -12113,7 +12097,7 @@
         <v>59</v>
       </c>
       <c r="M72" s="1" t="str">
-        <f>IF(ISBLANK(L72),"",VLOOKUP(L72,A:N,14,FALSE))</f>
+        <f t="shared" si="3"/>
         <v>To do</v>
       </c>
       <c r="N72" s="1" t="s">
@@ -12158,7 +12142,7 @@
         <v>64</v>
       </c>
       <c r="M73" s="1" t="str">
-        <f>IF(ISBLANK(L73),"",VLOOKUP(L73,A:N,14,FALSE))</f>
+        <f t="shared" si="3"/>
         <v>To do</v>
       </c>
       <c r="N73" s="1" t="s">
@@ -12203,7 +12187,7 @@
         <v>59</v>
       </c>
       <c r="M74" s="1" t="str">
-        <f>IF(ISBLANK(L74),"",VLOOKUP(L74,A:N,14,FALSE))</f>
+        <f t="shared" si="3"/>
         <v>To do</v>
       </c>
       <c r="N74" s="1" t="s">
@@ -12248,7 +12232,7 @@
         <v>64</v>
       </c>
       <c r="M75" s="1" t="str">
-        <f>IF(ISBLANK(L75),"",VLOOKUP(L75,A:N,14,FALSE))</f>
+        <f t="shared" si="3"/>
         <v>To do</v>
       </c>
       <c r="N75" s="1" t="s">
@@ -12293,7 +12277,7 @@
         <v>99</v>
       </c>
       <c r="M76" s="1" t="str">
-        <f>IF(ISBLANK(L76),"",VLOOKUP(L76,A:N,14,FALSE))</f>
+        <f t="shared" si="3"/>
         <v>To do</v>
       </c>
       <c r="N76" s="1" t="s">
@@ -12338,7 +12322,7 @@
         <v>100</v>
       </c>
       <c r="M77" s="1" t="str">
-        <f>IF(ISBLANK(L77),"",VLOOKUP(L77,A:N,14,FALSE))</f>
+        <f t="shared" si="3"/>
         <v>To do</v>
       </c>
       <c r="N77" s="1" t="s">
@@ -12383,7 +12367,7 @@
         <v>102</v>
       </c>
       <c r="M78" s="1" t="str">
-        <f>IF(ISBLANK(L78),"",VLOOKUP(L78,A:N,14,FALSE))</f>
+        <f t="shared" si="3"/>
         <v>To do</v>
       </c>
       <c r="N78" s="1" t="s">
@@ -12428,7 +12412,7 @@
         <v>103</v>
       </c>
       <c r="M79" s="1" t="str">
-        <f>IF(ISBLANK(L79),"",VLOOKUP(L79,A:N,14,FALSE))</f>
+        <f t="shared" si="3"/>
         <v>To do</v>
       </c>
       <c r="N79" s="1" t="s">
@@ -12470,7 +12454,7 @@
         <v>13.5</v>
       </c>
       <c r="M80" s="1" t="str">
-        <f>IF(ISBLANK(L80),"",VLOOKUP(L80,A:N,14,FALSE))</f>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="N80" s="1" t="s">
@@ -12512,7 +12496,7 @@
         <v>13.5</v>
       </c>
       <c r="M81" s="1" t="str">
-        <f>IF(ISBLANK(L81),"",VLOOKUP(L81,A:N,14,FALSE))</f>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="N81" s="1" t="s">
@@ -12557,7 +12541,7 @@
         <v>13.5</v>
       </c>
       <c r="M82" s="1" t="str">
-        <f>IF(ISBLANK(L82),"",VLOOKUP(L82,A:N,14,FALSE))</f>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="N82" s="1" t="s">
@@ -12602,7 +12586,7 @@
         <v>13.5</v>
       </c>
       <c r="M83" s="1" t="str">
-        <f>IF(ISBLANK(L83),"",VLOOKUP(L83,A:N,14,FALSE))</f>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="N83" s="1" t="s">
@@ -12644,7 +12628,7 @@
         <v>13.5</v>
       </c>
       <c r="M84" s="1" t="str">
-        <f>IF(ISBLANK(L84),"",VLOOKUP(L84,A:N,14,FALSE))</f>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="N84" s="1" t="s">
@@ -12686,7 +12670,7 @@
         <v>13.5</v>
       </c>
       <c r="M85" s="1" t="str">
-        <f>IF(ISBLANK(L85),"",VLOOKUP(L85,A:N,14,FALSE))</f>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="N85" s="1" t="s">
@@ -12731,7 +12715,7 @@
         <v>12.8</v>
       </c>
       <c r="M86" s="1" t="str">
-        <f>IF(ISBLANK(L86),"",VLOOKUP(L86,A:N,14,FALSE))</f>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="N86" s="1" t="s">
@@ -12776,7 +12760,7 @@
         <v>12.8</v>
       </c>
       <c r="M87" s="1" t="str">
-        <f>IF(ISBLANK(L87),"",VLOOKUP(L87,A:N,14,FALSE))</f>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="N87" s="1" t="s">
@@ -12821,7 +12805,7 @@
         <v>12.8</v>
       </c>
       <c r="M88" s="1" t="str">
-        <f>IF(ISBLANK(L88),"",VLOOKUP(L88,A:N,14,FALSE))</f>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="N88" s="1" t="s">
@@ -12866,7 +12850,7 @@
         <v>12.8</v>
       </c>
       <c r="M89" s="1" t="str">
-        <f>IF(ISBLANK(L89),"",VLOOKUP(L89,A:N,14,FALSE))</f>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="N89" s="1" t="s">
@@ -12908,7 +12892,7 @@
         <v>12.8</v>
       </c>
       <c r="M90" s="1" t="str">
-        <f>IF(ISBLANK(L90),"",VLOOKUP(L90,A:N,14,FALSE))</f>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="N90" s="1" t="s">
@@ -12953,7 +12937,7 @@
         <v>12.5</v>
       </c>
       <c r="M91" s="1" t="str">
-        <f>IF(ISBLANK(L91),"",VLOOKUP(L91,A:N,14,FALSE))</f>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="N91" s="1" t="s">
@@ -12995,7 +12979,7 @@
         <v>12.5</v>
       </c>
       <c r="M92" s="1" t="str">
-        <f>IF(ISBLANK(L92),"",VLOOKUP(L92,A:N,14,FALSE))</f>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="N92" s="1" t="s">
@@ -13037,7 +13021,7 @@
         <v>12.5</v>
       </c>
       <c r="M93" s="1" t="str">
-        <f>IF(ISBLANK(L93),"",VLOOKUP(L93,A:N,14,FALSE))</f>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="N93" s="1" t="s">
@@ -13079,7 +13063,7 @@
         <v>12.5</v>
       </c>
       <c r="M94" s="1" t="str">
-        <f>IF(ISBLANK(L94),"",VLOOKUP(L94,A:N,14,FALSE))</f>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="N94" s="1" t="s">
@@ -13121,7 +13105,7 @@
         <v>12.5</v>
       </c>
       <c r="M95" s="1" t="str">
-        <f>IF(ISBLANK(L95),"",VLOOKUP(L95,A:N,14,FALSE))</f>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="N95" s="1" t="s">
@@ -13163,7 +13147,7 @@
         <v>12.5</v>
       </c>
       <c r="M96" s="1" t="str">
-        <f>IF(ISBLANK(L96),"",VLOOKUP(L96,A:N,14,FALSE))</f>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="N96" s="1" t="s">
@@ -13205,7 +13189,7 @@
         <v>10</v>
       </c>
       <c r="M97" s="1" t="str">
-        <f>IF(ISBLANK(L97),"",VLOOKUP(L97,A:N,14,FALSE))</f>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="N97" s="1" t="s">
@@ -13244,7 +13228,7 @@
         <v>10</v>
       </c>
       <c r="M98" s="1" t="str">
-        <f>IF(ISBLANK(L98),"",VLOOKUP(L98,A:N,14,FALSE))</f>
+        <f t="shared" ref="M98:M129" si="4">IF(ISBLANK(L98),"",VLOOKUP(L98,A:N,14,FALSE))</f>
         <v/>
       </c>
       <c r="N98" s="1" t="s">
@@ -13283,7 +13267,7 @@
         <v>10</v>
       </c>
       <c r="M99" s="1" t="str">
-        <f>IF(ISBLANK(L99),"",VLOOKUP(L99,A:N,14,FALSE))</f>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="N99" s="1" t="s">
@@ -13325,7 +13309,7 @@
         <v>10</v>
       </c>
       <c r="M100" s="1" t="str">
-        <f>IF(ISBLANK(L100),"",VLOOKUP(L100,A:N,14,FALSE))</f>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="N100" s="1" t="s">
@@ -13367,7 +13351,7 @@
         <v>10</v>
       </c>
       <c r="M101" s="1" t="str">
-        <f>IF(ISBLANK(L101),"",VLOOKUP(L101,A:N,14,FALSE))</f>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="N101" s="1" t="s">
@@ -13412,7 +13396,7 @@
         <v>9.8000000000000007</v>
       </c>
       <c r="M102" s="1" t="str">
-        <f>IF(ISBLANK(L102),"",VLOOKUP(L102,A:N,14,FALSE))</f>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="N102" s="1" t="s">
@@ -13454,7 +13438,7 @@
         <v>9</v>
       </c>
       <c r="M103" s="1" t="str">
-        <f>IF(ISBLANK(L103),"",VLOOKUP(L103,A:N,14,FALSE))</f>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="N103" s="1" t="s">
@@ -13496,7 +13480,7 @@
         <v>9</v>
       </c>
       <c r="M104" s="1" t="str">
-        <f>IF(ISBLANK(L104),"",VLOOKUP(L104,A:N,14,FALSE))</f>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="N104" s="1" t="s">
@@ -13538,7 +13522,7 @@
         <v>9</v>
       </c>
       <c r="M105" s="1" t="str">
-        <f>IF(ISBLANK(L105),"",VLOOKUP(L105,A:N,14,FALSE))</f>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="N105" s="1" t="s">
@@ -13580,7 +13564,7 @@
         <v>9</v>
       </c>
       <c r="M106" s="1" t="str">
-        <f>IF(ISBLANK(L106),"",VLOOKUP(L106,A:N,14,FALSE))</f>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="N106" s="1" t="s">
@@ -13622,7 +13606,7 @@
         <v>9</v>
       </c>
       <c r="M107" s="1" t="str">
-        <f>IF(ISBLANK(L107),"",VLOOKUP(L107,A:N,14,FALSE))</f>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="N107" s="1" t="s">
@@ -13664,7 +13648,7 @@
         <v>9</v>
       </c>
       <c r="M108" s="1" t="str">
-        <f>IF(ISBLANK(L108),"",VLOOKUP(L108,A:N,14,FALSE))</f>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="N108" s="1" t="s">
@@ -13706,7 +13690,7 @@
         <v>9</v>
       </c>
       <c r="M109" s="1" t="str">
-        <f>IF(ISBLANK(L109),"",VLOOKUP(L109,A:N,14,FALSE))</f>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="N109" s="1" t="s">
@@ -13751,7 +13735,7 @@
         <v>9</v>
       </c>
       <c r="M110" s="1" t="str">
-        <f>IF(ISBLANK(L110),"",VLOOKUP(L110,A:N,14,FALSE))</f>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="N110" s="1" t="s">
@@ -13793,7 +13777,7 @@
         <v>9</v>
       </c>
       <c r="M111" s="1" t="str">
-        <f>IF(ISBLANK(L111),"",VLOOKUP(L111,A:N,14,FALSE))</f>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="N111" s="1" t="s">
@@ -13832,7 +13816,7 @@
         <v>9</v>
       </c>
       <c r="M112" s="1" t="str">
-        <f>IF(ISBLANK(L112),"",VLOOKUP(L112,A:N,14,FALSE))</f>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="N112" s="1" t="s">
@@ -13874,7 +13858,7 @@
         <v>7</v>
       </c>
       <c r="M113" s="1" t="str">
-        <f>IF(ISBLANK(L113),"",VLOOKUP(L113,A:N,14,FALSE))</f>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="N113" s="1" t="s">
@@ -13916,7 +13900,7 @@
         <v>6.75</v>
       </c>
       <c r="M114" s="1" t="str">
-        <f>IF(ISBLANK(L114),"",VLOOKUP(L114,A:N,14,FALSE))</f>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="N114" s="1" t="s">
@@ -13958,7 +13942,7 @@
         <v>2</v>
       </c>
       <c r="M115" s="1" t="str">
-        <f>IF(ISBLANK(L115),"",VLOOKUP(L115,A:N,14,FALSE))</f>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="N115" s="1" t="s">
@@ -14003,7 +13987,7 @@
         <v>27</v>
       </c>
       <c r="M116" s="1" t="str">
-        <f>IF(ISBLANK(L116),"",VLOOKUP(L116,A:N,14,FALSE))</f>
+        <f t="shared" si="4"/>
         <v>To do</v>
       </c>
       <c r="N116" s="1" t="s">
@@ -14045,7 +14029,7 @@
         <v>27</v>
       </c>
       <c r="M117" s="1" t="str">
-        <f>IF(ISBLANK(L117),"",VLOOKUP(L117,A:N,14,FALSE))</f>
+        <f t="shared" si="4"/>
         <v>To do</v>
       </c>
       <c r="N117" s="1" t="s">
@@ -14089,7 +14073,7 @@
       </c>
       <c r="L118"/>
       <c r="M118" s="1" t="str">
-        <f>IF(ISBLANK(L118),"",VLOOKUP(L118,A:N,14,FALSE))</f>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="N118" s="1" t="s">

</xml_diff>

<commit_message>
SigmaFox/modals/client-details: Extracted to lib with e-Questrian's own modal user as an example
</commit_message>
<xml_diff>
--- a/apps/e-questrian/e-Questrian - To do list.xlsx
+++ b/apps/e-questrian/e-Questrian - To do list.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rferreira/sigmafox/apps/e-questrian/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7DED31E2-BBD4-1F44-BBD3-2D88DB278BB3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3B0B11F-01E9-B545-8FB9-2810945C91A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="19820" activeTab="2" xr2:uid="{DC2B379E-A936-2146-8C4F-53C43AECE05C}"/>
   </bookViews>
@@ -22,7 +22,7 @@
   </definedNames>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="13" r:id="rId4"/>
+    <pivotCache cacheId="22" r:id="rId4"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -821,7 +821,7 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Ruben Ferreira" refreshedDate="45321.408745949077" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="118" xr:uid="{AEB2BF63-68F2-404E-AE9B-E794DFB00774}">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Ruben Ferreira" refreshedDate="45321.640190162034" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="118" xr:uid="{AEB2BF63-68F2-404E-AE9B-E794DFB00774}">
   <cacheSource type="worksheet">
     <worksheetSource ref="A1:N1048576" sheet="Issues 3-1-24"/>
   </cacheSource>
@@ -1458,7 +1458,7 @@
     <n v="32"/>
     <m/>
     <s v=""/>
-    <x v="1"/>
+    <x v="0"/>
   </r>
   <r>
     <n v="67"/>
@@ -1474,7 +1474,7 @@
     <n v="32"/>
     <m/>
     <s v=""/>
-    <x v="1"/>
+    <x v="0"/>
   </r>
   <r>
     <n v="84"/>
@@ -2776,7 +2776,69 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{936C0618-B7B4-0144-93D9-409C5361BBD7}" name="PivotTable7" cacheId="13" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{4DCC3165-0959-AA43-80CF-D9170B1DCB64}" name="PivotTable8" cacheId="22" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="A13:E15" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
+  <pivotFields count="14">
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField dataField="1" showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField axis="axisCol" showAll="0" sortType="ascending">
+      <items count="5">
+        <item x="0"/>
+        <item x="2"/>
+        <item x="1"/>
+        <item h="1" x="3"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+  </pivotFields>
+  <rowItems count="1">
+    <i/>
+  </rowItems>
+  <colFields count="1">
+    <field x="13"/>
+  </colFields>
+  <colItems count="4">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </colItems>
+  <dataFields count="1">
+    <dataField name="Sum of Impact S" fld="9" baseField="0" baseItem="0"/>
+  </dataFields>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{936C0618-B7B4-0144-93D9-409C5361BBD7}" name="PivotTable7" cacheId="22" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A7:E9" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="14">
     <pivotField showAll="0"/>
@@ -2837,8 +2899,8 @@
 </pivotTableDefinition>
 </file>
 
-<file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{4A183E6E-2837-3A40-90CB-E731BF47E9C0}" name="PivotTable6" cacheId="13" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{4A183E6E-2837-3A40-90CB-E731BF47E9C0}" name="PivotTable6" cacheId="22" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A1:E3" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="14">
     <pivotField showAll="0"/>
@@ -2886,68 +2948,6 @@
   </colItems>
   <dataFields count="1">
     <dataField name="Sum of Priority S" fld="10" baseField="0" baseItem="0"/>
-  </dataFields>
-  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
-    </ext>
-    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
-      <xpdl:pivotTableDefinition16/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
-</file>
-
-<file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{4DCC3165-0959-AA43-80CF-D9170B1DCB64}" name="PivotTable8" cacheId="13" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
-  <location ref="A13:E15" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
-  <pivotFields count="14">
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField dataField="1" showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField axis="axisCol" showAll="0" sortType="ascending">
-      <items count="5">
-        <item x="0"/>
-        <item x="2"/>
-        <item x="1"/>
-        <item h="1" x="3"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-  </pivotFields>
-  <rowItems count="1">
-    <i/>
-  </rowItems>
-  <colFields count="1">
-    <field x="13"/>
-  </colFields>
-  <colItems count="4">
-    <i>
-      <x/>
-    </i>
-    <i>
-      <x v="1"/>
-    </i>
-    <i>
-      <x v="2"/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
-  </colItems>
-  <dataFields count="1">
-    <dataField name="Sum of Impact S" fld="9" baseField="0" baseItem="0"/>
   </dataFields>
   <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
   <extLst>
@@ -3261,16 +3261,26 @@
   <dimension ref="A1:E17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="D2" sqref="D2:D3"/>
+      <pivotSelection pane="bottomRight" showHeader="1" extendable="1" start="2" max="4" activeRow="1" activeCol="3" click="1" r:id="rId3">
+        <pivotArea dataOnly="0" outline="0" fieldPosition="0">
+          <references count="1">
+            <reference field="13" count="1">
+              <x v="2"/>
+            </reference>
+          </references>
+        </pivotArea>
+      </pivotSelection>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="15.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="4.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="5.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="10.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
@@ -3299,13 +3309,13 @@
         <v>203</v>
       </c>
       <c r="B3" s="8">
-        <v>1671.4000000000003</v>
+        <v>1735.4000000000003</v>
       </c>
       <c r="C3" s="8">
         <v>103.2</v>
       </c>
       <c r="D3" s="8">
-        <v>1452.9976190476191</v>
+        <v>1388.9976190476193</v>
       </c>
       <c r="E3" s="8">
         <v>3227.5976190476194</v>
@@ -3314,7 +3324,7 @@
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="E5" s="7">
         <f>SUM(B3:C3)/GETPIVOTDATA("Priority S",$A$1)</f>
-        <v>0.54982070550778228</v>
+        <v>0.56964969522518227</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
@@ -3343,13 +3353,13 @@
         <v>180</v>
       </c>
       <c r="B9" s="8">
-        <v>157</v>
+        <v>165</v>
       </c>
       <c r="C9" s="8">
         <v>12</v>
       </c>
       <c r="D9" s="8">
-        <v>203</v>
+        <v>195</v>
       </c>
       <c r="E9" s="8">
         <v>372</v>
@@ -3358,7 +3368,7 @@
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="E11" s="7">
         <f>SUM(B9:C9)/GETPIVOTDATA("Importance S",$A$7)</f>
-        <v>0.45430107526881719</v>
+        <v>0.47580645161290325</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
@@ -3387,13 +3397,13 @@
         <v>181</v>
       </c>
       <c r="B15" s="8">
-        <v>161</v>
+        <v>169</v>
       </c>
       <c r="C15" s="8">
         <v>15</v>
       </c>
       <c r="D15" s="8">
-        <v>504</v>
+        <v>496</v>
       </c>
       <c r="E15" s="8">
         <v>680</v>
@@ -3402,7 +3412,7 @@
     <row r="17" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E17" s="7">
         <f>SUM(B15:C15)/GETPIVOTDATA("Impact S",$A$13)</f>
-        <v>0.25882352941176473</v>
+        <v>0.27058823529411763</v>
       </c>
     </row>
   </sheetData>
@@ -3841,7 +3851,7 @@
   <dimension ref="A1:XEY118"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="E37" sqref="E37"/>
+      <selection activeCell="O38" sqref="O38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="34.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -10541,79 +10551,79 @@
         <v>174</v>
       </c>
     </row>
-    <row r="37" spans="1:14" ht="68" x14ac:dyDescent="0.2">
-      <c r="A37">
+    <row r="37" spans="1:14" s="3" customFormat="1" ht="68" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A37" s="3">
         <v>58</v>
       </c>
-      <c r="B37" t="s">
+      <c r="B37" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C37" t="s">
+      <c r="C37" s="3" t="s">
         <v>104</v>
       </c>
-      <c r="E37" s="2" t="s">
+      <c r="E37" s="4" t="s">
         <v>106</v>
       </c>
-      <c r="F37" t="s">
+      <c r="F37" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="G37" t="s">
+      <c r="G37" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="H37" t="s">
+      <c r="H37" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="I37" s="1">
+      <c r="I37" s="5">
         <f>VLOOKUP(F37,'Source lists'!$E$1:F38,2,FALSE)</f>
         <v>4</v>
       </c>
-      <c r="J37" s="1">
+      <c r="J37" s="5">
         <f>VLOOKUP(G37,'Source lists'!$H$1:I39,2,FALSE)</f>
         <v>4</v>
       </c>
-      <c r="K37" s="1">
+      <c r="K37" s="5">
         <f>VLOOKUP(F37,'Source lists'!$E$2:$F$6,2,FALSE)*(VLOOKUP(G37,'Source lists'!$H$2:$I$7,2,FALSE)^2)/VLOOKUP(H37,'Source lists'!$K$2:$L$9,2,FALSE)</f>
         <v>32</v>
       </c>
-      <c r="M37" s="1" t="str">
+      <c r="M37" s="5" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="N37" s="1" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="38" spans="1:14" ht="68" x14ac:dyDescent="0.2">
-      <c r="A38">
+      <c r="N37" s="5" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="38" spans="1:14" s="3" customFormat="1" ht="17" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A38" s="3">
         <v>67</v>
       </c>
-      <c r="B38" t="s">
+      <c r="B38" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C38" t="s">
+      <c r="C38" s="3" t="s">
         <v>104</v>
       </c>
-      <c r="E38" s="2" t="s">
+      <c r="E38" s="4" t="s">
         <v>128</v>
       </c>
-      <c r="F38" t="s">
+      <c r="F38" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="G38" t="s">
+      <c r="G38" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="H38" t="s">
+      <c r="H38" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="I38" s="1">
+      <c r="I38" s="5">
         <f>VLOOKUP(F38,'Source lists'!$E$1:F39,2,FALSE)</f>
         <v>4</v>
       </c>
-      <c r="J38" s="1">
+      <c r="J38" s="5">
         <f>VLOOKUP(G38,'Source lists'!$H$1:I40,2,FALSE)</f>
         <v>4</v>
       </c>
-      <c r="K38" s="1">
+      <c r="K38" s="5">
         <f>VLOOKUP(F38,'Source lists'!$E$2:$F$6,2,FALSE)*(VLOOKUP(G38,'Source lists'!$H$2:$I$7,2,FALSE)^2)/VLOOKUP(H38,'Source lists'!$K$2:$L$9,2,FALSE)</f>
         <v>32</v>
       </c>
@@ -10621,11 +10631,11 @@
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="N38" s="1" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="39" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+      <c r="N38" s="5" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="39" spans="1:14" ht="34" x14ac:dyDescent="0.2">
       <c r="A39">
         <v>84</v>
       </c>
@@ -13228,7 +13238,7 @@
         <v>10</v>
       </c>
       <c r="M98" s="1" t="str">
-        <f t="shared" ref="M98:M129" si="4">IF(ISBLANK(L98),"",VLOOKUP(L98,A:N,14,FALSE))</f>
+        <f t="shared" ref="M98:M118" si="4">IF(ISBLANK(L98),"",VLOOKUP(L98,A:N,14,FALSE))</f>
         <v/>
       </c>
       <c r="N98" s="1" t="s">

</xml_diff>